<commit_message>
Updated guidance text in trans/BHNVFEAL to remove outdated information
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipM\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,12 +41,12 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="94">
   <si>
     <t>Sources:</t>
   </si>
@@ -289,18 +289,6 @@
   </si>
   <si>
     <t>Tables 35, 49, 55</t>
-  </si>
-  <si>
-    <t>https://greet.es.anl.gov/files/heavy-duty</t>
-  </si>
-  <si>
-    <t>Argonne National Laboratory</t>
-  </si>
-  <si>
-    <t>The GREET Model Expansion for Well-to-Wheels Analysis of Heavy-Duty Vehicles</t>
-  </si>
-  <si>
-    <t>Table 6</t>
   </si>
   <si>
     <t>Hydrogen vs. Gasoline Efficiency</t>
@@ -1231,7 +1219,7 @@
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1269,6 +1257,9 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="153"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="154">
@@ -5469,6 +5460,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6005,6 +5997,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7763,9 +7756,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7828,199 +7823,165 @@
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="25" t="s">
-        <v>8</v>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" s="5">
-        <v>2015</v>
+      <c r="B14" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="5" t="s">
-        <v>83</v>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="B17" s="5" t="s">
-        <v>81</v>
+      <c r="B17" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="B18" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="B19" s="5"/>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="B20" s="2" t="s">
-        <v>9</v>
+      <c r="B20" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="B21" s="7" t="s">
-        <v>96</v>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" s="7" t="s">
-        <v>12</v>
+      <c r="B23" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="B25" s="5"/>
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="B26" s="2" t="s">
-        <v>32</v>
+      <c r="A26" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="B27" s="7" t="s">
-        <v>20</v>
+      <c r="A27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="B28" s="7"/>
+      <c r="A28" s="20"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="B29" s="2" t="s">
-        <v>93</v>
+      <c r="A29" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="B30" s="7" t="s">
-        <v>92</v>
+      <c r="A30" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>1</v>
+      <c r="A32" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>34</v>
+      <c r="A33" s="20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="20"/>
+      <c r="A34" s="20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="20" t="s">
-        <v>36</v>
+      <c r="A36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="20" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="20" t="s">
-        <v>39</v>
+      <c r="A39" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="20" t="s">
-        <v>40</v>
+      <c r="A40" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="20" t="s">
-        <v>41</v>
+      <c r="A41" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>48</v>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="20" t="s">
-        <v>49</v>
+      <c r="A44" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="20" t="s">
-        <v>42</v>
+      <c r="A45" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8040,7 +8001,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -8750,7 +8711,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -8857,7 +8818,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -9017,7 +8978,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -9727,7 +9688,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9834,7 +9795,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -9994,7 +9955,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -10704,7 +10665,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -10811,7 +10772,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -10971,7 +10932,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -11681,7 +11642,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -11788,7 +11749,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -11948,7 +11909,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -12658,7 +12619,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -12765,7 +12726,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -12925,7 +12886,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -13635,7 +13596,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -13742,7 +13703,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
@@ -13902,7 +13863,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -14714,7 +14675,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <f>B$4*Calculations!$B$31</f>
@@ -14855,7 +14816,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
@@ -15015,7 +14976,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -15657,7 +15618,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -15764,7 +15725,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -17545,7 +17506,7 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17684,7 +17645,7 @@
       <c r="A14" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="30" t="s">
         <v>68</v>
       </c>
     </row>
@@ -17756,7 +17717,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" s="3"/>
       <c r="D24" s="2" t="s">
@@ -17765,18 +17726,18 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B25" s="26">
         <v>0.2</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B26" s="26">
         <v>0.5</v>
@@ -17785,7 +17746,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B27" s="8">
         <f>B26/B25</f>
@@ -17794,7 +17755,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B29" s="2"/>
       <c r="D29" s="2" t="s">
@@ -17803,18 +17764,18 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B30" s="27">
         <v>0.22500000000000001</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B31" s="8">
         <f>1-B30</f>
@@ -17833,11 +17794,11 @@
   <dimension ref="A1:BT14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C13" sqref="C13"/>
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
-      <selection pane="bottomRight" activeCell="W5" sqref="W5:AJ5"/>
+      <selection pane="bottomRight" activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21127,7 +21088,9 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -21136,7 +21099,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -21948,7 +21911,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <f>B$4*Calculations!$B$31</f>
@@ -22089,7 +22052,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
@@ -22249,7 +22212,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -23061,7 +23024,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <f>B$4*Calculations!$B$31</f>
@@ -23202,7 +23165,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
@@ -23353,7 +23316,9 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -23362,7 +23327,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -24174,7 +24139,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <f>B$4*Calculations!$B$31</f>
@@ -24315,7 +24280,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
@@ -24475,7 +24440,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -25287,7 +25252,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <f>B$4*Calculations!$B$31</f>
@@ -25428,7 +25393,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>

</xml_diff>

<commit_message>
Update transportation files for updated DOE hydrogen fuel cell research and correct start year in SYFAFE, SYVbT, and BAADTbVT
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\Model\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B4CFF3-7E7E-4173-83D4-9D12544D8158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6877" yWindow="187" windowWidth="12091" windowHeight="10141" firstSheet="16" activeTab="16" xr2:uid="{993692F4-C124-4710-B3D7-C2F6E29BEAF3}"/>
-    <workbookView xWindow="15" yWindow="60" windowWidth="12090" windowHeight="10140" firstSheet="4" activeTab="4" xr2:uid="{CB93BD1B-E6A1-4A15-B101-279FF1129CB1}"/>
+    <workbookView xWindow="6878" yWindow="188" windowWidth="12090" windowHeight="10140"/>
+    <workbookView xWindow="15" yWindow="60" windowWidth="12090" windowHeight="10140" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -43,7 +42,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -345,7 +344,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1288,160 +1287,160 @@
     </xf>
   </cellXfs>
   <cellStyles count="154">
-    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="8"/>
+    <cellStyle name="20% - Accent2 2" xfId="9"/>
+    <cellStyle name="20% - Accent3 2" xfId="10"/>
+    <cellStyle name="20% - Accent4 2" xfId="11"/>
+    <cellStyle name="20% - Accent5 2" xfId="12"/>
+    <cellStyle name="20% - Accent6 2" xfId="13"/>
+    <cellStyle name="40% - Accent1 2" xfId="14"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent3 2" xfId="16"/>
+    <cellStyle name="40% - Accent4 2" xfId="17"/>
+    <cellStyle name="40% - Accent5 2" xfId="18"/>
+    <cellStyle name="40% - Accent6 2" xfId="19"/>
+    <cellStyle name="60% - Accent1 2" xfId="20"/>
+    <cellStyle name="60% - Accent2 2" xfId="21"/>
+    <cellStyle name="60% - Accent3 2" xfId="22"/>
+    <cellStyle name="60% - Accent4 2" xfId="23"/>
+    <cellStyle name="60% - Accent5 2" xfId="24"/>
+    <cellStyle name="60% - Accent6 2" xfId="25"/>
+    <cellStyle name="Accent1 2" xfId="26"/>
+    <cellStyle name="Accent2 2" xfId="27"/>
+    <cellStyle name="Accent3 2" xfId="28"/>
+    <cellStyle name="Accent4 2" xfId="29"/>
+    <cellStyle name="Accent5 2" xfId="30"/>
+    <cellStyle name="Accent6 2" xfId="31"/>
+    <cellStyle name="Bad 2" xfId="32"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Body: normal cell 2" xfId="33"/>
+    <cellStyle name="Calculation 2" xfId="34"/>
+    <cellStyle name="Check Cell 2" xfId="35"/>
+    <cellStyle name="Column heading" xfId="36"/>
+    <cellStyle name="Comma 2" xfId="37"/>
+    <cellStyle name="Comma 2 2" xfId="38"/>
+    <cellStyle name="Comma 3" xfId="39"/>
+    <cellStyle name="Comma 4" xfId="40"/>
+    <cellStyle name="Comma 5" xfId="41"/>
+    <cellStyle name="Comma 6" xfId="42"/>
+    <cellStyle name="Comma 7" xfId="43"/>
+    <cellStyle name="Comma 8" xfId="44"/>
+    <cellStyle name="Corner heading" xfId="45"/>
+    <cellStyle name="Currency 2" xfId="46"/>
+    <cellStyle name="Currency 3" xfId="47"/>
+    <cellStyle name="Currency 3 2" xfId="48"/>
+    <cellStyle name="Data" xfId="49"/>
+    <cellStyle name="Data 2" xfId="50"/>
+    <cellStyle name="Data no deci" xfId="51"/>
+    <cellStyle name="Data Superscript" xfId="52"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
+    <cellStyle name="Explanatory Text 2" xfId="54"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56"/>
+    <cellStyle name="Good 2" xfId="57"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
+    <cellStyle name="Heading 1 2" xfId="59"/>
+    <cellStyle name="Heading 2 2" xfId="60"/>
+    <cellStyle name="Heading 3 2" xfId="61"/>
+    <cellStyle name="Heading 4 2" xfId="62"/>
+    <cellStyle name="Hed Side" xfId="63"/>
+    <cellStyle name="Hed Side 2" xfId="64"/>
+    <cellStyle name="Hed Side bold" xfId="65"/>
+    <cellStyle name="Hed Side Indent" xfId="66"/>
+    <cellStyle name="Hed Side Regular" xfId="67"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
+    <cellStyle name="Hed Top" xfId="69"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72"/>
+    <cellStyle name="Input 2" xfId="73"/>
+    <cellStyle name="Linked Cell 2" xfId="74"/>
+    <cellStyle name="Neutral 2" xfId="75"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 10" xfId="76"/>
+    <cellStyle name="Normal 11" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="78"/>
+    <cellStyle name="Normal 2 3" xfId="79"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Normal 3 2" xfId="81"/>
+    <cellStyle name="Normal 3 2 2" xfId="82"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="84"/>
+    <cellStyle name="Normal 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 3 2" xfId="86"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
+    <cellStyle name="Normal 3 3 3" xfId="88"/>
+    <cellStyle name="Normal 3 4" xfId="89"/>
+    <cellStyle name="Normal 3 4 2" xfId="90"/>
+    <cellStyle name="Normal 3 5" xfId="91"/>
+    <cellStyle name="Normal 3 6" xfId="92"/>
+    <cellStyle name="Normal 3 7" xfId="93"/>
+    <cellStyle name="Normal 4" xfId="94"/>
+    <cellStyle name="Normal 4 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 2" xfId="96"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 4 2 3" xfId="98"/>
+    <cellStyle name="Normal 4 3" xfId="99"/>
+    <cellStyle name="Normal 4 3 2" xfId="100"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
+    <cellStyle name="Normal 4 3 3" xfId="102"/>
+    <cellStyle name="Normal 4 4" xfId="103"/>
+    <cellStyle name="Normal 4 4 2" xfId="104"/>
+    <cellStyle name="Normal 4 5" xfId="105"/>
+    <cellStyle name="Normal 4 6" xfId="106"/>
+    <cellStyle name="Normal 4 7" xfId="107"/>
+    <cellStyle name="Normal 5" xfId="108"/>
+    <cellStyle name="Normal 5 2" xfId="109"/>
+    <cellStyle name="Normal 5 3" xfId="110"/>
+    <cellStyle name="Normal 6" xfId="111"/>
+    <cellStyle name="Normal 6 2" xfId="112"/>
+    <cellStyle name="Normal 7" xfId="113"/>
+    <cellStyle name="Normal 7 2" xfId="114"/>
+    <cellStyle name="Normal 8" xfId="115"/>
+    <cellStyle name="Normal 9" xfId="116"/>
+    <cellStyle name="Note 2" xfId="117"/>
+    <cellStyle name="Note 2 2" xfId="118"/>
+    <cellStyle name="Output 2" xfId="119"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Parent row 2" xfId="120"/>
+    <cellStyle name="Percent 2" xfId="121"/>
+    <cellStyle name="Percent 2 2" xfId="122"/>
+    <cellStyle name="Percent 3" xfId="123"/>
+    <cellStyle name="Percent 3 2" xfId="124"/>
+    <cellStyle name="Percent 4" xfId="125"/>
+    <cellStyle name="Reference" xfId="126"/>
+    <cellStyle name="Row heading" xfId="127"/>
+    <cellStyle name="Source Hed" xfId="128"/>
+    <cellStyle name="Source Letter" xfId="129"/>
+    <cellStyle name="Source Superscript" xfId="130"/>
+    <cellStyle name="Source Superscript 2" xfId="131"/>
+    <cellStyle name="Source Text" xfId="132"/>
+    <cellStyle name="Source Text 2" xfId="133"/>
+    <cellStyle name="State" xfId="134"/>
+    <cellStyle name="Superscript" xfId="135"/>
+    <cellStyle name="Table Data" xfId="136"/>
+    <cellStyle name="Table Head Top" xfId="137"/>
+    <cellStyle name="Table Hed Side" xfId="138"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Table title 2" xfId="139"/>
+    <cellStyle name="Title 2" xfId="140"/>
+    <cellStyle name="Title Text" xfId="141"/>
+    <cellStyle name="Title Text 1" xfId="142"/>
+    <cellStyle name="Title Text 2" xfId="143"/>
+    <cellStyle name="Title-1" xfId="144"/>
+    <cellStyle name="Title-2" xfId="145"/>
+    <cellStyle name="Title-3" xfId="146"/>
+    <cellStyle name="Total 2" xfId="147"/>
+    <cellStyle name="Warning Text 2" xfId="148"/>
+    <cellStyle name="Wrap" xfId="149"/>
+    <cellStyle name="Wrap Bold" xfId="150"/>
+    <cellStyle name="Wrap Title" xfId="151"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2463,6 +2462,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4430,6 +4430,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5428,6 +5429,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5676,202 +5678,202 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>8.070242239185747E-4</c:v>
+                  <c:v>8.122417554319157E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>8.0702422391857502E-4</c:v>
+                  <c:v>8.1224175543191505E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5922,7 +5924,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6451,7 +6453,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6487,6 +6489,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7556,23 +7559,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7608,23 +7594,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7800,10 +7769,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8022,7 +7993,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -8030,7 +8001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8827,131 +8798,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.0285041882251815E-3</v>
+        <v>1.2342050258702176E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.0354928896036072E-3</v>
+        <v>1.2425914675243284E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.0424815909820307E-3</v>
+        <v>1.2509779091784367E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.0494702923604564E-3</v>
+        <v>1.2593643508325475E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.0564589937388821E-3</v>
+        <v>1.2677507924866583E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.0634476951173056E-3</v>
+        <v>1.2761372341407666E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.0704363964957313E-3</v>
+        <v>1.2845236757948774E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.077425097874157E-3</v>
+        <v>1.2929101174489882E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.0844137992525827E-3</v>
+        <v>1.3012965591030991E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.0914025006310063E-3</v>
+        <v>1.3096830007572073E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.098391202009432E-3</v>
+        <v>1.3180694424113181E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.1053799033878577E-3</v>
+        <v>1.326455884065429E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.1123686047662812E-3</v>
+        <v>1.3348423257195372E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.1193573061447069E-3</v>
+        <v>1.343228767373648E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.1263460075231326E-3</v>
+        <v>1.3516152090277589E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.1333347089015561E-3</v>
+        <v>1.3600016506818671E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.1403234102799818E-3</v>
+        <v>1.368388092335978E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.1473121116584075E-3</v>
+        <v>1.3767745339900888E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.1543008130368332E-3</v>
+        <v>1.3851609756441996E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.1612895144152567E-3</v>
+        <v>1.3935474172983079E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.1682782157936824E-3</v>
+        <v>1.4019338589524187E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.1752669171721081E-3</v>
+        <v>1.4103203006065295E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.1822556185505317E-3</v>
+        <v>1.4187067422606378E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.1892443199289573E-3</v>
+        <v>1.4270931839147486E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>1.1901477808755785E-3</v>
+        <v>1.4281773370506941E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>1.1870043305566933E-3</v>
+        <v>1.4244051966680318E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.1959708032095119E-3</v>
+        <v>1.4351649638514141E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.2045165698477225E-3</v>
+        <v>1.4454198838172666E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.2133796453626963E-3</v>
+        <v>1.4560555744352354E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.222169687266617E-3</v>
+        <v>1.4666036247199402E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>1.2213828021307559E-3</v>
+        <v>1.465659362556907E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>1.2375089436638476E-3</v>
+        <v>1.485010732396617E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -8962,7 +8933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9759,131 +9730,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>2.2999517457206547E-4</v>
+        <v>2.7599420948647851E-4</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>2.3362740840636868E-4</v>
+        <v>2.8035289008764236E-4</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>2.3725964224067297E-4</v>
+        <v>2.8471157068880751E-4</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>2.4089187607497618E-4</v>
+        <v>2.8907025128997136E-4</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>2.4452410990928044E-4</v>
+        <v>2.9342893189113651E-4</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>2.4815634374358365E-4</v>
+        <v>2.9778761249230035E-4</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>2.5178857757788794E-4</v>
+        <v>3.021462930934655E-4</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>2.5542081141219114E-4</v>
+        <v>3.0650497369462935E-4</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>2.5905304524649544E-4</v>
+        <v>3.108636542957945E-4</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>2.6268527908079973E-4</v>
+        <v>3.1522233489695965E-4</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>2.6631751291510293E-4</v>
+        <v>3.195810154981235E-4</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>2.6994974674940722E-4</v>
+        <v>3.2393969609928865E-4</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>2.7358198058371043E-4</v>
+        <v>3.2829837670045249E-4</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>2.7721421441801472E-4</v>
+        <v>3.3265705730161764E-4</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>2.8084644825231793E-4</v>
+        <v>3.3701573790278149E-4</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>2.8447868208662222E-4</v>
+        <v>3.4137441850394664E-4</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>2.8811091592092543E-4</v>
+        <v>3.4573309910511049E-4</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>2.9174314975522972E-4</v>
+        <v>3.5009177970627564E-4</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>2.9537538358953401E-4</v>
+        <v>3.5445046030744079E-4</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>2.9900761742383721E-4</v>
+        <v>3.5880914090860464E-4</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>3.0263985125814151E-4</v>
+        <v>3.6316782150976978E-4</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>3.0627208509244471E-4</v>
+        <v>3.6752650211093363E-4</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>3.09904318926749E-4</v>
+        <v>3.7188518271209878E-4</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>3.1353655276105221E-4</v>
+        <v>3.7624386331326263E-4</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>3.0642860374827563E-4</v>
+        <v>3.6771432449793069E-4</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>3.1658202558688671E-4</v>
+        <v>3.7989843070426396E-4</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>3.2179980486067838E-4</v>
+        <v>3.8615976583281395E-4</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>3.3214901378975228E-4</v>
+        <v>3.9857881654770268E-4</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>3.4338648240875627E-4</v>
+        <v>4.1206377889050743E-4</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>3.56356040256355E-4</v>
+        <v>4.276272483076259E-4</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>3.642052905081176E-4</v>
+        <v>4.3704634860974103E-4</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>3.7982782509152056E-4</v>
+        <v>4.5579339010982462E-4</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -9894,7 +9865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10017,131 +9988,131 @@
       </c>
       <c r="B2" s="4">
         <f>B$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="C2" s="4">
         <f>C$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="D2" s="4">
         <f>D$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="E2" s="4">
         <f>E$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="F2" s="4">
         <f>F$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="G2" s="4">
         <f>G$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="H2" s="4">
         <f>H$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="I2" s="4">
         <f>I$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="J2" s="4">
         <f>J$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="K2" s="4">
         <f>K$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="L2" s="4">
         <f>L$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="M2" s="4">
         <f>M$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="N2" s="4">
         <f>N$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="O2" s="4">
         <f>O$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="P2" s="4">
         <f>P$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="Q2" s="4">
         <f>Q$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="R2" s="4">
         <f>R$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="S2" s="4">
         <f>S$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="T2" s="4">
         <f>T$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="U2" s="4">
         <f>U$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="V2" s="4">
         <f>V$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="W2" s="4">
         <f>W$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="X2" s="4">
         <f>X$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="Y2" s="4">
         <f>Y$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="Z2" s="4">
         <f>Z$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AA2" s="4">
         <f>AA$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AB2" s="4">
         <f>AB$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AC2" s="4">
         <f>AC$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AD2" s="4">
         <f>AD$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AE2" s="4">
         <f>AE$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AF2" s="4">
         <f>AF$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AG2" s="4">
         <f>AG$5/(1-'Other Values'!$B$3)</f>
-        <v>2.5933518777701359E-3</v>
+        <v>2.6101182829738698E-3</v>
       </c>
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
@@ -10354,131 +10325,131 @@
       </c>
       <c r="B5" s="4">
         <f>Extrapolations!E8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="C5" s="4">
         <f>Extrapolations!F8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="D5" s="4">
         <f>Extrapolations!G8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="E5" s="4">
         <f>Extrapolations!H8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="F5" s="4">
         <f>Extrapolations!I8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="G5" s="4">
         <f>Extrapolations!J8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="H5" s="4">
         <f>Extrapolations!K8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="I5" s="4">
         <f>Extrapolations!L8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="J5" s="4">
         <f>Extrapolations!M8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="K5" s="4">
         <f>Extrapolations!N8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="L5" s="4">
         <f>Extrapolations!O8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="M5" s="4">
         <f>Extrapolations!P8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="N5" s="4">
         <f>Extrapolations!Q8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="O5" s="4">
         <f>Extrapolations!R8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="P5" s="4">
         <f>Extrapolations!S8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>Extrapolations!T8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="R5" s="4">
         <f>Extrapolations!U8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="S5" s="4">
         <f>Extrapolations!V8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="T5" s="4">
         <f>Extrapolations!W8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="U5" s="4">
         <f>Extrapolations!X8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="V5" s="4">
         <f>Extrapolations!Y8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="W5" s="4">
         <f>Extrapolations!Z8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="X5" s="4">
         <f>Extrapolations!AA8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>Extrapolations!AB8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>Extrapolations!AC8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>Extrapolations!AD8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>Extrapolations!AE8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>Extrapolations!AF8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>Extrapolations!AG8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>Extrapolations!AH8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AF5" s="4">
         <f>Extrapolations!AI8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AG5" s="4">
         <f>Extrapolations!AJ8</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -10691,131 +10662,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>2.0175605597964369E-3</v>
+        <v>2.4367252662957466E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -10826,7 +10797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -11623,131 +11594,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>7.266015454415603E-3</v>
+        <v>8.7192185452987219E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>7.3306737458536664E-3</v>
+        <v>8.7968084950243979E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>7.3953320372917124E-3</v>
+        <v>8.8743984447500531E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>7.4599903287297757E-3</v>
+        <v>8.9519883944757291E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>7.5246486201678391E-3</v>
+        <v>9.0295783442014051E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>7.5893069116059024E-3</v>
+        <v>9.1071682939270811E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>7.6539652030439657E-3</v>
+        <v>9.1847582436527572E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>7.7186234944820117E-3</v>
+        <v>9.2623481933784124E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>7.7832817859200751E-3</v>
+        <v>9.3399381431040884E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>7.8479400773581384E-3</v>
+        <v>9.4175280928297644E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>7.9125983687962018E-3</v>
+        <v>9.4951180425554404E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>7.9772566602342478E-3</v>
+        <v>9.5727079922810956E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>8.0419149516723111E-3</v>
+        <v>9.6502979420067716E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>8.1065732431103744E-3</v>
+        <v>9.7278878917324476E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>8.1712315345484378E-3</v>
+        <v>9.8054778414581236E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>8.2358898259864838E-3</v>
+        <v>9.8830677911837788E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>8.3005481174245471E-3</v>
+        <v>9.9606577409094548E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>8.3652064088626105E-3</v>
+        <v>1.0038247690635131E-2</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>8.4298647003006738E-3</v>
+        <v>1.0115837640360807E-2</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>8.4945229917387198E-3</v>
+        <v>1.0193427590086462E-2</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>8.5591812831767831E-3</v>
+        <v>1.0271017539812138E-2</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>8.6238395746148465E-3</v>
+        <v>1.0348607489537814E-2</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>8.6884978660529098E-3</v>
+        <v>1.042619743926349E-2</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>8.7531561574909558E-3</v>
+        <v>1.0503787388989145E-2</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>8.8178144489290192E-3</v>
+        <v>1.0581377338714821E-2</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>8.8824727403670825E-3</v>
+        <v>1.0658967288440497E-2</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>8.9471310318051459E-3</v>
+        <v>1.0736557238166173E-2</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>9.0117893232432092E-3</v>
+        <v>1.0814147187891849E-2</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>9.0764476146812552E-3</v>
+        <v>1.0891737137617504E-2</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>9.1411059061193185E-3</v>
+        <v>1.0969327087343181E-2</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>9.2057641975573819E-3</v>
+        <v>1.1046917037068857E-2</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>9.2704224889954452E-3</v>
+        <v>1.1124506986794533E-2</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -11758,7 +11729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12555,131 +12526,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>2.5123529962890107E-5</v>
+        <v>3.0148235955468123E-5</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -12690,7 +12661,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13487,131 +13458,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.0463060748209536E-2</v>
+        <v>1.2555672897851441E-2</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.0544362764739312E-2</v>
+        <v>1.2653235317687172E-2</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.0625664781269122E-2</v>
+        <v>1.2750797737522945E-2</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.0706966797798933E-2</v>
+        <v>1.2848360157358718E-2</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.0788268814328709E-2</v>
+        <v>1.2945922577194449E-2</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.0869570830858519E-2</v>
+        <v>1.3043484997030222E-2</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.095087284738833E-2</v>
+        <v>1.3141047416865994E-2</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.1032174863918141E-2</v>
+        <v>1.3238609836701767E-2</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.1113476880447917E-2</v>
+        <v>1.3336172256537498E-2</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.1194778896977727E-2</v>
+        <v>1.3433734676373271E-2</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.1276080913507538E-2</v>
+        <v>1.3531297096209044E-2</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.1357382930037314E-2</v>
+        <v>1.3628859516044775E-2</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.1438684946567124E-2</v>
+        <v>1.3726421935880547E-2</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.1519986963096935E-2</v>
+        <v>1.382398435571632E-2</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.1601288979626746E-2</v>
+        <v>1.3921546775552093E-2</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.1682590996156521E-2</v>
+        <v>1.4019109195387824E-2</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.1763893012686332E-2</v>
+        <v>1.4116671615223597E-2</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.1845195029216143E-2</v>
+        <v>1.421423403505937E-2</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.1926497045745919E-2</v>
+        <v>1.4311796454895101E-2</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.2007799062275729E-2</v>
+        <v>1.4409358874730873E-2</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.208910107880554E-2</v>
+        <v>1.4506921294566646E-2</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.2170403095335351E-2</v>
+        <v>1.4604483714402419E-2</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.2251705111865126E-2</v>
+        <v>1.470204613423815E-2</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.2333007128394937E-2</v>
+        <v>1.4799608554073923E-2</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>1.2414309144924748E-2</v>
+        <v>1.4897170973909695E-2</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>1.2495611161454524E-2</v>
+        <v>1.4994733393745427E-2</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.2576913177984334E-2</v>
+        <v>1.5092295813581199E-2</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.2658215194514145E-2</v>
+        <v>1.5189858233416972E-2</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.2739517211043955E-2</v>
+        <v>1.5287420653252745E-2</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.2820819227573731E-2</v>
+        <v>1.5384983073088476E-2</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>1.2902121244103542E-2</v>
+        <v>1.5482545492924249E-2</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>1.2983423260633353E-2</v>
+        <v>1.5580107912760021E-2</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -13622,7 +13593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13879,7 +13850,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:AI3" si="0">B$4</f>
+        <f t="shared" ref="B3:AG3" si="0">B$4</f>
         <v>1.1107105081407272E-3</v>
       </c>
       <c r="C3" s="4">
@@ -14149,7 +14120,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:AI5" si="1">B$4</f>
+        <f t="shared" ref="B5:AG5" si="1">B$4</f>
         <v>1.1107105081407272E-3</v>
       </c>
       <c r="C5" s="4">
@@ -14555,131 +14526,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$4*Calculations!$B$27</f>
-        <v>2.7767762703518181E-3</v>
+        <v>3.3321315244221809E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -14690,13 +14661,13 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
@@ -15520,10 +15491,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:AI14"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16372,100 +16345,100 @@
         <v>5</v>
       </c>
       <c r="D14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="E14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="F14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="G14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="H14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="I14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="J14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="K14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="L14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="M14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="N14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="O14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="P14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="Q14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="R14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="S14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="T14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="U14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="V14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="W14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="X14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="Y14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="Z14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AA14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AB14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AC14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AD14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AE14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AF14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AG14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AH14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AI14" s="4">
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
@@ -17024,7 +16997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17132,11 +17105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -17372,7 +17345,7 @@
         <v>82</v>
       </c>
       <c r="B26" s="25">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D26" s="7"/>
     </row>
@@ -17382,7 +17355,7 @@
       </c>
       <c r="B27" s="8">
         <f>B26/B25</f>
-        <v>2.5</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -17422,7 +17395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -19090,267 +19063,267 @@
       <c r="D8" s="11"/>
       <c r="E8" s="4">
         <f t="shared" ref="E8:AL12" si="8">TREND($AM8:$BR8,$AM$1:$BR$1,E$1)</f>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AB8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AC8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AD8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AF8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AH8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AI8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AJ8" s="4">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AK8" s="33">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AL8" s="34">
         <f t="shared" si="8"/>
-        <v>8.070242239185747E-4</v>
+        <v>8.122417554319157E-4</v>
       </c>
       <c r="AM8" s="14">
         <f>BNVFE!D14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AN8" s="15">
         <f>BNVFE!E14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AO8" s="15">
         <f>BNVFE!F14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AP8" s="15">
         <f>BNVFE!G14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AQ8" s="15">
         <f>BNVFE!H14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AR8" s="15">
         <f>BNVFE!I14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AS8" s="15">
         <f>BNVFE!J14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AT8" s="15">
         <f>BNVFE!K14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AU8" s="15">
         <f>BNVFE!L14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AV8" s="15">
         <f>BNVFE!M14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AW8" s="15">
         <f>BNVFE!N14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AX8" s="15">
         <f>BNVFE!O14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AY8" s="15">
         <f>BNVFE!P14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="AZ8" s="15">
         <f>BNVFE!Q14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BA8" s="15">
         <f>BNVFE!R14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BB8" s="15">
         <f>BNVFE!S14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BC8" s="15">
         <f>BNVFE!T14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BD8" s="15">
         <f>BNVFE!U14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BE8" s="15">
         <f>BNVFE!V14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BF8" s="15">
         <f>BNVFE!W14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BG8" s="15">
         <f>BNVFE!X14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BH8" s="15">
         <f>BNVFE!Y14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BI8" s="15">
         <f>BNVFE!Z14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BJ8" s="15">
         <f>BNVFE!AA14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BK8" s="15">
         <f>BNVFE!AB14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BL8" s="15">
         <f>BNVFE!AC14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BM8" s="15">
         <f>BNVFE!AD14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BN8" s="15">
         <f>BNVFE!AE14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BO8" s="15">
         <f>BNVFE!AF14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BP8" s="15">
         <f>BNVFE!AG14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BQ8" s="15">
         <f>BNVFE!AH14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BR8" s="15">
         <f>BNVFE!AI14</f>
-        <v>8.0702422391857502E-4</v>
+        <v>8.1224175543191505E-4</v>
       </c>
       <c r="BS8" s="15"/>
       <c r="BT8" s="4"/>
@@ -19935,7 +19908,7 @@
         <v>4.3153075257314835E-3</v>
       </c>
       <c r="K11" s="29">
-        <f t="shared" ref="D11:AF12" si="9">TREND($AM11:$BR11,$AM$1:$BR$1,K$1)</f>
+        <f t="shared" ref="K11:AF12" si="9">TREND($AM11:$BR11,$AM$1:$BR$1,K$1)</f>
         <v>4.3478283323434078E-3</v>
       </c>
       <c r="L11" s="29">
@@ -20637,7 +20610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -20894,7 +20867,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:AI5" si="0">B$4</f>
+        <f t="shared" ref="B3:AG5" si="0">B$4</f>
         <v>3.0748825560000803E-4</v>
       </c>
       <c r="C3" s="4">
@@ -21570,131 +21543,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
-        <v>7.6872063900002008E-4</v>
+        <v>9.2246476680002399E-4</v>
       </c>
       <c r="C8" s="4">
         <f>C$4*Calculations!$B$27</f>
-        <v>7.8562465408047886E-4</v>
+        <v>9.4274958489657453E-4</v>
       </c>
       <c r="D8" s="4">
         <f>D$4*Calculations!$B$27</f>
-        <v>8.0252866916093765E-4</v>
+        <v>9.6303440299312507E-4</v>
       </c>
       <c r="E8" s="4">
         <f>E$4*Calculations!$B$27</f>
-        <v>8.1943268424139644E-4</v>
+        <v>9.8331922108967551E-4</v>
       </c>
       <c r="F8" s="4">
         <f>F$4*Calculations!$B$27</f>
-        <v>8.3633669932185522E-4</v>
+        <v>1.0036040391862261E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$4*Calculations!$B$27</f>
-        <v>8.5324071440231401E-4</v>
+        <v>1.0238888572827766E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$4*Calculations!$B$27</f>
-        <v>8.7014472948277279E-4</v>
+        <v>1.0441736753793271E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$4*Calculations!$B$27</f>
-        <v>8.8704874456323158E-4</v>
+        <v>1.0644584934758777E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$4*Calculations!$B$27</f>
-        <v>9.0395275964369037E-4</v>
+        <v>1.0847433115724282E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$4*Calculations!$B$27</f>
-        <v>9.2085677472414915E-4</v>
+        <v>1.1050281296689788E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$4*Calculations!$B$27</f>
-        <v>9.3776078980460794E-4</v>
+        <v>1.1253129477655293E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$4*Calculations!$B$27</f>
-        <v>9.5466480488506672E-4</v>
+        <v>1.1455977658620799E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$4*Calculations!$B$27</f>
-        <v>9.7156881996552551E-4</v>
+        <v>1.1658825839586304E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$4*Calculations!$B$27</f>
-        <v>9.8847283504598419E-4</v>
+        <v>1.1861674020551807E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$4*Calculations!$B$27</f>
-        <v>1.0200149884624322E-3</v>
+        <v>1.2240179861549186E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$4*Calculations!$B$27</f>
-        <v>1.0596934640509314E-3</v>
+        <v>1.2716321568611174E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$4*Calculations!$B$27</f>
-        <v>1.1076483687622431E-3</v>
+        <v>1.3291780425146915E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$4*Calculations!$B$27</f>
-        <v>1.1479243868073308E-3</v>
+        <v>1.3775092641687967E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$4*Calculations!$B$27</f>
-        <v>1.1966396740844649E-3</v>
+        <v>1.4359676089013577E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$4*Calculations!$B$27</f>
-        <v>1.2556893304475579E-3</v>
+        <v>1.5068271965370693E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$4*Calculations!$B$27</f>
-        <v>1.2619822221853316E-3</v>
+        <v>1.5143786666223975E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$4*Calculations!$B$27</f>
-        <v>1.2653284668730702E-3</v>
+        <v>1.518394160247684E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$4*Calculations!$B$27</f>
-        <v>1.2685621200488062E-3</v>
+        <v>1.5222745440585672E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$4*Calculations!$B$27</f>
-        <v>1.2726358258076298E-3</v>
+        <v>1.5271629909691554E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$4*Calculations!$B$27</f>
-        <v>1.279494655367044E-3</v>
+        <v>1.5353935864404525E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$4*Calculations!$B$27</f>
-        <v>1.2861787237707094E-3</v>
+        <v>1.5434144685248512E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$4*Calculations!$B$27</f>
-        <v>1.291913197649324E-3</v>
+        <v>1.5502958371791885E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$4*Calculations!$B$27</f>
-        <v>1.2982639965636309E-3</v>
+        <v>1.5579167958763567E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$4*Calculations!$B$27</f>
-        <v>1.3043571414638603E-3</v>
+        <v>1.565228569756632E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$4*Calculations!$B$27</f>
-        <v>1.3095804658189182E-3</v>
+        <v>1.5714965589827016E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$4*Calculations!$B$27</f>
-        <v>1.3138723197981339E-3</v>
+        <v>1.5766467837577606E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$4*Calculations!$B$27</f>
-        <v>1.3168481456887677E-3</v>
+        <v>1.5802177748265212E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -21705,7 +21678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -21962,7 +21935,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:AI3" si="0">B$4</f>
+        <f t="shared" ref="B3:AG3" si="0">B$4</f>
         <v>1.169525976045652E-4</v>
       </c>
       <c r="C3" s="4">
@@ -22232,7 +22205,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:AI5" si="1">B$4</f>
+        <f t="shared" ref="B5:AG5" si="1">B$4</f>
         <v>1.169525976045652E-4</v>
       </c>
       <c r="C5" s="4">
@@ -22638,131 +22611,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
-        <v>2.9238149401141303E-4</v>
+        <v>3.5085779281369554E-4</v>
       </c>
       <c r="C8" s="4">
         <f>C$4*Calculations!$B$27</f>
-        <v>2.9382293085211219E-4</v>
+        <v>3.5258751702253456E-4</v>
       </c>
       <c r="D8" s="4">
         <f>D$4*Calculations!$B$27</f>
-        <v>2.9526436769281136E-4</v>
+        <v>3.5431724123137362E-4</v>
       </c>
       <c r="E8" s="4">
         <f>E$4*Calculations!$B$27</f>
-        <v>2.9670580453351059E-4</v>
+        <v>3.5604696544021264E-4</v>
       </c>
       <c r="F8" s="4">
         <f>F$4*Calculations!$B$27</f>
-        <v>2.9814724137420975E-4</v>
+        <v>3.5777668964905165E-4</v>
       </c>
       <c r="G8" s="4">
         <f>G$4*Calculations!$B$27</f>
-        <v>2.9958867821490892E-4</v>
+        <v>3.5950641385789066E-4</v>
       </c>
       <c r="H8" s="4">
         <f>H$4*Calculations!$B$27</f>
-        <v>3.0103011505560814E-4</v>
+        <v>3.6123613806672973E-4</v>
       </c>
       <c r="I8" s="4">
         <f>I$4*Calculations!$B$27</f>
-        <v>3.0247155189630731E-4</v>
+        <v>3.6296586227556869E-4</v>
       </c>
       <c r="J8" s="4">
         <f>J$4*Calculations!$B$27</f>
-        <v>3.0391298873700648E-4</v>
+        <v>3.646955864844077E-4</v>
       </c>
       <c r="K8" s="4">
         <f>K$4*Calculations!$B$27</f>
-        <v>3.0535442557770565E-4</v>
+        <v>3.6642531069324671E-4</v>
       </c>
       <c r="L8" s="4">
         <f>L$4*Calculations!$B$27</f>
-        <v>3.0679586241840487E-4</v>
+        <v>3.6815503490208578E-4</v>
       </c>
       <c r="M8" s="4">
         <f>M$4*Calculations!$B$27</f>
-        <v>3.0823729925910404E-4</v>
+        <v>3.6988475911092479E-4</v>
       </c>
       <c r="N8" s="4">
         <f>N$4*Calculations!$B$27</f>
-        <v>3.0967873609980321E-4</v>
+        <v>3.7161448331976375E-4</v>
       </c>
       <c r="O8" s="4">
         <f>O$4*Calculations!$B$27</f>
-        <v>3.1256160978120122E-4</v>
+        <v>3.750739317374414E-4</v>
       </c>
       <c r="P8" s="4">
         <f>P$4*Calculations!$B$27</f>
-        <v>3.1434287741956897E-4</v>
+        <v>3.7721145290348275E-4</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$4*Calculations!$B$27</f>
-        <v>3.1868729041468845E-4</v>
+        <v>3.8242474849762605E-4</v>
       </c>
       <c r="R8" s="4">
         <f>R$4*Calculations!$B$27</f>
-        <v>3.2203835203692025E-4</v>
+        <v>3.8644602244430421E-4</v>
       </c>
       <c r="S8" s="4">
         <f>S$4*Calculations!$B$27</f>
-        <v>3.264251593678409E-4</v>
+        <v>3.9171019124140902E-4</v>
       </c>
       <c r="T8" s="4">
         <f>T$4*Calculations!$B$27</f>
-        <v>3.316866222318138E-4</v>
+        <v>3.980239466781765E-4</v>
       </c>
       <c r="U8" s="4">
         <f>U$4*Calculations!$B$27</f>
-        <v>3.3797409857564992E-4</v>
+        <v>4.0556891829077982E-4</v>
       </c>
       <c r="V8" s="4">
         <f>V$4*Calculations!$B$27</f>
-        <v>3.4420870131810481E-4</v>
+        <v>4.130504415817257E-4</v>
       </c>
       <c r="W8" s="4">
         <f>W$4*Calculations!$B$27</f>
-        <v>3.4939541900461503E-4</v>
+        <v>4.1927450280553795E-4</v>
       </c>
       <c r="X8" s="4">
         <f>X$4*Calculations!$B$27</f>
-        <v>3.4952864055911551E-4</v>
+        <v>4.1943436867093855E-4</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$4*Calculations!$B$27</f>
-        <v>3.5136620571732131E-4</v>
+        <v>4.2163944686078548E-4</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$4*Calculations!$B$27</f>
-        <v>3.5264604568544775E-4</v>
+        <v>4.2317525482253723E-4</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$4*Calculations!$B$27</f>
-        <v>3.5327444885288356E-4</v>
+        <v>4.2392933862346019E-4</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$4*Calculations!$B$27</f>
-        <v>3.5291946113748794E-4</v>
+        <v>4.2350335336498543E-4</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$4*Calculations!$B$27</f>
-        <v>3.5237655217636708E-4</v>
+        <v>4.228518626116404E-4</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$4*Calculations!$B$27</f>
-        <v>3.518375651582058E-4</v>
+        <v>4.2220507818984689E-4</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$4*Calculations!$B$27</f>
-        <v>3.5118695839835316E-4</v>
+        <v>4.2142435007802369E-4</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$4*Calculations!$B$27</f>
-        <v>3.5082800723795613E-4</v>
+        <v>4.2099360868554726E-4</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$4*Calculations!$B$27</f>
-        <v>3.50443615325874E-4</v>
+        <v>4.2053233839104873E-4</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -22773,7 +22746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -23030,7 +23003,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:AI4" si="0">B$5</f>
+        <f t="shared" ref="B3:AG4" si="0">B$5</f>
         <v>8.2962674808847244E-4</v>
       </c>
       <c r="C3" s="4">
@@ -23706,131 +23679,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$4*Calculations!$B$27</f>
-        <v>2.074066870221181E-3</v>
+        <v>2.4888802442654171E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$4*Calculations!$B$27</f>
-        <v>2.0844976872009461E-3</v>
+        <v>2.5013972246411349E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$4*Calculations!$B$27</f>
-        <v>2.0949285041807113E-3</v>
+        <v>2.5139142050168532E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$4*Calculations!$B$27</f>
-        <v>2.1053593211604765E-3</v>
+        <v>2.5264311853925715E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$4*Calculations!$B$27</f>
-        <v>2.1157901381402416E-3</v>
+        <v>2.5389481657682898E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$4*Calculations!$B$27</f>
-        <v>2.1262209551200072E-3</v>
+        <v>2.5514651461440081E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$4*Calculations!$B$27</f>
-        <v>2.1366517720997724E-3</v>
+        <v>2.5639821265197264E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$4*Calculations!$B$27</f>
-        <v>2.1470825890795371E-3</v>
+        <v>2.5764991068954442E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$4*Calculations!$B$27</f>
-        <v>2.1575134060593023E-3</v>
+        <v>2.5890160872711625E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$4*Calculations!$B$27</f>
-        <v>2.1679442230390679E-3</v>
+        <v>2.6015330676468808E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$4*Calculations!$B$27</f>
-        <v>2.1783750400188326E-3</v>
+        <v>2.6140500480225991E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$4*Calculations!$B$27</f>
-        <v>2.1888058569985978E-3</v>
+        <v>2.6265670283983169E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$4*Calculations!$B$27</f>
-        <v>2.1992366739783629E-3</v>
+        <v>2.6390840087740352E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$4*Calculations!$B$27</f>
-        <v>2.2096674909581281E-3</v>
+        <v>2.6516009891497535E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$4*Calculations!$B$27</f>
-        <v>2.2200983079378933E-3</v>
+        <v>2.6641179695254718E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$4*Calculations!$B$27</f>
-        <v>2.2305291249176584E-3</v>
+        <v>2.67663494990119E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$4*Calculations!$B$27</f>
-        <v>2.2409599418974236E-3</v>
+        <v>2.6891519302769079E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$4*Calculations!$B$27</f>
-        <v>2.2618215758569513E-3</v>
+        <v>2.7141858910283414E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$4*Calculations!$B$27</f>
-        <v>2.2763608733602607E-3</v>
+        <v>2.7316330480323127E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$4*Calculations!$B$27</f>
-        <v>2.3131504377265758E-3</v>
+        <v>2.7757805252718905E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$4*Calculations!$B$27</f>
-        <v>2.3124895490410548E-3</v>
+        <v>2.7749874588492655E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -23841,7 +23814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -24098,7 +24071,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:AI4" si="0">B$5</f>
+        <f t="shared" ref="B3:AG4" si="0">B$5</f>
         <v>7.8040477200267344E-4</v>
       </c>
       <c r="C3" s="4">
@@ -24774,131 +24747,131 @@
       </c>
       <c r="B8" s="4">
         <f>B$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$4*Calculations!$B$27</f>
-        <v>1.9510119300066835E-3</v>
+        <v>2.34121431600802E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$4*Calculations!$B$27</f>
-        <v>1.9608238838348972E-3</v>
+        <v>2.3529886606018765E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$4*Calculations!$B$27</f>
-        <v>1.9706358376631113E-3</v>
+        <v>2.3647630051957329E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$4*Calculations!$B$27</f>
-        <v>1.9804477914913249E-3</v>
+        <v>2.3765373497895898E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$4*Calculations!$B$27</f>
-        <v>1.990259745319539E-3</v>
+        <v>2.3883116943834463E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$4*Calculations!$B$27</f>
-        <v>2.0000716991477527E-3</v>
+        <v>2.4000860389773028E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$4*Calculations!$B$27</f>
-        <v>2.0098836529759663E-3</v>
+        <v>2.4118603835711593E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$4*Calculations!$B$27</f>
-        <v>2.0196956068041804E-3</v>
+        <v>2.4236347281650162E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$4*Calculations!$B$27</f>
-        <v>2.0295075606323941E-3</v>
+        <v>2.4354090727588726E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$4*Calculations!$B$27</f>
-        <v>2.0393195144606082E-3</v>
+        <v>2.4471834173527291E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$4*Calculations!$B$27</f>
-        <v>2.0491314682888218E-3</v>
+        <v>2.4589577619465856E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$4*Calculations!$B$27</f>
-        <v>2.0589434221170355E-3</v>
+        <v>2.4707321065404425E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$4*Calculations!$B$27</f>
-        <v>2.0687553759452496E-3</v>
+        <v>2.482506451134299E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$4*Calculations!$B$27</f>
-        <v>2.0785673297734632E-3</v>
+        <v>2.4942807957281554E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$4*Calculations!$B$27</f>
-        <v>2.0883792836016769E-3</v>
+        <v>2.5060551403220119E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$4*Calculations!$B$27</f>
-        <v>2.098191237429891E-3</v>
+        <v>2.5178294849158688E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$4*Calculations!$B$27</f>
-        <v>2.1080031912581046E-3</v>
+        <v>2.5296038295097253E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$4*Calculations!$B$27</f>
-        <v>2.1276270989145302E-3</v>
+        <v>2.5531525186974356E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$4*Calculations!$B$27</f>
-        <v>2.1590641096528242E-3</v>
+        <v>2.5908769315833888E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$4*Calculations!$B$27</f>
-        <v>2.2163451968687251E-3</v>
+        <v>2.6596142362424698E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$4*Calculations!$B$27</f>
-        <v>2.2402453220033178E-3</v>
+        <v>2.6882943864039808E-3</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>

</xml_diff>

<commit_message>
Update BHNVFEAL xlsx file
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A6B8EF-092C-4AB2-9FFB-9E2AFA6EDC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -42,7 +43,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,6 +52,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -58,14 +60,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -382,7 +384,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1339,162 +1341,162 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="156">
-    <cellStyle name="20% - Accent1 2" xfId="8"/>
-    <cellStyle name="20% - Accent2 2" xfId="9"/>
-    <cellStyle name="20% - Accent3 2" xfId="10"/>
-    <cellStyle name="20% - Accent4 2" xfId="11"/>
-    <cellStyle name="20% - Accent5 2" xfId="12"/>
-    <cellStyle name="20% - Accent6 2" xfId="13"/>
-    <cellStyle name="40% - Accent1 2" xfId="14"/>
-    <cellStyle name="40% - Accent2 2" xfId="15"/>
-    <cellStyle name="40% - Accent3 2" xfId="16"/>
-    <cellStyle name="40% - Accent4 2" xfId="17"/>
-    <cellStyle name="40% - Accent5 2" xfId="18"/>
-    <cellStyle name="40% - Accent6 2" xfId="19"/>
-    <cellStyle name="60% - Accent1 2" xfId="20"/>
-    <cellStyle name="60% - Accent2 2" xfId="21"/>
-    <cellStyle name="60% - Accent3 2" xfId="22"/>
-    <cellStyle name="60% - Accent4 2" xfId="23"/>
-    <cellStyle name="60% - Accent5 2" xfId="24"/>
-    <cellStyle name="60% - Accent6 2" xfId="25"/>
-    <cellStyle name="Accent1 2" xfId="26"/>
-    <cellStyle name="Accent2 2" xfId="27"/>
-    <cellStyle name="Accent3 2" xfId="28"/>
-    <cellStyle name="Accent4 2" xfId="29"/>
-    <cellStyle name="Accent5 2" xfId="30"/>
-    <cellStyle name="Accent6 2" xfId="31"/>
-    <cellStyle name="Bad 2" xfId="32"/>
-    <cellStyle name="Body: normal cell" xfId="4"/>
-    <cellStyle name="Body: normal cell 2" xfId="33"/>
-    <cellStyle name="Calculation 2" xfId="34"/>
-    <cellStyle name="Check Cell 2" xfId="35"/>
-    <cellStyle name="Column heading" xfId="36"/>
+    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Comma" xfId="154" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="37"/>
-    <cellStyle name="Comma 2 2" xfId="38"/>
-    <cellStyle name="Comma 3" xfId="39"/>
-    <cellStyle name="Comma 4" xfId="40"/>
-    <cellStyle name="Comma 5" xfId="41"/>
-    <cellStyle name="Comma 6" xfId="42"/>
-    <cellStyle name="Comma 7" xfId="43"/>
-    <cellStyle name="Comma 8" xfId="44"/>
-    <cellStyle name="Corner heading" xfId="45"/>
-    <cellStyle name="Currency 2" xfId="46"/>
-    <cellStyle name="Currency 3" xfId="47"/>
-    <cellStyle name="Currency 3 2" xfId="48"/>
-    <cellStyle name="Data" xfId="49"/>
-    <cellStyle name="Data 2" xfId="50"/>
-    <cellStyle name="Data no deci" xfId="51"/>
-    <cellStyle name="Data Superscript" xfId="52"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
-    <cellStyle name="Explanatory Text 2" xfId="54"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
-    <cellStyle name="Footnotes: top row" xfId="2"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56"/>
-    <cellStyle name="Good 2" xfId="57"/>
-    <cellStyle name="Header: bottom row" xfId="5"/>
-    <cellStyle name="Header: bottom row 2" xfId="58"/>
-    <cellStyle name="Heading 1 2" xfId="59"/>
-    <cellStyle name="Heading 2 2" xfId="60"/>
-    <cellStyle name="Heading 3 2" xfId="61"/>
-    <cellStyle name="Heading 4 2" xfId="62"/>
-    <cellStyle name="Hed Side" xfId="63"/>
-    <cellStyle name="Hed Side 2" xfId="64"/>
-    <cellStyle name="Hed Side bold" xfId="65"/>
-    <cellStyle name="Hed Side Indent" xfId="66"/>
-    <cellStyle name="Hed Side Regular" xfId="67"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
-    <cellStyle name="Hed Top" xfId="69"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71"/>
+    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72"/>
-    <cellStyle name="Input 2" xfId="73"/>
-    <cellStyle name="Linked Cell 2" xfId="74"/>
-    <cellStyle name="Neutral 2" xfId="75"/>
+    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76"/>
-    <cellStyle name="Normal 11" xfId="77"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="78"/>
-    <cellStyle name="Normal 2 3" xfId="79"/>
-    <cellStyle name="Normal 3" xfId="80"/>
-    <cellStyle name="Normal 3 2" xfId="81"/>
-    <cellStyle name="Normal 3 2 2" xfId="82"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
-    <cellStyle name="Normal 3 2 3" xfId="84"/>
-    <cellStyle name="Normal 3 3" xfId="85"/>
-    <cellStyle name="Normal 3 3 2" xfId="86"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
-    <cellStyle name="Normal 3 3 3" xfId="88"/>
-    <cellStyle name="Normal 3 4" xfId="89"/>
-    <cellStyle name="Normal 3 4 2" xfId="90"/>
-    <cellStyle name="Normal 3 5" xfId="91"/>
-    <cellStyle name="Normal 3 6" xfId="92"/>
-    <cellStyle name="Normal 3 7" xfId="93"/>
-    <cellStyle name="Normal 4" xfId="94"/>
-    <cellStyle name="Normal 4 2" xfId="95"/>
-    <cellStyle name="Normal 4 2 2" xfId="96"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
-    <cellStyle name="Normal 4 2 3" xfId="98"/>
-    <cellStyle name="Normal 4 3" xfId="99"/>
-    <cellStyle name="Normal 4 3 2" xfId="100"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
-    <cellStyle name="Normal 4 3 3" xfId="102"/>
-    <cellStyle name="Normal 4 4" xfId="103"/>
-    <cellStyle name="Normal 4 4 2" xfId="104"/>
-    <cellStyle name="Normal 4 5" xfId="105"/>
-    <cellStyle name="Normal 4 6" xfId="106"/>
-    <cellStyle name="Normal 4 7" xfId="107"/>
-    <cellStyle name="Normal 5" xfId="108"/>
-    <cellStyle name="Normal 5 2" xfId="109"/>
-    <cellStyle name="Normal 5 3" xfId="110"/>
-    <cellStyle name="Normal 6" xfId="111"/>
-    <cellStyle name="Normal 6 2" xfId="112"/>
-    <cellStyle name="Normal 7" xfId="113"/>
-    <cellStyle name="Normal 7 2" xfId="114"/>
-    <cellStyle name="Normal 8" xfId="115"/>
-    <cellStyle name="Normal 9" xfId="116"/>
-    <cellStyle name="Note 2" xfId="117"/>
-    <cellStyle name="Note 2 2" xfId="118"/>
-    <cellStyle name="Output 2" xfId="119"/>
-    <cellStyle name="Parent row" xfId="3"/>
-    <cellStyle name="Parent row 2" xfId="120"/>
+    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
     <cellStyle name="Percent" xfId="155" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="121"/>
-    <cellStyle name="Percent 2 2" xfId="122"/>
-    <cellStyle name="Percent 3" xfId="123"/>
-    <cellStyle name="Percent 3 2" xfId="124"/>
-    <cellStyle name="Percent 4" xfId="125"/>
-    <cellStyle name="Reference" xfId="126"/>
-    <cellStyle name="Row heading" xfId="127"/>
-    <cellStyle name="Source Hed" xfId="128"/>
-    <cellStyle name="Source Letter" xfId="129"/>
-    <cellStyle name="Source Superscript" xfId="130"/>
-    <cellStyle name="Source Superscript 2" xfId="131"/>
-    <cellStyle name="Source Text" xfId="132"/>
-    <cellStyle name="Source Text 2" xfId="133"/>
-    <cellStyle name="State" xfId="134"/>
-    <cellStyle name="Superscript" xfId="135"/>
-    <cellStyle name="Table Data" xfId="136"/>
-    <cellStyle name="Table Head Top" xfId="137"/>
-    <cellStyle name="Table Hed Side" xfId="138"/>
-    <cellStyle name="Table title" xfId="7"/>
-    <cellStyle name="Table title 2" xfId="139"/>
-    <cellStyle name="Title 2" xfId="140"/>
-    <cellStyle name="Title Text" xfId="141"/>
-    <cellStyle name="Title Text 1" xfId="142"/>
-    <cellStyle name="Title Text 2" xfId="143"/>
-    <cellStyle name="Title-1" xfId="144"/>
-    <cellStyle name="Title-2" xfId="145"/>
-    <cellStyle name="Title-3" xfId="146"/>
-    <cellStyle name="Total 2" xfId="147"/>
-    <cellStyle name="Warning Text 2" xfId="148"/>
-    <cellStyle name="Wrap" xfId="149"/>
-    <cellStyle name="Wrap Bold" xfId="150"/>
-    <cellStyle name="Wrap Title" xfId="151"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
+    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1524,7 +1526,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1776,133 +1777,133 @@
                   <c:v>3.142498616321923E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>3.2092630056054029E-4</c:v>
+                  <c:v>3.1859095271137485E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>3.2760273948888828E-4</c:v>
+                  <c:v>3.2293204379055739E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>3.3427917841723627E-4</c:v>
+                  <c:v>3.2727313486973994E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>3.4095561734558426E-4</c:v>
+                  <c:v>3.3161422594892248E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>3.4763205627393225E-4</c:v>
+                  <c:v>3.3595531702810503E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>3.5430849520228023E-4</c:v>
+                  <c:v>3.4029640810728757E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>3.6098493413062822E-4</c:v>
+                  <c:v>3.4463749918647011E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>3.6766137305897621E-4</c:v>
+                  <c:v>3.4897859026565266E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>3.743378119873242E-4</c:v>
+                  <c:v>3.533196813448352E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>3.8101425091567219E-4</c:v>
+                  <c:v>3.5766077242401775E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>3.8769068984402017E-4</c:v>
+                  <c:v>3.6200186350320029E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>3.9436712877236816E-4</c:v>
+                  <c:v>3.6634295458238284E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>4.010435677007162E-4</c:v>
+                  <c:v>3.7068404566156505E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>4.1543936179917892E-4</c:v>
+                  <c:v>3.8286968063361244E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>4.232456921304615E-4</c:v>
+                  <c:v>3.8999540362380768E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.284224989356039E-4</c:v>
+                  <c:v>3.9439145706872869E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.3223887309206766E-4</c:v>
+                  <c:v>3.9758791642567675E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>4.3661930301858122E-4</c:v>
+                  <c:v>4.1670440259151796E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>4.4073837767711228E-4</c:v>
+                  <c:v>4.5449874343080136E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>4.4130433819121803E-4</c:v>
+                  <c:v>4.5571840174311271E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>4.4139330713525239E-4</c:v>
+                  <c:v>4.5632492494806224E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.4143859386227608E-4</c:v>
+                  <c:v>4.5682343934192723E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>4.4252278985937798E-4</c:v>
+                  <c:v>4.5864796428233097E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.4258101673758966E-4</c:v>
+                  <c:v>4.5942511490356416E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>4.4262644410952699E-4</c:v>
+                  <c:v>4.6038567019040524E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.4263525674443374E-4</c:v>
+                  <c:v>4.6137990440500237E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>4.428907913418545E-4</c:v>
+                  <c:v>4.627584500454361E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>4.4235185104972023E-4</c:v>
+                  <c:v>4.6332164296180965E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>4.4180682000362565E-4</c:v>
+                  <c:v>4.6388593065941057E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.415169210975881E-4</c:v>
+                  <c:v>4.6479081055883617E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>4.4141525513386555E-4</c:v>
+                  <c:v>4.6598088096797761E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>4.4094858868260617E-4</c:v>
+                  <c:v>4.6672534660756901E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>4.406528424788466E-4</c:v>
+                  <c:v>4.6768413007742366E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>4.4046477188487546E-4</c:v>
+                  <c:v>4.6835837126328925E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>4.4016736396697124E-4</c:v>
+                  <c:v>4.6888408232764332E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>4.3991921468742256E-4</c:v>
+                  <c:v>4.6949898925199146E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>4.3980677282836695E-4</c:v>
+                  <c:v>4.7032072339820558E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>4.3981133028276362E-4</c:v>
+                  <c:v>4.7135545011319722E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>4.3960459654073496E-4</c:v>
+                  <c:v>4.7215508696463892E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>4.3945697770705547E-4</c:v>
+                  <c:v>4.730119981602886E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>4.3919624527100954E-4</c:v>
+                  <c:v>4.737905892831368E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>4.3913823303573507E-4</c:v>
+                  <c:v>4.7491927991846777E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>4.3909651675542918E-4</c:v>
+                  <c:v>4.7615242132589445E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,7 +1989,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2988,7 +2988,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3452,7 +3451,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3961,7 +3959,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4470,7 +4467,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4967,7 +4963,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5464,7 +5459,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5992,7 +5986,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6519,7 +6512,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7586,6 +7578,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7621,6 +7630,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7796,17 +7822,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" customWidth="1"/>
-    <col min="2" max="2" width="107.3984375" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="107.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8016,7 +8042,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -8024,7 +8050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8034,9 +8060,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -9054,7 +9080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9064,9 +9090,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -9958,7 +9984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9968,9 +9994,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -10862,7 +10888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10872,11 +10898,11 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -11802,7 +11828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -11812,9 +11838,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -12706,7 +12732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12716,10 +12742,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -13729,7 +13755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13739,9 +13765,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -14633,7 +14659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -14643,9 +14669,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -15663,7 +15689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -15673,9 +15699,9 @@
       <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -16492,18 +16518,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:AH20"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.3984375" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -16680,97 +16706,97 @@
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>4.010435677007162E-4</v>
+        <v>3.7068404566156505E-4</v>
       </c>
       <c r="E8" s="4">
-        <v>4.1543936179917892E-4</v>
+        <v>3.8286968063361244E-4</v>
       </c>
       <c r="F8" s="4">
-        <v>4.232456921304615E-4</v>
+        <v>3.8999540362380768E-4</v>
       </c>
       <c r="G8" s="4">
-        <v>4.284224989356039E-4</v>
+        <v>3.9439145706872869E-4</v>
       </c>
       <c r="H8" s="4">
-        <v>4.3223887309206766E-4</v>
+        <v>3.9758791642567675E-4</v>
       </c>
       <c r="I8" s="4">
-        <v>4.3661930301858122E-4</v>
+        <v>4.1670440259151796E-4</v>
       </c>
       <c r="J8" s="4">
-        <v>4.4073837767711228E-4</v>
+        <v>4.5449874343080136E-4</v>
       </c>
       <c r="K8" s="4">
-        <v>4.4130433819121803E-4</v>
+        <v>4.5571840174311271E-4</v>
       </c>
       <c r="L8" s="4">
-        <v>4.4139330713525239E-4</v>
+        <v>4.5632492494806224E-4</v>
       </c>
       <c r="M8" s="4">
-        <v>4.4143859386227608E-4</v>
+        <v>4.5682343934192723E-4</v>
       </c>
       <c r="N8" s="4">
-        <v>4.4252278985937798E-4</v>
+        <v>4.5864796428233097E-4</v>
       </c>
       <c r="O8" s="4">
-        <v>4.4258101673758966E-4</v>
+        <v>4.5942511490356416E-4</v>
       </c>
       <c r="P8" s="4">
-        <v>4.4262644410952699E-4</v>
+        <v>4.6038567019040524E-4</v>
       </c>
       <c r="Q8" s="4">
-        <v>4.4263525674443374E-4</v>
+        <v>4.6137990440500237E-4</v>
       </c>
       <c r="R8" s="4">
-        <v>4.428907913418545E-4</v>
+        <v>4.627584500454361E-4</v>
       </c>
       <c r="S8" s="4">
-        <v>4.4235185104972023E-4</v>
+        <v>4.6332164296180965E-4</v>
       </c>
       <c r="T8" s="4">
-        <v>4.4180682000362565E-4</v>
+        <v>4.6388593065941057E-4</v>
       </c>
       <c r="U8" s="4">
-        <v>4.415169210975881E-4</v>
+        <v>4.6479081055883617E-4</v>
       </c>
       <c r="V8" s="4">
-        <v>4.4141525513386555E-4</v>
+        <v>4.6598088096797761E-4</v>
       </c>
       <c r="W8" s="4">
-        <v>4.4094858868260617E-4</v>
+        <v>4.6672534660756901E-4</v>
       </c>
       <c r="X8" s="4">
-        <v>4.406528424788466E-4</v>
+        <v>4.6768413007742366E-4</v>
       </c>
       <c r="Y8" s="4">
-        <v>4.4046477188487546E-4</v>
+        <v>4.6835837126328925E-4</v>
       </c>
       <c r="Z8" s="4">
-        <v>4.4016736396697124E-4</v>
+        <v>4.6888408232764332E-4</v>
       </c>
       <c r="AA8" s="4">
-        <v>4.3991921468742256E-4</v>
+        <v>4.6949898925199146E-4</v>
       </c>
       <c r="AB8" s="4">
-        <v>4.3980677282836695E-4</v>
+        <v>4.7032072339820558E-4</v>
       </c>
       <c r="AC8" s="4">
-        <v>4.3981133028276362E-4</v>
+        <v>4.7135545011319722E-4</v>
       </c>
       <c r="AD8" s="4">
-        <v>4.3960459654073496E-4</v>
+        <v>4.7215508696463892E-4</v>
       </c>
       <c r="AE8" s="4">
-        <v>4.3945697770705547E-4</v>
+        <v>4.730119981602886E-4</v>
       </c>
       <c r="AF8" s="4">
-        <v>4.3919624527100954E-4</v>
+        <v>4.737905892831368E-4</v>
       </c>
       <c r="AG8" s="4">
-        <v>4.3913823303573507E-4</v>
+        <v>4.7491927991846777E-4</v>
       </c>
       <c r="AH8" s="4">
-        <v>4.3909651675542918E-4</v>
+        <v>4.7615242132589445E-4</v>
       </c>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
@@ -18864,14 +18890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -19243,14 +19269,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="50.3984375" customWidth="1"/>
+    <col min="1" max="1" width="50.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -19350,18 +19376,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="42.1328125" customWidth="1"/>
-    <col min="2" max="2" width="26.3984375" customWidth="1"/>
-    <col min="3" max="3" width="42.86328125" customWidth="1"/>
+    <col min="1" max="1" width="42.08984375" customWidth="1"/>
+    <col min="2" max="2" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -19519,7 +19545,7 @@
       </c>
       <c r="D16" s="4">
         <f>BNVFE!D8</f>
-        <v>4.010435677007162E-4</v>
+        <v>3.7068404566156505E-4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -19537,7 +19563,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.5">
+    <row r="20" spans="1:4" ht="29">
       <c r="A20" s="22" t="s">
         <v>68</v>
       </c>
@@ -19555,7 +19581,7 @@
         <v>6.7042622950819668</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.5">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="22" t="s">
         <v>70</v>
       </c>
@@ -19639,7 +19665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BT15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -19647,11 +19673,11 @@
       <selection pane="topRight" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="15" max="15" width="11.3984375" customWidth="1"/>
-    <col min="39" max="39" width="9.1328125" style="13"/>
+    <col min="15" max="15" width="11.36328125" customWidth="1"/>
+    <col min="39" max="39" width="9.08984375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -19897,175 +19923,175 @@
       </c>
       <c r="AB2" s="17">
         <f>($AN$2-$AA$2)/COUNT($AB$1:$AN$1)+AA2</f>
-        <v>3.2092630056054029E-4</v>
+        <v>3.1859095271137485E-4</v>
       </c>
       <c r="AC2" s="17">
         <f t="shared" ref="AC2:AM2" si="0">($AN$2-$AA$2)/COUNT($AB$1:$AN$1)+AB2</f>
-        <v>3.2760273948888828E-4</v>
+        <v>3.2293204379055739E-4</v>
       </c>
       <c r="AD2" s="17">
         <f t="shared" si="0"/>
-        <v>3.3427917841723627E-4</v>
+        <v>3.2727313486973994E-4</v>
       </c>
       <c r="AE2" s="17">
         <f t="shared" si="0"/>
-        <v>3.4095561734558426E-4</v>
+        <v>3.3161422594892248E-4</v>
       </c>
       <c r="AF2" s="17">
         <f t="shared" si="0"/>
-        <v>3.4763205627393225E-4</v>
+        <v>3.3595531702810503E-4</v>
       </c>
       <c r="AG2" s="17">
         <f t="shared" si="0"/>
-        <v>3.5430849520228023E-4</v>
+        <v>3.4029640810728757E-4</v>
       </c>
       <c r="AH2" s="17">
         <f t="shared" si="0"/>
-        <v>3.6098493413062822E-4</v>
+        <v>3.4463749918647011E-4</v>
       </c>
       <c r="AI2" s="17">
         <f t="shared" si="0"/>
-        <v>3.6766137305897621E-4</v>
+        <v>3.4897859026565266E-4</v>
       </c>
       <c r="AJ2" s="17">
         <f t="shared" si="0"/>
-        <v>3.743378119873242E-4</v>
+        <v>3.533196813448352E-4</v>
       </c>
       <c r="AK2" s="17">
         <f t="shared" si="0"/>
-        <v>3.8101425091567219E-4</v>
+        <v>3.5766077242401775E-4</v>
       </c>
       <c r="AL2" s="17">
         <f t="shared" si="0"/>
-        <v>3.8769068984402017E-4</v>
+        <v>3.6200186350320029E-4</v>
       </c>
       <c r="AM2" s="31">
         <f t="shared" si="0"/>
-        <v>3.9436712877236816E-4</v>
+        <v>3.6634295458238284E-4</v>
       </c>
       <c r="AN2" s="15">
         <f>BNVFE!D8</f>
-        <v>4.010435677007162E-4</v>
+        <v>3.7068404566156505E-4</v>
       </c>
       <c r="AO2" s="15">
         <f>BNVFE!E8</f>
-        <v>4.1543936179917892E-4</v>
+        <v>3.8286968063361244E-4</v>
       </c>
       <c r="AP2" s="15">
         <f>BNVFE!F8</f>
-        <v>4.232456921304615E-4</v>
+        <v>3.8999540362380768E-4</v>
       </c>
       <c r="AQ2" s="15">
         <f>BNVFE!G8</f>
-        <v>4.284224989356039E-4</v>
+        <v>3.9439145706872869E-4</v>
       </c>
       <c r="AR2" s="15">
         <f>BNVFE!H8</f>
-        <v>4.3223887309206766E-4</v>
+        <v>3.9758791642567675E-4</v>
       </c>
       <c r="AS2" s="15">
         <f>BNVFE!I8</f>
-        <v>4.3661930301858122E-4</v>
+        <v>4.1670440259151796E-4</v>
       </c>
       <c r="AT2" s="15">
         <f>BNVFE!J8</f>
-        <v>4.4073837767711228E-4</v>
+        <v>4.5449874343080136E-4</v>
       </c>
       <c r="AU2" s="15">
         <f>BNVFE!K8</f>
-        <v>4.4130433819121803E-4</v>
+        <v>4.5571840174311271E-4</v>
       </c>
       <c r="AV2" s="15">
         <f>BNVFE!L8</f>
-        <v>4.4139330713525239E-4</v>
+        <v>4.5632492494806224E-4</v>
       </c>
       <c r="AW2" s="15">
         <f>BNVFE!M8</f>
-        <v>4.4143859386227608E-4</v>
+        <v>4.5682343934192723E-4</v>
       </c>
       <c r="AX2" s="15">
         <f>BNVFE!N8</f>
-        <v>4.4252278985937798E-4</v>
+        <v>4.5864796428233097E-4</v>
       </c>
       <c r="AY2" s="15">
         <f>BNVFE!O8</f>
-        <v>4.4258101673758966E-4</v>
+        <v>4.5942511490356416E-4</v>
       </c>
       <c r="AZ2" s="15">
         <f>BNVFE!P8</f>
-        <v>4.4262644410952699E-4</v>
+        <v>4.6038567019040524E-4</v>
       </c>
       <c r="BA2" s="15">
         <f>BNVFE!Q8</f>
-        <v>4.4263525674443374E-4</v>
+        <v>4.6137990440500237E-4</v>
       </c>
       <c r="BB2" s="15">
         <f>BNVFE!R8</f>
-        <v>4.428907913418545E-4</v>
+        <v>4.627584500454361E-4</v>
       </c>
       <c r="BC2" s="15">
         <f>BNVFE!S8</f>
-        <v>4.4235185104972023E-4</v>
+        <v>4.6332164296180965E-4</v>
       </c>
       <c r="BD2" s="15">
         <f>BNVFE!T8</f>
-        <v>4.4180682000362565E-4</v>
+        <v>4.6388593065941057E-4</v>
       </c>
       <c r="BE2" s="15">
         <f>BNVFE!U8</f>
-        <v>4.415169210975881E-4</v>
+        <v>4.6479081055883617E-4</v>
       </c>
       <c r="BF2" s="15">
         <f>BNVFE!V8</f>
-        <v>4.4141525513386555E-4</v>
+        <v>4.6598088096797761E-4</v>
       </c>
       <c r="BG2" s="15">
         <f>BNVFE!W8</f>
-        <v>4.4094858868260617E-4</v>
+        <v>4.6672534660756901E-4</v>
       </c>
       <c r="BH2" s="15">
         <f>BNVFE!X8</f>
-        <v>4.406528424788466E-4</v>
+        <v>4.6768413007742366E-4</v>
       </c>
       <c r="BI2" s="15">
         <f>BNVFE!Y8</f>
-        <v>4.4046477188487546E-4</v>
+        <v>4.6835837126328925E-4</v>
       </c>
       <c r="BJ2" s="15">
         <f>BNVFE!Z8</f>
-        <v>4.4016736396697124E-4</v>
+        <v>4.6888408232764332E-4</v>
       </c>
       <c r="BK2" s="15">
         <f>BNVFE!AA8</f>
-        <v>4.3991921468742256E-4</v>
+        <v>4.6949898925199146E-4</v>
       </c>
       <c r="BL2" s="15">
         <f>BNVFE!AB8</f>
-        <v>4.3980677282836695E-4</v>
+        <v>4.7032072339820558E-4</v>
       </c>
       <c r="BM2" s="15">
         <f>BNVFE!AC8</f>
-        <v>4.3981133028276362E-4</v>
+        <v>4.7135545011319722E-4</v>
       </c>
       <c r="BN2" s="15">
         <f>BNVFE!AD8</f>
-        <v>4.3960459654073496E-4</v>
+        <v>4.7215508696463892E-4</v>
       </c>
       <c r="BO2" s="15">
         <f>BNVFE!AE8</f>
-        <v>4.3945697770705547E-4</v>
+        <v>4.730119981602886E-4</v>
       </c>
       <c r="BP2" s="15">
         <f>BNVFE!AF8</f>
-        <v>4.3919624527100954E-4</v>
+        <v>4.737905892831368E-4</v>
       </c>
       <c r="BQ2" s="15">
         <f>BNVFE!AG8</f>
-        <v>4.3913823303573507E-4</v>
+        <v>4.7491927991846777E-4</v>
       </c>
       <c r="BR2" s="15">
         <f>BNVFE!AH8</f>
-        <v>4.3909651675542918E-4</v>
+        <v>4.7615242132589445E-4</v>
       </c>
       <c r="BS2" s="15"/>
       <c r="BT2" s="4"/>
@@ -23090,7 +23116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -23100,9 +23126,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -23344,123 +23370,123 @@
       </c>
       <c r="C3" s="4">
         <f>BNVFE!C25*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.0495642992099084E-4</v>
+        <v>3.0273729318629119E-4</v>
       </c>
       <c r="D3" s="4">
         <f>BNVFE!D25*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.1206914647141513E-4</v>
+        <v>3.0761991621687003E-4</v>
       </c>
       <c r="E3" s="4">
         <f>BNVFE!E25*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.1882187840910213E-4</v>
+        <v>3.1213979915246134E-4</v>
       </c>
       <c r="F3" s="4">
         <f>BNVFE!F25*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.2511303052032729E-4</v>
+        <v>3.1620568917810511E-4</v>
       </c>
       <c r="G3" s="4">
         <f>BNVFE!G25*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.3132507899165593E-4</v>
+        <v>3.2019608072131204E-4</v>
       </c>
       <c r="H3" s="4">
         <f>BNVFE!H25*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.3654940106272427E-4</v>
+        <v>3.2323964534612426E-4</v>
       </c>
       <c r="I3" s="4">
         <f>BNVFE!I25*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.4251086081258395E-4</v>
+        <v>3.2700003616200409E-4</v>
       </c>
       <c r="J3" s="4">
         <f>BNVFE!J25*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.4855887390285254E-4</v>
+        <v>3.3084678824742565E-4</v>
       </c>
       <c r="K3" s="4">
         <f>BNVFE!K25*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.5467038374657962E-4</v>
+        <v>3.347565299442292E-4</v>
       </c>
       <c r="L3" s="4">
         <f>BNVFE!L25*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.606941984468817E-4</v>
+        <v>3.3858619543846379E-4</v>
       </c>
       <c r="M3" s="4">
         <f>BNVFE!M25*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.6680695227320973E-4</v>
+        <v>3.4250190615166639E-4</v>
       </c>
       <c r="N3" s="4">
         <f>BNVFE!N25*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.7287562060881878E-4</v>
+        <v>3.4637865729529685E-4</v>
       </c>
       <c r="O3" s="4">
         <f>BNVFE!O25*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.7896305858214533E-4</v>
+        <v>3.5027505993149845E-4</v>
       </c>
       <c r="P3" s="4">
         <f>BNVFE!P25*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.9236503637815238E-4</v>
+        <v>3.6160433984711515E-4</v>
       </c>
       <c r="Q3" s="4">
         <f>BNVFE!Q25*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.9958069974953693E-4</v>
+        <v>3.6818953902328103E-4</v>
       </c>
       <c r="R3" s="4">
         <f>BNVFE!R25*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>4.0425029377326959E-4</v>
+        <v>3.7213933156593097E-4</v>
       </c>
       <c r="S3" s="4">
         <f>BNVFE!S25*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>4.0766085158771333E-4</v>
+        <v>3.7498022200458688E-4</v>
       </c>
       <c r="T3" s="4">
         <f>BNVFE!T25*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>4.1161322090888235E-4</v>
+        <v>3.9283888763458292E-4</v>
       </c>
       <c r="U3" s="4">
         <f>BNVFE!U25*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>4.1531514899510258E-4</v>
+        <v>4.2828177192306375E-4</v>
       </c>
       <c r="V3" s="4">
         <f>BNVFE!V25*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>4.1564996463107134E-4</v>
+        <v>4.2922609449666765E-4</v>
       </c>
       <c r="W3" s="4">
         <f>BNVFE!W25*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.1549338417832383E-4</v>
+        <v>4.2954884971441691E-4</v>
       </c>
       <c r="X3" s="4">
         <f>BNVFE!X25*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.1532681156711845E-4</v>
+        <v>4.2980161940757162E-4</v>
       </c>
       <c r="Y3" s="4">
         <f>BNVFE!Y25*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.1611003974718208E-4</v>
+        <v>4.3127275480689105E-4</v>
       </c>
       <c r="Z3" s="4">
         <f>BNVFE!Z25*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.159197079205367E-4</v>
+        <v>4.3174910892155335E-4</v>
       </c>
       <c r="AA3" s="4">
         <f>BNVFE!AA25*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.1570872142824807E-4</v>
+        <v>4.3238794442968778E-4</v>
       </c>
       <c r="AB3" s="4">
         <f>BNVFE!AB25*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.1548706556389424E-4</v>
+        <v>4.3308204592944482E-4</v>
       </c>
       <c r="AC3" s="4">
         <f>BNVFE!AC25*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.1544768876733244E-4</v>
+        <v>4.3408427605020098E-4</v>
       </c>
       <c r="AD3" s="4">
         <f>BNVFE!AD25*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.1466296916326439E-4</v>
+        <v>4.3432016321901044E-4</v>
       </c>
       <c r="AE3" s="4">
         <f>BNVFE!AE25*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.1384514251470114E-4</v>
+        <v>4.3452688005751722E-4</v>
       </c>
       <c r="AF3" s="4">
         <f>BNVFE!AF25*('BHNVFEAL-LDVs-psgr'!AF$4/BNVFE!AF$26)</f>
-        <v>4.1327648701805351E-4</v>
+        <v>4.3506172517354685E-4</v>
       </c>
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
@@ -23475,123 +23501,123 @@
       </c>
       <c r="C4" s="29">
         <f>Extrapolations!AB2</f>
-        <v>3.2092630056054029E-4</v>
+        <v>3.1859095271137485E-4</v>
       </c>
       <c r="D4" s="29">
         <f>Extrapolations!AC2</f>
-        <v>3.2760273948888828E-4</v>
+        <v>3.2293204379055739E-4</v>
       </c>
       <c r="E4" s="29">
         <f>Extrapolations!AD2</f>
-        <v>3.3427917841723627E-4</v>
+        <v>3.2727313486973994E-4</v>
       </c>
       <c r="F4" s="29">
         <f>Extrapolations!AE2</f>
-        <v>3.4095561734558426E-4</v>
+        <v>3.3161422594892248E-4</v>
       </c>
       <c r="G4" s="29">
         <f>Extrapolations!AF2</f>
-        <v>3.4763205627393225E-4</v>
+        <v>3.3595531702810503E-4</v>
       </c>
       <c r="H4" s="29">
         <f>Extrapolations!AG2</f>
-        <v>3.5430849520228023E-4</v>
+        <v>3.4029640810728757E-4</v>
       </c>
       <c r="I4" s="29">
         <f>Extrapolations!AH2</f>
-        <v>3.6098493413062822E-4</v>
+        <v>3.4463749918647011E-4</v>
       </c>
       <c r="J4" s="29">
         <f>Extrapolations!AI2</f>
-        <v>3.6766137305897621E-4</v>
+        <v>3.4897859026565266E-4</v>
       </c>
       <c r="K4" s="29">
         <f>Extrapolations!AJ2</f>
-        <v>3.743378119873242E-4</v>
+        <v>3.533196813448352E-4</v>
       </c>
       <c r="L4" s="29">
         <f>Extrapolations!AK2</f>
-        <v>3.8101425091567219E-4</v>
+        <v>3.5766077242401775E-4</v>
       </c>
       <c r="M4" s="29">
         <f>Extrapolations!AL2</f>
-        <v>3.8769068984402017E-4</v>
+        <v>3.6200186350320029E-4</v>
       </c>
       <c r="N4" s="29">
         <f>Extrapolations!AM2</f>
-        <v>3.9436712877236816E-4</v>
+        <v>3.6634295458238284E-4</v>
       </c>
       <c r="O4" s="29">
         <f>Extrapolations!AN2</f>
-        <v>4.010435677007162E-4</v>
+        <v>3.7068404566156505E-4</v>
       </c>
       <c r="P4" s="29">
         <f>Extrapolations!AO2</f>
-        <v>4.1543936179917892E-4</v>
+        <v>3.8286968063361244E-4</v>
       </c>
       <c r="Q4" s="29">
         <f>Extrapolations!AP2</f>
-        <v>4.232456921304615E-4</v>
+        <v>3.8999540362380768E-4</v>
       </c>
       <c r="R4" s="29">
         <f>Extrapolations!AQ2</f>
-        <v>4.284224989356039E-4</v>
+        <v>3.9439145706872869E-4</v>
       </c>
       <c r="S4" s="29">
         <f>Extrapolations!AR2</f>
-        <v>4.3223887309206766E-4</v>
+        <v>3.9758791642567675E-4</v>
       </c>
       <c r="T4" s="29">
         <f>Extrapolations!AS2</f>
-        <v>4.3661930301858122E-4</v>
+        <v>4.1670440259151796E-4</v>
       </c>
       <c r="U4" s="29">
         <f>Extrapolations!AT2</f>
-        <v>4.4073837767711228E-4</v>
+        <v>4.5449874343080136E-4</v>
       </c>
       <c r="V4" s="29">
         <f>Extrapolations!AU2</f>
-        <v>4.4130433819121803E-4</v>
+        <v>4.5571840174311271E-4</v>
       </c>
       <c r="W4" s="29">
         <f>Extrapolations!AV2</f>
-        <v>4.4139330713525239E-4</v>
+        <v>4.5632492494806224E-4</v>
       </c>
       <c r="X4" s="29">
         <f>Extrapolations!AW2</f>
-        <v>4.4143859386227608E-4</v>
+        <v>4.5682343934192723E-4</v>
       </c>
       <c r="Y4" s="29">
         <f>Extrapolations!AX2</f>
-        <v>4.4252278985937798E-4</v>
+        <v>4.5864796428233097E-4</v>
       </c>
       <c r="Z4" s="29">
         <f>Extrapolations!AY2</f>
-        <v>4.4258101673758966E-4</v>
+        <v>4.5942511490356416E-4</v>
       </c>
       <c r="AA4" s="29">
         <f>Extrapolations!AZ2</f>
-        <v>4.4262644410952699E-4</v>
+        <v>4.6038567019040524E-4</v>
       </c>
       <c r="AB4" s="29">
         <f>Extrapolations!BA2</f>
-        <v>4.4263525674443374E-4</v>
+        <v>4.6137990440500237E-4</v>
       </c>
       <c r="AC4" s="29">
         <f>Extrapolations!BB2</f>
-        <v>4.428907913418545E-4</v>
+        <v>4.627584500454361E-4</v>
       </c>
       <c r="AD4" s="29">
         <f>Extrapolations!BC2</f>
-        <v>4.4235185104972023E-4</v>
+        <v>4.6332164296180965E-4</v>
       </c>
       <c r="AE4" s="29">
         <f>Extrapolations!BD2</f>
-        <v>4.4180682000362565E-4</v>
+        <v>4.6388593065941057E-4</v>
       </c>
       <c r="AF4" s="29">
         <f>Extrapolations!BE2</f>
-        <v>4.415169210975881E-4</v>
+        <v>4.6479081055883617E-4</v>
       </c>
       <c r="AH4" s="29"/>
       <c r="AI4" s="29"/>
@@ -23606,123 +23632,123 @@
       </c>
       <c r="C5" s="4">
         <f>BNVFE!C27*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.3247079907851041E-4</v>
+        <v>3.3005144309496473E-4</v>
       </c>
       <c r="D5" s="4">
         <f>BNVFE!D27*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.3608525156768267E-4</v>
+        <v>3.3129361905197572E-4</v>
       </c>
       <c r="E5" s="4">
         <f>BNVFE!E27*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.4140601212844754E-4</v>
+        <v>3.3425059969841139E-4</v>
       </c>
       <c r="F5" s="4">
         <f>BNVFE!F27*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.4682483192820804E-4</v>
+        <v>3.3732263769440833E-4</v>
       </c>
       <c r="G5" s="4">
         <f>BNVFE!G27*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.5399117808755025E-4</v>
+        <v>3.4210083999227872E-4</v>
       </c>
       <c r="H5" s="4">
         <f>BNVFE!H27*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.5770234384308779E-4</v>
+        <v>3.4355603783043959E-4</v>
       </c>
       <c r="I5" s="4">
         <f>BNVFE!I27*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.6308195251352201E-4</v>
+        <v>3.4663955274299627E-4</v>
       </c>
       <c r="J5" s="4">
         <f>BNVFE!J27*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.6931237060169403E-4</v>
+        <v>3.5054569205335479E-4</v>
       </c>
       <c r="K5" s="4">
         <f>BNVFE!K27*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.7541688009215464E-4</v>
+        <v>3.5433816247802349E-4</v>
       </c>
       <c r="L5" s="4">
         <f>BNVFE!L27*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.8060604014518434E-4</v>
+        <v>3.5727758208629781E-4</v>
       </c>
       <c r="M5" s="4">
         <f>BNVFE!M27*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.8660972321779061E-4</v>
+        <v>3.6099252295587557E-4</v>
       </c>
       <c r="N5" s="4">
         <f>BNVFE!N27*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.926877010252523E-4</v>
+        <v>3.6478286887036809E-4</v>
       </c>
       <c r="O5" s="4">
         <f>BNVFE!O27*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.9870114016606978E-4</v>
+        <v>3.6851894295167754E-4</v>
       </c>
       <c r="P5" s="4">
         <f>BNVFE!P27*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>4.1235135875181372E-4</v>
+        <v>3.8002377134032826E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>BNVFE!Q27*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>4.2000791936622607E-4</v>
+        <v>3.8701199110595277E-4</v>
       </c>
       <c r="R5" s="4">
         <f>BNVFE!R27*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>4.2525292156963163E-4</v>
+        <v>3.9147364990695831E-4</v>
       </c>
       <c r="S5" s="4">
         <f>BNVFE!S27*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>4.2886235816476826E-4</v>
+        <v>3.9448208393744698E-4</v>
       </c>
       <c r="T5" s="4">
         <f>BNVFE!T27*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>4.3285917396080627E-4</v>
+        <v>4.1311577899687946E-4</v>
       </c>
       <c r="U5" s="4">
         <f>BNVFE!U27*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>4.3707582192698479E-4</v>
+        <v>4.5072183842209402E-4</v>
       </c>
       <c r="V5" s="4">
         <f>BNVFE!V27*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>4.3740782672530476E-4</v>
+        <v>4.5169462081927711E-4</v>
       </c>
       <c r="W5" s="4">
         <f>BNVFE!W27*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.3733077971452199E-4</v>
+        <v>4.521249688309292E-4</v>
       </c>
       <c r="X5" s="4">
         <f>BNVFE!X27*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.3727737730799265E-4</v>
+        <v>4.525171976933608E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>BNVFE!Y27*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.3826191917219735E-4</v>
+        <v>4.542318308954683E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>BNVFE!Z27*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.381057457924663E-4</v>
+        <v>4.5477952055940612E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>BNVFE!AA27*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.3788374849786256E-4</v>
+        <v>4.5545268634648259E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>BNVFE!AB27*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.3769898244799599E-4</v>
+        <v>4.5623458954744165E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>BNVFE!AC27*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.3777480871824145E-4</v>
+        <v>4.5741296931825801E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>BNVFE!AD27*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.3716325908544007E-4</v>
+        <v>4.5788708459420266E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>BNVFE!AE27*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.363360192507078E-4</v>
+        <v>4.5814172893183499E-4</v>
       </c>
       <c r="AF5" s="4">
         <f>BNVFE!AF27*('BHNVFEAL-LDVs-psgr'!AF$4/BNVFE!AF$26)</f>
-        <v>4.3573558513369061E-4</v>
+        <v>4.5870472030867576E-4</v>
       </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -23737,123 +23763,123 @@
       </c>
       <c r="C6" s="4">
         <f>BNVFE!C28*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>5.2428092566616732E-4</v>
+        <v>5.2046578701914962E-4</v>
       </c>
       <c r="D6" s="4">
         <f>BNVFE!D28*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>5.3102064816912329E-4</v>
+        <v>5.2344978395413549E-4</v>
       </c>
       <c r="E6" s="4">
         <f>BNVFE!E28*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>5.3833911588692471E-4</v>
+        <v>5.2705624955022199E-4</v>
       </c>
       <c r="F6" s="4">
         <f>BNVFE!F28*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>5.5418108584188324E-4</v>
+        <v>5.3899781223055879E-4</v>
       </c>
       <c r="G6" s="4">
         <f>BNVFE!G28*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>5.8181999979491409E-4</v>
+        <v>5.6227703675971281E-4</v>
       </c>
       <c r="H6" s="4">
         <f>BNVFE!H28*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>6.1507401996100622E-4</v>
+        <v>5.9074925537233765E-4</v>
       </c>
       <c r="I6" s="4">
         <f>BNVFE!I28*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>6.2764405946183748E-4</v>
+        <v>5.992207944996859E-4</v>
       </c>
       <c r="J6" s="4">
         <f>BNVFE!J28*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>6.3817589517729746E-4</v>
+        <v>6.0574686534929938E-4</v>
       </c>
       <c r="K6" s="4">
         <f>BNVFE!K28*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>6.4869543049513468E-4</v>
+        <v>6.1227280668123567E-4</v>
       </c>
       <c r="L6" s="4">
         <f>BNVFE!L28*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>6.581047918396357E-4</v>
+        <v>6.1776762317850031E-4</v>
       </c>
       <c r="M6" s="4">
         <f>BNVFE!M28*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>6.6834810198910361E-4</v>
+        <v>6.2406259610263957E-4</v>
       </c>
       <c r="N6" s="4">
         <f>BNVFE!N28*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>6.7910400948621805E-4</v>
+        <v>6.3084611052237143E-4</v>
       </c>
       <c r="O6" s="4">
         <f>BNVFE!O28*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>6.8981170811608045E-4</v>
+        <v>6.3759206057134501E-4</v>
       </c>
       <c r="P6" s="4">
         <f>BNVFE!P28*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>7.1344718240657083E-4</v>
+        <v>6.575142367202969E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>BNVFE!Q28*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>7.2661438980298719E-4</v>
+        <v>6.6953137976117814E-4</v>
       </c>
       <c r="R6" s="4">
         <f>BNVFE!R28*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>7.356760015799844E-4</v>
+        <v>6.7723877927624405E-4</v>
       </c>
       <c r="S6" s="4">
         <f>BNVFE!S28*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>7.4187120383651457E-4</v>
+        <v>6.8239819357187139E-4</v>
       </c>
       <c r="T6" s="4">
         <f>BNVFE!T28*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>7.4853261641737515E-4</v>
+        <v>7.143908539728348E-4</v>
       </c>
       <c r="U6" s="4">
         <f>BNVFE!U28*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>7.5506233584725639E-4</v>
+        <v>7.7863626186398447E-4</v>
       </c>
       <c r="V6" s="4">
         <f>BNVFE!V28*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>7.5521763030150985E-4</v>
+        <v>7.7988485873460188E-4</v>
       </c>
       <c r="W6" s="4">
         <f>BNVFE!W28*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>7.5422055105138291E-4</v>
+        <v>7.7973460582479433E-4</v>
       </c>
       <c r="X6" s="4">
         <f>BNVFE!X28*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>7.5304546398064301E-4</v>
+        <v>7.7929031040680061E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>BNVFE!Y28*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>7.5349566500976337E-4</v>
+        <v>7.8095244080447995E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>BNVFE!Z28*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>7.5171922103753558E-4</v>
+        <v>7.8032874533602939E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>BNVFE!AA28*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>7.4943614758610189E-4</v>
+        <v>7.795053089642472E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>BNVFE!AB28*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>7.4699197436416847E-4</v>
+        <v>7.7862547203833433E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>BNVFE!AC28*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>7.4464449629104302E-4</v>
+        <v>7.7804853854486272E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>BNVFE!AD28*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>7.4057257931631681E-4</v>
+        <v>7.7567959389579684E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>BNVFE!AE28*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>7.3602635790278052E-4</v>
+        <v>7.728089666492378E-4</v>
       </c>
       <c r="AF6" s="4">
         <f>BNVFE!AF28*('BHNVFEAL-LDVs-psgr'!AF$4/BNVFE!AF$26)</f>
-        <v>7.3135170735541761E-4</v>
+        <v>7.6990379444637376E-4</v>
       </c>
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
@@ -23868,123 +23894,123 @@
       </c>
       <c r="C7" s="4">
         <f>BNVFE!C29*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>2.898398018603075E-4</v>
+        <v>2.8773066728113853E-4</v>
       </c>
       <c r="D7" s="4">
         <f>BNVFE!D29*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>2.9639229529668671E-4</v>
+        <v>2.9216657294521781E-4</v>
       </c>
       <c r="E7" s="4">
         <f>BNVFE!E29*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.0225117678650028E-4</v>
+        <v>2.9591639722626953E-4</v>
       </c>
       <c r="F7" s="4">
         <f>BNVFE!F29*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.0778031687736323E-4</v>
+        <v>2.99347851600729E-4</v>
       </c>
       <c r="G7" s="4">
         <f>BNVFE!G29*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.1364712087038462E-4</v>
+        <v>3.0311191394826462E-4</v>
       </c>
       <c r="H7" s="4">
         <f>BNVFE!H29*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.1818917619505965E-4</v>
+        <v>3.0560552519627761E-4</v>
       </c>
       <c r="I7" s="4">
         <f>BNVFE!I29*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.2376820979030025E-4</v>
+        <v>3.0910615814739656E-4</v>
       </c>
       <c r="J7" s="4">
         <f>BNVFE!J29*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.2959142944700965E-4</v>
+        <v>3.1284317809912674E-4</v>
       </c>
       <c r="K7" s="4">
         <f>BNVFE!K29*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.3540222212257912E-4</v>
+        <v>3.1657022733976996E-4</v>
       </c>
       <c r="L7" s="4">
         <f>BNVFE!L29*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.4090374402748674E-4</v>
+        <v>3.2000875588796858E-4</v>
       </c>
       <c r="M7" s="4">
         <f>BNVFE!M29*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.4686163891380382E-4</v>
+        <v>3.2387819195526624E-4</v>
       </c>
       <c r="N7" s="4">
         <f>BNVFE!N29*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.5254200312831522E-4</v>
+        <v>3.2748996966977387E-4</v>
       </c>
       <c r="O7" s="4">
         <f>BNVFE!O29*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.582922320064483E-4</v>
+        <v>3.3116904193405711E-4</v>
       </c>
       <c r="P7" s="4">
         <f>BNVFE!P29*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.7083340468707854E-4</v>
+        <v>3.417607484421509E-4</v>
       </c>
       <c r="Q7" s="4">
         <f>BNVFE!Q29*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.7782282401531729E-4</v>
+        <v>3.4814096750386184E-4</v>
       </c>
       <c r="R7" s="4">
         <f>BNVFE!R29*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.8233661580785696E-4</v>
+        <v>3.519663308388775E-4</v>
       </c>
       <c r="S7" s="4">
         <f>BNVFE!S29*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.8550736662354158E-4</v>
+        <v>3.5460269819358875E-4</v>
       </c>
       <c r="T7" s="4">
         <f>BNVFE!T29*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.8922118122167398E-4</v>
+        <v>3.7146818447016827E-4</v>
       </c>
       <c r="U7" s="4">
         <f>BNVFE!U29*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.9278680995063548E-4</v>
+        <v>4.0505007188083468E-4</v>
       </c>
       <c r="V7" s="4">
         <f>BNVFE!V29*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.9308720014886002E-4</v>
+        <v>4.0592637573368492E-4</v>
       </c>
       <c r="W7" s="4">
         <f>BNVFE!W29*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.9293845521070378E-4</v>
+        <v>4.0623092417730792E-4</v>
       </c>
       <c r="X7" s="4">
         <f>BNVFE!X29*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.9281882697013573E-4</v>
+        <v>4.0650919532138791E-4</v>
       </c>
       <c r="Y7" s="4">
         <f>BNVFE!Y29*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.9354272058642249E-4</v>
+        <v>4.0788310069284843E-4</v>
       </c>
       <c r="Z7" s="4">
         <f>BNVFE!Z29*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.9331686794151E-4</v>
+        <v>4.0828603219255716E-4</v>
       </c>
       <c r="AA7" s="4">
         <f>BNVFE!AA29*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.930117319368427E-4</v>
+        <v>4.0878029771683217E-4</v>
       </c>
       <c r="AB7" s="4">
         <f>BNVFE!AB29*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.9280440477488073E-4</v>
+        <v>4.0943882341830048E-4</v>
       </c>
       <c r="AC7" s="4">
         <f>BNVFE!AC29*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.9272510536214313E-4</v>
+        <v>4.1034237921428937E-4</v>
       </c>
       <c r="AD7" s="4">
         <f>BNVFE!AD29*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.9200385857580093E-4</v>
+        <v>4.1058689224812239E-4</v>
       </c>
       <c r="AE7" s="4">
         <f>BNVFE!AE29*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.9112433694300379E-4</v>
+        <v>4.1067061175031487E-4</v>
       </c>
       <c r="AF7" s="4">
         <f>BNVFE!AF29*('BHNVFEAL-LDVs-psgr'!AF$4/BNVFE!AF$26)</f>
-        <v>3.9051236766252144E-4</v>
+        <v>4.1109763007020822E-4</v>
       </c>
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
@@ -24161,7 +24187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -24171,9 +24197,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -25191,7 +25217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -25201,9 +25227,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">

</xml_diff>

<commit_message>
update bcdtrtsy, bhnvfeal, bnvfe, syfafe to match epa 2021 inventory. updated calibration sheet
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C752FB79-D71E-41B0-B3B0-DB2CFF5FF23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F09EAEE-3EAE-4E97-9875-D813368FD5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="75" windowWidth="15405" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3696,181 +3696,181 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>3.4326338356696702E-3</c:v>
+                  <c:v>1.1807374066651309E-3</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>3.3755616799663441E-3</c:v>
+                  <c:v>1.1611060587428182E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>3.318489524263018E-3</c:v>
+                  <c:v>1.1414747108205057E-3</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>3.2614173685596914E-3</c:v>
+                  <c:v>1.121843362898193E-3</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>3.2043452128563653E-3</c:v>
+                  <c:v>1.1022120149758803E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>3.1472730571530387E-3</c:v>
+                  <c:v>1.0825806670535676E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>3.0902009014497122E-3</c:v>
+                  <c:v>1.0629493191312547E-3</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>3.0331287457463856E-3</c:v>
+                  <c:v>1.043317971208942E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>2.9760565900430595E-3</c:v>
+                  <c:v>1.0236866232866293E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>2.9189844343397329E-3</c:v>
+                  <c:v>1.0040552753643166E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>2.8619122786364064E-3</c:v>
+                  <c:v>9.8442392744200395E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>2.8048401229330798E-3</c:v>
+                  <c:v>9.6479257951969115E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>2.7477679672297532E-3</c:v>
+                  <c:v>9.4516123159737835E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>2.6906958115264271E-3</c:v>
+                  <c:v>9.2552988367506565E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>2.6336236558231006E-3</c:v>
+                  <c:v>9.0589853575275296E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>2.5765515001197744E-3</c:v>
+                  <c:v>8.8626718783044037E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>2.5194793444164483E-3</c:v>
+                  <c:v>8.6663583990812768E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>2.4624071887131217E-3</c:v>
+                  <c:v>8.4700449198581499E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>2.4053350330097956E-3</c:v>
+                  <c:v>8.2737314406350229E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>2.2911907216031429E-3</c:v>
+                  <c:v>7.8811044821887691E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>2.4416893404631888E-3</c:v>
+                  <c:v>8.3987808713595574E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>2.5184424936439019E-3</c:v>
+                  <c:v>8.6627919001452318E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>2.5972597245510895E-3</c:v>
+                  <c:v>8.9339028233518841E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>2.6712322131487161E-3</c:v>
+                  <c:v>9.1883490839571541E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>2.7413284684994969E-3</c:v>
+                  <c:v>9.4294621030615396E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>2.8030530706552449E-3</c:v>
+                  <c:v>9.6417787967895108E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>2.8293185238036926E-3</c:v>
+                  <c:v>9.7321251737118614E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>2.8691599474660314E-3</c:v>
+                  <c:v>9.8691693837994168E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>2.9102408430290473E-3</c:v>
+                  <c:v>1.0010477057185716E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>2.9488442594546977E-3</c:v>
+                  <c:v>1.0143262842040467E-3</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>2.9718288652678219E-3</c:v>
+                  <c:v>1.022232395126511E-3</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>2.973873170030446E-3</c:v>
+                  <c:v>1.0229355831795947E-3</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>2.9741148395886286E-3</c:v>
+                  <c:v>1.0230187112675467E-3</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.9740804199848872E-3</c:v>
+                  <c:v>1.0230068718125956E-3</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>2.974117402750609E-3</c:v>
+                  <c:v>1.0230195929290854E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>2.9740189040973501E-3</c:v>
+                  <c:v>1.0229857119356625E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>2.9738284977787817E-3</c:v>
+                  <c:v>1.0229202170784881E-3</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>2.9731170372461332E-3</c:v>
+                  <c:v>1.022675493025624E-3</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>2.9728588902180751E-3</c:v>
+                  <c:v>1.0225866971134939E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>2.9723678616157684E-3</c:v>
+                  <c:v>1.0224177959529731E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>2.970316965865194E-3</c:v>
+                  <c:v>1.0217123407702182E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>2.9689965712791254E-3</c:v>
+                  <c:v>1.0212581591260447E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>2.969104224082315E-3</c:v>
+                  <c:v>1.0212951889106777E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>2.9694304779858613E-3</c:v>
+                  <c:v>1.0214074118294128E-3</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>2.9701628099803533E-3</c:v>
+                  <c:v>1.0216593151262368E-3</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>2.9710357497177878E-3</c:v>
+                  <c:v>1.021959583856051E-3</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>2.9721562176693601E-3</c:v>
+                  <c:v>1.0223449959001912E-3</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>2.973041607050701E-3</c:v>
+                  <c:v>1.0226495469860513E-3</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>2.9740906726328101E-3</c:v>
+                  <c:v>1.0230103984587512E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7788,14 +7788,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="107.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.40625" customWidth="1"/>
+    <col min="2" max="2" width="107.40625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8023,12 +8023,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -9022,12 +9022,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -9899,12 +9899,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -10776,14 +10776,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="2" max="2" width="10.40625" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -11688,12 +11688,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -12565,12 +12565,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -13556,12 +13556,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -14433,12 +14433,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -14539,123 +14539,123 @@
       </c>
       <c r="B2" s="4">
         <f t="array" ref="B2:B8">TRANSPOSE(SYFAFE!B7:H7)</f>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:AE8" si="0">C2</f>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="K2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="L2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="N2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="O2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="P2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="Q2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="R2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="T2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="U2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="V2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="W2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="X2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="Y2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="Z2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AA2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AB2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
@@ -14665,123 +14665,123 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:C8" si="1">B3</f>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:Q3" si="2">C3</f>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="F3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="J3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="K3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Q3" s="4">
         <f t="shared" si="2"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="R3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="V3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="W3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="X3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AB3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AC3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AD3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -14791,123 +14791,123 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AA4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AC4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AE4" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -14917,123 +14917,123 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="T5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="U5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="V5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="W5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Y5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="Z5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AA5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AB5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AC5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AD5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AE5" s="4">
         <f t="shared" si="0"/>
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -15043,123 +15043,123 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="O6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="T6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="U6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="V6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="W6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="X6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="Y6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AA6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AB6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AC6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AD6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AE6" s="4">
         <f t="shared" si="0"/>
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -15169,123 +15169,123 @@
         <v>84</v>
       </c>
       <c r="B7" s="4">
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="K7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="T7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="U7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="V7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="W7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="X7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="Y7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="Z7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AA7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AB7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AC7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AD7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AE7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -15295,123 +15295,123 @@
         <v>85</v>
       </c>
       <c r="B8" s="4">
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AB8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AC8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AD8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" si="0"/>
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4"/>
@@ -15432,12 +15432,12 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="30">
+    <row r="1" spans="1:31">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -16206,15 +16206,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.40625" customWidth="1"/>
+    <col min="2" max="2" width="16.40625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -16598,94 +16598,94 @@
         <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>2.2911907216031429E-3</v>
+        <v>7.8811044821887691E-4</v>
       </c>
       <c r="E10" s="4">
-        <v>2.4416893404631888E-3</v>
+        <v>8.3987808713595574E-4</v>
       </c>
       <c r="F10" s="4">
-        <v>2.5184424936439019E-3</v>
+        <v>8.6627919001452318E-4</v>
       </c>
       <c r="G10" s="4">
-        <v>2.5972597245510895E-3</v>
+        <v>8.9339028233518841E-4</v>
       </c>
       <c r="H10" s="4">
-        <v>2.6712322131487161E-3</v>
+        <v>9.1883490839571541E-4</v>
       </c>
       <c r="I10" s="4">
-        <v>2.7413284684994969E-3</v>
+        <v>9.4294621030615396E-4</v>
       </c>
       <c r="J10" s="4">
-        <v>2.8030530706552449E-3</v>
+        <v>9.6417787967895108E-4</v>
       </c>
       <c r="K10" s="4">
-        <v>2.8293185238036926E-3</v>
+        <v>9.7321251737118614E-4</v>
       </c>
       <c r="L10" s="4">
-        <v>2.8691599474660314E-3</v>
+        <v>9.8691693837994168E-4</v>
       </c>
       <c r="M10" s="4">
-        <v>2.9102408430290473E-3</v>
+        <v>1.0010477057185716E-3</v>
       </c>
       <c r="N10" s="4">
-        <v>2.9488442594546977E-3</v>
+        <v>1.0143262842040467E-3</v>
       </c>
       <c r="O10" s="4">
-        <v>2.9718288652678219E-3</v>
+        <v>1.022232395126511E-3</v>
       </c>
       <c r="P10" s="4">
-        <v>2.973873170030446E-3</v>
+        <v>1.0229355831795947E-3</v>
       </c>
       <c r="Q10" s="4">
-        <v>2.9741148395886286E-3</v>
+        <v>1.0230187112675467E-3</v>
       </c>
       <c r="R10" s="4">
-        <v>2.9740804199848872E-3</v>
+        <v>1.0230068718125956E-3</v>
       </c>
       <c r="S10" s="4">
-        <v>2.974117402750609E-3</v>
+        <v>1.0230195929290854E-3</v>
       </c>
       <c r="T10" s="4">
-        <v>2.9740189040973501E-3</v>
+        <v>1.0229857119356625E-3</v>
       </c>
       <c r="U10" s="4">
-        <v>2.9738284977787817E-3</v>
+        <v>1.0229202170784881E-3</v>
       </c>
       <c r="V10" s="4">
-        <v>2.9731170372461332E-3</v>
+        <v>1.022675493025624E-3</v>
       </c>
       <c r="W10" s="4">
-        <v>2.9728588902180751E-3</v>
+        <v>1.0225866971134939E-3</v>
       </c>
       <c r="X10" s="4">
-        <v>2.9723678616157684E-3</v>
+        <v>1.0224177959529731E-3</v>
       </c>
       <c r="Y10" s="4">
-        <v>2.970316965865194E-3</v>
+        <v>1.0217123407702182E-3</v>
       </c>
       <c r="Z10" s="4">
-        <v>2.9689965712791254E-3</v>
+        <v>1.0212581591260447E-3</v>
       </c>
       <c r="AA10" s="4">
-        <v>2.969104224082315E-3</v>
+        <v>1.0212951889106777E-3</v>
       </c>
       <c r="AB10" s="4">
-        <v>2.9694304779858613E-3</v>
+        <v>1.0214074118294128E-3</v>
       </c>
       <c r="AC10" s="4">
-        <v>2.9701628099803533E-3</v>
+        <v>1.0216593151262368E-3</v>
       </c>
       <c r="AD10" s="4">
-        <v>2.9710357497177878E-3</v>
+        <v>1.021959583856051E-3</v>
       </c>
       <c r="AE10" s="4">
-        <v>2.9721562176693601E-3</v>
+        <v>1.0223449959001912E-3</v>
       </c>
       <c r="AF10" s="4">
-        <v>2.973041607050701E-3</v>
+        <v>1.0226495469860513E-3</v>
       </c>
       <c r="AG10" s="4">
-        <v>2.9740906726328101E-3</v>
+        <v>1.0230103984587512E-3</v>
       </c>
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
@@ -18512,11 +18512,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -18575,25 +18575,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="C3">
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="D3">
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="E3">
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="F3">
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="G3">
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="H3">
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -18679,25 +18679,25 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>4.1164543276724285E-3</v>
+        <v>4.5678462664228052E-3</v>
       </c>
       <c r="C7">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="D7">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="E7">
-        <v>1.2927707805913415E-3</v>
+        <v>1.4345302324303027E-3</v>
       </c>
       <c r="F7">
-        <v>2.8457967314859398E-3</v>
+        <v>3.1578540511261791E-3</v>
       </c>
       <c r="G7">
-        <v>1.0018973549582896E-3</v>
+        <v>1.1117609301334846E-3</v>
       </c>
       <c r="H7">
-        <v>3.8783123417740241E-3</v>
+        <v>4.3035906972909077E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -18893,9 +18893,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.40625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -19002,11 +19002,11 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="42.1328125" customWidth="1"/>
+    <col min="2" max="2" width="26.40625" customWidth="1"/>
+    <col min="3" max="3" width="42.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -19176,7 +19176,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="29.5">
       <c r="A20" s="13" t="s">
         <v>68</v>
       </c>
@@ -19194,7 +19194,7 @@
         <v>6.7042622950819668</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="29.5">
       <c r="A22" s="13" t="s">
         <v>70</v>
       </c>
@@ -19286,11 +19286,11 @@
       <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" style="26"/>
+    <col min="15" max="15" width="11.40625" customWidth="1"/>
+    <col min="40" max="40" width="8.7265625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -19937,239 +19937,239 @@
       <c r="K4" s="9"/>
       <c r="L4" s="4">
         <f>L5/M5*M4</f>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4:AI4" si="1">M5/N5*N4</f>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4326338356696702E-3</v>
+        <v>1.1807374066651309E-3</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="1"/>
-        <v>3.3755616799663441E-3</v>
+        <v>1.1611060587428182E-3</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="1"/>
-        <v>3.318489524263018E-3</v>
+        <v>1.1414747108205057E-3</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="1"/>
-        <v>3.2614173685596914E-3</v>
+        <v>1.121843362898193E-3</v>
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="1"/>
-        <v>3.2043452128563653E-3</v>
+        <v>1.1022120149758803E-3</v>
       </c>
       <c r="AA4" s="4">
         <f t="shared" si="1"/>
-        <v>3.1472730571530387E-3</v>
+        <v>1.0825806670535676E-3</v>
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="1"/>
-        <v>3.0902009014497122E-3</v>
+        <v>1.0629493191312547E-3</v>
       </c>
       <c r="AC4" s="4">
         <f t="shared" si="1"/>
-        <v>3.0331287457463856E-3</v>
+        <v>1.043317971208942E-3</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="1"/>
-        <v>2.9760565900430595E-3</v>
+        <v>1.0236866232866293E-3</v>
       </c>
       <c r="AE4" s="4">
         <f t="shared" si="1"/>
-        <v>2.9189844343397329E-3</v>
+        <v>1.0040552753643166E-3</v>
       </c>
       <c r="AF4" s="4">
         <f t="shared" si="1"/>
-        <v>2.8619122786364064E-3</v>
+        <v>9.8442392744200395E-4</v>
       </c>
       <c r="AG4" s="4">
         <f>AG5/AH5*AH4</f>
-        <v>2.8048401229330798E-3</v>
+        <v>9.6479257951969115E-4</v>
       </c>
       <c r="AH4" s="4">
         <f t="shared" si="1"/>
-        <v>2.7477679672297532E-3</v>
+        <v>9.4516123159737835E-4</v>
       </c>
       <c r="AI4" s="4">
         <f t="shared" si="1"/>
-        <v>2.6906958115264271E-3</v>
+        <v>9.2552988367506565E-4</v>
       </c>
       <c r="AJ4" s="4">
         <f>AJ5/AK5*AK4</f>
-        <v>2.6336236558231006E-3</v>
+        <v>9.0589853575275296E-4</v>
       </c>
       <c r="AK4" s="19">
         <f>AK5/AL5*AL4</f>
-        <v>2.5765515001197744E-3</v>
+        <v>8.8626718783044037E-4</v>
       </c>
       <c r="AL4" s="19">
         <f>AL5/AM5*AM4</f>
-        <v>2.5194793444164483E-3</v>
+        <v>8.6663583990812768E-4</v>
       </c>
       <c r="AM4" s="19">
         <f>AM5/AN5*AN4</f>
-        <v>2.4624071887131217E-3</v>
+        <v>8.4700449198581499E-4</v>
       </c>
       <c r="AN4" s="29">
         <f>AN5/AO5*AO4</f>
-        <v>2.4053350330097956E-3</v>
+        <v>8.2737314406350229E-4</v>
       </c>
       <c r="AO4" s="10">
         <f>BNVFE!D10</f>
-        <v>2.2911907216031429E-3</v>
+        <v>7.8811044821887691E-4</v>
       </c>
       <c r="AP4" s="10">
         <f>BNVFE!E10</f>
-        <v>2.4416893404631888E-3</v>
+        <v>8.3987808713595574E-4</v>
       </c>
       <c r="AQ4" s="10">
         <f>BNVFE!F10</f>
-        <v>2.5184424936439019E-3</v>
+        <v>8.6627919001452318E-4</v>
       </c>
       <c r="AR4" s="10">
         <f>BNVFE!G10</f>
-        <v>2.5972597245510895E-3</v>
+        <v>8.9339028233518841E-4</v>
       </c>
       <c r="AS4" s="10">
         <f>BNVFE!H10</f>
-        <v>2.6712322131487161E-3</v>
+        <v>9.1883490839571541E-4</v>
       </c>
       <c r="AT4" s="10">
         <f>BNVFE!I10</f>
-        <v>2.7413284684994969E-3</v>
+        <v>9.4294621030615396E-4</v>
       </c>
       <c r="AU4" s="10">
         <f>BNVFE!J10</f>
-        <v>2.8030530706552449E-3</v>
+        <v>9.6417787967895108E-4</v>
       </c>
       <c r="AV4" s="10">
         <f>BNVFE!K10</f>
-        <v>2.8293185238036926E-3</v>
+        <v>9.7321251737118614E-4</v>
       </c>
       <c r="AW4" s="10">
         <f>BNVFE!L10</f>
-        <v>2.8691599474660314E-3</v>
+        <v>9.8691693837994168E-4</v>
       </c>
       <c r="AX4" s="10">
         <f>BNVFE!M10</f>
-        <v>2.9102408430290473E-3</v>
+        <v>1.0010477057185716E-3</v>
       </c>
       <c r="AY4" s="10">
         <f>BNVFE!N10</f>
-        <v>2.9488442594546977E-3</v>
+        <v>1.0143262842040467E-3</v>
       </c>
       <c r="AZ4" s="10">
         <f>BNVFE!O10</f>
-        <v>2.9718288652678219E-3</v>
+        <v>1.022232395126511E-3</v>
       </c>
       <c r="BA4" s="10">
         <f>BNVFE!P10</f>
-        <v>2.973873170030446E-3</v>
+        <v>1.0229355831795947E-3</v>
       </c>
       <c r="BB4" s="10">
         <f>BNVFE!Q10</f>
-        <v>2.9741148395886286E-3</v>
+        <v>1.0230187112675467E-3</v>
       </c>
       <c r="BC4" s="10">
         <f>BNVFE!R10</f>
-        <v>2.9740804199848872E-3</v>
+        <v>1.0230068718125956E-3</v>
       </c>
       <c r="BD4" s="10">
         <f>BNVFE!S10</f>
-        <v>2.974117402750609E-3</v>
+        <v>1.0230195929290854E-3</v>
       </c>
       <c r="BE4" s="10">
         <f>BNVFE!T10</f>
-        <v>2.9740189040973501E-3</v>
+        <v>1.0229857119356625E-3</v>
       </c>
       <c r="BF4" s="10">
         <f>BNVFE!U10</f>
-        <v>2.9738284977787817E-3</v>
+        <v>1.0229202170784881E-3</v>
       </c>
       <c r="BG4" s="10">
         <f>BNVFE!V10</f>
-        <v>2.9731170372461332E-3</v>
+        <v>1.022675493025624E-3</v>
       </c>
       <c r="BH4" s="10">
         <f>BNVFE!W10</f>
-        <v>2.9728588902180751E-3</v>
+        <v>1.0225866971134939E-3</v>
       </c>
       <c r="BI4" s="10">
         <f>BNVFE!X10</f>
-        <v>2.9723678616157684E-3</v>
+        <v>1.0224177959529731E-3</v>
       </c>
       <c r="BJ4" s="10">
         <f>BNVFE!Y10</f>
-        <v>2.970316965865194E-3</v>
+        <v>1.0217123407702182E-3</v>
       </c>
       <c r="BK4" s="10">
         <f>BNVFE!Z10</f>
-        <v>2.9689965712791254E-3</v>
+        <v>1.0212581591260447E-3</v>
       </c>
       <c r="BL4" s="10">
         <f>BNVFE!AA10</f>
-        <v>2.969104224082315E-3</v>
+        <v>1.0212951889106777E-3</v>
       </c>
       <c r="BM4" s="10">
         <f>BNVFE!AB10</f>
-        <v>2.9694304779858613E-3</v>
+        <v>1.0214074118294128E-3</v>
       </c>
       <c r="BN4" s="10">
         <f>BNVFE!AC10</f>
-        <v>2.9701628099803533E-3</v>
+        <v>1.0216593151262368E-3</v>
       </c>
       <c r="BO4" s="10">
         <f>BNVFE!AD10</f>
-        <v>2.9710357497177878E-3</v>
+        <v>1.021959583856051E-3</v>
       </c>
       <c r="BP4" s="10">
         <f>BNVFE!AE10</f>
-        <v>2.9721562176693601E-3</v>
+        <v>1.0223449959001912E-3</v>
       </c>
       <c r="BQ4" s="10">
         <f>BNVFE!AF10</f>
-        <v>2.973041607050701E-3</v>
+        <v>1.0226495469860513E-3</v>
       </c>
       <c r="BR4" s="10">
         <f>BNVFE!AG10</f>
-        <v>2.9740906726328101E-3</v>
+        <v>1.0230103984587512E-3</v>
       </c>
       <c r="BS4" s="10"/>
       <c r="BT4" s="4"/>
@@ -22740,12 +22740,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -23779,12 +23779,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -24778,12 +24778,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -24884,123 +24884,123 @@
       </c>
       <c r="B2" s="4">
         <f t="array" ref="B2:B8">TRANSPOSE(SYFAFE!B3:H3)</f>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:AE8" si="0">C2</f>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="K2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="L2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="N2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="O2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="P2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="Q2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="R2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="T2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="U2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="V2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="W2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="X2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="Y2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="Z2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AA2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AB2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>2.8703352303668895E-3</v>
+        <v>3.4003581782857295E-3</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
@@ -25010,123 +25010,123 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:C8" si="1">B3</f>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:Q3" si="2">C3</f>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="F3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="J3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="K3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="Q3" s="4">
         <f t="shared" si="2"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="R3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="V3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="W3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="X3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AB3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AC3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AD3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>7.9831680311033635E-4</v>
+        <v>2.8226770072497282E-3</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -25136,123 +25136,123 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AA4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AC4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AE4" s="4">
         <f t="shared" si="0"/>
-        <v>8.9290515403996041E-4</v>
+        <v>9.1563612345912568E-4</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -25262,123 +25262,123 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="T5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="U5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="V5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="W5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="Y5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="Z5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AA5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AB5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AC5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AD5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AE5" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671645E-4</v>
+        <v>1.0581562199094108E-3</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -25388,123 +25388,123 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="O6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="T6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="U6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="V6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="W6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="X6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="Y6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AA6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AB6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AC6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AD6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AE6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9806327342263117E-3</v>
+        <v>2.3463672970163861E-3</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -25514,123 +25514,123 @@
         <v>84</v>
       </c>
       <c r="B7" s="4">
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="K7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="T7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="U7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="V7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="W7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="X7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="Y7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="Z7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AA7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AB7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AC7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AD7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AE7" s="4">
         <f t="shared" si="0"/>
-        <v>8.9321857227671634E-4</v>
+        <v>3.076266427557592E-3</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -25640,123 +25640,123 @@
         <v>85</v>
       </c>
       <c r="B8" s="4">
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AB8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AC8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AD8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" si="0"/>
-        <v>2.679655716830149E-3</v>
+        <v>3.1744686597282318E-3</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4"/>

</xml_diff>

<commit_message>
Remove efficiency adjustment for HDVs that had been incorrectly applied
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F09EAEE-3EAE-4E97-9875-D813368FD5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21AF18-E41A-4B31-8D96-6A3A3B048707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="75" windowWidth="15405" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3233,136 +3233,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>5.2911336018791888E-5</c:v>
+                  <c:v>7.5108389563240119E-5</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>5.4633355406983469E-5</c:v>
+                  <c:v>7.7552820431472588E-5</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>5.6355374795175051E-5</c:v>
+                  <c:v>7.9997251299705058E-5</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>5.8077394183367066E-5</c:v>
+                  <c:v>8.2441682167937527E-5</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>5.9799413571558647E-5</c:v>
+                  <c:v>8.4886113036169997E-5</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>6.1521432959750228E-5</c:v>
+                  <c:v>8.7330543904402466E-5</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>6.3243452347942243E-5</c:v>
+                  <c:v>8.9774974772634936E-5</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>6.4965471736133824E-5</c:v>
+                  <c:v>9.2219405640867405E-5</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>6.6687491124325406E-5</c:v>
+                  <c:v>9.4663836509099875E-5</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>6.8409510512516987E-5</c:v>
+                  <c:v>9.7108267377332344E-5</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>7.0131529900709002E-5</c:v>
+                  <c:v>9.9552698245564814E-5</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>7.1853549288900583E-5</c:v>
+                  <c:v>1.0199712911379728E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>7.3575568677092164E-5</c:v>
+                  <c:v>1.0444155998202975E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>7.5297588065284179E-5</c:v>
+                  <c:v>1.0688599085026222E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>7.5722348919915995E-5</c:v>
+                  <c:v>1.0748894488887501E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>8.0144525754122377E-5</c:v>
+                  <c:v>1.1376628742778099E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>8.0922650602619964E-5</c:v>
+                  <c:v>1.1487084665170681E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>8.2247994269403775E-5</c:v>
+                  <c:v>1.1675219072501874E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>8.3280711603233847E-5</c:v>
+                  <c:v>1.1821814758141852E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>8.2910808979344075E-5</c:v>
+                  <c:v>1.1769306557695523E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>8.2709536945446978E-5</c:v>
+                  <c:v>1.1740735707916262E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>8.1373982016617121E-5</c:v>
+                  <c:v>1.1551151797500483E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>8.0659892904163668E-5</c:v>
+                  <c:v>1.1449785838376007E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>7.9807124660185322E-5</c:v>
+                  <c:v>1.13287341804607E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>7.8987634533903321E-5</c:v>
+                  <c:v>1.1212406398402511E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>7.8028009936033827E-5</c:v>
+                  <c:v>1.1076186329973974E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>7.7122766808563597E-5</c:v>
+                  <c:v>1.0947685788155618E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>7.6319490121400875E-5</c:v>
+                  <c:v>1.0833659526703707E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>7.5555840180256291E-5</c:v>
+                  <c:v>1.0725258337875167E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.4865315441272314E-5</c:v>
+                  <c:v>1.0627237374881068E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>7.4241753709387812E-5</c:v>
+                  <c:v>1.053872190542009E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>7.3666550441435144E-5</c:v>
+                  <c:v>1.0457070988285631E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>7.3143235881095107E-5</c:v>
+                  <c:v>1.0382785746559407E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>7.268369834764319E-5</c:v>
+                  <c:v>1.0317553743970813E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>7.2282905818000628E-5</c:v>
+                  <c:v>1.0260660677729319E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>7.1941486288945263E-5</c:v>
+                  <c:v>1.0212195692865432E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>7.1603868596124793E-5</c:v>
+                  <c:v>1.0164270384030296E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>7.129639337962048E-5</c:v>
+                  <c:v>1.0120623842325044E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>7.1056851476574028E-5</c:v>
+                  <c:v>1.0086620530512349E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>7.082859882864499E-5</c:v>
+                  <c:v>1.0054219744424832E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>7.0341451089990512E-5</c:v>
+                  <c:v>9.9850684341711718E-5</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>7.0180331309609449E-5</c:v>
+                  <c:v>9.9621972535475967E-5</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>7.008295989492991E-5</c:v>
+                  <c:v>9.9483752435656976E-5</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>7.001263722126285E-5</c:v>
+                  <c:v>9.9383928406132565E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3696,181 +3696,181 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1.1807374066651309E-3</c:v>
+                  <c:v>1.1807374066651307E-3</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>1.1611060587428182E-3</c:v>
+                  <c:v>1.177387347221569E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.1414747108205057E-3</c:v>
+                  <c:v>1.1740372877780075E-3</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>1.121843362898193E-3</c:v>
+                  <c:v>1.1706872283344459E-3</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.1022120149758803E-3</c:v>
+                  <c:v>1.1673371688908844E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1.0825806670535676E-3</c:v>
+                  <c:v>1.163987109447323E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.0629493191312547E-3</c:v>
+                  <c:v>1.1606370500037615E-3</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>1.043317971208942E-3</c:v>
+                  <c:v>1.1572869905602E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>1.0236866232866293E-3</c:v>
+                  <c:v>1.1539369311166386E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>1.0040552753643166E-3</c:v>
+                  <c:v>1.1505868716730771E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>9.8442392744200395E-4</c:v>
+                  <c:v>1.1472368122295155E-3</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>9.6479257951969115E-4</c:v>
+                  <c:v>1.143886752785954E-3</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>9.4516123159737835E-4</c:v>
+                  <c:v>1.1405366933423926E-3</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>9.2552988367506565E-4</c:v>
+                  <c:v>1.1371866338988309E-3</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>9.0589853575275296E-4</c:v>
+                  <c:v>1.1338365744552694E-3</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>8.8626718783044037E-4</c:v>
+                  <c:v>1.130486515011708E-3</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>8.6663583990812768E-4</c:v>
+                  <c:v>1.1271364555681463E-3</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>8.4700449198581499E-4</c:v>
+                  <c:v>1.1237863961245848E-3</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>8.2737314406350229E-4</c:v>
+                  <c:v>1.1204363366810234E-3</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>7.8811044821887691E-4</c:v>
+                  <c:v>1.1137362177939013E-3</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>8.3987808713595574E-4</c:v>
+                  <c:v>1.1868928349938494E-3</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>8.6627919001452318E-4</c:v>
+                  <c:v>1.2242021544325342E-3</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>8.9339028233518841E-4</c:v>
+                  <c:v>1.2625148116111296E-3</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>9.1883490839571541E-4</c:v>
+                  <c:v>1.2984724640643824E-3</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>9.4294621030615396E-4</c:v>
+                  <c:v>1.3325458991476347E-3</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>9.6417787967895108E-4</c:v>
+                  <c:v>1.3625499159680566E-3</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>9.7321251737118614E-4</c:v>
+                  <c:v>1.3753174198569201E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>9.8691693837994168E-4</c:v>
+                  <c:v>1.3946841343267524E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.0010477057185716E-3</c:v>
+                  <c:v>1.4146533498165595E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>1.0143262842040467E-3</c:v>
+                  <c:v>1.4334182752321722E-3</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.022232395126511E-3</c:v>
+                  <c:v>1.4445909758303492E-3</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>1.0229355831795947E-3</c:v>
+                  <c:v>1.4455847020325701E-3</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>1.0230187112675467E-3</c:v>
+                  <c:v>1.4457021763821076E-3</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>1.0230068718125956E-3</c:v>
+                  <c:v>1.4456854451868699E-3</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>1.0230195929290854E-3</c:v>
+                  <c:v>1.4457034223221783E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>1.0229857119356625E-3</c:v>
+                  <c:v>1.4456555426251702E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>1.0229202170784881E-3</c:v>
+                  <c:v>1.4455629870770495E-3</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>1.022675493025624E-3</c:v>
+                  <c:v>1.4452171497116701E-3</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>1.0225866971134939E-3</c:v>
+                  <c:v>1.4450916657473916E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>1.0224177959529731E-3</c:v>
+                  <c:v>1.4448529792281048E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.0217123407702182E-3</c:v>
+                  <c:v>1.443856049179987E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.0212581591260447E-3</c:v>
+                  <c:v>1.4432142120520614E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.0212951889106777E-3</c:v>
+                  <c:v>1.443266541535037E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.0214074118294128E-3</c:v>
+                  <c:v>1.4434251319069122E-3</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>1.0216593151262368E-3</c:v>
+                  <c:v>1.4437811147842976E-3</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>1.021959583856051E-3</c:v>
+                  <c:v>1.4442054463741406E-3</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>1.0223449959001912E-3</c:v>
+                  <c:v>1.4447501001765403E-3</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>1.0226495469860513E-3</c:v>
+                  <c:v>1.4451804834752992E-3</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>1.0230103984587512E-3</c:v>
+                  <c:v>1.4456904289471535E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4237,148 +4237,148 @@
                   <c:v>7.8040477200267344E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>7.6742949272979222E-4</c:v>
+                  <c:v>7.7819056047563108E-4</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>7.54454213456911E-4</c:v>
+                  <c:v>7.7597634894858872E-4</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>7.4147893418402978E-4</c:v>
+                  <c:v>7.7376213742154636E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>7.2850365491114856E-4</c:v>
+                  <c:v>7.71547925894504E-4</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>7.1552837563826734E-4</c:v>
+                  <c:v>7.6933371436746164E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>7.0255309636538612E-4</c:v>
+                  <c:v>7.6711950284041929E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>6.895778170925049E-4</c:v>
+                  <c:v>7.6490529131337693E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>6.7660253781962369E-4</c:v>
+                  <c:v>7.6269107978633457E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>6.6362725854674247E-4</c:v>
+                  <c:v>7.6047686825929221E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>6.5065197927386125E-4</c:v>
+                  <c:v>7.5826265673224985E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>6.3767670000098003E-4</c:v>
+                  <c:v>7.5604844520520749E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>6.2470142072809881E-4</c:v>
+                  <c:v>7.5383423367816514E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>6.1172614145521759E-4</c:v>
+                  <c:v>7.5162002215112278E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>5.9875086218233637E-4</c:v>
+                  <c:v>7.4940581062408042E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>5.8577558290945516E-4</c:v>
+                  <c:v>7.4719159909703806E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>5.7280030363657394E-4</c:v>
+                  <c:v>7.449773875699957E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>5.5982502436369272E-4</c:v>
+                  <c:v>7.4276317604295334E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>5.468497450908115E-4</c:v>
+                  <c:v>7.4054896451591099E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>5.2089918654504906E-4</c:v>
+                  <c:v>7.3612054146182692E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>5.5511484890837198E-4</c:v>
+                  <c:v>7.8447318350072194E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>5.7256457698191549E-4</c:v>
+                  <c:v>8.0913266389472246E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>5.9048357040231516E-4</c:v>
+                  <c:v>8.3445529729440947E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>6.0730111805293394E-4</c:v>
+                  <c:v>8.582213975349269E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>6.2323740919090079E-4</c:v>
+                  <c:v>8.8074213007663328E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>6.3727041602424229E-4</c:v>
+                  <c:v>9.0057319308330108E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>6.4324183213127449E-4</c:v>
+                  <c:v>9.0901183566816969E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>6.5229972721649369E-4</c:v>
+                  <c:v>9.2181220627128113E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>6.616394146024239E-4</c:v>
+                  <c:v>9.3501079807791388E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>6.7041585037635684E-4</c:v>
+                  <c:v>9.4741341804908898E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>6.7564137017190565E-4</c:v>
+                  <c:v>9.5479798028431191E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>6.7610614016152745E-4</c:v>
+                  <c:v>9.5545478057360543E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>6.7616108341661443E-4</c:v>
+                  <c:v>9.5553242488507497E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>6.7615325816513226E-4</c:v>
+                  <c:v>9.5552136645283517E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>6.761616661481077E-4</c:v>
+                  <c:v>9.5553324838534815E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>6.7613927260929199E-4</c:v>
+                  <c:v>9.5550160244627959E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>6.7609598398407189E-4</c:v>
+                  <c:v>9.5544042814027313E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>6.7593423437099028E-4</c:v>
+                  <c:v>9.5521184799302321E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>6.7587554498487476E-4</c:v>
+                  <c:v>9.5512890975122625E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>6.7576391028022079E-4</c:v>
+                  <c:v>9.5497115062746795E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>6.7529764183818757E-4</c:v>
+                  <c:v>9.5431223276604333E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>6.749974518717581E-4</c:v>
+                  <c:v>9.5388801248246955E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>6.7502192659447849E-4</c:v>
+                  <c:v>9.5392259949394229E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>6.750960999888459E-4</c:v>
+                  <c:v>9.5402741931442593E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>6.7526259470123058E-4</c:v>
+                  <c:v>9.5426270510675759E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>6.7546105639839315E-4</c:v>
+                  <c:v>9.5454316577121671E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>6.7571579330834156E-4</c:v>
+                  <c:v>9.5490315303348411E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>6.7591708541561474E-4</c:v>
+                  <c:v>9.5518761355641295E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>6.7615558909110566E-4</c:v>
+                  <c:v>9.555246604539279E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7788,14 +7788,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.40625" customWidth="1"/>
-    <col min="2" max="2" width="107.40625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="107.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8023,12 +8023,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -9022,12 +9022,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -9899,12 +9899,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -10776,14 +10776,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
-    <col min="2" max="2" width="10.40625" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -11688,12 +11688,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -12565,12 +12565,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -13556,12 +13556,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -14433,12 +14433,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -15432,12 +15432,12 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -16206,15 +16206,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.40625" customWidth="1"/>
-    <col min="2" max="2" width="16.40625" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -16493,94 +16493,94 @@
         <v>4</v>
       </c>
       <c r="D9" s="4">
-        <v>7.5722348919915995E-5</v>
+        <v>1.0748894488887501E-4</v>
       </c>
       <c r="E9" s="4">
-        <v>8.0144525754122377E-5</v>
+        <v>1.1376628742778099E-4</v>
       </c>
       <c r="F9" s="4">
-        <v>8.0922650602619964E-5</v>
+        <v>1.1487084665170681E-4</v>
       </c>
       <c r="G9" s="4">
-        <v>8.2247994269403775E-5</v>
+        <v>1.1675219072501874E-4</v>
       </c>
       <c r="H9" s="4">
-        <v>8.3280711603233847E-5</v>
+        <v>1.1821814758141852E-4</v>
       </c>
       <c r="I9" s="4">
-        <v>8.2910808979344075E-5</v>
+        <v>1.1769306557695523E-4</v>
       </c>
       <c r="J9" s="4">
-        <v>8.2709536945446978E-5</v>
+        <v>1.1740735707916262E-4</v>
       </c>
       <c r="K9" s="4">
-        <v>8.1373982016617121E-5</v>
+        <v>1.1551151797500483E-4</v>
       </c>
       <c r="L9" s="4">
-        <v>8.0659892904163668E-5</v>
+        <v>1.1449785838376007E-4</v>
       </c>
       <c r="M9" s="4">
-        <v>7.9807124660185322E-5</v>
+        <v>1.13287341804607E-4</v>
       </c>
       <c r="N9" s="4">
-        <v>7.8987634533903321E-5</v>
+        <v>1.1212406398402511E-4</v>
       </c>
       <c r="O9" s="4">
-        <v>7.8028009936033827E-5</v>
+        <v>1.1076186329973974E-4</v>
       </c>
       <c r="P9" s="4">
-        <v>7.7122766808563597E-5</v>
+        <v>1.0947685788155618E-4</v>
       </c>
       <c r="Q9" s="4">
-        <v>7.6319490121400875E-5</v>
+        <v>1.0833659526703707E-4</v>
       </c>
       <c r="R9" s="4">
-        <v>7.5555840180256291E-5</v>
+        <v>1.0725258337875167E-4</v>
       </c>
       <c r="S9" s="4">
-        <v>7.4865315441272314E-5</v>
+        <v>1.0627237374881068E-4</v>
       </c>
       <c r="T9" s="4">
-        <v>7.4241753709387812E-5</v>
+        <v>1.053872190542009E-4</v>
       </c>
       <c r="U9" s="4">
-        <v>7.3666550441435144E-5</v>
+        <v>1.0457070988285631E-4</v>
       </c>
       <c r="V9" s="4">
-        <v>7.3143235881095107E-5</v>
+        <v>1.0382785746559407E-4</v>
       </c>
       <c r="W9" s="4">
-        <v>7.268369834764319E-5</v>
+        <v>1.0317553743970813E-4</v>
       </c>
       <c r="X9" s="4">
-        <v>7.2282905818000628E-5</v>
+        <v>1.0260660677729319E-4</v>
       </c>
       <c r="Y9" s="4">
-        <v>7.1941486288945263E-5</v>
+        <v>1.0212195692865432E-4</v>
       </c>
       <c r="Z9" s="4">
-        <v>7.1603868596124793E-5</v>
+        <v>1.0164270384030296E-4</v>
       </c>
       <c r="AA9" s="4">
-        <v>7.129639337962048E-5</v>
+        <v>1.0120623842325044E-4</v>
       </c>
       <c r="AB9" s="4">
-        <v>7.1056851476574028E-5</v>
+        <v>1.0086620530512349E-4</v>
       </c>
       <c r="AC9" s="4">
-        <v>7.082859882864499E-5</v>
+        <v>1.0054219744424832E-4</v>
       </c>
       <c r="AD9" s="4">
-        <v>7.0341451089990512E-5</v>
+        <v>9.9850684341711718E-5</v>
       </c>
       <c r="AE9" s="4">
-        <v>7.0180331309609449E-5</v>
+        <v>9.9621972535475967E-5</v>
       </c>
       <c r="AF9" s="4">
-        <v>7.008295989492991E-5</v>
+        <v>9.9483752435656976E-5</v>
       </c>
       <c r="AG9" s="4">
-        <v>7.001263722126285E-5</v>
+        <v>9.9383928406132565E-5</v>
       </c>
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
@@ -16598,94 +16598,94 @@
         <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>7.8811044821887691E-4</v>
+        <v>1.1137362177939013E-3</v>
       </c>
       <c r="E10" s="4">
-        <v>8.3987808713595574E-4</v>
+        <v>1.1868928349938494E-3</v>
       </c>
       <c r="F10" s="4">
-        <v>8.6627919001452318E-4</v>
+        <v>1.2242021544325342E-3</v>
       </c>
       <c r="G10" s="4">
-        <v>8.9339028233518841E-4</v>
+        <v>1.2625148116111296E-3</v>
       </c>
       <c r="H10" s="4">
-        <v>9.1883490839571541E-4</v>
+        <v>1.2984724640643824E-3</v>
       </c>
       <c r="I10" s="4">
-        <v>9.4294621030615396E-4</v>
+        <v>1.3325458991476347E-3</v>
       </c>
       <c r="J10" s="4">
-        <v>9.6417787967895108E-4</v>
+        <v>1.3625499159680566E-3</v>
       </c>
       <c r="K10" s="4">
-        <v>9.7321251737118614E-4</v>
+        <v>1.3753174198569201E-3</v>
       </c>
       <c r="L10" s="4">
-        <v>9.8691693837994168E-4</v>
+        <v>1.3946841343267524E-3</v>
       </c>
       <c r="M10" s="4">
-        <v>1.0010477057185716E-3</v>
+        <v>1.4146533498165595E-3</v>
       </c>
       <c r="N10" s="4">
-        <v>1.0143262842040467E-3</v>
+        <v>1.4334182752321722E-3</v>
       </c>
       <c r="O10" s="4">
-        <v>1.022232395126511E-3</v>
+        <v>1.4445909758303492E-3</v>
       </c>
       <c r="P10" s="4">
-        <v>1.0229355831795947E-3</v>
+        <v>1.4455847020325701E-3</v>
       </c>
       <c r="Q10" s="4">
-        <v>1.0230187112675467E-3</v>
+        <v>1.4457021763821076E-3</v>
       </c>
       <c r="R10" s="4">
-        <v>1.0230068718125956E-3</v>
+        <v>1.4456854451868699E-3</v>
       </c>
       <c r="S10" s="4">
-        <v>1.0230195929290854E-3</v>
+        <v>1.4457034223221783E-3</v>
       </c>
       <c r="T10" s="4">
-        <v>1.0229857119356625E-3</v>
+        <v>1.4456555426251702E-3</v>
       </c>
       <c r="U10" s="4">
-        <v>1.0229202170784881E-3</v>
+        <v>1.4455629870770495E-3</v>
       </c>
       <c r="V10" s="4">
-        <v>1.022675493025624E-3</v>
+        <v>1.4452171497116701E-3</v>
       </c>
       <c r="W10" s="4">
-        <v>1.0225866971134939E-3</v>
+        <v>1.4450916657473916E-3</v>
       </c>
       <c r="X10" s="4">
-        <v>1.0224177959529731E-3</v>
+        <v>1.4448529792281048E-3</v>
       </c>
       <c r="Y10" s="4">
-        <v>1.0217123407702182E-3</v>
+        <v>1.443856049179987E-3</v>
       </c>
       <c r="Z10" s="4">
-        <v>1.0212581591260447E-3</v>
+        <v>1.4432142120520614E-3</v>
       </c>
       <c r="AA10" s="4">
-        <v>1.0212951889106777E-3</v>
+        <v>1.443266541535037E-3</v>
       </c>
       <c r="AB10" s="4">
-        <v>1.0214074118294128E-3</v>
+        <v>1.4434251319069122E-3</v>
       </c>
       <c r="AC10" s="4">
-        <v>1.0216593151262368E-3</v>
+        <v>1.4437811147842976E-3</v>
       </c>
       <c r="AD10" s="4">
-        <v>1.021959583856051E-3</v>
+        <v>1.4442054463741406E-3</v>
       </c>
       <c r="AE10" s="4">
-        <v>1.0223449959001912E-3</v>
+        <v>1.4447501001765403E-3</v>
       </c>
       <c r="AF10" s="4">
-        <v>1.0226495469860513E-3</v>
+        <v>1.4451804834752992E-3</v>
       </c>
       <c r="AG10" s="4">
-        <v>1.0230103984587512E-3</v>
+        <v>1.4456904289471535E-3</v>
       </c>
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
@@ -16703,94 +16703,94 @@
         <v>5</v>
       </c>
       <c r="D11" s="4">
-        <v>5.2089918654504906E-4</v>
+        <v>7.3612054146182692E-4</v>
       </c>
       <c r="E11" s="4">
-        <v>5.5511484890837198E-4</v>
+        <v>7.8447318350072194E-4</v>
       </c>
       <c r="F11" s="4">
-        <v>5.7256457698191549E-4</v>
+        <v>8.0913266389472246E-4</v>
       </c>
       <c r="G11" s="4">
-        <v>5.9048357040231516E-4</v>
+        <v>8.3445529729440947E-4</v>
       </c>
       <c r="H11" s="4">
-        <v>6.0730111805293394E-4</v>
+        <v>8.582213975349269E-4</v>
       </c>
       <c r="I11" s="4">
-        <v>6.2323740919090079E-4</v>
+        <v>8.8074213007663328E-4</v>
       </c>
       <c r="J11" s="4">
-        <v>6.3727041602424229E-4</v>
+        <v>9.0057319308330108E-4</v>
       </c>
       <c r="K11" s="4">
-        <v>6.4324183213127449E-4</v>
+        <v>9.0901183566816969E-4</v>
       </c>
       <c r="L11" s="4">
-        <v>6.5229972721649369E-4</v>
+        <v>9.2181220627128113E-4</v>
       </c>
       <c r="M11" s="4">
-        <v>6.616394146024239E-4</v>
+        <v>9.3501079807791388E-4</v>
       </c>
       <c r="N11" s="4">
-        <v>6.7041585037635684E-4</v>
+        <v>9.4741341804908898E-4</v>
       </c>
       <c r="O11" s="4">
-        <v>6.7564137017190565E-4</v>
+        <v>9.5479798028431191E-4</v>
       </c>
       <c r="P11" s="4">
-        <v>6.7610614016152745E-4</v>
+        <v>9.5545478057360543E-4</v>
       </c>
       <c r="Q11" s="4">
-        <v>6.7616108341661443E-4</v>
+        <v>9.5553242488507497E-4</v>
       </c>
       <c r="R11" s="4">
-        <v>6.7615325816513226E-4</v>
+        <v>9.5552136645283517E-4</v>
       </c>
       <c r="S11" s="4">
-        <v>6.761616661481077E-4</v>
+        <v>9.5553324838534815E-4</v>
       </c>
       <c r="T11" s="4">
-        <v>6.7613927260929199E-4</v>
+        <v>9.5550160244627959E-4</v>
       </c>
       <c r="U11" s="4">
-        <v>6.7609598398407189E-4</v>
+        <v>9.5544042814027313E-4</v>
       </c>
       <c r="V11" s="4">
-        <v>6.7593423437099028E-4</v>
+        <v>9.5521184799302321E-4</v>
       </c>
       <c r="W11" s="4">
-        <v>6.7587554498487476E-4</v>
+        <v>9.5512890975122625E-4</v>
       </c>
       <c r="X11" s="4">
-        <v>6.7576391028022079E-4</v>
+        <v>9.5497115062746795E-4</v>
       </c>
       <c r="Y11" s="4">
-        <v>6.7529764183818757E-4</v>
+        <v>9.5431223276604333E-4</v>
       </c>
       <c r="Z11" s="4">
-        <v>6.749974518717581E-4</v>
+        <v>9.5388801248246955E-4</v>
       </c>
       <c r="AA11" s="4">
-        <v>6.7502192659447849E-4</v>
+        <v>9.5392259949394229E-4</v>
       </c>
       <c r="AB11" s="4">
-        <v>6.750960999888459E-4</v>
+        <v>9.5402741931442593E-4</v>
       </c>
       <c r="AC11" s="4">
-        <v>6.7526259470123058E-4</v>
+        <v>9.5426270510675759E-4</v>
       </c>
       <c r="AD11" s="4">
-        <v>6.7546105639839315E-4</v>
+        <v>9.5454316577121671E-4</v>
       </c>
       <c r="AE11" s="4">
-        <v>6.7571579330834156E-4</v>
+        <v>9.5490315303348411E-4</v>
       </c>
       <c r="AF11" s="4">
-        <v>6.7591708541561474E-4</v>
+        <v>9.5518761355641295E-4</v>
       </c>
       <c r="AG11" s="4">
-        <v>6.7615558909110566E-4</v>
+        <v>9.555246604539279E-4</v>
       </c>
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
@@ -18512,11 +18512,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -18893,9 +18893,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.40625" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -19002,11 +19002,11 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.1328125" customWidth="1"/>
-    <col min="2" max="2" width="26.40625" customWidth="1"/>
-    <col min="3" max="3" width="42.86328125" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -19176,7 +19176,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29.5">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" s="13" t="s">
         <v>68</v>
       </c>
@@ -19194,7 +19194,7 @@
         <v>6.7042622950819668</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="29.5">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="13" t="s">
         <v>70</v>
       </c>
@@ -19286,11 +19286,11 @@
       <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="15" max="15" width="11.40625" customWidth="1"/>
-    <col min="40" max="40" width="8.7265625" style="26"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -19742,179 +19742,179 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="4" cm="1">
         <f t="array" ref="AA3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AA1)</f>
-        <v>5.2911336018791888E-5</v>
+        <v>7.5108389563240119E-5</v>
       </c>
       <c r="AB3" s="4" cm="1">
         <f t="array" ref="AB3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AB1)</f>
-        <v>5.4633355406983469E-5</v>
+        <v>7.7552820431472588E-5</v>
       </c>
       <c r="AC3" s="4" cm="1">
         <f t="array" ref="AC3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AC1)</f>
-        <v>5.6355374795175051E-5</v>
+        <v>7.9997251299705058E-5</v>
       </c>
       <c r="AD3" s="4" cm="1">
         <f t="array" ref="AD3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AD1)</f>
-        <v>5.8077394183367066E-5</v>
+        <v>8.2441682167937527E-5</v>
       </c>
       <c r="AE3" s="4" cm="1">
         <f t="array" ref="AE3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AE1)</f>
-        <v>5.9799413571558647E-5</v>
+        <v>8.4886113036169997E-5</v>
       </c>
       <c r="AF3" s="4" cm="1">
         <f t="array" ref="AF3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AF1)</f>
-        <v>6.1521432959750228E-5</v>
+        <v>8.7330543904402466E-5</v>
       </c>
       <c r="AG3" s="4" cm="1">
         <f t="array" ref="AG3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AG1)</f>
-        <v>6.3243452347942243E-5</v>
+        <v>8.9774974772634936E-5</v>
       </c>
       <c r="AH3" s="4" cm="1">
         <f t="array" ref="AH3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AH1)</f>
-        <v>6.4965471736133824E-5</v>
+        <v>9.2219405640867405E-5</v>
       </c>
       <c r="AI3" s="4" cm="1">
         <f t="array" ref="AI3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AI1)</f>
-        <v>6.6687491124325406E-5</v>
+        <v>9.4663836509099875E-5</v>
       </c>
       <c r="AJ3" s="4" cm="1">
         <f t="array" ref="AJ3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AJ1)</f>
-        <v>6.8409510512516987E-5</v>
+        <v>9.7108267377332344E-5</v>
       </c>
       <c r="AK3" s="4" cm="1">
         <f t="array" ref="AK3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AK1)</f>
-        <v>7.0131529900709002E-5</v>
+        <v>9.9552698245564814E-5</v>
       </c>
       <c r="AL3" s="4" cm="1">
         <f t="array" ref="AL3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AL1)</f>
-        <v>7.1853549288900583E-5</v>
+        <v>1.0199712911379728E-4</v>
       </c>
       <c r="AM3" s="4" cm="1">
         <f t="array" ref="AM3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AM1)</f>
-        <v>7.3575568677092164E-5</v>
+        <v>1.0444155998202975E-4</v>
       </c>
       <c r="AN3" s="28" cm="1">
         <f t="array" ref="AN3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AN1)</f>
-        <v>7.5297588065284179E-5</v>
+        <v>1.0688599085026222E-4</v>
       </c>
       <c r="AO3" s="10">
         <f>BNVFE!D9</f>
-        <v>7.5722348919915995E-5</v>
+        <v>1.0748894488887501E-4</v>
       </c>
       <c r="AP3" s="10">
         <f>BNVFE!E9</f>
-        <v>8.0144525754122377E-5</v>
+        <v>1.1376628742778099E-4</v>
       </c>
       <c r="AQ3" s="10">
         <f>BNVFE!F9</f>
-        <v>8.0922650602619964E-5</v>
+        <v>1.1487084665170681E-4</v>
       </c>
       <c r="AR3" s="10">
         <f>BNVFE!G9</f>
-        <v>8.2247994269403775E-5</v>
+        <v>1.1675219072501874E-4</v>
       </c>
       <c r="AS3" s="10">
         <f>BNVFE!H9</f>
-        <v>8.3280711603233847E-5</v>
+        <v>1.1821814758141852E-4</v>
       </c>
       <c r="AT3" s="10">
         <f>BNVFE!I9</f>
-        <v>8.2910808979344075E-5</v>
+        <v>1.1769306557695523E-4</v>
       </c>
       <c r="AU3" s="10">
         <f>BNVFE!J9</f>
-        <v>8.2709536945446978E-5</v>
+        <v>1.1740735707916262E-4</v>
       </c>
       <c r="AV3" s="10">
         <f>BNVFE!K9</f>
-        <v>8.1373982016617121E-5</v>
+        <v>1.1551151797500483E-4</v>
       </c>
       <c r="AW3" s="10">
         <f>BNVFE!L9</f>
-        <v>8.0659892904163668E-5</v>
+        <v>1.1449785838376007E-4</v>
       </c>
       <c r="AX3" s="10">
         <f>BNVFE!M9</f>
-        <v>7.9807124660185322E-5</v>
+        <v>1.13287341804607E-4</v>
       </c>
       <c r="AY3" s="10">
         <f>BNVFE!N9</f>
-        <v>7.8987634533903321E-5</v>
+        <v>1.1212406398402511E-4</v>
       </c>
       <c r="AZ3" s="10">
         <f>BNVFE!O9</f>
-        <v>7.8028009936033827E-5</v>
+        <v>1.1076186329973974E-4</v>
       </c>
       <c r="BA3" s="10">
         <f>BNVFE!P9</f>
-        <v>7.7122766808563597E-5</v>
+        <v>1.0947685788155618E-4</v>
       </c>
       <c r="BB3" s="10">
         <f>BNVFE!Q9</f>
-        <v>7.6319490121400875E-5</v>
+        <v>1.0833659526703707E-4</v>
       </c>
       <c r="BC3" s="10">
         <f>BNVFE!R9</f>
-        <v>7.5555840180256291E-5</v>
+        <v>1.0725258337875167E-4</v>
       </c>
       <c r="BD3" s="10">
         <f>BNVFE!S9</f>
-        <v>7.4865315441272314E-5</v>
+        <v>1.0627237374881068E-4</v>
       </c>
       <c r="BE3" s="10">
         <f>BNVFE!T9</f>
-        <v>7.4241753709387812E-5</v>
+        <v>1.053872190542009E-4</v>
       </c>
       <c r="BF3" s="10">
         <f>BNVFE!U9</f>
-        <v>7.3666550441435144E-5</v>
+        <v>1.0457070988285631E-4</v>
       </c>
       <c r="BG3" s="10">
         <f>BNVFE!V9</f>
-        <v>7.3143235881095107E-5</v>
+        <v>1.0382785746559407E-4</v>
       </c>
       <c r="BH3" s="10">
         <f>BNVFE!W9</f>
-        <v>7.268369834764319E-5</v>
+        <v>1.0317553743970813E-4</v>
       </c>
       <c r="BI3" s="10">
         <f>BNVFE!X9</f>
-        <v>7.2282905818000628E-5</v>
+        <v>1.0260660677729319E-4</v>
       </c>
       <c r="BJ3" s="10">
         <f>BNVFE!Y9</f>
-        <v>7.1941486288945263E-5</v>
+        <v>1.0212195692865432E-4</v>
       </c>
       <c r="BK3" s="10">
         <f>BNVFE!Z9</f>
-        <v>7.1603868596124793E-5</v>
+        <v>1.0164270384030296E-4</v>
       </c>
       <c r="BL3" s="10">
         <f>BNVFE!AA9</f>
-        <v>7.129639337962048E-5</v>
+        <v>1.0120623842325044E-4</v>
       </c>
       <c r="BM3" s="10">
         <f>BNVFE!AB9</f>
-        <v>7.1056851476574028E-5</v>
+        <v>1.0086620530512349E-4</v>
       </c>
       <c r="BN3" s="10">
         <f>BNVFE!AC9</f>
-        <v>7.082859882864499E-5</v>
+        <v>1.0054219744424832E-4</v>
       </c>
       <c r="BO3" s="10">
         <f>BNVFE!AD9</f>
-        <v>7.0341451089990512E-5</v>
+        <v>9.9850684341711718E-5</v>
       </c>
       <c r="BP3" s="10">
         <f>BNVFE!AE9</f>
-        <v>7.0180331309609449E-5</v>
+        <v>9.9621972535475967E-5</v>
       </c>
       <c r="BQ3" s="10">
         <f>BNVFE!AF9</f>
-        <v>7.008295989492991E-5</v>
+        <v>9.9483752435656976E-5</v>
       </c>
       <c r="BR3" s="10">
         <f>BNVFE!AG9</f>
-        <v>7.001263722126285E-5</v>
+        <v>9.9383928406132565E-5</v>
       </c>
       <c r="BS3" s="10"/>
       <c r="BT3" s="4"/>
@@ -19937,239 +19937,239 @@
       <c r="K4" s="9"/>
       <c r="L4" s="4">
         <f>L5/M5*M4</f>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4:AI4" si="1">M5/N5*N4</f>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651309E-3</v>
+        <v>1.1807374066651307E-3</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1611060587428182E-3</v>
+        <v>1.177387347221569E-3</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1414747108205057E-3</v>
+        <v>1.1740372877780075E-3</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="1"/>
-        <v>1.121843362898193E-3</v>
+        <v>1.1706872283344459E-3</v>
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1022120149758803E-3</v>
+        <v>1.1673371688908844E-3</v>
       </c>
       <c r="AA4" s="4">
         <f t="shared" si="1"/>
-        <v>1.0825806670535676E-3</v>
+        <v>1.163987109447323E-3</v>
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="1"/>
-        <v>1.0629493191312547E-3</v>
+        <v>1.1606370500037615E-3</v>
       </c>
       <c r="AC4" s="4">
         <f t="shared" si="1"/>
-        <v>1.043317971208942E-3</v>
+        <v>1.1572869905602E-3</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="1"/>
-        <v>1.0236866232866293E-3</v>
+        <v>1.1539369311166386E-3</v>
       </c>
       <c r="AE4" s="4">
         <f t="shared" si="1"/>
-        <v>1.0040552753643166E-3</v>
+        <v>1.1505868716730771E-3</v>
       </c>
       <c r="AF4" s="4">
         <f t="shared" si="1"/>
-        <v>9.8442392744200395E-4</v>
+        <v>1.1472368122295155E-3</v>
       </c>
       <c r="AG4" s="4">
         <f>AG5/AH5*AH4</f>
-        <v>9.6479257951969115E-4</v>
+        <v>1.143886752785954E-3</v>
       </c>
       <c r="AH4" s="4">
         <f t="shared" si="1"/>
-        <v>9.4516123159737835E-4</v>
+        <v>1.1405366933423926E-3</v>
       </c>
       <c r="AI4" s="4">
         <f t="shared" si="1"/>
-        <v>9.2552988367506565E-4</v>
+        <v>1.1371866338988309E-3</v>
       </c>
       <c r="AJ4" s="4">
         <f>AJ5/AK5*AK4</f>
-        <v>9.0589853575275296E-4</v>
+        <v>1.1338365744552694E-3</v>
       </c>
       <c r="AK4" s="19">
         <f>AK5/AL5*AL4</f>
-        <v>8.8626718783044037E-4</v>
+        <v>1.130486515011708E-3</v>
       </c>
       <c r="AL4" s="19">
         <f>AL5/AM5*AM4</f>
-        <v>8.6663583990812768E-4</v>
+        <v>1.1271364555681463E-3</v>
       </c>
       <c r="AM4" s="19">
         <f>AM5/AN5*AN4</f>
-        <v>8.4700449198581499E-4</v>
+        <v>1.1237863961245848E-3</v>
       </c>
       <c r="AN4" s="29">
         <f>AN5/AO5*AO4</f>
-        <v>8.2737314406350229E-4</v>
+        <v>1.1204363366810234E-3</v>
       </c>
       <c r="AO4" s="10">
         <f>BNVFE!D10</f>
-        <v>7.8811044821887691E-4</v>
+        <v>1.1137362177939013E-3</v>
       </c>
       <c r="AP4" s="10">
         <f>BNVFE!E10</f>
-        <v>8.3987808713595574E-4</v>
+        <v>1.1868928349938494E-3</v>
       </c>
       <c r="AQ4" s="10">
         <f>BNVFE!F10</f>
-        <v>8.6627919001452318E-4</v>
+        <v>1.2242021544325342E-3</v>
       </c>
       <c r="AR4" s="10">
         <f>BNVFE!G10</f>
-        <v>8.9339028233518841E-4</v>
+        <v>1.2625148116111296E-3</v>
       </c>
       <c r="AS4" s="10">
         <f>BNVFE!H10</f>
-        <v>9.1883490839571541E-4</v>
+        <v>1.2984724640643824E-3</v>
       </c>
       <c r="AT4" s="10">
         <f>BNVFE!I10</f>
-        <v>9.4294621030615396E-4</v>
+        <v>1.3325458991476347E-3</v>
       </c>
       <c r="AU4" s="10">
         <f>BNVFE!J10</f>
-        <v>9.6417787967895108E-4</v>
+        <v>1.3625499159680566E-3</v>
       </c>
       <c r="AV4" s="10">
         <f>BNVFE!K10</f>
-        <v>9.7321251737118614E-4</v>
+        <v>1.3753174198569201E-3</v>
       </c>
       <c r="AW4" s="10">
         <f>BNVFE!L10</f>
-        <v>9.8691693837994168E-4</v>
+        <v>1.3946841343267524E-3</v>
       </c>
       <c r="AX4" s="10">
         <f>BNVFE!M10</f>
-        <v>1.0010477057185716E-3</v>
+        <v>1.4146533498165595E-3</v>
       </c>
       <c r="AY4" s="10">
         <f>BNVFE!N10</f>
-        <v>1.0143262842040467E-3</v>
+        <v>1.4334182752321722E-3</v>
       </c>
       <c r="AZ4" s="10">
         <f>BNVFE!O10</f>
-        <v>1.022232395126511E-3</v>
+        <v>1.4445909758303492E-3</v>
       </c>
       <c r="BA4" s="10">
         <f>BNVFE!P10</f>
-        <v>1.0229355831795947E-3</v>
+        <v>1.4455847020325701E-3</v>
       </c>
       <c r="BB4" s="10">
         <f>BNVFE!Q10</f>
-        <v>1.0230187112675467E-3</v>
+        <v>1.4457021763821076E-3</v>
       </c>
       <c r="BC4" s="10">
         <f>BNVFE!R10</f>
-        <v>1.0230068718125956E-3</v>
+        <v>1.4456854451868699E-3</v>
       </c>
       <c r="BD4" s="10">
         <f>BNVFE!S10</f>
-        <v>1.0230195929290854E-3</v>
+        <v>1.4457034223221783E-3</v>
       </c>
       <c r="BE4" s="10">
         <f>BNVFE!T10</f>
-        <v>1.0229857119356625E-3</v>
+        <v>1.4456555426251702E-3</v>
       </c>
       <c r="BF4" s="10">
         <f>BNVFE!U10</f>
-        <v>1.0229202170784881E-3</v>
+        <v>1.4455629870770495E-3</v>
       </c>
       <c r="BG4" s="10">
         <f>BNVFE!V10</f>
-        <v>1.022675493025624E-3</v>
+        <v>1.4452171497116701E-3</v>
       </c>
       <c r="BH4" s="10">
         <f>BNVFE!W10</f>
-        <v>1.0225866971134939E-3</v>
+        <v>1.4450916657473916E-3</v>
       </c>
       <c r="BI4" s="10">
         <f>BNVFE!X10</f>
-        <v>1.0224177959529731E-3</v>
+        <v>1.4448529792281048E-3</v>
       </c>
       <c r="BJ4" s="10">
         <f>BNVFE!Y10</f>
-        <v>1.0217123407702182E-3</v>
+        <v>1.443856049179987E-3</v>
       </c>
       <c r="BK4" s="10">
         <f>BNVFE!Z10</f>
-        <v>1.0212581591260447E-3</v>
+        <v>1.4432142120520614E-3</v>
       </c>
       <c r="BL4" s="10">
         <f>BNVFE!AA10</f>
-        <v>1.0212951889106777E-3</v>
+        <v>1.443266541535037E-3</v>
       </c>
       <c r="BM4" s="10">
         <f>BNVFE!AB10</f>
-        <v>1.0214074118294128E-3</v>
+        <v>1.4434251319069122E-3</v>
       </c>
       <c r="BN4" s="10">
         <f>BNVFE!AC10</f>
-        <v>1.0216593151262368E-3</v>
+        <v>1.4437811147842976E-3</v>
       </c>
       <c r="BO4" s="10">
         <f>BNVFE!AD10</f>
-        <v>1.021959583856051E-3</v>
+        <v>1.4442054463741406E-3</v>
       </c>
       <c r="BP4" s="10">
         <f>BNVFE!AE10</f>
-        <v>1.0223449959001912E-3</v>
+        <v>1.4447501001765403E-3</v>
       </c>
       <c r="BQ4" s="10">
         <f>BNVFE!AF10</f>
-        <v>1.0226495469860513E-3</v>
+        <v>1.4451804834752992E-3</v>
       </c>
       <c r="BR4" s="10">
         <f>BNVFE!AG10</f>
-        <v>1.0230103984587512E-3</v>
+        <v>1.4456904289471535E-3</v>
       </c>
       <c r="BS4" s="10"/>
       <c r="BT4" s="4"/>
@@ -20236,195 +20236,195 @@
       </c>
       <c r="W5" s="4">
         <f>($AO$5-$V$5)/COUNT($V$1:$AO$1)+V5</f>
-        <v>7.6742949272979222E-4</v>
+        <v>7.7819056047563108E-4</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" ref="X5:AN5" si="3">($AO$5-$V$5)/COUNT($V$1:$AO$1)+W5</f>
-        <v>7.54454213456911E-4</v>
+        <v>7.7597634894858872E-4</v>
       </c>
       <c r="Y5" s="4">
         <f t="shared" si="3"/>
-        <v>7.4147893418402978E-4</v>
+        <v>7.7376213742154636E-4</v>
       </c>
       <c r="Z5" s="4">
         <f t="shared" si="3"/>
-        <v>7.2850365491114856E-4</v>
+        <v>7.71547925894504E-4</v>
       </c>
       <c r="AA5" s="4">
         <f t="shared" si="3"/>
-        <v>7.1552837563826734E-4</v>
+        <v>7.6933371436746164E-4</v>
       </c>
       <c r="AB5" s="4">
         <f t="shared" si="3"/>
-        <v>7.0255309636538612E-4</v>
+        <v>7.6711950284041929E-4</v>
       </c>
       <c r="AC5" s="4">
         <f t="shared" si="3"/>
-        <v>6.895778170925049E-4</v>
+        <v>7.6490529131337693E-4</v>
       </c>
       <c r="AD5" s="4">
         <f t="shared" si="3"/>
-        <v>6.7660253781962369E-4</v>
+        <v>7.6269107978633457E-4</v>
       </c>
       <c r="AE5" s="4">
         <f t="shared" si="3"/>
-        <v>6.6362725854674247E-4</v>
+        <v>7.6047686825929221E-4</v>
       </c>
       <c r="AF5" s="4">
         <f t="shared" si="3"/>
-        <v>6.5065197927386125E-4</v>
+        <v>7.5826265673224985E-4</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="3"/>
-        <v>6.3767670000098003E-4</v>
+        <v>7.5604844520520749E-4</v>
       </c>
       <c r="AH5" s="4">
         <f t="shared" si="3"/>
-        <v>6.2470142072809881E-4</v>
+        <v>7.5383423367816514E-4</v>
       </c>
       <c r="AI5" s="4">
         <f t="shared" si="3"/>
-        <v>6.1172614145521759E-4</v>
+        <v>7.5162002215112278E-4</v>
       </c>
       <c r="AJ5" s="4">
         <f t="shared" si="3"/>
-        <v>5.9875086218233637E-4</v>
+        <v>7.4940581062408042E-4</v>
       </c>
       <c r="AK5" s="4">
         <f t="shared" si="3"/>
-        <v>5.8577558290945516E-4</v>
+        <v>7.4719159909703806E-4</v>
       </c>
       <c r="AL5" s="4">
         <f t="shared" si="3"/>
-        <v>5.7280030363657394E-4</v>
+        <v>7.449773875699957E-4</v>
       </c>
       <c r="AM5" s="4">
         <f t="shared" si="3"/>
-        <v>5.5982502436369272E-4</v>
+        <v>7.4276317604295334E-4</v>
       </c>
       <c r="AN5" s="28">
         <f t="shared" si="3"/>
-        <v>5.468497450908115E-4</v>
+        <v>7.4054896451591099E-4</v>
       </c>
       <c r="AO5" s="10">
         <f>BNVFE!D11</f>
-        <v>5.2089918654504906E-4</v>
+        <v>7.3612054146182692E-4</v>
       </c>
       <c r="AP5" s="10">
         <f>BNVFE!E11</f>
-        <v>5.5511484890837198E-4</v>
+        <v>7.8447318350072194E-4</v>
       </c>
       <c r="AQ5" s="10">
         <f>BNVFE!F11</f>
-        <v>5.7256457698191549E-4</v>
+        <v>8.0913266389472246E-4</v>
       </c>
       <c r="AR5" s="10">
         <f>BNVFE!G11</f>
-        <v>5.9048357040231516E-4</v>
+        <v>8.3445529729440947E-4</v>
       </c>
       <c r="AS5" s="10">
         <f>BNVFE!H11</f>
-        <v>6.0730111805293394E-4</v>
+        <v>8.582213975349269E-4</v>
       </c>
       <c r="AT5" s="10">
         <f>BNVFE!I11</f>
-        <v>6.2323740919090079E-4</v>
+        <v>8.8074213007663328E-4</v>
       </c>
       <c r="AU5" s="10">
         <f>BNVFE!J11</f>
-        <v>6.3727041602424229E-4</v>
+        <v>9.0057319308330108E-4</v>
       </c>
       <c r="AV5" s="10">
         <f>BNVFE!K11</f>
-        <v>6.4324183213127449E-4</v>
+        <v>9.0901183566816969E-4</v>
       </c>
       <c r="AW5" s="10">
         <f>BNVFE!L11</f>
-        <v>6.5229972721649369E-4</v>
+        <v>9.2181220627128113E-4</v>
       </c>
       <c r="AX5" s="10">
         <f>BNVFE!M11</f>
-        <v>6.616394146024239E-4</v>
+        <v>9.3501079807791388E-4</v>
       </c>
       <c r="AY5" s="10">
         <f>BNVFE!N11</f>
-        <v>6.7041585037635684E-4</v>
+        <v>9.4741341804908898E-4</v>
       </c>
       <c r="AZ5" s="10">
         <f>BNVFE!O11</f>
-        <v>6.7564137017190565E-4</v>
+        <v>9.5479798028431191E-4</v>
       </c>
       <c r="BA5" s="10">
         <f>BNVFE!P11</f>
-        <v>6.7610614016152745E-4</v>
+        <v>9.5545478057360543E-4</v>
       </c>
       <c r="BB5" s="10">
         <f>BNVFE!Q11</f>
-        <v>6.7616108341661443E-4</v>
+        <v>9.5553242488507497E-4</v>
       </c>
       <c r="BC5" s="10">
         <f>BNVFE!R11</f>
-        <v>6.7615325816513226E-4</v>
+        <v>9.5552136645283517E-4</v>
       </c>
       <c r="BD5" s="10">
         <f>BNVFE!S11</f>
-        <v>6.761616661481077E-4</v>
+        <v>9.5553324838534815E-4</v>
       </c>
       <c r="BE5" s="10">
         <f>BNVFE!T11</f>
-        <v>6.7613927260929199E-4</v>
+        <v>9.5550160244627959E-4</v>
       </c>
       <c r="BF5" s="10">
         <f>BNVFE!U11</f>
-        <v>6.7609598398407189E-4</v>
+        <v>9.5544042814027313E-4</v>
       </c>
       <c r="BG5" s="10">
         <f>BNVFE!V11</f>
-        <v>6.7593423437099028E-4</v>
+        <v>9.5521184799302321E-4</v>
       </c>
       <c r="BH5" s="10">
         <f>BNVFE!W11</f>
-        <v>6.7587554498487476E-4</v>
+        <v>9.5512890975122625E-4</v>
       </c>
       <c r="BI5" s="10">
         <f>BNVFE!X11</f>
-        <v>6.7576391028022079E-4</v>
+        <v>9.5497115062746795E-4</v>
       </c>
       <c r="BJ5" s="10">
         <f>BNVFE!Y11</f>
-        <v>6.7529764183818757E-4</v>
+        <v>9.5431223276604333E-4</v>
       </c>
       <c r="BK5" s="10">
         <f>BNVFE!Z11</f>
-        <v>6.749974518717581E-4</v>
+        <v>9.5388801248246955E-4</v>
       </c>
       <c r="BL5" s="10">
         <f>BNVFE!AA11</f>
-        <v>6.7502192659447849E-4</v>
+        <v>9.5392259949394229E-4</v>
       </c>
       <c r="BM5" s="10">
         <f>BNVFE!AB11</f>
-        <v>6.750960999888459E-4</v>
+        <v>9.5402741931442593E-4</v>
       </c>
       <c r="BN5" s="10">
         <f>BNVFE!AC11</f>
-        <v>6.7526259470123058E-4</v>
+        <v>9.5426270510675759E-4</v>
       </c>
       <c r="BO5" s="10">
         <f>BNVFE!AD11</f>
-        <v>6.7546105639839315E-4</v>
+        <v>9.5454316577121671E-4</v>
       </c>
       <c r="BP5" s="10">
         <f>BNVFE!AE11</f>
-        <v>6.7571579330834156E-4</v>
+        <v>9.5490315303348411E-4</v>
       </c>
       <c r="BQ5" s="10">
         <f>BNVFE!AF11</f>
-        <v>6.7591708541561474E-4</v>
+        <v>9.5518761355641295E-4</v>
       </c>
       <c r="BR5" s="10">
         <f>BNVFE!AG11</f>
-        <v>6.7615558909110566E-4</v>
+        <v>9.555246604539279E-4</v>
       </c>
       <c r="BS5" s="10"/>
       <c r="BT5" s="4"/>
@@ -22740,12 +22740,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -23779,12 +23779,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -24778,12 +24778,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="30">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
updated transportation files with apta passenger rail data - avlo, baadtbvt, bhnvfeal, bnvfe, syfafe, syvbt, ttle, tts
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21AF18-E41A-4B31-8D96-6A3A3B048707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4895BA9-0971-484C-8231-CFE662F3F61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -385,14 +385,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="44">
     <font>
@@ -1294,7 +1293,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1327,8 +1326,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="154" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="155" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -1336,6 +1333,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="43" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="154" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="156">
     <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -5704,199 +5707,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>5.6550914138770239E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.5917423769000218E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>5.5283933399230198E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>5.4650443029460177E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>5.401695265969033E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>5.338346228992031E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>5.2749971920150289E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>5.2116481550380268E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>5.1482991180610421E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>5.0849500810840401E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>5.021601044107038E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>4.9582520071300533E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>4.8949029701530512E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4.8315539331760492E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>4.7682048961990471E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>4.7048558592220624E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>4.6415068222450603E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>4.5781577852680583E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>4.5148087482910562E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>4.4514597113140715E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.3881106743370694E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>4.3247616373600674E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>4.2614126003830653E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>4.1980635634060806E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>4.1347145264290786E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>4.0713654894520765E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>4.0080164524750744E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>3.9446674154980897E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>3.8813183785210877E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>3.8179693415440856E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>3.7546203045671009E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>3.6912712675900988E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>3.6279222306130968E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>3.5645731936360947E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>3.50122415665911E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>3.8258341226368855E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>3.0425177990638558E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>3.1369602145278982E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>3.1866725580745358E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>3.2176784865192677E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.2673519826153288E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.3038240919707824E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>3.3340389823551702E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>3.3475402773417714E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>3.3555107094994109E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>3.3533649804280095E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>3.3530916094466514E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>3.3543094523282268E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>3.3562165718775656E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>3.3577393040427292E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>3.3592389782957394E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>3.3615828155893885E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>3.3637923107499002E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>3.3656727929620473E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>3.3676884833871952E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>3.3691991114356807E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>3.3705013729136348E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>3.3713686099786852E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>3.3722694633495147E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>3.3729739602263772E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>3.3742953237129352E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>3.3751721202413692E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>3.3760101841942016E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>3.3764787130259203E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>3.3772719520374359E-4</c:v>
+                  <c:v>7.1745362435245036E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7788,8 +7791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10770,907 +10773,902 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="30" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:32" ht="30">
+      <c r="A1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="30">
         <v>2021</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="30">
         <v>2022</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="30">
         <v>2023</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="30">
         <v>2024</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="30">
         <v>2025</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="30">
         <v>2026</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="30">
         <v>2027</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="30">
         <v>2028</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="30">
         <v>2029</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="30">
         <v>2030</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="30">
         <v>2031</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="30">
         <v>2032</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="30">
         <v>2033</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="30">
         <v>2034</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="30">
         <v>2035</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="30">
         <v>2036</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="30">
         <v>2037</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="30">
         <v>2038</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="30">
         <v>2039</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="30">
         <v>2040</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="30">
         <v>2041</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="30">
         <v>2042</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="30">
         <v>2043</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="30">
         <v>2044</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="30">
         <v>2045</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="30">
         <v>2046</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="30">
         <v>2047</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="30">
         <v>2048</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="30">
         <v>2049</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="30">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
+    <row r="2" spans="1:32" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
         <f>Extrapolations!G9</f>
-        <v>1.7968922323952086E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="C2" s="4">
         <f>Extrapolations!H9</f>
-        <v>1.7765351800131182E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="D2" s="4">
         <f>Extrapolations!I9</f>
-        <v>1.7561781276310348E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="E2" s="4">
         <f>Extrapolations!J9</f>
-        <v>1.7358210752489514E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="F2" s="4">
         <f>Extrapolations!K9</f>
-        <v>1.7154640228668611E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="G2" s="4">
         <f>Extrapolations!L9</f>
-        <v>1.6951069704847777E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="H2" s="4">
         <f>Extrapolations!M9</f>
-        <v>1.6747499181026873E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="I2" s="4">
         <f>Extrapolations!N9</f>
-        <v>1.6543928657206039E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="J2" s="4">
         <f>Extrapolations!O9</f>
-        <v>1.6340358133385205E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="K2" s="4">
         <f>Extrapolations!P9</f>
-        <v>1.6136787609564301E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="L2" s="4">
         <f>Extrapolations!Q9</f>
-        <v>1.5933217085743467E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="M2" s="4">
         <f>Extrapolations!R9</f>
-        <v>1.5729646561922633E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="N2" s="4">
         <f>Extrapolations!S9</f>
-        <v>1.552607603810173E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="O2" s="4">
         <f>Extrapolations!T9</f>
-        <v>1.5322505514280896E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="P2" s="4">
         <f>Extrapolations!U9</f>
-        <v>1.5118934990460062E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Q2" s="4">
         <f>Extrapolations!V9</f>
-        <v>1.4915364466639158E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="R2" s="4">
         <f>Extrapolations!W9</f>
-        <v>1.4711793942818324E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="S2" s="4">
         <f>Extrapolations!X9</f>
-        <v>1.450822341899749E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="T2" s="4">
         <f>Extrapolations!Y9</f>
-        <v>1.4304652895176587E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="U2" s="4">
         <f>Extrapolations!Z9</f>
-        <v>1.4101082371355753E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="V2" s="4">
         <f>Extrapolations!AA9</f>
-        <v>1.3897511847534849E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="W2" s="4">
         <f>Extrapolations!AB9</f>
-        <v>1.3693941323714015E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="X2" s="4">
         <f>Extrapolations!AC9</f>
-        <v>1.3490370799893181E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Y2" s="4">
         <f>Extrapolations!AD9</f>
-        <v>1.3286800276072278E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Z2" s="4">
         <f>Extrapolations!AE9</f>
-        <v>1.3083229752251443E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AA2" s="4">
         <f>Extrapolations!AF9</f>
-        <v>1.2879659228430609E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AB2" s="4">
         <f>Extrapolations!AG9</f>
-        <v>1.2676088704609706E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AC2" s="4">
         <f>Extrapolations!AH9</f>
-        <v>1.2472518180788872E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AD2" s="4">
         <f>Extrapolations!AI9</f>
-        <v>1.2268947656968038E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AE2" s="4">
         <f>Extrapolations!AJ9</f>
-        <v>1.2065377133147134E-3</v>
-      </c>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
     </row>
-    <row r="3" spans="1:34">
-      <c r="A3" t="s">
+    <row r="3" spans="1:32">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
+      <c r="B3" s="30">
+        <v>0</v>
+      </c>
+      <c r="C3" s="30">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
+        <v>0</v>
+      </c>
+      <c r="K3" s="30">
+        <v>0</v>
+      </c>
+      <c r="L3" s="30">
+        <v>0</v>
+      </c>
+      <c r="M3" s="30">
+        <v>0</v>
+      </c>
+      <c r="N3" s="30">
+        <v>0</v>
+      </c>
+      <c r="O3" s="30">
+        <v>0</v>
+      </c>
+      <c r="P3" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>0</v>
+      </c>
+      <c r="R3" s="30">
+        <v>0</v>
+      </c>
+      <c r="S3" s="30">
+        <v>0</v>
+      </c>
+      <c r="T3" s="30">
+        <v>0</v>
+      </c>
+      <c r="U3" s="30">
+        <v>0</v>
+      </c>
+      <c r="V3" s="30">
+        <v>0</v>
+      </c>
+      <c r="W3" s="30">
+        <v>0</v>
+      </c>
+      <c r="X3" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
-      <c r="A4" t="s">
+    <row r="4" spans="1:32">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
+      <c r="B4" s="30">
+        <v>0</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0</v>
+      </c>
+      <c r="K4" s="30">
+        <v>0</v>
+      </c>
+      <c r="L4" s="30">
+        <v>0</v>
+      </c>
+      <c r="M4" s="30">
+        <v>0</v>
+      </c>
+      <c r="N4" s="30">
+        <v>0</v>
+      </c>
+      <c r="O4" s="30">
+        <v>0</v>
+      </c>
+      <c r="P4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>0</v>
+      </c>
+      <c r="R4" s="30">
+        <v>0</v>
+      </c>
+      <c r="S4" s="30">
+        <v>0</v>
+      </c>
+      <c r="T4" s="30">
+        <v>0</v>
+      </c>
+      <c r="U4" s="30">
+        <v>0</v>
+      </c>
+      <c r="V4" s="30">
+        <v>0</v>
+      </c>
+      <c r="W4" s="30">
+        <v>0</v>
+      </c>
+      <c r="X4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
-      <c r="A5" t="s">
+    <row r="5" spans="1:32">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="22">
-        <f>Extrapolations!Q6</f>
-        <v>4.2882977835183994E-4</v>
-      </c>
-      <c r="C5" s="22">
-        <f>Extrapolations!R6</f>
-        <v>4.3401682022130295E-4</v>
-      </c>
-      <c r="D5" s="22">
-        <f>Extrapolations!S6</f>
-        <v>4.3920386209076769E-4</v>
-      </c>
-      <c r="E5" s="22">
-        <f>Extrapolations!T6</f>
-        <v>4.4439090396023069E-4</v>
-      </c>
-      <c r="F5" s="22">
-        <f>Extrapolations!U6</f>
-        <v>4.4957794582969543E-4</v>
-      </c>
-      <c r="G5" s="22">
-        <f>Extrapolations!V6</f>
-        <v>4.5476498769915844E-4</v>
-      </c>
-      <c r="H5" s="22">
-        <f>Extrapolations!W6</f>
-        <v>4.5995202956862317E-4</v>
-      </c>
-      <c r="I5" s="22">
-        <f>Extrapolations!X6</f>
-        <v>4.6513907143808618E-4</v>
-      </c>
-      <c r="J5" s="22">
-        <f>Extrapolations!Y6</f>
-        <v>4.7032611330755092E-4</v>
-      </c>
-      <c r="K5" s="22">
-        <f>Extrapolations!Z6</f>
-        <v>4.7551315517701392E-4</v>
-      </c>
-      <c r="L5" s="22">
-        <f>Extrapolations!AA6</f>
-        <v>4.8070019704647866E-4</v>
-      </c>
-      <c r="M5" s="22">
-        <f>Extrapolations!AB6</f>
-        <v>4.8588723891594167E-4</v>
-      </c>
-      <c r="N5" s="22">
-        <f>Extrapolations!AC6</f>
-        <v>4.9107428078540641E-4</v>
-      </c>
-      <c r="O5" s="22">
-        <f>Extrapolations!AD6</f>
-        <v>4.9626132265486941E-4</v>
-      </c>
-      <c r="P5" s="22">
-        <f>Extrapolations!AE6</f>
-        <v>5.0144836452433242E-4</v>
-      </c>
-      <c r="Q5" s="22">
-        <f>Extrapolations!AF6</f>
-        <v>5.0663540639379716E-4</v>
-      </c>
-      <c r="R5" s="22">
-        <f>Extrapolations!AG6</f>
-        <v>5.1182244826326016E-4</v>
-      </c>
-      <c r="S5" s="22">
-        <f>Extrapolations!AH6</f>
-        <v>5.170094901327249E-4</v>
-      </c>
-      <c r="T5" s="22">
-        <f>Extrapolations!AI6</f>
-        <v>5.2219653200218791E-4</v>
-      </c>
-      <c r="U5" s="22">
-        <f>Extrapolations!AJ6</f>
-        <v>5.2738357387165265E-4</v>
-      </c>
-      <c r="V5" s="22">
-        <f>Extrapolations!AK6</f>
-        <v>5.3257061574111565E-4</v>
-      </c>
-      <c r="W5" s="22">
-        <f>Extrapolations!AL6</f>
-        <v>5.3775765761058039E-4</v>
-      </c>
-      <c r="X5" s="22">
-        <f>Extrapolations!AM6</f>
-        <v>5.429446994800434E-4</v>
-      </c>
-      <c r="Y5" s="22">
-        <f>Extrapolations!AN6</f>
-        <v>5.4813174134950814E-4</v>
-      </c>
-      <c r="Z5" s="22">
-        <f>Extrapolations!AO6</f>
-        <v>5.7245968727451246E-4</v>
-      </c>
-      <c r="AA5" s="22">
-        <f>Extrapolations!AP6</f>
-        <v>5.6525537747016295E-4</v>
-      </c>
-      <c r="AB5" s="22">
-        <f>Extrapolations!AQ6</f>
-        <v>5.6816948983254214E-4</v>
-      </c>
-      <c r="AC5" s="22">
-        <f>Extrapolations!AR6</f>
-        <v>5.7128317518608321E-4</v>
-      </c>
-      <c r="AD5" s="22">
-        <f>Extrapolations!AS6</f>
-        <v>5.7537137435165198E-4</v>
-      </c>
-      <c r="AE5" s="22">
-        <f>Extrapolations!AT6</f>
-        <v>5.8053804811384778E-4</v>
-      </c>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
+      <c r="B5" s="31">
+        <f>Extrapolations!G8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="C5" s="31">
+        <f>Extrapolations!H8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="D5" s="31">
+        <f>Extrapolations!I8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="E5" s="31">
+        <f>Extrapolations!J8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="F5" s="31">
+        <f>Extrapolations!K8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="G5" s="31">
+        <f>Extrapolations!L8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="H5" s="31">
+        <f>Extrapolations!M8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="I5" s="31">
+        <f>Extrapolations!N8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="J5" s="31">
+        <f>Extrapolations!O8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="K5" s="31">
+        <f>Extrapolations!P8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="L5" s="31">
+        <f>Extrapolations!Q8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="M5" s="31">
+        <f>Extrapolations!R8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="N5" s="31">
+        <f>Extrapolations!S8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="O5" s="31">
+        <f>Extrapolations!T8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="P5" s="31">
+        <f>Extrapolations!U8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="Q5" s="31">
+        <f>Extrapolations!V8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="R5" s="31">
+        <f>Extrapolations!W8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="S5" s="31">
+        <f>Extrapolations!X8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="T5" s="31">
+        <f>Extrapolations!Y8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="U5" s="31">
+        <f>Extrapolations!Z8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="V5" s="31">
+        <f>Extrapolations!AA8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="W5" s="31">
+        <f>Extrapolations!AB8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="X5" s="31">
+        <f>Extrapolations!AC8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="Y5" s="31">
+        <f>Extrapolations!AD8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="Z5" s="31">
+        <f>Extrapolations!AE8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AA5" s="31">
+        <f>Extrapolations!AF8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AB5" s="31">
+        <f>Extrapolations!AG8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AC5" s="31">
+        <f>Extrapolations!AH8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AD5" s="31">
+        <f>Extrapolations!AI8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AE5" s="31">
+        <f>Extrapolations!AJ8</f>
+        <v>7.1745362435245036E-5</v>
+      </c>
     </row>
-    <row r="6" spans="1:34">
-      <c r="A6" t="s">
+    <row r="6" spans="1:32">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
+      <c r="B6" s="30">
+        <v>0</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
+        <v>0</v>
+      </c>
+      <c r="K6" s="30">
+        <v>0</v>
+      </c>
+      <c r="L6" s="30">
+        <v>0</v>
+      </c>
+      <c r="M6" s="30">
+        <v>0</v>
+      </c>
+      <c r="N6" s="30">
+        <v>0</v>
+      </c>
+      <c r="O6" s="30">
+        <v>0</v>
+      </c>
+      <c r="P6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0</v>
+      </c>
+      <c r="R6" s="30">
+        <v>0</v>
+      </c>
+      <c r="S6" s="30">
+        <v>0</v>
+      </c>
+      <c r="T6" s="30">
+        <v>0</v>
+      </c>
+      <c r="U6" s="30">
+        <v>0</v>
+      </c>
+      <c r="V6" s="30">
+        <v>0</v>
+      </c>
+      <c r="W6" s="30">
+        <v>0</v>
+      </c>
+      <c r="X6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
-      <c r="A7" t="s">
+    <row r="7" spans="1:32">
+      <c r="A7" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
+      <c r="B7" s="30">
+        <v>0</v>
+      </c>
+      <c r="C7" s="30">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
+        <v>0</v>
+      </c>
+      <c r="K7" s="30">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30">
+        <v>0</v>
+      </c>
+      <c r="M7" s="30">
+        <v>0</v>
+      </c>
+      <c r="N7" s="30">
+        <v>0</v>
+      </c>
+      <c r="O7" s="30">
+        <v>0</v>
+      </c>
+      <c r="P7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0</v>
+      </c>
+      <c r="R7" s="30">
+        <v>0</v>
+      </c>
+      <c r="S7" s="30">
+        <v>0</v>
+      </c>
+      <c r="T7" s="30">
+        <v>0</v>
+      </c>
+      <c r="U7" s="30">
+        <v>0</v>
+      </c>
+      <c r="V7" s="30">
+        <v>0</v>
+      </c>
+      <c r="W7" s="30">
+        <v>0</v>
+      </c>
+      <c r="X7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
-      <c r="A8" t="s">
+    <row r="8" spans="1:32" s="4" customFormat="1">
+      <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.2864893350555196E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.3020504606639086E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.3176115862723028E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.3331727118806919E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.3487338374890861E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.3642949630974751E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.3798560887058693E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.3954172143142583E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.4109783399226525E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.4265394655310416E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.4421005911394358E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.4576617167478248E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.473222842356219E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.488783967964608E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.504345093572997E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.5199062191813913E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.5354673447897803E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.5510284703981745E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.5665895960065635E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.5821507216149577E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.5977118472233467E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.613272972831741E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.62883409844013E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.6443952240485242E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>1.7173790618235372E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>1.6957661324104886E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.7045084694976261E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.7138495255582494E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.7261141230549557E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.7416141443415431E-3</v>
-      </c>
-      <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
+        <v>2.1523608730573507E-4</v>
+      </c>
     </row>
-    <row r="13" spans="1:34">
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="23"/>
+    <row r="13" spans="1:32">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="32"/>
+      <c r="AC13" s="32"/>
+      <c r="AD13" s="32"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11685,7 +11683,7 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16207,7 +16205,7 @@
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17018,94 +17016,94 @@
         <v>5</v>
       </c>
       <c r="D14" s="4">
-        <v>3.8258341226368855E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="E14" s="4">
-        <v>3.0425177990638558E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="F14" s="4">
-        <v>3.1369602145278982E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="G14" s="4">
-        <v>3.1866725580745358E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="H14" s="4">
-        <v>3.2176784865192677E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="I14" s="4">
-        <v>3.2673519826153288E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="J14" s="4">
-        <v>3.3038240919707824E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="K14" s="4">
-        <v>3.3340389823551702E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="L14" s="4">
-        <v>3.3475402773417714E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="M14" s="4">
-        <v>3.3555107094994109E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="N14" s="4">
-        <v>3.3533649804280095E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="O14" s="4">
-        <v>3.3530916094466514E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="P14" s="4">
-        <v>3.3543094523282268E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Q14" s="4">
-        <v>3.3562165718775656E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="R14" s="4">
-        <v>3.3577393040427292E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="S14" s="4">
-        <v>3.3592389782957394E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="T14" s="4">
-        <v>3.3615828155893885E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="U14" s="4">
-        <v>3.3637923107499002E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="V14" s="4">
-        <v>3.3656727929620473E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="W14" s="4">
-        <v>3.3676884833871952E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="X14" s="4">
-        <v>3.3691991114356807E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Y14" s="4">
-        <v>3.3705013729136348E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Z14" s="4">
-        <v>3.3713686099786852E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AA14" s="4">
-        <v>3.3722694633495147E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AB14" s="4">
-        <v>3.3729739602263772E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AC14" s="4">
-        <v>3.3742953237129352E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AD14" s="4">
-        <v>3.3751721202413692E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AE14" s="4">
-        <v>3.3760101841942016E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AF14" s="4">
-        <v>3.3764787130259203E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AG14" s="4">
-        <v>3.3772719520374359E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
@@ -17123,94 +17121,94 @@
         <v>2</v>
       </c>
       <c r="D15" s="4">
-        <v>1.2294220931562134E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="E15" s="4">
-        <v>9.7770537903301043E-4</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="F15" s="4">
-        <v>1.0080542097404184E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="G15" s="4">
-        <v>1.0240291452707345E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="H15" s="4">
-        <v>1.0339928217467291E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="I15" s="4">
-        <v>1.049955273747318E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="J15" s="4">
-        <v>1.0616754935969699E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="K15" s="4">
-        <v>1.0713849719983116E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="L15" s="4">
-        <v>1.0757235789035442E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="M15" s="4">
-        <v>1.0782848570647235E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="N15" s="4">
-        <v>1.0775953324691067E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="O15" s="4">
-        <v>1.0775074853975044E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="P15" s="4">
-        <v>1.0778988361191009E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Q15" s="4">
-        <v>1.0785116841499065E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="R15" s="4">
-        <v>1.0790010102695979E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="S15" s="4">
-        <v>1.0794829267876918E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="T15" s="4">
-        <v>1.0802361129581342E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="U15" s="4">
-        <v>1.0809461286247785E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="V15" s="4">
-        <v>1.0815504168148291E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="W15" s="4">
-        <v>1.0821981538212447E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="X15" s="4">
-        <v>1.0826835903137368E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Y15" s="4">
-        <v>1.0831020687371974E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="Z15" s="4">
-        <v>1.0833807531687749E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AA15" s="4">
-        <v>1.0836702401149649E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AB15" s="4">
-        <v>1.0838966283997708E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AC15" s="4">
-        <v>1.0843212452052544E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AD15" s="4">
-        <v>1.0846030015461477E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AE15" s="4">
-        <v>1.0848723112720957E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AF15" s="4">
-        <v>1.0850228718239992E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AG15" s="4">
-        <v>1.0852777771687293E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
@@ -18627,16 +18625,16 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>1.232672246515414E-3</v>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="C5">
-        <v>4.2170366328158899E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="D5">
-        <v>4.2170366328158899E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="E5">
-        <v>4.2170366328158899E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -18645,7 +18643,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.2651109898447668E-3</v>
+        <v>2.1523608730573507E-4</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -19282,15 +19280,15 @@
   <dimension ref="A1:BT15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" style="26"/>
+    <col min="40" max="40" width="8.7109375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -19405,7 +19403,7 @@
       <c r="AM1">
         <v>2019</v>
       </c>
-      <c r="AN1" s="27">
+      <c r="AN1" s="25">
         <v>2020</v>
       </c>
       <c r="AO1">
@@ -19582,7 +19580,7 @@
         <f t="shared" si="0"/>
         <v>3.4824495702621549E-4</v>
       </c>
-      <c r="AN2" s="28">
+      <c r="AN2" s="26">
         <f t="shared" si="0"/>
         <v>3.5107788164238408E-4</v>
       </c>
@@ -19792,7 +19790,7 @@
         <f t="array" ref="AM3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AM1)</f>
         <v>1.0444155998202975E-4</v>
       </c>
-      <c r="AN3" s="28" cm="1">
+      <c r="AN3" s="26" cm="1">
         <f t="array" ref="AN3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AN1)</f>
         <v>1.0688599085026222E-4</v>
       </c>
@@ -20047,7 +20045,7 @@
         <f>AM5/AN5*AN4</f>
         <v>1.1237863961245848E-3</v>
       </c>
-      <c r="AN4" s="29">
+      <c r="AN4" s="27">
         <f>AN5/AO5*AO4</f>
         <v>1.1204363366810234E-3</v>
       </c>
@@ -20230,7 +20228,7 @@
         <f>V5</f>
         <v>7.8040477200267344E-4</v>
       </c>
-      <c r="V5" s="25">
+      <c r="V5" s="23">
         <f>Calculations!B22</f>
         <v>7.8040477200267344E-4</v>
       </c>
@@ -20302,7 +20300,7 @@
         <f t="shared" si="3"/>
         <v>7.4276317604295334E-4</v>
       </c>
-      <c r="AN5" s="28">
+      <c r="AN5" s="26">
         <f t="shared" si="3"/>
         <v>7.4054896451591099E-4</v>
       </c>
@@ -20545,7 +20543,7 @@
         <f t="shared" si="4"/>
         <v>5.429446994800434E-4</v>
       </c>
-      <c r="AN6" s="28">
+      <c r="AN6" s="26">
         <f t="shared" si="4"/>
         <v>5.4813174134950814E-4</v>
       </c>
@@ -20788,7 +20786,7 @@
         <f t="shared" si="5"/>
         <v>4.6159076773102222E-5</v>
       </c>
-      <c r="AN7" s="28">
+      <c r="AN7" s="26">
         <f t="shared" si="5"/>
         <v>4.6599105683549815E-5</v>
       </c>
@@ -20926,264 +20924,264 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="4">
-        <f>TREND($AO8:$AT8,$AO$1:$AT$1,F$1)</f>
-        <v>5.6550914138770239E-4</v>
+        <f>SYFAFE!$E$5</f>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" ref="G8:AN9" si="6">TREND($AO8:$AT8,$AO$1:$AT$1,G$1)</f>
-        <v>5.5917423769000218E-4</v>
+        <f>F8</f>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="6"/>
-        <v>5.5283933399230198E-4</v>
+        <f t="shared" ref="H8:BR8" si="6">G8</f>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="6"/>
-        <v>5.4650443029460177E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="6"/>
-        <v>5.401695265969033E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="6"/>
-        <v>5.338346228992031E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>5.2749971920150289E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="6"/>
-        <v>5.2116481550380268E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="6"/>
-        <v>5.1482991180610421E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="6"/>
-        <v>5.0849500810840401E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="6"/>
-        <v>5.021601044107038E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="6"/>
-        <v>4.9582520071300533E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="6"/>
-        <v>4.8949029701530512E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="6"/>
-        <v>4.8315539331760492E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="6"/>
-        <v>4.7682048961990471E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="6"/>
-        <v>4.7048558592220624E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" si="6"/>
-        <v>4.6415068222450603E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" si="6"/>
-        <v>4.5781577852680583E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="6"/>
-        <v>4.5148087482910562E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="6"/>
-        <v>4.4514597113140715E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="6"/>
-        <v>4.3881106743370694E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" si="6"/>
-        <v>4.3247616373600674E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AB8" s="4">
         <f t="shared" si="6"/>
-        <v>4.2614126003830653E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AC8" s="4">
         <f t="shared" si="6"/>
-        <v>4.1980635634060806E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AD8" s="4">
         <f t="shared" si="6"/>
-        <v>4.1347145264290786E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" si="6"/>
-        <v>4.0713654894520765E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AF8" s="4">
         <f t="shared" si="6"/>
-        <v>4.0080164524750744E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="6"/>
-        <v>3.9446674154980897E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AH8" s="4">
         <f t="shared" si="6"/>
-        <v>3.8813183785210877E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AI8" s="4">
         <f t="shared" si="6"/>
-        <v>3.8179693415440856E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AJ8" s="4">
         <f t="shared" si="6"/>
-        <v>3.7546203045671009E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AK8" s="4">
         <f t="shared" si="6"/>
-        <v>3.6912712675900988E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AL8" s="4">
         <f t="shared" si="6"/>
-        <v>3.6279222306130968E-4</v>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="AM8" s="4">
         <f t="shared" si="6"/>
-        <v>3.5645731936360947E-4</v>
-      </c>
-      <c r="AN8" s="28">
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AN8" s="4">
         <f t="shared" si="6"/>
-        <v>3.50122415665911E-4</v>
-      </c>
-      <c r="AO8" s="10">
-        <f>BNVFE!D14</f>
-        <v>3.8258341226368855E-4</v>
-      </c>
-      <c r="AP8" s="10">
-        <f>BNVFE!E14</f>
-        <v>3.0425177990638558E-4</v>
-      </c>
-      <c r="AQ8" s="10">
-        <f>BNVFE!F14</f>
-        <v>3.1369602145278982E-4</v>
-      </c>
-      <c r="AR8" s="10">
-        <f>BNVFE!G14</f>
-        <v>3.1866725580745358E-4</v>
-      </c>
-      <c r="AS8" s="10">
-        <f>BNVFE!H14</f>
-        <v>3.2176784865192677E-4</v>
-      </c>
-      <c r="AT8" s="10">
-        <f>BNVFE!I14</f>
-        <v>3.2673519826153288E-4</v>
-      </c>
-      <c r="AU8" s="10">
-        <f>BNVFE!J14</f>
-        <v>3.3038240919707824E-4</v>
-      </c>
-      <c r="AV8" s="10">
-        <f>BNVFE!K14</f>
-        <v>3.3340389823551702E-4</v>
-      </c>
-      <c r="AW8" s="10">
-        <f>BNVFE!L14</f>
-        <v>3.3475402773417714E-4</v>
-      </c>
-      <c r="AX8" s="10">
-        <f>BNVFE!M14</f>
-        <v>3.3555107094994109E-4</v>
-      </c>
-      <c r="AY8" s="10">
-        <f>BNVFE!N14</f>
-        <v>3.3533649804280095E-4</v>
-      </c>
-      <c r="AZ8" s="10">
-        <f>BNVFE!O14</f>
-        <v>3.3530916094466514E-4</v>
-      </c>
-      <c r="BA8" s="10">
-        <f>BNVFE!P14</f>
-        <v>3.3543094523282268E-4</v>
-      </c>
-      <c r="BB8" s="10">
-        <f>BNVFE!Q14</f>
-        <v>3.3562165718775656E-4</v>
-      </c>
-      <c r="BC8" s="10">
-        <f>BNVFE!R14</f>
-        <v>3.3577393040427292E-4</v>
-      </c>
-      <c r="BD8" s="10">
-        <f>BNVFE!S14</f>
-        <v>3.3592389782957394E-4</v>
-      </c>
-      <c r="BE8" s="10">
-        <f>BNVFE!T14</f>
-        <v>3.3615828155893885E-4</v>
-      </c>
-      <c r="BF8" s="10">
-        <f>BNVFE!U14</f>
-        <v>3.3637923107499002E-4</v>
-      </c>
-      <c r="BG8" s="10">
-        <f>BNVFE!V14</f>
-        <v>3.3656727929620473E-4</v>
-      </c>
-      <c r="BH8" s="10">
-        <f>BNVFE!W14</f>
-        <v>3.3676884833871952E-4</v>
-      </c>
-      <c r="BI8" s="10">
-        <f>BNVFE!X14</f>
-        <v>3.3691991114356807E-4</v>
-      </c>
-      <c r="BJ8" s="10">
-        <f>BNVFE!Y14</f>
-        <v>3.3705013729136348E-4</v>
-      </c>
-      <c r="BK8" s="10">
-        <f>BNVFE!Z14</f>
-        <v>3.3713686099786852E-4</v>
-      </c>
-      <c r="BL8" s="10">
-        <f>BNVFE!AA14</f>
-        <v>3.3722694633495147E-4</v>
-      </c>
-      <c r="BM8" s="10">
-        <f>BNVFE!AB14</f>
-        <v>3.3729739602263772E-4</v>
-      </c>
-      <c r="BN8" s="10">
-        <f>BNVFE!AC14</f>
-        <v>3.3742953237129352E-4</v>
-      </c>
-      <c r="BO8" s="10">
-        <f>BNVFE!AD14</f>
-        <v>3.3751721202413692E-4</v>
-      </c>
-      <c r="BP8" s="10">
-        <f>BNVFE!AE14</f>
-        <v>3.3760101841942016E-4</v>
-      </c>
-      <c r="BQ8" s="10">
-        <f>BNVFE!AF14</f>
-        <v>3.3764787130259203E-4</v>
-      </c>
-      <c r="BR8" s="10">
-        <f>BNVFE!AG14</f>
-        <v>3.3772719520374359E-4</v>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AO8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AP8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AQ8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AR8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AS8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AT8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AU8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AV8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AW8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AX8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AY8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="AZ8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BA8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BB8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BC8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BD8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BE8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BF8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BG8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BH8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BI8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BJ8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BK8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BL8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BM8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BN8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BO8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BP8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BQ8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
+      </c>
+      <c r="BR8" s="4">
+        <f t="shared" si="6"/>
+        <v>7.1745362435245036E-5</v>
       </c>
       <c r="BS8" s="10"/>
       <c r="BT8" s="4"/>
@@ -21199,264 +21197,264 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="19">
-        <f>TREND($AO9:$AT9,$AO$1:$AT$1,F$1)</f>
-        <v>1.817249284777292E-3</v>
-      </c>
-      <c r="G9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.7968922323952086E-3</v>
-      </c>
-      <c r="H9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.7765351800131182E-3</v>
-      </c>
-      <c r="I9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.7561781276310348E-3</v>
-      </c>
-      <c r="J9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.7358210752489514E-3</v>
-      </c>
-      <c r="K9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.7154640228668611E-3</v>
-      </c>
-      <c r="L9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.6951069704847777E-3</v>
-      </c>
-      <c r="M9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.6747499181026873E-3</v>
-      </c>
-      <c r="N9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.6543928657206039E-3</v>
-      </c>
-      <c r="O9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.6340358133385205E-3</v>
-      </c>
-      <c r="P9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.6136787609564301E-3</v>
-      </c>
-      <c r="Q9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.5933217085743467E-3</v>
-      </c>
-      <c r="R9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.5729646561922633E-3</v>
-      </c>
-      <c r="S9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.552607603810173E-3</v>
-      </c>
-      <c r="T9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.5322505514280896E-3</v>
-      </c>
-      <c r="U9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.5118934990460062E-3</v>
-      </c>
-      <c r="V9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.4915364466639158E-3</v>
-      </c>
-      <c r="W9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.4711793942818324E-3</v>
-      </c>
-      <c r="X9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.450822341899749E-3</v>
-      </c>
-      <c r="Y9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.4304652895176587E-3</v>
-      </c>
-      <c r="Z9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.4101082371355753E-3</v>
-      </c>
-      <c r="AA9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.3897511847534849E-3</v>
-      </c>
-      <c r="AB9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.3693941323714015E-3</v>
-      </c>
-      <c r="AC9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.3490370799893181E-3</v>
-      </c>
-      <c r="AD9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.3286800276072278E-3</v>
-      </c>
-      <c r="AE9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.3083229752251443E-3</v>
-      </c>
-      <c r="AF9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2879659228430609E-3</v>
-      </c>
-      <c r="AG9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2676088704609706E-3</v>
-      </c>
-      <c r="AH9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2472518180788872E-3</v>
-      </c>
-      <c r="AI9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2268947656968038E-3</v>
-      </c>
-      <c r="AJ9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2065377133147134E-3</v>
-      </c>
-      <c r="AK9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.18618066093263E-3</v>
-      </c>
-      <c r="AL9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.1658236085505466E-3</v>
-      </c>
-      <c r="AM9" s="19">
-        <f t="shared" si="6"/>
-        <v>1.1454665561684563E-3</v>
-      </c>
-      <c r="AN9" s="29">
-        <f t="shared" si="6"/>
-        <v>1.1251095037863729E-3</v>
-      </c>
-      <c r="AO9" s="10">
-        <f>BNVFE!D15</f>
-        <v>1.2294220931562134E-3</v>
-      </c>
-      <c r="AP9" s="10">
-        <f>BNVFE!E15</f>
-        <v>9.7770537903301043E-4</v>
-      </c>
-      <c r="AQ9" s="10">
-        <f>BNVFE!F15</f>
-        <v>1.0080542097404184E-3</v>
-      </c>
-      <c r="AR9" s="10">
-        <f>BNVFE!G15</f>
-        <v>1.0240291452707345E-3</v>
-      </c>
-      <c r="AS9" s="10">
-        <f>BNVFE!H15</f>
-        <v>1.0339928217467291E-3</v>
-      </c>
-      <c r="AT9" s="10">
-        <f>BNVFE!I15</f>
-        <v>1.049955273747318E-3</v>
-      </c>
-      <c r="AU9" s="10">
-        <f>BNVFE!J15</f>
-        <v>1.0616754935969699E-3</v>
-      </c>
-      <c r="AV9" s="10">
-        <f>BNVFE!K15</f>
-        <v>1.0713849719983116E-3</v>
-      </c>
-      <c r="AW9" s="10">
-        <f>BNVFE!L15</f>
-        <v>1.0757235789035442E-3</v>
-      </c>
-      <c r="AX9" s="10">
-        <f>BNVFE!M15</f>
-        <v>1.0782848570647235E-3</v>
-      </c>
-      <c r="AY9" s="10">
-        <f>BNVFE!N15</f>
-        <v>1.0775953324691067E-3</v>
-      </c>
-      <c r="AZ9" s="10">
-        <f>BNVFE!O15</f>
-        <v>1.0775074853975044E-3</v>
-      </c>
-      <c r="BA9" s="10">
-        <f>BNVFE!P15</f>
-        <v>1.0778988361191009E-3</v>
-      </c>
-      <c r="BB9" s="10">
-        <f>BNVFE!Q15</f>
-        <v>1.0785116841499065E-3</v>
-      </c>
-      <c r="BC9" s="10">
-        <f>BNVFE!R15</f>
-        <v>1.0790010102695979E-3</v>
-      </c>
-      <c r="BD9" s="10">
-        <f>BNVFE!S15</f>
-        <v>1.0794829267876918E-3</v>
-      </c>
-      <c r="BE9" s="10">
-        <f>BNVFE!T15</f>
-        <v>1.0802361129581342E-3</v>
-      </c>
-      <c r="BF9" s="10">
-        <f>BNVFE!U15</f>
-        <v>1.0809461286247785E-3</v>
-      </c>
-      <c r="BG9" s="10">
-        <f>BNVFE!V15</f>
-        <v>1.0815504168148291E-3</v>
-      </c>
-      <c r="BH9" s="10">
-        <f>BNVFE!W15</f>
-        <v>1.0821981538212447E-3</v>
-      </c>
-      <c r="BI9" s="10">
-        <f>BNVFE!X15</f>
-        <v>1.0826835903137368E-3</v>
-      </c>
-      <c r="BJ9" s="10">
-        <f>BNVFE!Y15</f>
-        <v>1.0831020687371974E-3</v>
-      </c>
-      <c r="BK9" s="10">
-        <f>BNVFE!Z15</f>
-        <v>1.0833807531687749E-3</v>
-      </c>
-      <c r="BL9" s="10">
-        <f>BNVFE!AA15</f>
-        <v>1.0836702401149649E-3</v>
-      </c>
-      <c r="BM9" s="10">
-        <f>BNVFE!AB15</f>
-        <v>1.0838966283997708E-3</v>
-      </c>
-      <c r="BN9" s="10">
-        <f>BNVFE!AC15</f>
-        <v>1.0843212452052544E-3</v>
-      </c>
-      <c r="BO9" s="10">
-        <f>BNVFE!AD15</f>
-        <v>1.0846030015461477E-3</v>
-      </c>
-      <c r="BP9" s="10">
-        <f>BNVFE!AE15</f>
-        <v>1.0848723112720957E-3</v>
-      </c>
-      <c r="BQ9" s="10">
-        <f>BNVFE!AF15</f>
-        <v>1.0850228718239992E-3</v>
-      </c>
-      <c r="BR9" s="10">
-        <f>BNVFE!AG15</f>
-        <v>1.0852777771687293E-3</v>
+        <f>SYFAFE!$B$5</f>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="G9" s="4">
+        <f>F9</f>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" ref="H9:BR9" si="7">G9</f>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="R9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="W9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="X9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="Y9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="Z9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AA9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AB9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AC9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AD9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AE9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AF9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AG9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AH9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AI9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AJ9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AK9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AL9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AM9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AN9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AO9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AP9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AQ9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AR9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AS9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AT9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AU9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AV9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AW9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AX9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AY9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="AZ9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BA9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BB9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BC9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BD9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BE9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BF9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BG9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BH9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BI9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BJ9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BK9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BL9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BM9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BN9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BO9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BP9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BQ9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
+      </c>
+      <c r="BR9" s="4">
+        <f t="shared" si="7"/>
+        <v>7.5686214263268839E-4</v>
       </c>
       <c r="BS9" s="10"/>
       <c r="BT9" s="4"/>
@@ -21476,139 +21474,139 @@
         <v>3.2890937975528366E-3</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" ref="G10:AN13" si="7">TREND($AO10:$BR10,$AO$1:$BR$1,G$1)</f>
+        <f t="shared" ref="G10:AN13" si="8">TREND($AO10:$BR10,$AO$1:$BR$1,G$1)</f>
         <v>3.2917330420467188E-3</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.294372286540601E-3</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2970115310344832E-3</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2996507755283645E-3</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3022900200222467E-3</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3049292645161289E-3</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3075685090100111E-3</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3102077535038933E-3</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3128469979977755E-3</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3154862424916577E-3</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.318125486985539E-3</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3207647314794212E-3</v>
       </c>
       <c r="S10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3234039759733034E-3</v>
       </c>
       <c r="T10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3260432204671856E-3</v>
       </c>
       <c r="U10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3286824649610678E-3</v>
       </c>
       <c r="V10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.33132170945495E-3</v>
       </c>
       <c r="W10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3339609539488322E-3</v>
       </c>
       <c r="X10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3366001984427144E-3</v>
       </c>
       <c r="Y10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3392394429365957E-3</v>
       </c>
       <c r="Z10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3418786874304779E-3</v>
       </c>
       <c r="AA10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3445179319243601E-3</v>
       </c>
       <c r="AB10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3471571764182423E-3</v>
       </c>
       <c r="AC10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3497964209121245E-3</v>
       </c>
       <c r="AD10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3524356654060067E-3</v>
       </c>
       <c r="AE10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3550749098998889E-3</v>
       </c>
       <c r="AF10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3577141543937711E-3</v>
       </c>
       <c r="AG10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3603533988876525E-3</v>
       </c>
       <c r="AH10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3629926433815347E-3</v>
       </c>
       <c r="AI10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3656318878754169E-3</v>
       </c>
       <c r="AJ10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3682711323692991E-3</v>
       </c>
       <c r="AK10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3709103768631813E-3</v>
       </c>
       <c r="AL10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3735496213570635E-3</v>
       </c>
       <c r="AM10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3761888658509456E-3</v>
       </c>
-      <c r="AN10" s="28">
-        <f t="shared" si="7"/>
+      <c r="AN10" s="26">
+        <f t="shared" si="8"/>
         <v>3.3788281103448278E-3</v>
       </c>
       <c r="AO10" s="10">
@@ -21750,135 +21748,135 @@
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="T11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="U11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="V11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="X11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="Y11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="Z11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AA11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AB11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AC11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AD11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AE11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AF11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AG11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AH11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AI11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AJ11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AK11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AL11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AM11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
-      <c r="AN11" s="28">
-        <f t="shared" si="7"/>
+      <c r="AN11" s="26">
+        <f t="shared" si="8"/>
         <v>1.2594546332724645E-5</v>
       </c>
       <c r="AO11" s="10">
@@ -22020,135 +22018,135 @@
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="V12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="X12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="Y12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AA12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AB12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AC12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AD12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AE12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AF12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AG12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AH12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AI12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AJ12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AK12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AL12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AM12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
-      <c r="AN12" s="28">
-        <f t="shared" si="7"/>
+      <c r="AN12" s="26">
+        <f t="shared" si="8"/>
         <v>5.2454271866069317E-3</v>
       </c>
       <c r="AO12" s="10">
@@ -22306,71 +22304,71 @@
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="X13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="Y13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="Z13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AA13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AB13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AC13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AD13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AE13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AF13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AG13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AH13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AI13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AJ13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AK13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AL13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AM13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
-      <c r="AN13" s="28">
-        <f t="shared" si="7"/>
+      <c r="AN13" s="26">
+        <f t="shared" si="8"/>
         <v>1.4345302324303025E-3</v>
       </c>
       <c r="AO13" s="10">
@@ -22524,74 +22522,74 @@
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
       <c r="W14">
-        <f t="shared" ref="W14:AM14" si="8">$AO14</f>
+        <f t="shared" ref="W14:AM14" si="9">$AO14</f>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK14" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AL14" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AM14" s="20">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AN14" s="30">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AN14" s="28">
         <f>$AO14</f>
         <v>0</v>
       </c>
@@ -22718,10 +22716,10 @@
       <c r="BS14" s="11"/>
     </row>
     <row r="15" spans="1:72">
-      <c r="E15" s="24"/>
+      <c r="E15" s="22"/>
       <c r="X15" s="4"/>
       <c r="AH15" s="4"/>
-      <c r="AN15" s="27"/>
+      <c r="AN15" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22737,7 +22735,7 @@
   <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Edits for BAU aviation emissions
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4895BA9-0971-484C-8231-CFE662F3F61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A472C0A-45AB-4862-9C04-77E6914BDDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1293,7 +1293,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1333,10 +1333,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="43" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="154" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -4715,169 +4711,169 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>4.236427364823752E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>4.2882977835183994E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>4.3401682022130295E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4.3920386209076769E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>4.4439090396023069E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>4.4957794582969543E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>4.5476498769915844E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>4.5995202956862317E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>4.6513907143808618E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>4.7032611330755092E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.7551315517701392E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>4.8070019704647866E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>4.8588723891594167E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>4.9107428078540641E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>4.9626132265486941E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>5.0144836452433242E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>5.0663540639379716E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>5.1182244826326016E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>5.170094901327249E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>5.2219653200218791E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>5.2738357387165265E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>5.3257061574111565E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>5.3775765761058039E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>5.429446994800434E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>5.4813174134950814E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
                   <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>5.6525537747016295E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>5.6816948983254214E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>5.7128317518608321E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>5.7537137435165198E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>5.8053804811384778E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>5.8402553055494823E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>5.8760417107298871E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>5.9096130220580865E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>5.946019196444121E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>5.9865845018156332E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>6.0321943227520944E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>6.0839429137508894E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>6.1395089969970801E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>6.1977379967962927E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>6.2567088851316315E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>6.3167004143386532E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>6.3779136032516399E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>6.437466870978497E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>6.4981143154692399E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>6.5593323238593052E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>6.6206558943440969E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>6.6830617483670774E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>6.7444724581067943E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>6.8055623616867665E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>6.8655076394605308E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>6.9253674881163997E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>6.9843365885812099E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>7.0421403083949718E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>7.0992567085904998E-4</c:v>
+                  <c:v>5.7245968727451246E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9131,99 +9127,99 @@
       </c>
       <c r="B2" s="4">
         <f>B$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3780336177922486E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="C2" s="4">
         <f>C$5/(1-'Other Values'!$B$3)</f>
-        <v>1.394702045298585E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="D2" s="4">
         <f>D$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4113704728049271E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="E2" s="4">
         <f>E$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4280389003112637E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="F2" s="4">
         <f>F$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4447073278176057E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="G2" s="4">
         <f>G$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4613757553239421E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="H2" s="4">
         <f>H$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4780441828302841E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="I2" s="4">
         <f>I$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4947126103366205E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="J2" s="4">
         <f>J$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5113810378429625E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="K2" s="4">
         <f>K$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5280494653492991E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="L2" s="4">
         <f>L$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5447178928556411E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="M2" s="4">
         <f>M$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5613863203619775E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="N2" s="4">
         <f>N$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5780547478683195E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="O2" s="4">
         <f>O$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5947231753746559E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="P2" s="4">
         <f>P$5/(1-'Other Values'!$B$3)</f>
-        <v>1.6113916028809925E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="Q2" s="4">
         <f>Q$5/(1-'Other Values'!$B$3)</f>
-        <v>1.6280600303873345E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="R2" s="4">
         <f>R$5/(1-'Other Values'!$B$3)</f>
-        <v>1.6447284578936709E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="S2" s="4">
         <f>S$5/(1-'Other Values'!$B$3)</f>
-        <v>1.661396885400013E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="T2" s="4">
         <f>T$5/(1-'Other Values'!$B$3)</f>
-        <v>1.6780653129063493E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="U2" s="4">
         <f>U$5/(1-'Other Values'!$B$3)</f>
-        <v>1.6947337404126914E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="V2" s="4">
         <f>V$5/(1-'Other Values'!$B$3)</f>
-        <v>1.711402167919028E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="W2" s="4">
         <f>W$5/(1-'Other Values'!$B$3)</f>
-        <v>1.72807059542537E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="X2" s="4">
         <f>X$5/(1-'Other Values'!$B$3)</f>
-        <v>1.7447390229317064E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="Y2" s="4">
         <f>Y$5/(1-'Other Values'!$B$3)</f>
-        <v>1.7614074504380484E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="Z2" s="4">
         <f>Z$5/(1-'Other Values'!$B$3)</f>
@@ -9231,23 +9227,23 @@
       </c>
       <c r="AA2" s="4">
         <f>AA$5/(1-'Other Values'!$B$3)</f>
-        <v>1.8164338208636196E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="AB2" s="4">
         <f>AB$5/(1-'Other Values'!$B$3)</f>
-        <v>1.8257982470394711E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="AC2" s="4">
         <f>AC$5/(1-'Other Values'!$B$3)</f>
-        <v>1.8358039959613347E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="AD2" s="4">
         <f>AD$5/(1-'Other Values'!$B$3)</f>
-        <v>1.8489413203048922E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="AE2" s="4">
         <f>AE$5/(1-'Other Values'!$B$3)</f>
-        <v>1.865544295415052E-3</v>
+        <v>1.8395846877216544E-3</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
@@ -9448,99 +9444,99 @@
       </c>
       <c r="B5" s="4">
         <f>Extrapolations!Q6</f>
-        <v>4.2882977835183994E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="C5" s="4">
         <f>Extrapolations!R6</f>
-        <v>4.3401682022130295E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="D5" s="4">
         <f>Extrapolations!S6</f>
-        <v>4.3920386209076769E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="E5" s="4">
         <f>Extrapolations!T6</f>
-        <v>4.4439090396023069E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="F5" s="4">
         <f>Extrapolations!U6</f>
-        <v>4.4957794582969543E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="G5" s="4">
         <f>Extrapolations!V6</f>
-        <v>4.5476498769915844E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="H5" s="4">
         <f>Extrapolations!W6</f>
-        <v>4.5995202956862317E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="I5" s="4">
         <f>Extrapolations!X6</f>
-        <v>4.6513907143808618E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="J5" s="4">
         <f>Extrapolations!Y6</f>
-        <v>4.7032611330755092E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="K5" s="4">
         <f>Extrapolations!Z6</f>
-        <v>4.7551315517701392E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="L5" s="4">
         <f>Extrapolations!AA6</f>
-        <v>4.8070019704647866E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="M5" s="4">
         <f>Extrapolations!AB6</f>
-        <v>4.8588723891594167E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="N5" s="4">
         <f>Extrapolations!AC6</f>
-        <v>4.9107428078540641E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="O5" s="4">
         <f>Extrapolations!AD6</f>
-        <v>4.9626132265486941E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="P5" s="4">
         <f>Extrapolations!AE6</f>
-        <v>5.0144836452433242E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>Extrapolations!AF6</f>
-        <v>5.0663540639379716E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="R5" s="4">
         <f>Extrapolations!AG6</f>
-        <v>5.1182244826326016E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="S5" s="4">
         <f>Extrapolations!AH6</f>
-        <v>5.170094901327249E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="T5" s="4">
         <f>Extrapolations!AI6</f>
-        <v>5.2219653200218791E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="U5" s="4">
         <f>Extrapolations!AJ6</f>
-        <v>5.2738357387165265E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="V5" s="4">
         <f>Extrapolations!AK6</f>
-        <v>5.3257061574111565E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="W5" s="4">
         <f>Extrapolations!AL6</f>
-        <v>5.3775765761058039E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="X5" s="4">
         <f>Extrapolations!AM6</f>
-        <v>5.429446994800434E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>Extrapolations!AN6</f>
-        <v>5.4813174134950814E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>Extrapolations!AO6</f>
@@ -9548,23 +9544,23 @@
       </c>
       <c r="AA5" s="4">
         <f>Extrapolations!AP6</f>
-        <v>5.6525537747016295E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>Extrapolations!AQ6</f>
-        <v>5.6816948983254214E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>Extrapolations!AR6</f>
-        <v>5.7128317518608321E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>Extrapolations!AS6</f>
-        <v>5.7537137435165198E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>Extrapolations!AT6</f>
-        <v>5.8053804811384778E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -9765,99 +9761,99 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.2864893350555196E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.3020504606639086E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.3176115862723028E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.3331727118806919E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.3487338374890861E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.3642949630974751E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.3798560887058693E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.3954172143142583E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.4109783399226525E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.4265394655310416E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.4421005911394358E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.4576617167478248E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.473222842356219E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.488783967964608E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.504345093572997E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.5199062191813913E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.5354673447897803E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.5510284703981745E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.5665895960065635E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.5821507216149577E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.5977118472233467E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.613272972831741E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.62883409844013E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.6443952240485242E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
@@ -9865,23 +9861,23 @@
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>1.6957661324104886E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.7045084694976261E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.7138495255582494E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.7261141230549557E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.7416141443415431E-3</v>
+        <v>1.7173790618235372E-3</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4"/>
@@ -10775,110 +10771,109 @@
   </sheetPr>
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="30">
+      <c r="B1">
         <v>2021</v>
       </c>
-      <c r="C1" s="30">
+      <c r="C1">
         <v>2022</v>
       </c>
-      <c r="D1" s="30">
+      <c r="D1">
         <v>2023</v>
       </c>
-      <c r="E1" s="30">
+      <c r="E1">
         <v>2024</v>
       </c>
-      <c r="F1" s="30">
+      <c r="F1">
         <v>2025</v>
       </c>
-      <c r="G1" s="30">
+      <c r="G1">
         <v>2026</v>
       </c>
-      <c r="H1" s="30">
+      <c r="H1">
         <v>2027</v>
       </c>
-      <c r="I1" s="30">
+      <c r="I1">
         <v>2028</v>
       </c>
-      <c r="J1" s="30">
+      <c r="J1">
         <v>2029</v>
       </c>
-      <c r="K1" s="30">
+      <c r="K1">
         <v>2030</v>
       </c>
-      <c r="L1" s="30">
+      <c r="L1">
         <v>2031</v>
       </c>
-      <c r="M1" s="30">
+      <c r="M1">
         <v>2032</v>
       </c>
-      <c r="N1" s="30">
+      <c r="N1">
         <v>2033</v>
       </c>
-      <c r="O1" s="30">
+      <c r="O1">
         <v>2034</v>
       </c>
-      <c r="P1" s="30">
+      <c r="P1">
         <v>2035</v>
       </c>
-      <c r="Q1" s="30">
+      <c r="Q1">
         <v>2036</v>
       </c>
-      <c r="R1" s="30">
+      <c r="R1">
         <v>2037</v>
       </c>
-      <c r="S1" s="30">
+      <c r="S1">
         <v>2038</v>
       </c>
-      <c r="T1" s="30">
+      <c r="T1">
         <v>2039</v>
       </c>
-      <c r="U1" s="30">
+      <c r="U1">
         <v>2040</v>
       </c>
-      <c r="V1" s="30">
+      <c r="V1">
         <v>2041</v>
       </c>
-      <c r="W1" s="30">
+      <c r="W1">
         <v>2042</v>
       </c>
-      <c r="X1" s="30">
+      <c r="X1">
         <v>2043</v>
       </c>
-      <c r="Y1" s="30">
+      <c r="Y1">
         <v>2044</v>
       </c>
-      <c r="Z1" s="30">
+      <c r="Z1">
         <v>2045</v>
       </c>
-      <c r="AA1" s="30">
+      <c r="AA1">
         <v>2046</v>
       </c>
-      <c r="AB1" s="30">
+      <c r="AB1">
         <v>2047</v>
       </c>
-      <c r="AC1" s="30">
+      <c r="AC1">
         <v>2048</v>
       </c>
-      <c r="AD1" s="30">
+      <c r="AD1">
         <v>2049</v>
       </c>
-      <c r="AE1" s="30">
+      <c r="AE1">
         <v>2050</v>
       </c>
     </row>
@@ -11008,507 +11003,507 @@
       </c>
     </row>
     <row r="3" spans="1:32">
-      <c r="A3" s="30" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="30">
-        <v>0</v>
-      </c>
-      <c r="C3" s="30">
-        <v>0</v>
-      </c>
-      <c r="D3" s="30">
-        <v>0</v>
-      </c>
-      <c r="E3" s="30">
-        <v>0</v>
-      </c>
-      <c r="F3" s="30">
-        <v>0</v>
-      </c>
-      <c r="G3" s="30">
-        <v>0</v>
-      </c>
-      <c r="H3" s="30">
-        <v>0</v>
-      </c>
-      <c r="I3" s="30">
-        <v>0</v>
-      </c>
-      <c r="J3" s="30">
-        <v>0</v>
-      </c>
-      <c r="K3" s="30">
-        <v>0</v>
-      </c>
-      <c r="L3" s="30">
-        <v>0</v>
-      </c>
-      <c r="M3" s="30">
-        <v>0</v>
-      </c>
-      <c r="N3" s="30">
-        <v>0</v>
-      </c>
-      <c r="O3" s="30">
-        <v>0</v>
-      </c>
-      <c r="P3" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="30">
-        <v>0</v>
-      </c>
-      <c r="R3" s="30">
-        <v>0</v>
-      </c>
-      <c r="S3" s="30">
-        <v>0</v>
-      </c>
-      <c r="T3" s="30">
-        <v>0</v>
-      </c>
-      <c r="U3" s="30">
-        <v>0</v>
-      </c>
-      <c r="V3" s="30">
-        <v>0</v>
-      </c>
-      <c r="W3" s="30">
-        <v>0</v>
-      </c>
-      <c r="X3" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="30">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="30" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="30">
-        <v>0</v>
-      </c>
-      <c r="C4" s="30">
-        <v>0</v>
-      </c>
-      <c r="D4" s="30">
-        <v>0</v>
-      </c>
-      <c r="E4" s="30">
-        <v>0</v>
-      </c>
-      <c r="F4" s="30">
-        <v>0</v>
-      </c>
-      <c r="G4" s="30">
-        <v>0</v>
-      </c>
-      <c r="H4" s="30">
-        <v>0</v>
-      </c>
-      <c r="I4" s="30">
-        <v>0</v>
-      </c>
-      <c r="J4" s="30">
-        <v>0</v>
-      </c>
-      <c r="K4" s="30">
-        <v>0</v>
-      </c>
-      <c r="L4" s="30">
-        <v>0</v>
-      </c>
-      <c r="M4" s="30">
-        <v>0</v>
-      </c>
-      <c r="N4" s="30">
-        <v>0</v>
-      </c>
-      <c r="O4" s="30">
-        <v>0</v>
-      </c>
-      <c r="P4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="30">
-        <v>0</v>
-      </c>
-      <c r="R4" s="30">
-        <v>0</v>
-      </c>
-      <c r="S4" s="30">
-        <v>0</v>
-      </c>
-      <c r="T4" s="30">
-        <v>0</v>
-      </c>
-      <c r="U4" s="30">
-        <v>0</v>
-      </c>
-      <c r="V4" s="30">
-        <v>0</v>
-      </c>
-      <c r="W4" s="30">
-        <v>0</v>
-      </c>
-      <c r="X4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="30">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="30" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="29">
         <f>Extrapolations!G8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <f>Extrapolations!H8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <f>Extrapolations!I8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <f>Extrapolations!J8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="29">
         <f>Extrapolations!K8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="29">
         <f>Extrapolations!L8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="29">
         <f>Extrapolations!M8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="29">
         <f>Extrapolations!N8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="29">
         <f>Extrapolations!O8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="29">
         <f>Extrapolations!P8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="29">
         <f>Extrapolations!Q8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="29">
         <f>Extrapolations!R8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="29">
         <f>Extrapolations!S8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="29">
         <f>Extrapolations!T8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="P5" s="31">
+      <c r="P5" s="29">
         <f>Extrapolations!U8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="29">
         <f>Extrapolations!V8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="29">
         <f>Extrapolations!W8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="S5" s="31">
+      <c r="S5" s="29">
         <f>Extrapolations!X8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="29">
         <f>Extrapolations!Y8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="U5" s="31">
+      <c r="U5" s="29">
         <f>Extrapolations!Z8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="V5" s="31">
+      <c r="V5" s="29">
         <f>Extrapolations!AA8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="W5" s="31">
+      <c r="W5" s="29">
         <f>Extrapolations!AB8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="29">
         <f>Extrapolations!AC8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="Y5" s="31">
+      <c r="Y5" s="29">
         <f>Extrapolations!AD8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="Z5" s="31">
+      <c r="Z5" s="29">
         <f>Extrapolations!AE8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="AA5" s="31">
+      <c r="AA5" s="29">
         <f>Extrapolations!AF8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="AB5" s="31">
+      <c r="AB5" s="29">
         <f>Extrapolations!AG8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="AC5" s="31">
+      <c r="AC5" s="29">
         <f>Extrapolations!AH8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="AD5" s="31">
+      <c r="AD5" s="29">
         <f>Extrapolations!AI8</f>
         <v>7.1745362435245036E-5</v>
       </c>
-      <c r="AE5" s="31">
+      <c r="AE5" s="29">
         <f>Extrapolations!AJ8</f>
         <v>7.1745362435245036E-5</v>
       </c>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="30" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30">
-        <v>0</v>
-      </c>
-      <c r="C6" s="30">
-        <v>0</v>
-      </c>
-      <c r="D6" s="30">
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
-        <v>0</v>
-      </c>
-      <c r="K6" s="30">
-        <v>0</v>
-      </c>
-      <c r="L6" s="30">
-        <v>0</v>
-      </c>
-      <c r="M6" s="30">
-        <v>0</v>
-      </c>
-      <c r="N6" s="30">
-        <v>0</v>
-      </c>
-      <c r="O6" s="30">
-        <v>0</v>
-      </c>
-      <c r="P6" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="30">
-        <v>0</v>
-      </c>
-      <c r="R6" s="30">
-        <v>0</v>
-      </c>
-      <c r="S6" s="30">
-        <v>0</v>
-      </c>
-      <c r="T6" s="30">
-        <v>0</v>
-      </c>
-      <c r="U6" s="30">
-        <v>0</v>
-      </c>
-      <c r="V6" s="30">
-        <v>0</v>
-      </c>
-      <c r="W6" s="30">
-        <v>0</v>
-      </c>
-      <c r="X6" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="30">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="30" t="s">
+      <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="30">
-        <v>0</v>
-      </c>
-      <c r="C7" s="30">
-        <v>0</v>
-      </c>
-      <c r="D7" s="30">
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
-        <v>0</v>
-      </c>
-      <c r="G7" s="30">
-        <v>0</v>
-      </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0</v>
-      </c>
-      <c r="K7" s="30">
-        <v>0</v>
-      </c>
-      <c r="L7" s="30">
-        <v>0</v>
-      </c>
-      <c r="M7" s="30">
-        <v>0</v>
-      </c>
-      <c r="N7" s="30">
-        <v>0</v>
-      </c>
-      <c r="O7" s="30">
-        <v>0</v>
-      </c>
-      <c r="P7" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="30">
-        <v>0</v>
-      </c>
-      <c r="R7" s="30">
-        <v>0</v>
-      </c>
-      <c r="S7" s="30">
-        <v>0</v>
-      </c>
-      <c r="T7" s="30">
-        <v>0</v>
-      </c>
-      <c r="U7" s="30">
-        <v>0</v>
-      </c>
-      <c r="V7" s="30">
-        <v>0</v>
-      </c>
-      <c r="W7" s="30">
-        <v>0</v>
-      </c>
-      <c r="X7" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="30">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
         <v>0</v>
       </c>
     </row>
@@ -11638,37 +11633,37 @@
       </c>
     </row>
     <row r="13" spans="1:32">
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="32"/>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="32"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16204,8 +16199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16809,91 +16804,91 @@
         <v>5.7245968727451246E-4</v>
       </c>
       <c r="E12" s="4">
-        <v>5.6525537747016295E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="F12" s="4">
-        <v>5.6816948983254214E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="G12" s="4">
-        <v>5.7128317518608321E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="H12" s="4">
-        <v>5.7537137435165198E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="I12" s="4">
-        <v>5.8053804811384778E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="J12" s="4">
-        <v>5.8402553055494823E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="K12" s="4">
-        <v>5.8760417107298871E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="L12" s="4">
-        <v>5.9096130220580865E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="M12" s="4">
-        <v>5.946019196444121E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="N12" s="4">
-        <v>5.9865845018156332E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="O12" s="4">
-        <v>6.0321943227520944E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="P12" s="4">
-        <v>6.0839429137508894E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Q12" s="4">
-        <v>6.1395089969970801E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="R12" s="4">
-        <v>6.1977379967962927E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="S12" s="4">
-        <v>6.2567088851316315E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="T12" s="4">
-        <v>6.3167004143386532E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="U12" s="4">
-        <v>6.3779136032516399E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="V12" s="4">
-        <v>6.437466870978497E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="W12" s="4">
-        <v>6.4981143154692399E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="X12" s="4">
-        <v>6.5593323238593052E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Y12" s="4">
-        <v>6.6206558943440969E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Z12" s="4">
-        <v>6.6830617483670774E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AA12" s="4">
-        <v>6.7444724581067943E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AB12" s="4">
-        <v>6.8055623616867665E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AC12" s="4">
-        <v>6.8655076394605308E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AD12" s="4">
-        <v>6.9253674881163997E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AE12" s="4">
-        <v>6.9843365885812099E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AF12" s="4">
-        <v>7.0421403083949718E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AG12" s="4">
-        <v>7.0992567085904998E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
@@ -20449,103 +20444,103 @@
       <c r="O6" s="9"/>
       <c r="P6" s="4">
         <f>TREND($AO6:$BR6,$AO$1:$BR$1,P$1)</f>
-        <v>4.236427364823752E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" ref="Q6:AN6" si="4">TREND($AO6:$BR6,$AO$1:$BR$1,Q$1)</f>
-        <v>4.2882977835183994E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="4"/>
-        <v>4.3401682022130295E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="4"/>
-        <v>4.3920386209076769E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="T6" s="4">
         <f t="shared" si="4"/>
-        <v>4.4439090396023069E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="U6" s="4">
         <f t="shared" si="4"/>
-        <v>4.4957794582969543E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="V6" s="4">
         <f t="shared" si="4"/>
-        <v>4.5476498769915844E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="W6" s="4">
         <f t="shared" si="4"/>
-        <v>4.5995202956862317E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="X6" s="4">
         <f t="shared" si="4"/>
-        <v>4.6513907143808618E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Y6" s="4">
         <f t="shared" si="4"/>
-        <v>4.7032611330755092E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="4"/>
-        <v>4.7551315517701392E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AA6" s="4">
         <f t="shared" si="4"/>
-        <v>4.8070019704647866E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AB6" s="4">
         <f t="shared" si="4"/>
-        <v>4.8588723891594167E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AC6" s="4">
         <f t="shared" si="4"/>
-        <v>4.9107428078540641E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AD6" s="4">
         <f t="shared" si="4"/>
-        <v>4.9626132265486941E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AE6" s="4">
         <f t="shared" si="4"/>
-        <v>5.0144836452433242E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AF6" s="4">
         <f t="shared" si="4"/>
-        <v>5.0663540639379716E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="4"/>
-        <v>5.1182244826326016E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AH6" s="4">
         <f t="shared" si="4"/>
-        <v>5.170094901327249E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AI6" s="4">
         <f t="shared" si="4"/>
-        <v>5.2219653200218791E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AJ6" s="4">
         <f t="shared" si="4"/>
-        <v>5.2738357387165265E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AK6" s="4">
         <f t="shared" si="4"/>
-        <v>5.3257061574111565E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AL6" s="4">
         <f t="shared" si="4"/>
-        <v>5.3775765761058039E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AM6" s="4">
         <f t="shared" si="4"/>
-        <v>5.429446994800434E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AN6" s="26">
         <f t="shared" si="4"/>
-        <v>5.4813174134950814E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AO6" s="10">
         <f>BNVFE!D12</f>
@@ -20553,119 +20548,119 @@
       </c>
       <c r="AP6" s="10">
         <f>BNVFE!E12</f>
-        <v>5.6525537747016295E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AQ6" s="10">
         <f>BNVFE!F12</f>
-        <v>5.6816948983254214E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AR6" s="10">
         <f>BNVFE!G12</f>
-        <v>5.7128317518608321E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AS6" s="10">
         <f>BNVFE!H12</f>
-        <v>5.7537137435165198E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AT6" s="10">
         <f>BNVFE!I12</f>
-        <v>5.8053804811384778E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AU6" s="10">
         <f>BNVFE!J12</f>
-        <v>5.8402553055494823E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AV6" s="10">
         <f>BNVFE!K12</f>
-        <v>5.8760417107298871E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AW6" s="10">
         <f>BNVFE!L12</f>
-        <v>5.9096130220580865E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AX6" s="10">
         <f>BNVFE!M12</f>
-        <v>5.946019196444121E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AY6" s="10">
         <f>BNVFE!N12</f>
-        <v>5.9865845018156332E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="AZ6" s="10">
         <f>BNVFE!O12</f>
-        <v>6.0321943227520944E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BA6" s="10">
         <f>BNVFE!P12</f>
-        <v>6.0839429137508894E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BB6" s="10">
         <f>BNVFE!Q12</f>
-        <v>6.1395089969970801E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BC6" s="10">
         <f>BNVFE!R12</f>
-        <v>6.1977379967962927E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BD6" s="10">
         <f>BNVFE!S12</f>
-        <v>6.2567088851316315E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BE6" s="10">
         <f>BNVFE!T12</f>
-        <v>6.3167004143386532E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BF6" s="10">
         <f>BNVFE!U12</f>
-        <v>6.3779136032516399E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BG6" s="10">
         <f>BNVFE!V12</f>
-        <v>6.437466870978497E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BH6" s="10">
         <f>BNVFE!W12</f>
-        <v>6.4981143154692399E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BI6" s="10">
         <f>BNVFE!X12</f>
-        <v>6.5593323238593052E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BJ6" s="10">
         <f>BNVFE!Y12</f>
-        <v>6.6206558943440969E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BK6" s="10">
         <f>BNVFE!Z12</f>
-        <v>6.6830617483670774E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BL6" s="10">
         <f>BNVFE!AA12</f>
-        <v>6.7444724581067943E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BM6" s="10">
         <f>BNVFE!AB12</f>
-        <v>6.8055623616867665E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BN6" s="10">
         <f>BNVFE!AC12</f>
-        <v>6.8655076394605308E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BO6" s="10">
         <f>BNVFE!AD12</f>
-        <v>6.9253674881163997E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BP6" s="10">
         <f>BNVFE!AE12</f>
-        <v>6.9843365885812099E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BQ6" s="10">
         <f>BNVFE!AF12</f>
-        <v>7.0421403083949718E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BR6" s="10">
         <f>BNVFE!AG12</f>
-        <v>7.0992567085904998E-4</v>
+        <v>5.7245968727451246E-4</v>
       </c>
       <c r="BS6" s="10"/>
       <c r="BT6" s="4"/>

</xml_diff>

<commit_message>
Port recent BNVFE edits into BHNVFEAL
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A472C0A-45AB-4862-9C04-77E6914BDDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3687D9-89B6-4A02-8B8A-CFEA5EACE775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1773,133 +1773,133 @@
                   <c:v>3.142498616321923E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>3.170827862483609E-4</c:v>
+                  <c:v>3.1689948446677165E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>3.199157108645295E-4</c:v>
+                  <c:v>3.1954910730135099E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>3.227486354806981E-4</c:v>
+                  <c:v>3.2219873013593033E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>3.255815600968667E-4</c:v>
+                  <c:v>3.2484835297050968E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>3.284144847130353E-4</c:v>
+                  <c:v>3.2749797580508902E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>3.312474093292039E-4</c:v>
+                  <c:v>3.3014759863966836E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>3.3408033394537249E-4</c:v>
+                  <c:v>3.3279722147424771E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>3.3691325856154109E-4</c:v>
+                  <c:v>3.3544684430882705E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>3.3974618317770969E-4</c:v>
+                  <c:v>3.3809646714340639E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>3.4257910779387829E-4</c:v>
+                  <c:v>3.4074608997798574E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>3.4541203241004689E-4</c:v>
+                  <c:v>3.4339571281256508E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>3.4824495702621549E-4</c:v>
+                  <c:v>3.4604533564714442E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>3.5107788164238408E-4</c:v>
+                  <c:v>3.4869495848172376E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>3.5391080625855263E-4</c:v>
+                  <c:v>3.5134458131630327E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>3.6152338546126896E-4</c:v>
+                  <c:v>3.6011837400814692E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>3.6806778318324615E-4</c:v>
+                  <c:v>3.6765672079173311E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>3.7326311577328699E-4</c:v>
+                  <c:v>3.736430585304968E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>3.8684273091170592E-4</c:v>
+                  <c:v>3.8928883765267276E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.9133628030331842E-4</c:v>
+                  <c:v>3.9446747162568221E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.9460271712590122E-4</c:v>
+                  <c:v>3.9823101405773444E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>4.0654622240144441E-4</c:v>
+                  <c:v>4.1199473204362889E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.0753465089361259E-4</c:v>
+                  <c:v>4.1313289936177025E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>4.0771889354095417E-4</c:v>
+                  <c:v>4.1334468996044436E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.0791884576015625E-4</c:v>
+                  <c:v>4.1357470435096535E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>4.0852284515353123E-4</c:v>
+                  <c:v>4.1427122401939349E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.09583671112226E-4</c:v>
+                  <c:v>4.154939817739491E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>4.1078673798239525E-4</c:v>
+                  <c:v>4.1688094432107664E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>4.122748024320864E-4</c:v>
+                  <c:v>4.1859603308611211E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>4.1373149805260076E-4</c:v>
+                  <c:v>4.2027564609660228E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.1495700440447459E-4</c:v>
+                  <c:v>4.2168774723272802E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>4.1601549646964788E-4</c:v>
+                  <c:v>4.2290738034426306E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>4.1779365223495714E-4</c:v>
+                  <c:v>4.2495638955627015E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>4.1809544457369974E-4</c:v>
+                  <c:v>4.2530341133255339E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>4.1838332983416382E-4</c:v>
+                  <c:v>4.2563408484261415E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>4.1848122624012197E-4</c:v>
+                  <c:v>4.257457185090017E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>4.1826563698301188E-4</c:v>
+                  <c:v>4.2549536074558018E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>4.1769414168042572E-4</c:v>
+                  <c:v>4.2483576932089885E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>4.1714393092982577E-4</c:v>
+                  <c:v>4.2420044731809718E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>4.1708664938544884E-4</c:v>
+                  <c:v>4.2413535117129356E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>4.165029094218215E-4</c:v>
+                  <c:v>4.2346108578435258E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>4.1616572999280917E-4</c:v>
+                  <c:v>4.2307229280284277E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>4.1755377409260071E-4</c:v>
+                  <c:v>4.2467076402359958E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>4.1711981834238049E-4</c:v>
+                  <c:v>4.2417015147939801E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16200,7 +16200,7 @@
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D8" sqref="D8:AG20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16381,94 +16381,94 @@
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>3.5391080625855263E-4</v>
+        <v>3.5134458131630327E-4</v>
       </c>
       <c r="E8" s="4">
-        <v>3.6152338546126896E-4</v>
+        <v>3.6011837400814692E-4</v>
       </c>
       <c r="F8" s="4">
-        <v>3.6806778318324615E-4</v>
+        <v>3.6765672079173311E-4</v>
       </c>
       <c r="G8" s="4">
-        <v>3.7326311577328699E-4</v>
+        <v>3.736430585304968E-4</v>
       </c>
       <c r="H8" s="4">
-        <v>3.8684273091170592E-4</v>
+        <v>3.8928883765267276E-4</v>
       </c>
       <c r="I8" s="4">
-        <v>3.9133628030331842E-4</v>
+        <v>3.9446747162568221E-4</v>
       </c>
       <c r="J8" s="4">
-        <v>3.9460271712590122E-4</v>
+        <v>3.9823101405773444E-4</v>
       </c>
       <c r="K8" s="4">
-        <v>4.0654622240144441E-4</v>
+        <v>4.1199473204362889E-4</v>
       </c>
       <c r="L8" s="4">
-        <v>4.0753465089361259E-4</v>
+        <v>4.1313289936177025E-4</v>
       </c>
       <c r="M8" s="4">
-        <v>4.0771889354095417E-4</v>
+        <v>4.1334468996044436E-4</v>
       </c>
       <c r="N8" s="4">
-        <v>4.0791884576015625E-4</v>
+        <v>4.1357470435096535E-4</v>
       </c>
       <c r="O8" s="4">
-        <v>4.0852284515353123E-4</v>
+        <v>4.1427122401939349E-4</v>
       </c>
       <c r="P8" s="4">
-        <v>4.09583671112226E-4</v>
+        <v>4.154939817739491E-4</v>
       </c>
       <c r="Q8" s="4">
-        <v>4.1078673798239525E-4</v>
+        <v>4.1688094432107664E-4</v>
       </c>
       <c r="R8" s="4">
-        <v>4.122748024320864E-4</v>
+        <v>4.1859603308611211E-4</v>
       </c>
       <c r="S8" s="4">
-        <v>4.1373149805260076E-4</v>
+        <v>4.2027564609660228E-4</v>
       </c>
       <c r="T8" s="4">
-        <v>4.1495700440447459E-4</v>
+        <v>4.2168774723272802E-4</v>
       </c>
       <c r="U8" s="4">
-        <v>4.1601549646964788E-4</v>
+        <v>4.2290738034426306E-4</v>
       </c>
       <c r="V8" s="4">
-        <v>4.1779365223495714E-4</v>
+        <v>4.2495638955627015E-4</v>
       </c>
       <c r="W8" s="4">
-        <v>4.1809544457369974E-4</v>
+        <v>4.2530341133255339E-4</v>
       </c>
       <c r="X8" s="4">
-        <v>4.1838332983416382E-4</v>
+        <v>4.2563408484261415E-4</v>
       </c>
       <c r="Y8" s="4">
-        <v>4.1848122624012197E-4</v>
+        <v>4.257457185090017E-4</v>
       </c>
       <c r="Z8" s="4">
-        <v>4.1826563698301188E-4</v>
+        <v>4.2549536074558018E-4</v>
       </c>
       <c r="AA8" s="4">
-        <v>4.1769414168042572E-4</v>
+        <v>4.2483576932089885E-4</v>
       </c>
       <c r="AB8" s="4">
-        <v>4.1714393092982577E-4</v>
+        <v>4.2420044731809718E-4</v>
       </c>
       <c r="AC8" s="4">
-        <v>4.1708664938544884E-4</v>
+        <v>4.2413535117129356E-4</v>
       </c>
       <c r="AD8" s="4">
-        <v>4.165029094218215E-4</v>
+        <v>4.2346108578435258E-4</v>
       </c>
       <c r="AE8" s="4">
-        <v>4.1616572999280917E-4</v>
+        <v>4.2307229280284277E-4</v>
       </c>
       <c r="AF8" s="4">
-        <v>4.1755377409260071E-4</v>
+        <v>4.2467076402359958E-4</v>
       </c>
       <c r="AG8" s="4">
-        <v>4.1711981834238049E-4</v>
+        <v>4.2417015147939801E-4</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -19151,7 +19151,7 @@
       </c>
       <c r="D16" s="4">
         <f>BNVFE!D8</f>
-        <v>3.5391080625855263E-4</v>
+        <v>3.5134458131630327E-4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -19529,175 +19529,175 @@
       </c>
       <c r="AB2" s="4">
         <f>($AO$2-$AA$2)/COUNT($AB$1:$AO$1)+AA2</f>
-        <v>3.170827862483609E-4</v>
+        <v>3.1689948446677165E-4</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" ref="AC2:AN2" si="0">($AO$2-$AA$2)/COUNT($AB$1:$AO$1)+AB2</f>
-        <v>3.199157108645295E-4</v>
+        <v>3.1954910730135099E-4</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>3.227486354806981E-4</v>
+        <v>3.2219873013593033E-4</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>3.255815600968667E-4</v>
+        <v>3.2484835297050968E-4</v>
       </c>
       <c r="AF2" s="4">
         <f t="shared" si="0"/>
-        <v>3.284144847130353E-4</v>
+        <v>3.2749797580508902E-4</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" si="0"/>
-        <v>3.312474093292039E-4</v>
+        <v>3.3014759863966836E-4</v>
       </c>
       <c r="AH2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3408033394537249E-4</v>
+        <v>3.3279722147424771E-4</v>
       </c>
       <c r="AI2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3691325856154109E-4</v>
+        <v>3.3544684430882705E-4</v>
       </c>
       <c r="AJ2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3974618317770969E-4</v>
+        <v>3.3809646714340639E-4</v>
       </c>
       <c r="AK2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4257910779387829E-4</v>
+        <v>3.4074608997798574E-4</v>
       </c>
       <c r="AL2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4541203241004689E-4</v>
+        <v>3.4339571281256508E-4</v>
       </c>
       <c r="AM2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4824495702621549E-4</v>
+        <v>3.4604533564714442E-4</v>
       </c>
       <c r="AN2" s="26">
         <f t="shared" si="0"/>
-        <v>3.5107788164238408E-4</v>
+        <v>3.4869495848172376E-4</v>
       </c>
       <c r="AO2" s="10">
         <f>BNVFE!D8</f>
-        <v>3.5391080625855263E-4</v>
+        <v>3.5134458131630327E-4</v>
       </c>
       <c r="AP2" s="10">
         <f>BNVFE!E8</f>
-        <v>3.6152338546126896E-4</v>
+        <v>3.6011837400814692E-4</v>
       </c>
       <c r="AQ2" s="10">
         <f>BNVFE!F8</f>
-        <v>3.6806778318324615E-4</v>
+        <v>3.6765672079173311E-4</v>
       </c>
       <c r="AR2" s="10">
         <f>BNVFE!G8</f>
-        <v>3.7326311577328699E-4</v>
+        <v>3.736430585304968E-4</v>
       </c>
       <c r="AS2" s="10">
         <f>BNVFE!H8</f>
-        <v>3.8684273091170592E-4</v>
+        <v>3.8928883765267276E-4</v>
       </c>
       <c r="AT2" s="10">
         <f>BNVFE!I8</f>
-        <v>3.9133628030331842E-4</v>
+        <v>3.9446747162568221E-4</v>
       </c>
       <c r="AU2" s="10">
         <f>BNVFE!J8</f>
-        <v>3.9460271712590122E-4</v>
+        <v>3.9823101405773444E-4</v>
       </c>
       <c r="AV2" s="10">
         <f>BNVFE!K8</f>
-        <v>4.0654622240144441E-4</v>
+        <v>4.1199473204362889E-4</v>
       </c>
       <c r="AW2" s="10">
         <f>BNVFE!L8</f>
-        <v>4.0753465089361259E-4</v>
+        <v>4.1313289936177025E-4</v>
       </c>
       <c r="AX2" s="10">
         <f>BNVFE!M8</f>
-        <v>4.0771889354095417E-4</v>
+        <v>4.1334468996044436E-4</v>
       </c>
       <c r="AY2" s="10">
         <f>BNVFE!N8</f>
-        <v>4.0791884576015625E-4</v>
+        <v>4.1357470435096535E-4</v>
       </c>
       <c r="AZ2" s="10">
         <f>BNVFE!O8</f>
-        <v>4.0852284515353123E-4</v>
+        <v>4.1427122401939349E-4</v>
       </c>
       <c r="BA2" s="10">
         <f>BNVFE!P8</f>
-        <v>4.09583671112226E-4</v>
+        <v>4.154939817739491E-4</v>
       </c>
       <c r="BB2" s="10">
         <f>BNVFE!Q8</f>
-        <v>4.1078673798239525E-4</v>
+        <v>4.1688094432107664E-4</v>
       </c>
       <c r="BC2" s="10">
         <f>BNVFE!R8</f>
-        <v>4.122748024320864E-4</v>
+        <v>4.1859603308611211E-4</v>
       </c>
       <c r="BD2" s="10">
         <f>BNVFE!S8</f>
-        <v>4.1373149805260076E-4</v>
+        <v>4.2027564609660228E-4</v>
       </c>
       <c r="BE2" s="10">
         <f>BNVFE!T8</f>
-        <v>4.1495700440447459E-4</v>
+        <v>4.2168774723272802E-4</v>
       </c>
       <c r="BF2" s="10">
         <f>BNVFE!U8</f>
-        <v>4.1601549646964788E-4</v>
+        <v>4.2290738034426306E-4</v>
       </c>
       <c r="BG2" s="10">
         <f>BNVFE!V8</f>
-        <v>4.1779365223495714E-4</v>
+        <v>4.2495638955627015E-4</v>
       </c>
       <c r="BH2" s="10">
         <f>BNVFE!W8</f>
-        <v>4.1809544457369974E-4</v>
+        <v>4.2530341133255339E-4</v>
       </c>
       <c r="BI2" s="10">
         <f>BNVFE!X8</f>
-        <v>4.1838332983416382E-4</v>
+        <v>4.2563408484261415E-4</v>
       </c>
       <c r="BJ2" s="10">
         <f>BNVFE!Y8</f>
-        <v>4.1848122624012197E-4</v>
+        <v>4.257457185090017E-4</v>
       </c>
       <c r="BK2" s="10">
         <f>BNVFE!Z8</f>
-        <v>4.1826563698301188E-4</v>
+        <v>4.2549536074558018E-4</v>
       </c>
       <c r="BL2" s="10">
         <f>BNVFE!AA8</f>
-        <v>4.1769414168042572E-4</v>
+        <v>4.2483576932089885E-4</v>
       </c>
       <c r="BM2" s="10">
         <f>BNVFE!AB8</f>
-        <v>4.1714393092982577E-4</v>
+        <v>4.2420044731809718E-4</v>
       </c>
       <c r="BN2" s="10">
         <f>BNVFE!AC8</f>
-        <v>4.1708664938544884E-4</v>
+        <v>4.2413535117129356E-4</v>
       </c>
       <c r="BO2" s="10">
         <f>BNVFE!AD8</f>
-        <v>4.165029094218215E-4</v>
+        <v>4.2346108578435258E-4</v>
       </c>
       <c r="BP2" s="10">
         <f>BNVFE!AE8</f>
-        <v>4.1616572999280917E-4</v>
+        <v>4.2307229280284277E-4</v>
       </c>
       <c r="BQ2" s="10">
         <f>BNVFE!AF8</f>
-        <v>4.1755377409260071E-4</v>
+        <v>4.2467076402359958E-4</v>
       </c>
       <c r="BR2" s="10">
         <f>BNVFE!AG8</f>
-        <v>4.1711981834238049E-4</v>
+        <v>4.2417015147939801E-4</v>
       </c>
       <c r="BS2" s="10"/>
       <c r="BT2" s="4"/>
@@ -22966,123 +22966,123 @@
       </c>
       <c r="B3" s="4">
         <f>BNVFE!B25*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.6512977295439592E-4</v>
+        <v>3.6491869578213529E-4</v>
       </c>
       <c r="C3" s="4">
         <f>BNVFE!C25*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.5474795033263841E-4</v>
+        <v>3.5434143118335762E-4</v>
       </c>
       <c r="D3" s="4">
         <f>BNVFE!D25*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.5999582362156076E-4</v>
+        <v>3.5938245579985413E-4</v>
       </c>
       <c r="E3" s="4">
         <f>BNVFE!E25*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.575411527957111E-4</v>
+        <v>3.5673597291661197E-4</v>
       </c>
       <c r="F3" s="4">
         <f>BNVFE!F25*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.5098955393113139E-4</v>
+        <v>3.5001004459842016E-4</v>
       </c>
       <c r="G3" s="4">
         <f>BNVFE!G25*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.2529070551256162E-4</v>
+        <v>3.2421067232572473E-4</v>
       </c>
       <c r="H3" s="4">
         <f>BNVFE!H25*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.2405957424546739E-4</v>
+        <v>3.2281494881004815E-4</v>
       </c>
       <c r="I3" s="4">
         <f>BNVFE!I25*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.2305318872919765E-4</v>
+        <v>3.216471004014191E-4</v>
       </c>
       <c r="J3" s="4">
         <f>BNVFE!J25*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.2314699001954232E-4</v>
+        <v>3.2157787520010301E-4</v>
       </c>
       <c r="K3" s="4">
         <f>BNVFE!K25*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.2324770853401079E-4</v>
+        <v>3.21518126095359E-4</v>
       </c>
       <c r="L3" s="4">
         <f>BNVFE!L25*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.2427274517001246E-4</v>
+        <v>3.2237982474551686E-4</v>
       </c>
       <c r="M3" s="4">
         <f>BNVFE!M25*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.2437797979064292E-4</v>
+        <v>3.2232910952030141E-4</v>
       </c>
       <c r="N3" s="4">
         <f>BNVFE!N25*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.2523361399085606E-4</v>
+        <v>3.230261074746993E-4</v>
       </c>
       <c r="O3" s="4">
         <f>BNVFE!O25*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.2615971146515569E-4</v>
+        <v>3.2379471109806533E-4</v>
       </c>
       <c r="P3" s="4">
         <f>BNVFE!P25*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.3177243986842866E-4</v>
+        <v>3.3048305141780151E-4</v>
       </c>
       <c r="Q3" s="4">
         <f>BNVFE!Q25*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3631690935380739E-4</v>
+        <v>3.3594130670836631E-4</v>
       </c>
       <c r="R3" s="4">
         <f>BNVFE!R25*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.4057057772530629E-4</v>
+        <v>3.4091724290291815E-4</v>
       </c>
       <c r="S3" s="4">
         <f>BNVFE!S25*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.5254040910253097E-4</v>
+        <v>3.5476961338184239E-4</v>
       </c>
       <c r="T3" s="4">
         <f>BNVFE!T25*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.5622167214823523E-4</v>
+        <v>3.5907190164345085E-4</v>
       </c>
       <c r="U3" s="4">
         <f>BNVFE!U25*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.5932586621187509E-4</v>
+        <v>3.626297992090949E-4</v>
       </c>
       <c r="V3" s="4">
         <f>BNVFE!V25*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.6998069835868409E-4</v>
+        <v>3.7493915890105976E-4</v>
       </c>
       <c r="W3" s="4">
         <f>BNVFE!W25*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.7043547142435307E-4</v>
+        <v>3.7552409347380434E-4</v>
       </c>
       <c r="X3" s="4">
         <f>BNVFE!X25*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.7063277045978053E-4</v>
+        <v>3.7574684426413548E-4</v>
       </c>
       <c r="Y3" s="4">
         <f>BNVFE!Y25*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.7027223527136152E-4</v>
+        <v>3.7540611772019785E-4</v>
       </c>
       <c r="Z3" s="4">
         <f>BNVFE!Z25*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.707899458345789E-4</v>
+        <v>3.7600738009461071E-4</v>
       </c>
       <c r="AA3" s="4">
         <f>BNVFE!AA25*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.6942231456915355E-4</v>
+        <v>3.7475309506278861E-4</v>
       </c>
       <c r="AB3" s="4">
         <f>BNVFE!AB25*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.7062339495815715E-4</v>
+        <v>3.7612176000740666E-4</v>
       </c>
       <c r="AC3" s="4">
         <f>BNVFE!AC25*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.7138471662628673E-4</v>
+        <v>3.7707899733741858E-4</v>
       </c>
       <c r="AD3" s="4">
         <f>BNVFE!AD25*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.7275932113182964E-4</v>
+        <v>3.7865539671164459E-4</v>
       </c>
       <c r="AE3" s="4">
         <f>BNVFE!AE25*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.7333739446942469E-4</v>
+        <v>3.793930531609804E-4</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -23093,123 +23093,123 @@
       </c>
       <c r="B4" s="4">
         <f>Extrapolations!AB2</f>
-        <v>3.170827862483609E-4</v>
+        <v>3.1689948446677165E-4</v>
       </c>
       <c r="C4" s="4">
         <f>Extrapolations!AC2</f>
-        <v>3.199157108645295E-4</v>
+        <v>3.1954910730135099E-4</v>
       </c>
       <c r="D4" s="4">
         <f>Extrapolations!AD2</f>
-        <v>3.227486354806981E-4</v>
+        <v>3.2219873013593033E-4</v>
       </c>
       <c r="E4" s="4">
         <f>Extrapolations!AE2</f>
-        <v>3.255815600968667E-4</v>
+        <v>3.2484835297050968E-4</v>
       </c>
       <c r="F4" s="4">
         <f>Extrapolations!AF2</f>
-        <v>3.284144847130353E-4</v>
+        <v>3.2749797580508902E-4</v>
       </c>
       <c r="G4" s="4">
         <f>Extrapolations!AG2</f>
-        <v>3.312474093292039E-4</v>
+        <v>3.3014759863966836E-4</v>
       </c>
       <c r="H4" s="4">
         <f>Extrapolations!AH2</f>
-        <v>3.3408033394537249E-4</v>
+        <v>3.3279722147424771E-4</v>
       </c>
       <c r="I4" s="4">
         <f>Extrapolations!AI2</f>
-        <v>3.3691325856154109E-4</v>
+        <v>3.3544684430882705E-4</v>
       </c>
       <c r="J4" s="4">
         <f>Extrapolations!AJ2</f>
-        <v>3.3974618317770969E-4</v>
+        <v>3.3809646714340639E-4</v>
       </c>
       <c r="K4" s="4">
         <f>Extrapolations!AK2</f>
-        <v>3.4257910779387829E-4</v>
+        <v>3.4074608997798574E-4</v>
       </c>
       <c r="L4" s="4">
         <f>Extrapolations!AL2</f>
-        <v>3.4541203241004689E-4</v>
+        <v>3.4339571281256508E-4</v>
       </c>
       <c r="M4" s="4">
         <f>Extrapolations!AM2</f>
-        <v>3.4824495702621549E-4</v>
+        <v>3.4604533564714442E-4</v>
       </c>
       <c r="N4" s="4">
         <f>Extrapolations!AN2</f>
-        <v>3.5107788164238408E-4</v>
+        <v>3.4869495848172376E-4</v>
       </c>
       <c r="O4" s="4">
         <f>Extrapolations!AO2</f>
-        <v>3.5391080625855263E-4</v>
+        <v>3.5134458131630327E-4</v>
       </c>
       <c r="P4" s="4">
         <f>Extrapolations!AP2</f>
-        <v>3.6152338546126896E-4</v>
+        <v>3.6011837400814692E-4</v>
       </c>
       <c r="Q4" s="4">
         <f>Extrapolations!AQ2</f>
-        <v>3.6806778318324615E-4</v>
+        <v>3.6765672079173311E-4</v>
       </c>
       <c r="R4" s="4">
         <f>Extrapolations!AR2</f>
-        <v>3.7326311577328699E-4</v>
+        <v>3.736430585304968E-4</v>
       </c>
       <c r="S4" s="4">
         <f>Extrapolations!AS2</f>
-        <v>3.8684273091170592E-4</v>
+        <v>3.8928883765267276E-4</v>
       </c>
       <c r="T4" s="4">
         <f>Extrapolations!AT2</f>
-        <v>3.9133628030331842E-4</v>
+        <v>3.9446747162568221E-4</v>
       </c>
       <c r="U4" s="4">
         <f>Extrapolations!AU2</f>
-        <v>3.9460271712590122E-4</v>
+        <v>3.9823101405773444E-4</v>
       </c>
       <c r="V4" s="4">
         <f>Extrapolations!AV2</f>
-        <v>4.0654622240144441E-4</v>
+        <v>4.1199473204362889E-4</v>
       </c>
       <c r="W4" s="4">
         <f>Extrapolations!AW2</f>
-        <v>4.0753465089361259E-4</v>
+        <v>4.1313289936177025E-4</v>
       </c>
       <c r="X4" s="4">
         <f>Extrapolations!AX2</f>
-        <v>4.0771889354095417E-4</v>
+        <v>4.1334468996044436E-4</v>
       </c>
       <c r="Y4" s="4">
         <f>Extrapolations!AY2</f>
-        <v>4.0791884576015625E-4</v>
+        <v>4.1357470435096535E-4</v>
       </c>
       <c r="Z4" s="4">
         <f>Extrapolations!AZ2</f>
-        <v>4.0852284515353123E-4</v>
+        <v>4.1427122401939349E-4</v>
       </c>
       <c r="AA4" s="4">
         <f>Extrapolations!BA2</f>
-        <v>4.09583671112226E-4</v>
+        <v>4.154939817739491E-4</v>
       </c>
       <c r="AB4" s="4">
         <f>Extrapolations!BB2</f>
-        <v>4.1078673798239525E-4</v>
+        <v>4.1688094432107664E-4</v>
       </c>
       <c r="AC4" s="4">
         <f>Extrapolations!BC2</f>
-        <v>4.122748024320864E-4</v>
+        <v>4.1859603308611211E-4</v>
       </c>
       <c r="AD4" s="4">
         <f>Extrapolations!BD2</f>
-        <v>4.1373149805260076E-4</v>
+        <v>4.2027564609660228E-4</v>
       </c>
       <c r="AE4" s="4">
         <f>Extrapolations!BE2</f>
-        <v>4.1495700440447459E-4</v>
+        <v>4.2168774723272802E-4</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -23220,123 +23220,123 @@
       </c>
       <c r="B5" s="4">
         <f>BNVFE!B27*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.5658241110255779E-4</v>
+        <v>3.5637627505836616E-4</v>
       </c>
       <c r="C5" s="4">
         <f>BNVFE!C27*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.546826203139623E-4</v>
+        <v>3.5427617602883105E-4</v>
       </c>
       <c r="D5" s="4">
         <f>BNVFE!D27*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.5321445226457391E-4</v>
+        <v>3.5261263867406798E-4</v>
       </c>
       <c r="E5" s="4">
         <f>BNVFE!E27*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.524765095404888E-4</v>
+        <v>3.5168273519838039E-4</v>
       </c>
       <c r="F5" s="4">
         <f>BNVFE!F27*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.4444165282567749E-4</v>
+        <v>3.4348041677252866E-4</v>
       </c>
       <c r="G5" s="4">
         <f>BNVFE!G27*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.1958904086234162E-4</v>
+        <v>3.1852793839482163E-4</v>
       </c>
       <c r="H5" s="4">
         <f>BNVFE!H27*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.1833343353394986E-4</v>
+        <v>3.1711080066083321E-4</v>
       </c>
       <c r="I5" s="4">
         <f>BNVFE!I27*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.1412412398046098E-4</v>
+        <v>3.1275689938831239E-4</v>
       </c>
       <c r="J5" s="4">
         <f>BNVFE!J27*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.1380528787726191E-4</v>
+        <v>3.12281533849422E-4</v>
       </c>
       <c r="K5" s="4">
         <f>BNVFE!K27*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.1412454613579944E-4</v>
+        <v>3.1244377846381834E-4</v>
       </c>
       <c r="L5" s="4">
         <f>BNVFE!L27*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.1593684912226372E-4</v>
+        <v>3.1409258893246343E-4</v>
       </c>
       <c r="M5" s="4">
         <f>BNVFE!M27*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.1696816235110396E-4</v>
+        <v>3.149660947480407E-4</v>
       </c>
       <c r="N5" s="4">
         <f>BNVFE!N27*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.1872195023581305E-4</v>
+        <v>3.1655864130425985E-4</v>
       </c>
       <c r="O5" s="4">
         <f>BNVFE!O27*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.204519818383183E-4</v>
+        <v>3.1812836850398589E-4</v>
       </c>
       <c r="P5" s="4">
         <f>BNVFE!P27*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.2661274550379422E-4</v>
+        <v>3.2534340950334998E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>BNVFE!Q27*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3159751139569607E-4</v>
+        <v>3.3122717942891744E-4</v>
       </c>
       <c r="R5" s="4">
         <f>BNVFE!R27*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.3626742360268452E-4</v>
+        <v>3.3660970862010116E-4</v>
       </c>
       <c r="S5" s="4">
         <f>BNVFE!S27*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.4855286672866461E-4</v>
+        <v>3.5075685674517315E-4</v>
       </c>
       <c r="T5" s="4">
         <f>BNVFE!T27*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.5224997356011041E-4</v>
+        <v>3.5506842438112659E-4</v>
       </c>
       <c r="U5" s="4">
         <f>BNVFE!U27*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.5572055564458207E-4</v>
+        <v>3.5899133849685383E-4</v>
       </c>
       <c r="V5" s="4">
         <f>BNVFE!V27*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.6666645963201293E-4</v>
+        <v>3.7158050293309159E-4</v>
       </c>
       <c r="W5" s="4">
         <f>BNVFE!W27*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.6745317163350868E-4</v>
+        <v>3.7250082623344597E-4</v>
       </c>
       <c r="X5" s="4">
         <f>BNVFE!X27*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.6812816732604984E-4</v>
+        <v>3.732076820565791E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>BNVFE!Y27*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.6829543482855682E-4</v>
+        <v>3.7340190863010219E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>BNVFE!Z27*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.6916794586512564E-4</v>
+        <v>3.7436255674953617E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>BNVFE!AA27*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.6836027015493497E-4</v>
+        <v>3.7367572530025347E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>BNVFE!AB27*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.6989680254038607E-4</v>
+        <v>3.753843882637504E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>BNVFE!AC27*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.7101492304657024E-4</v>
+        <v>3.767035338732028E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>BNVFE!AD27*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.7218016517873024E-4</v>
+        <v>3.7806708002914585E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>BNVFE!AE27*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.7301391239035468E-4</v>
+        <v>3.7906432409328105E-4</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -23347,123 +23347,123 @@
       </c>
       <c r="B6" s="4">
         <f>BNVFE!B28*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>5.7733679111085859E-4</v>
+        <v>5.770030395892457E-4</v>
       </c>
       <c r="C6" s="4">
         <f>BNVFE!C28*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>5.1624349374592988E-4</v>
+        <v>5.1565191072000234E-4</v>
       </c>
       <c r="D6" s="4">
         <f>BNVFE!D28*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>5.0741882465691354E-4</v>
+        <v>5.0655427468507849E-4</v>
       </c>
       <c r="E6" s="4">
         <f>BNVFE!E28*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>5.1345781970387209E-4</v>
+        <v>5.1230151671061109E-4</v>
       </c>
       <c r="F6" s="4">
         <f>BNVFE!F28*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>5.0721121114026969E-4</v>
+        <v>5.057957327894093E-4</v>
       </c>
       <c r="G6" s="4">
         <f>BNVFE!G28*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>4.7306733810797443E-4</v>
+        <v>4.7149665558890241E-4</v>
       </c>
       <c r="H6" s="4">
         <f>BNVFE!H28*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>4.7481949081841583E-4</v>
+        <v>4.7299583719891884E-4</v>
       </c>
       <c r="I6" s="4">
         <f>BNVFE!I28*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>4.7320913259414843E-4</v>
+        <v>4.7114949083498103E-4</v>
       </c>
       <c r="J6" s="4">
         <f>BNVFE!J28*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>4.7463592657213656E-4</v>
+        <v>4.7233122224492742E-4</v>
       </c>
       <c r="K6" s="4">
         <f>BNVFE!K28*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>4.7740258867597427E-4</v>
+        <v>4.7484817881709057E-4</v>
       </c>
       <c r="L6" s="4">
         <f>BNVFE!L28*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>4.8006153857130626E-4</v>
+        <v>4.7725921150277634E-4</v>
       </c>
       <c r="M6" s="4">
         <f>BNVFE!M28*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>4.8249268977570829E-4</v>
+        <v>4.7944511876494916E-4</v>
       </c>
       <c r="N6" s="4">
         <f>BNVFE!N28*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>4.8553787759081645E-4</v>
+        <v>4.8224231408656933E-4</v>
       </c>
       <c r="O6" s="4">
         <f>BNVFE!O28*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>4.8878116836815273E-4</v>
+        <v>4.8523699169033819E-4</v>
       </c>
       <c r="P6" s="4">
         <f>BNVFE!P28*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>4.9839012649989111E-4</v>
+        <v>4.9645320107814599E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>BNVFE!Q28*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>5.0688524375738135E-4</v>
+        <v>5.0631914840744451E-4</v>
       </c>
       <c r="R6" s="4">
         <f>BNVFE!R28*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>5.1408893015787694E-4</v>
+        <v>5.1461221884438588E-4</v>
       </c>
       <c r="S6" s="4">
         <f>BNVFE!S28*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>5.3298064486994104E-4</v>
+        <v>5.3635081947590716E-4</v>
       </c>
       <c r="T6" s="4">
         <f>BNVFE!T28*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>5.3904493880410056E-4</v>
+        <v>5.4335798852553027E-4</v>
       </c>
       <c r="U6" s="4">
         <f>BNVFE!U28*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>5.4440423055981968E-4</v>
+        <v>5.4940992391592244E-4</v>
       </c>
       <c r="V6" s="4">
         <f>BNVFE!V28*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>5.6091264450523141E-4</v>
+        <v>5.6842996426768682E-4</v>
       </c>
       <c r="W6" s="4">
         <f>BNVFE!W28*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>5.6228352121743142E-4</v>
+        <v>5.7000753402081756E-4</v>
       </c>
       <c r="X6" s="4">
         <f>BNVFE!X28*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>5.6300211186441568E-4</v>
+        <v>5.707705408366043E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>BNVFE!Y28*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>5.6370242333199415E-4</v>
+        <v>5.7151824558879846E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>BNVFE!Z28*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>5.6505007903216167E-4</v>
+        <v>5.7300097326242578E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>BNVFE!AA28*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>5.6472680383080583E-4</v>
+        <v>5.7287583682467122E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>BNVFE!AB28*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>5.6695236229259763E-4</v>
+        <v>5.7536335602862711E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>BNVFE!AC28*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>5.6913462321645978E-4</v>
+        <v>5.7786091743895448E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>BNVFE!AD28*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>5.7051355681803149E-4</v>
+        <v>5.7953758615710883E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>BNVFE!AE28*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>5.7222367877689934E-4</v>
+        <v>5.8150534020495943E-4</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -23474,123 +23474,123 @@
       </c>
       <c r="B7" s="4">
         <f>BNVFE!B29*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.1763216261773128E-4</v>
+        <v>3.1744854324820717E-4</v>
       </c>
       <c r="C7" s="4">
         <f>BNVFE!C29*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.0669186158966625E-4</v>
+        <v>3.0634041173760126E-4</v>
       </c>
       <c r="D7" s="4">
         <f>BNVFE!D29*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.1685245989931227E-4</v>
+        <v>3.1631260057212433E-4</v>
       </c>
       <c r="E7" s="4">
         <f>BNVFE!E29*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.1739782303062078E-4</v>
+        <v>3.1668304561611668E-4</v>
       </c>
       <c r="F7" s="4">
         <f>BNVFE!F29*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.1192088323962313E-4</v>
+        <v>3.1105040315615982E-4</v>
       </c>
       <c r="G7" s="4">
         <f>BNVFE!G29*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>2.9142107044187574E-4</v>
+        <v>2.904534915283473E-4</v>
       </c>
       <c r="H7" s="4">
         <f>BNVFE!H29*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>2.9074753100539563E-4</v>
+        <v>2.896308481447913E-4</v>
       </c>
       <c r="I7" s="4">
         <f>BNVFE!I29*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>2.8982606084405671E-4</v>
+        <v>2.8856459352085231E-4</v>
       </c>
       <c r="J7" s="4">
         <f>BNVFE!J29*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>2.8983551626977824E-4</v>
+        <v>2.8842815300220999E-4</v>
       </c>
       <c r="K7" s="4">
         <f>BNVFE!K29*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>2.9017394439876564E-4</v>
+        <v>2.8862132779813285E-4</v>
       </c>
       <c r="L7" s="4">
         <f>BNVFE!L29*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>2.9163668386046073E-4</v>
+        <v>2.8993427425732799E-4</v>
       </c>
       <c r="M7" s="4">
         <f>BNVFE!M29*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>2.925881148990673E-4</v>
+        <v>2.9074003911273041E-4</v>
       </c>
       <c r="N7" s="4">
         <f>BNVFE!N29*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>2.9426018427939119E-4</v>
+        <v>2.9226290833281419E-4</v>
       </c>
       <c r="O7" s="4">
         <f>BNVFE!O29*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>2.9593459855706646E-4</v>
+        <v>2.937887619941194E-4</v>
       </c>
       <c r="P7" s="4">
         <f>BNVFE!P29*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.0150773383604229E-4</v>
+        <v>3.0033596504796238E-4</v>
       </c>
       <c r="Q7" s="4">
         <f>BNVFE!Q29*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.0595864748126056E-4</v>
+        <v>3.0561694929662176E-4</v>
       </c>
       <c r="R7" s="4">
         <f>BNVFE!R29*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.1002205402131999E-4</v>
+        <v>3.1033762400137736E-4</v>
       </c>
       <c r="S7" s="4">
         <f>BNVFE!S29*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.2110959644743808E-4</v>
+        <v>3.231400555609079E-4</v>
       </c>
       <c r="T7" s="4">
         <f>BNVFE!T29*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.2436399554231139E-4</v>
+        <v>3.2695932283305509E-4</v>
       </c>
       <c r="U7" s="4">
         <f>BNVFE!U29*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.2731318390816493E-4</v>
+        <v>3.3032276638030907E-4</v>
       </c>
       <c r="V7" s="4">
         <f>BNVFE!V29*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.3702991066531066E-4</v>
+        <v>3.4154676660143898E-4</v>
       </c>
       <c r="W7" s="4">
         <f>BNVFE!W29*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.3741002097795717E-4</v>
+        <v>3.420449768741958E-4</v>
       </c>
       <c r="X7" s="4">
         <f>BNVFE!X29*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.3750948921623593E-4</v>
+        <v>3.4216652058283842E-4</v>
       </c>
       <c r="Y7" s="4">
         <f>BNVFE!Y29*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.3717526117842833E-4</v>
+        <v>3.418502489054371E-4</v>
       </c>
       <c r="Z7" s="4">
         <f>BNVFE!Z29*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.375039228412405E-4</v>
+        <v>3.422529850790624E-4</v>
       </c>
       <c r="AA7" s="4">
         <f>BNVFE!AA29*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.3608556774951192E-4</v>
+        <v>3.4093529749808124E-4</v>
       </c>
       <c r="AB7" s="4">
         <f>BNVFE!AB29*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.3718406040280117E-4</v>
+        <v>3.4218633785776896E-4</v>
       </c>
       <c r="AC7" s="4">
         <f>BNVFE!AC29*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.378358588691025E-4</v>
+        <v>3.4301574950155089E-4</v>
       </c>
       <c r="AD7" s="4">
         <f>BNVFE!AD29*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.3847440572982264E-4</v>
+        <v>3.4382818379754854E-4</v>
       </c>
       <c r="AE7" s="4">
         <f>BNVFE!AE29*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.3885840983958386E-4</v>
+        <v>3.4435480774975858E-4</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>

</xml_diff>

<commit_message>
Adjust ratio of tested to onroad LDV efficiency
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3687D9-89B6-4A02-8B8A-CFEA5EACE775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BBB26-2C5B-4C09-BC97-E4961155787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1773,133 +1773,133 @@
                   <c:v>3.142498616321923E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>3.1689948446677165E-4</c:v>
+                  <c:v>3.1934654476143933E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>3.1954910730135099E-4</c:v>
+                  <c:v>3.2444322789068635E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>3.2219873013593033E-4</c:v>
+                  <c:v>3.2953991101993338E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>3.2484835297050968E-4</c:v>
+                  <c:v>3.346365941491804E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>3.2749797580508902E-4</c:v>
+                  <c:v>3.3973327727842743E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>3.3014759863966836E-4</c:v>
+                  <c:v>3.4482996040767445E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>3.3279722147424771E-4</c:v>
+                  <c:v>3.4992664353692148E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>3.3544684430882705E-4</c:v>
+                  <c:v>3.550233266661685E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>3.3809646714340639E-4</c:v>
+                  <c:v>3.6012000979541552E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>3.4074608997798574E-4</c:v>
+                  <c:v>3.6521669292466255E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>3.4339571281256508E-4</c:v>
+                  <c:v>3.7031337605390957E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>3.4604533564714442E-4</c:v>
+                  <c:v>3.754100591831566E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>3.4869495848172376E-4</c:v>
+                  <c:v>3.8050674231240362E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>3.5134458131630327E-4</c:v>
+                  <c:v>3.8560342544165043E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>3.6011837400814692E-4</c:v>
+                  <c:v>3.938977091004229E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>3.6765672079173311E-4</c:v>
+                  <c:v>4.0102815590911211E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>3.736430585304968E-4</c:v>
+                  <c:v>4.0668872915977704E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>3.8928883765267276E-4</c:v>
+                  <c:v>4.2148439524556525E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.9446747162568221E-4</c:v>
+                  <c:v>4.2638034079782157E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.9823101405773444E-4</c:v>
+                  <c:v>4.2993928617474374E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>4.1199473204362889E-4</c:v>
+                  <c:v>4.4295232919176118E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.1313289936177025E-4</c:v>
+                  <c:v>4.4402927119422075E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>4.1334468996044436E-4</c:v>
+                  <c:v>4.4423001272194757E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.1357470435096535E-4</c:v>
+                  <c:v>4.4444787060954387E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>4.1427122401939349E-4</c:v>
+                  <c:v>4.4510595798899477E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.154939817739491E-4</c:v>
+                  <c:v>4.4626178063197816E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>4.1688094432107664E-4</c:v>
+                  <c:v>4.4757258182247277E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>4.1859603308611211E-4</c:v>
+                  <c:v>4.4919390205042781E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>4.2027564609660228E-4</c:v>
+                  <c:v>4.5078104437884211E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.2168774723272802E-4</c:v>
+                  <c:v>4.5211629450069859E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>4.2290738034426306E-4</c:v>
+                  <c:v>4.5326957425061224E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>4.2495638955627015E-4</c:v>
+                  <c:v>4.5520696339484528E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>4.2530341133255339E-4</c:v>
+                  <c:v>4.5553578115777672E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>4.2563408484261415E-4</c:v>
+                  <c:v>4.5584944646724456E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>4.257457185090017E-4</c:v>
+                  <c:v>4.559561094704881E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>4.2549536074558018E-4</c:v>
+                  <c:v>4.5572121425237108E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>4.2483576932089885E-4</c:v>
+                  <c:v>4.550985416964502E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>4.2420044731809718E-4</c:v>
+                  <c:v>4.5449905971852166E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>4.2413535117129356E-4</c:v>
+                  <c:v>4.5443664862698183E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>4.2346108578435258E-4</c:v>
+                  <c:v>4.5380063490385911E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>4.2307229280284277E-4</c:v>
+                  <c:v>4.5343326114607497E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>4.2467076402359958E-4</c:v>
+                  <c:v>4.5494560422822621E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>4.2417015147939801E-4</c:v>
+                  <c:v>4.5447278785524218E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16200,7 +16200,7 @@
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:AG20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16381,94 +16381,94 @@
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>3.5134458131630327E-4</v>
+        <v>3.8560342544165043E-4</v>
       </c>
       <c r="E8" s="4">
-        <v>3.6011837400814692E-4</v>
+        <v>3.938977091004229E-4</v>
       </c>
       <c r="F8" s="4">
-        <v>3.6765672079173311E-4</v>
+        <v>4.0102815590911211E-4</v>
       </c>
       <c r="G8" s="4">
-        <v>3.736430585304968E-4</v>
+        <v>4.0668872915977704E-4</v>
       </c>
       <c r="H8" s="4">
-        <v>3.8928883765267276E-4</v>
+        <v>4.2148439524556525E-4</v>
       </c>
       <c r="I8" s="4">
-        <v>3.9446747162568221E-4</v>
+        <v>4.2638034079782157E-4</v>
       </c>
       <c r="J8" s="4">
-        <v>3.9823101405773444E-4</v>
+        <v>4.2993928617474374E-4</v>
       </c>
       <c r="K8" s="4">
-        <v>4.1199473204362889E-4</v>
+        <v>4.4295232919176118E-4</v>
       </c>
       <c r="L8" s="4">
-        <v>4.1313289936177025E-4</v>
+        <v>4.4402927119422075E-4</v>
       </c>
       <c r="M8" s="4">
-        <v>4.1334468996044436E-4</v>
+        <v>4.4423001272194757E-4</v>
       </c>
       <c r="N8" s="4">
-        <v>4.1357470435096535E-4</v>
+        <v>4.4444787060954387E-4</v>
       </c>
       <c r="O8" s="4">
-        <v>4.1427122401939349E-4</v>
+        <v>4.4510595798899477E-4</v>
       </c>
       <c r="P8" s="4">
-        <v>4.154939817739491E-4</v>
+        <v>4.4626178063197816E-4</v>
       </c>
       <c r="Q8" s="4">
-        <v>4.1688094432107664E-4</v>
+        <v>4.4757258182247277E-4</v>
       </c>
       <c r="R8" s="4">
-        <v>4.1859603308611211E-4</v>
+        <v>4.4919390205042781E-4</v>
       </c>
       <c r="S8" s="4">
-        <v>4.2027564609660228E-4</v>
+        <v>4.5078104437884211E-4</v>
       </c>
       <c r="T8" s="4">
-        <v>4.2168774723272802E-4</v>
+        <v>4.5211629450069859E-4</v>
       </c>
       <c r="U8" s="4">
-        <v>4.2290738034426306E-4</v>
+        <v>4.5326957425061224E-4</v>
       </c>
       <c r="V8" s="4">
-        <v>4.2495638955627015E-4</v>
+        <v>4.5520696339484528E-4</v>
       </c>
       <c r="W8" s="4">
-        <v>4.2530341133255339E-4</v>
+        <v>4.5553578115777672E-4</v>
       </c>
       <c r="X8" s="4">
-        <v>4.2563408484261415E-4</v>
+        <v>4.5584944646724456E-4</v>
       </c>
       <c r="Y8" s="4">
-        <v>4.257457185090017E-4</v>
+        <v>4.559561094704881E-4</v>
       </c>
       <c r="Z8" s="4">
-        <v>4.2549536074558018E-4</v>
+        <v>4.5572121425237108E-4</v>
       </c>
       <c r="AA8" s="4">
-        <v>4.2483576932089885E-4</v>
+        <v>4.550985416964502E-4</v>
       </c>
       <c r="AB8" s="4">
-        <v>4.2420044731809718E-4</v>
+        <v>4.5449905971852166E-4</v>
       </c>
       <c r="AC8" s="4">
-        <v>4.2413535117129356E-4</v>
+        <v>4.5443664862698183E-4</v>
       </c>
       <c r="AD8" s="4">
-        <v>4.2346108578435258E-4</v>
+        <v>4.5380063490385911E-4</v>
       </c>
       <c r="AE8" s="4">
-        <v>4.2307229280284277E-4</v>
+        <v>4.5343326114607497E-4</v>
       </c>
       <c r="AF8" s="4">
-        <v>4.2467076402359958E-4</v>
+        <v>4.5494560422822621E-4</v>
       </c>
       <c r="AG8" s="4">
-        <v>4.2417015147939801E-4</v>
+        <v>4.5447278785524218E-4</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -19143,7 +19143,7 @@
       </c>
       <c r="B16">
         <f>TREND(C16:D16,C13:D13,B13)</f>
-        <v>3.1424986163219263E-4</v>
+        <v>3.142498616321935E-4</v>
       </c>
       <c r="C16">
         <f>C15*$B$2/$B$9</f>
@@ -19151,7 +19151,7 @@
       </c>
       <c r="D16" s="4">
         <f>BNVFE!D8</f>
-        <v>3.5134458131630327E-4</v>
+        <v>3.8560342544165043E-4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -19529,175 +19529,175 @@
       </c>
       <c r="AB2" s="4">
         <f>($AO$2-$AA$2)/COUNT($AB$1:$AO$1)+AA2</f>
-        <v>3.1689948446677165E-4</v>
+        <v>3.1934654476143933E-4</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" ref="AC2:AN2" si="0">($AO$2-$AA$2)/COUNT($AB$1:$AO$1)+AB2</f>
-        <v>3.1954910730135099E-4</v>
+        <v>3.2444322789068635E-4</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>3.2219873013593033E-4</v>
+        <v>3.2953991101993338E-4</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>3.2484835297050968E-4</v>
+        <v>3.346365941491804E-4</v>
       </c>
       <c r="AF2" s="4">
         <f t="shared" si="0"/>
-        <v>3.2749797580508902E-4</v>
+        <v>3.3973327727842743E-4</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3014759863966836E-4</v>
+        <v>3.4482996040767445E-4</v>
       </c>
       <c r="AH2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3279722147424771E-4</v>
+        <v>3.4992664353692148E-4</v>
       </c>
       <c r="AI2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3544684430882705E-4</v>
+        <v>3.550233266661685E-4</v>
       </c>
       <c r="AJ2" s="4">
         <f t="shared" si="0"/>
-        <v>3.3809646714340639E-4</v>
+        <v>3.6012000979541552E-4</v>
       </c>
       <c r="AK2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4074608997798574E-4</v>
+        <v>3.6521669292466255E-4</v>
       </c>
       <c r="AL2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4339571281256508E-4</v>
+        <v>3.7031337605390957E-4</v>
       </c>
       <c r="AM2" s="4">
         <f t="shared" si="0"/>
-        <v>3.4604533564714442E-4</v>
+        <v>3.754100591831566E-4</v>
       </c>
       <c r="AN2" s="26">
         <f t="shared" si="0"/>
-        <v>3.4869495848172376E-4</v>
+        <v>3.8050674231240362E-4</v>
       </c>
       <c r="AO2" s="10">
         <f>BNVFE!D8</f>
-        <v>3.5134458131630327E-4</v>
+        <v>3.8560342544165043E-4</v>
       </c>
       <c r="AP2" s="10">
         <f>BNVFE!E8</f>
-        <v>3.6011837400814692E-4</v>
+        <v>3.938977091004229E-4</v>
       </c>
       <c r="AQ2" s="10">
         <f>BNVFE!F8</f>
-        <v>3.6765672079173311E-4</v>
+        <v>4.0102815590911211E-4</v>
       </c>
       <c r="AR2" s="10">
         <f>BNVFE!G8</f>
-        <v>3.736430585304968E-4</v>
+        <v>4.0668872915977704E-4</v>
       </c>
       <c r="AS2" s="10">
         <f>BNVFE!H8</f>
-        <v>3.8928883765267276E-4</v>
+        <v>4.2148439524556525E-4</v>
       </c>
       <c r="AT2" s="10">
         <f>BNVFE!I8</f>
-        <v>3.9446747162568221E-4</v>
+        <v>4.2638034079782157E-4</v>
       </c>
       <c r="AU2" s="10">
         <f>BNVFE!J8</f>
-        <v>3.9823101405773444E-4</v>
+        <v>4.2993928617474374E-4</v>
       </c>
       <c r="AV2" s="10">
         <f>BNVFE!K8</f>
-        <v>4.1199473204362889E-4</v>
+        <v>4.4295232919176118E-4</v>
       </c>
       <c r="AW2" s="10">
         <f>BNVFE!L8</f>
-        <v>4.1313289936177025E-4</v>
+        <v>4.4402927119422075E-4</v>
       </c>
       <c r="AX2" s="10">
         <f>BNVFE!M8</f>
-        <v>4.1334468996044436E-4</v>
+        <v>4.4423001272194757E-4</v>
       </c>
       <c r="AY2" s="10">
         <f>BNVFE!N8</f>
-        <v>4.1357470435096535E-4</v>
+        <v>4.4444787060954387E-4</v>
       </c>
       <c r="AZ2" s="10">
         <f>BNVFE!O8</f>
-        <v>4.1427122401939349E-4</v>
+        <v>4.4510595798899477E-4</v>
       </c>
       <c r="BA2" s="10">
         <f>BNVFE!P8</f>
-        <v>4.154939817739491E-4</v>
+        <v>4.4626178063197816E-4</v>
       </c>
       <c r="BB2" s="10">
         <f>BNVFE!Q8</f>
-        <v>4.1688094432107664E-4</v>
+        <v>4.4757258182247277E-4</v>
       </c>
       <c r="BC2" s="10">
         <f>BNVFE!R8</f>
-        <v>4.1859603308611211E-4</v>
+        <v>4.4919390205042781E-4</v>
       </c>
       <c r="BD2" s="10">
         <f>BNVFE!S8</f>
-        <v>4.2027564609660228E-4</v>
+        <v>4.5078104437884211E-4</v>
       </c>
       <c r="BE2" s="10">
         <f>BNVFE!T8</f>
-        <v>4.2168774723272802E-4</v>
+        <v>4.5211629450069859E-4</v>
       </c>
       <c r="BF2" s="10">
         <f>BNVFE!U8</f>
-        <v>4.2290738034426306E-4</v>
+        <v>4.5326957425061224E-4</v>
       </c>
       <c r="BG2" s="10">
         <f>BNVFE!V8</f>
-        <v>4.2495638955627015E-4</v>
+        <v>4.5520696339484528E-4</v>
       </c>
       <c r="BH2" s="10">
         <f>BNVFE!W8</f>
-        <v>4.2530341133255339E-4</v>
+        <v>4.5553578115777672E-4</v>
       </c>
       <c r="BI2" s="10">
         <f>BNVFE!X8</f>
-        <v>4.2563408484261415E-4</v>
+        <v>4.5584944646724456E-4</v>
       </c>
       <c r="BJ2" s="10">
         <f>BNVFE!Y8</f>
-        <v>4.257457185090017E-4</v>
+        <v>4.559561094704881E-4</v>
       </c>
       <c r="BK2" s="10">
         <f>BNVFE!Z8</f>
-        <v>4.2549536074558018E-4</v>
+        <v>4.5572121425237108E-4</v>
       </c>
       <c r="BL2" s="10">
         <f>BNVFE!AA8</f>
-        <v>4.2483576932089885E-4</v>
+        <v>4.550985416964502E-4</v>
       </c>
       <c r="BM2" s="10">
         <f>BNVFE!AB8</f>
-        <v>4.2420044731809718E-4</v>
+        <v>4.5449905971852166E-4</v>
       </c>
       <c r="BN2" s="10">
         <f>BNVFE!AC8</f>
-        <v>4.2413535117129356E-4</v>
+        <v>4.5443664862698183E-4</v>
       </c>
       <c r="BO2" s="10">
         <f>BNVFE!AD8</f>
-        <v>4.2346108578435258E-4</v>
+        <v>4.5380063490385911E-4</v>
       </c>
       <c r="BP2" s="10">
         <f>BNVFE!AE8</f>
-        <v>4.2307229280284277E-4</v>
+        <v>4.5343326114607497E-4</v>
       </c>
       <c r="BQ2" s="10">
         <f>BNVFE!AF8</f>
-        <v>4.2467076402359958E-4</v>
+        <v>4.5494560422822621E-4</v>
       </c>
       <c r="BR2" s="10">
         <f>BNVFE!AG8</f>
-        <v>4.2417015147939801E-4</v>
+        <v>4.5447278785524218E-4</v>
       </c>
       <c r="BS2" s="10"/>
       <c r="BT2" s="4"/>
@@ -22966,123 +22966,123 @@
       </c>
       <c r="B3" s="4">
         <f>BNVFE!B25*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.6491869578213529E-4</v>
+        <v>3.6773655474057739E-4</v>
       </c>
       <c r="C3" s="4">
         <f>BNVFE!C25*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.5434143118335762E-4</v>
+        <v>3.5976842082089582E-4</v>
       </c>
       <c r="D3" s="4">
         <f>BNVFE!D25*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.5938245579985413E-4</v>
+        <v>3.6757085434956571E-4</v>
       </c>
       <c r="E3" s="4">
         <f>BNVFE!E25*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.5673597291661197E-4</v>
+        <v>3.67485043084539E-4</v>
       </c>
       <c r="F3" s="4">
         <f>BNVFE!F25*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.5001004459842016E-4</v>
+        <v>3.6308639538755298E-4</v>
       </c>
       <c r="G3" s="4">
         <f>BNVFE!G25*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.2421067232572473E-4</v>
+        <v>3.3862900642764912E-4</v>
       </c>
       <c r="H3" s="4">
         <f>BNVFE!H25*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.2281494881004815E-4</v>
+        <v>3.3943057282821812E-4</v>
       </c>
       <c r="I3" s="4">
         <f>BNVFE!I25*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.216471004014191E-4</v>
+        <v>3.4041823774591409E-4</v>
       </c>
       <c r="J3" s="4">
         <f>BNVFE!J25*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.2157787520010301E-4</v>
+        <v>3.4252539976387765E-4</v>
       </c>
       <c r="K3" s="4">
         <f>BNVFE!K25*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.21518126095359E-4</v>
+        <v>3.4460787718934045E-4</v>
       </c>
       <c r="L3" s="4">
         <f>BNVFE!L25*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.2237982474551686E-4</v>
+        <v>3.4765012147470174E-4</v>
       </c>
       <c r="M3" s="4">
         <f>BNVFE!M25*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.2232910952030141E-4</v>
+        <v>3.4968132096095504E-4</v>
       </c>
       <c r="N3" s="4">
         <f>BNVFE!N25*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.230261074746993E-4</v>
+        <v>3.5249609679543592E-4</v>
       </c>
       <c r="O3" s="4">
         <f>BNVFE!O25*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.2379471109806533E-4</v>
+        <v>3.5536722744245131E-4</v>
       </c>
       <c r="P3" s="4">
         <f>BNVFE!P25*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.3048305141780151E-4</v>
+        <v>3.6148257419113056E-4</v>
       </c>
       <c r="Q3" s="4">
         <f>BNVFE!Q25*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3594130670836631E-4</v>
+        <v>3.664339997180947E-4</v>
       </c>
       <c r="R3" s="4">
         <f>BNVFE!R25*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.4091724290291815E-4</v>
+        <v>3.7106858296827262E-4</v>
       </c>
       <c r="S3" s="4">
         <f>BNVFE!S25*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.5476961338184239E-4</v>
+        <v>3.8411030958242069E-4</v>
       </c>
       <c r="T3" s="4">
         <f>BNVFE!T25*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.5907190164345085E-4</v>
+        <v>3.8812122876113119E-4</v>
       </c>
       <c r="U3" s="4">
         <f>BNVFE!U25*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.626297992090949E-4</v>
+        <v>3.9150340258291803E-4</v>
       </c>
       <c r="V3" s="4">
         <f>BNVFE!V25*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.7493915890105976E-4</v>
+        <v>4.03112372133042E-4</v>
       </c>
       <c r="W3" s="4">
         <f>BNVFE!W25*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.7552409347380434E-4</v>
+        <v>4.0360787000657248E-4</v>
       </c>
       <c r="X3" s="4">
         <f>BNVFE!X25*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.7574684426413548E-4</v>
+        <v>4.0382283711848821E-4</v>
       </c>
       <c r="Y3" s="4">
         <f>BNVFE!Y25*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.7540611772019785E-4</v>
+        <v>4.0343001609921412E-4</v>
       </c>
       <c r="Z3" s="4">
         <f>BNVFE!Z25*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.7600738009461071E-4</v>
+        <v>4.0399408750656777E-4</v>
       </c>
       <c r="AA3" s="4">
         <f>BNVFE!AA25*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.7475309506278861E-4</v>
+        <v>4.0250398522270639E-4</v>
       </c>
       <c r="AB3" s="4">
         <f>BNVFE!AB25*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.7612176000740666E-4</v>
+        <v>4.0381262204317188E-4</v>
       </c>
       <c r="AC3" s="4">
         <f>BNVFE!AC25*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.7707899733741858E-4</v>
+        <v>4.0464211986551089E-4</v>
       </c>
       <c r="AD3" s="4">
         <f>BNVFE!AD25*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.7865539671164459E-4</v>
+        <v>4.061398198412998E-4</v>
       </c>
       <c r="AE3" s="4">
         <f>BNVFE!AE25*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.793930531609804E-4</v>
+        <v>4.0676965949352643E-4</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -23093,123 +23093,123 @@
       </c>
       <c r="B4" s="4">
         <f>Extrapolations!AB2</f>
-        <v>3.1689948446677165E-4</v>
+        <v>3.1934654476143933E-4</v>
       </c>
       <c r="C4" s="4">
         <f>Extrapolations!AC2</f>
-        <v>3.1954910730135099E-4</v>
+        <v>3.2444322789068635E-4</v>
       </c>
       <c r="D4" s="4">
         <f>Extrapolations!AD2</f>
-        <v>3.2219873013593033E-4</v>
+        <v>3.2953991101993338E-4</v>
       </c>
       <c r="E4" s="4">
         <f>Extrapolations!AE2</f>
-        <v>3.2484835297050968E-4</v>
+        <v>3.346365941491804E-4</v>
       </c>
       <c r="F4" s="4">
         <f>Extrapolations!AF2</f>
-        <v>3.2749797580508902E-4</v>
+        <v>3.3973327727842743E-4</v>
       </c>
       <c r="G4" s="4">
         <f>Extrapolations!AG2</f>
-        <v>3.3014759863966836E-4</v>
+        <v>3.4482996040767445E-4</v>
       </c>
       <c r="H4" s="4">
         <f>Extrapolations!AH2</f>
-        <v>3.3279722147424771E-4</v>
+        <v>3.4992664353692148E-4</v>
       </c>
       <c r="I4" s="4">
         <f>Extrapolations!AI2</f>
-        <v>3.3544684430882705E-4</v>
+        <v>3.550233266661685E-4</v>
       </c>
       <c r="J4" s="4">
         <f>Extrapolations!AJ2</f>
-        <v>3.3809646714340639E-4</v>
+        <v>3.6012000979541552E-4</v>
       </c>
       <c r="K4" s="4">
         <f>Extrapolations!AK2</f>
-        <v>3.4074608997798574E-4</v>
+        <v>3.6521669292466255E-4</v>
       </c>
       <c r="L4" s="4">
         <f>Extrapolations!AL2</f>
-        <v>3.4339571281256508E-4</v>
+        <v>3.7031337605390957E-4</v>
       </c>
       <c r="M4" s="4">
         <f>Extrapolations!AM2</f>
-        <v>3.4604533564714442E-4</v>
+        <v>3.754100591831566E-4</v>
       </c>
       <c r="N4" s="4">
         <f>Extrapolations!AN2</f>
-        <v>3.4869495848172376E-4</v>
+        <v>3.8050674231240362E-4</v>
       </c>
       <c r="O4" s="4">
         <f>Extrapolations!AO2</f>
-        <v>3.5134458131630327E-4</v>
+        <v>3.8560342544165043E-4</v>
       </c>
       <c r="P4" s="4">
         <f>Extrapolations!AP2</f>
-        <v>3.6011837400814692E-4</v>
+        <v>3.938977091004229E-4</v>
       </c>
       <c r="Q4" s="4">
         <f>Extrapolations!AQ2</f>
-        <v>3.6765672079173311E-4</v>
+        <v>4.0102815590911211E-4</v>
       </c>
       <c r="R4" s="4">
         <f>Extrapolations!AR2</f>
-        <v>3.736430585304968E-4</v>
+        <v>4.0668872915977704E-4</v>
       </c>
       <c r="S4" s="4">
         <f>Extrapolations!AS2</f>
-        <v>3.8928883765267276E-4</v>
+        <v>4.2148439524556525E-4</v>
       </c>
       <c r="T4" s="4">
         <f>Extrapolations!AT2</f>
-        <v>3.9446747162568221E-4</v>
+        <v>4.2638034079782157E-4</v>
       </c>
       <c r="U4" s="4">
         <f>Extrapolations!AU2</f>
-        <v>3.9823101405773444E-4</v>
+        <v>4.2993928617474374E-4</v>
       </c>
       <c r="V4" s="4">
         <f>Extrapolations!AV2</f>
-        <v>4.1199473204362889E-4</v>
+        <v>4.4295232919176118E-4</v>
       </c>
       <c r="W4" s="4">
         <f>Extrapolations!AW2</f>
-        <v>4.1313289936177025E-4</v>
+        <v>4.4402927119422075E-4</v>
       </c>
       <c r="X4" s="4">
         <f>Extrapolations!AX2</f>
-        <v>4.1334468996044436E-4</v>
+        <v>4.4423001272194757E-4</v>
       </c>
       <c r="Y4" s="4">
         <f>Extrapolations!AY2</f>
-        <v>4.1357470435096535E-4</v>
+        <v>4.4444787060954387E-4</v>
       </c>
       <c r="Z4" s="4">
         <f>Extrapolations!AZ2</f>
-        <v>4.1427122401939349E-4</v>
+        <v>4.4510595798899477E-4</v>
       </c>
       <c r="AA4" s="4">
         <f>Extrapolations!BA2</f>
-        <v>4.154939817739491E-4</v>
+        <v>4.4626178063197816E-4</v>
       </c>
       <c r="AB4" s="4">
         <f>Extrapolations!BB2</f>
-        <v>4.1688094432107664E-4</v>
+        <v>4.4757258182247277E-4</v>
       </c>
       <c r="AC4" s="4">
         <f>Extrapolations!BC2</f>
-        <v>4.1859603308611211E-4</v>
+        <v>4.4919390205042781E-4</v>
       </c>
       <c r="AD4" s="4">
         <f>Extrapolations!BD2</f>
-        <v>4.2027564609660228E-4</v>
+        <v>4.5078104437884211E-4</v>
       </c>
       <c r="AE4" s="4">
         <f>Extrapolations!BE2</f>
-        <v>4.2168774723272802E-4</v>
+        <v>4.5211629450069859E-4</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -23220,123 +23220,123 @@
       </c>
       <c r="B5" s="4">
         <f>BNVFE!B27*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.5637627505836616E-4</v>
+        <v>3.5912817045549592E-4</v>
       </c>
       <c r="C5" s="4">
         <f>BNVFE!C27*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.5427617602883105E-4</v>
+        <v>3.5970216623752401E-4</v>
       </c>
       <c r="D5" s="4">
         <f>BNVFE!D27*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.5261263867406798E-4</v>
+        <v>3.6064678940271876E-4</v>
       </c>
       <c r="E5" s="4">
         <f>BNVFE!E27*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.5168273519838039E-4</v>
+        <v>3.6227954259795134E-4</v>
       </c>
       <c r="F5" s="4">
         <f>BNVFE!F27*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.4348041677252866E-4</v>
+        <v>3.5631282112271915E-4</v>
       </c>
       <c r="G5" s="4">
         <f>BNVFE!G27*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.1852793839482163E-4</v>
+        <v>3.3269354930339661E-4</v>
       </c>
       <c r="H5" s="4">
         <f>BNVFE!H27*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.1711080066083321E-4</v>
+        <v>3.3343282619064117E-4</v>
       </c>
       <c r="I5" s="4">
         <f>BNVFE!I27*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.1275689938831239E-4</v>
+        <v>3.3100920978231121E-4</v>
       </c>
       <c r="J5" s="4">
         <f>BNVFE!J27*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.12281533849422E-4</v>
+        <v>3.326234964208629E-4</v>
       </c>
       <c r="K5" s="4">
         <f>BNVFE!K27*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.1244377846381834E-4</v>
+        <v>3.3488185734666483E-4</v>
       </c>
       <c r="L5" s="4">
         <f>BNVFE!L27*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.1409258893246343E-4</v>
+        <v>3.387132764367971E-4</v>
       </c>
       <c r="M5" s="4">
         <f>BNVFE!M27*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.149660947480407E-4</v>
+        <v>3.4169349530148885E-4</v>
       </c>
       <c r="N5" s="4">
         <f>BNVFE!N27*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.1655864130425985E-4</v>
+        <v>3.4543859732872489E-4</v>
       </c>
       <c r="O5" s="4">
         <f>BNVFE!O27*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.1812836850398589E-4</v>
+        <v>3.4914837213574049E-4</v>
       </c>
       <c r="P5" s="4">
         <f>BNVFE!P27*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.2534340950334998E-4</v>
+        <v>3.5586083055954025E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>BNVFE!Q27*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3122717942891744E-4</v>
+        <v>3.6129198091988776E-4</v>
       </c>
       <c r="R5" s="4">
         <f>BNVFE!R27*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.3660970862010116E-4</v>
+        <v>3.6638008253103504E-4</v>
       </c>
       <c r="S5" s="4">
         <f>BNVFE!S27*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.5075685674517315E-4</v>
+        <v>3.797656838426424E-4</v>
       </c>
       <c r="T5" s="4">
         <f>BNVFE!T27*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.5506842438112659E-4</v>
+        <v>3.8379386561392104E-4</v>
       </c>
       <c r="U5" s="4">
         <f>BNVFE!U27*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.5899133849685383E-4</v>
+        <v>3.8757523740699085E-4</v>
       </c>
       <c r="V5" s="4">
         <f>BNVFE!V27*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.7158050293309159E-4</v>
+        <v>3.9950134420415153E-4</v>
       </c>
       <c r="W5" s="4">
         <f>BNVFE!W27*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.7250082623344597E-4</v>
+        <v>4.0035850605750056E-4</v>
       </c>
       <c r="X5" s="4">
         <f>BNVFE!X27*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.732076820565791E-4</v>
+        <v>4.0109394743594799E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>BNVFE!Y27*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.7340190863010219E-4</v>
+        <v>4.012761936991058E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>BNVFE!Z27*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.7436255674953617E-4</v>
+        <v>4.0222683786844709E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>BNVFE!AA27*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.7367572530025347E-4</v>
+        <v>4.0134683501182901E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>BNVFE!AB27*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.753843882637504E-4</v>
+        <v>4.0302096346638407E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>BNVFE!AC27*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.767035338732028E-4</v>
+        <v>4.0423921136844502E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>BNVFE!AD27*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.7806708002914585E-4</v>
+        <v>4.0550880062563649E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>BNVFE!AE27*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.7906432409328105E-4</v>
+        <v>4.0641720967975257E-4</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -23347,123 +23347,123 @@
       </c>
       <c r="B6" s="4">
         <f>BNVFE!B28*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>5.770030395892457E-4</v>
+        <v>5.8145858873744711E-4</v>
       </c>
       <c r="C6" s="4">
         <f>BNVFE!C28*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>5.1565191072000234E-4</v>
+        <v>5.2354948444348316E-4</v>
       </c>
       <c r="D6" s="4">
         <f>BNVFE!D28*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>5.0655427468507849E-4</v>
+        <v>5.1809592960240015E-4</v>
       </c>
       <c r="E6" s="4">
         <f>BNVFE!E28*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>5.1230151671061109E-4</v>
+        <v>5.2773804503500592E-4</v>
       </c>
       <c r="F6" s="4">
         <f>BNVFE!F28*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>5.057957327894093E-4</v>
+        <v>5.2469222599488079E-4</v>
       </c>
       <c r="G6" s="4">
         <f>BNVFE!G28*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>4.7149665558890241E-4</v>
+        <v>4.9246510878464057E-4</v>
       </c>
       <c r="H6" s="4">
         <f>BNVFE!H28*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>4.7299583719891884E-4</v>
+        <v>4.9734142906827569E-4</v>
       </c>
       <c r="I6" s="4">
         <f>BNVFE!I28*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>4.7114949083498103E-4</v>
+        <v>4.9864550056494565E-4</v>
       </c>
       <c r="J6" s="4">
         <f>BNVFE!J28*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>4.7233122224492742E-4</v>
+        <v>5.0309879253892425E-4</v>
       </c>
       <c r="K6" s="4">
         <f>BNVFE!K28*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>4.7484817881709057E-4</v>
+        <v>5.0894929277128537E-4</v>
       </c>
       <c r="L6" s="4">
         <f>BNVFE!L28*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>4.7725921150277634E-4</v>
+        <v>5.1466999519847565E-4</v>
       </c>
       <c r="M6" s="4">
         <f>BNVFE!M28*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>4.7944511876494916E-4</v>
+        <v>5.2012988435178866E-4</v>
       </c>
       <c r="N6" s="4">
         <f>BNVFE!N28*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>4.8224231408656933E-4</v>
+        <v>5.2623775444660776E-4</v>
       </c>
       <c r="O6" s="4">
         <f>BNVFE!O28*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>4.8523699169033819E-4</v>
+        <v>5.3255139284003441E-4</v>
       </c>
       <c r="P6" s="4">
         <f>BNVFE!P28*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>4.9645320107814599E-4</v>
+        <v>5.4302083063339991E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>BNVFE!Q28*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>5.0631914840744451E-4</v>
+        <v>5.522766833965494E-4</v>
       </c>
       <c r="R6" s="4">
         <f>BNVFE!R28*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>5.1461221884438588E-4</v>
+        <v>5.601254580107081E-4</v>
       </c>
       <c r="S6" s="4">
         <f>BNVFE!S28*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>5.3635081947590716E-4</v>
+        <v>5.807089207832928E-4</v>
       </c>
       <c r="T6" s="4">
         <f>BNVFE!T28*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>5.4335798852553027E-4</v>
+        <v>5.8731627063682789E-4</v>
       </c>
       <c r="U6" s="4">
         <f>BNVFE!U28*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>5.4940992391592244E-4</v>
+        <v>5.931554855531328E-4</v>
       </c>
       <c r="V6" s="4">
         <f>BNVFE!V28*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>5.6842996426768682E-4</v>
+        <v>6.1114222360517459E-4</v>
       </c>
       <c r="W6" s="4">
         <f>BNVFE!W28*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>5.7000753402081756E-4</v>
+        <v>6.1263586196471168E-4</v>
       </c>
       <c r="X6" s="4">
         <f>BNVFE!X28*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>5.707705408366043E-4</v>
+        <v>6.1341880221425316E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>BNVFE!Y28*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>5.7151824558879846E-4</v>
+        <v>6.1418182638870312E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>BNVFE!Z28*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>5.7300097326242578E-4</v>
+        <v>6.1565016430071618E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>BNVFE!AA28*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>5.7287583682467122E-4</v>
+        <v>6.1529793989050126E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>BNVFE!AB28*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>5.7536335602862711E-4</v>
+        <v>6.1772279652446511E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>BNVFE!AC28*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>5.7786091743895448E-4</v>
+        <v>6.2010047833741867E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>BNVFE!AD28*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>5.7953758615710883E-4</v>
+        <v>6.2160289507864192E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>BNVFE!AE28*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>5.8150534020495943E-4</v>
+        <v>6.234661580070439E-4</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -23474,123 +23474,123 @@
       </c>
       <c r="B7" s="4">
         <f>BNVFE!B29*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.1744854324820717E-4</v>
+        <v>3.1989984330977049E-4</v>
       </c>
       <c r="C7" s="4">
         <f>BNVFE!C29*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.0634041173760126E-4</v>
+        <v>3.1103223181211821E-4</v>
       </c>
       <c r="D7" s="4">
         <f>BNVFE!D29*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.1631260057212433E-4</v>
+        <v>3.2351966813477334E-4</v>
       </c>
       <c r="E7" s="4">
         <f>BNVFE!E29*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.1668304561611668E-4</v>
+        <v>3.2622525200054595E-4</v>
       </c>
       <c r="F7" s="4">
         <f>BNVFE!F29*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.1105040315615982E-4</v>
+        <v>3.2267122446555342E-4</v>
       </c>
       <c r="G7" s="4">
         <f>BNVFE!G29*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>2.904534915283473E-4</v>
+        <v>3.0337057242480451E-4</v>
       </c>
       <c r="H7" s="4">
         <f>BNVFE!H29*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>2.896308481447913E-4</v>
+        <v>3.0453845169467914E-4</v>
       </c>
       <c r="I7" s="4">
         <f>BNVFE!I29*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>2.8856459352085231E-4</v>
+        <v>3.0540505504212268E-4</v>
       </c>
       <c r="J7" s="4">
         <f>BNVFE!J29*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>2.8842815300220999E-4</v>
+        <v>3.0721631066429536E-4</v>
       </c>
       <c r="K7" s="4">
         <f>BNVFE!K29*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>2.8862132779813285E-4</v>
+        <v>3.093486028050069E-4</v>
       </c>
       <c r="L7" s="4">
         <f>BNVFE!L29*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>2.8993427425732799E-4</v>
+        <v>3.1266127073803886E-4</v>
       </c>
       <c r="M7" s="4">
         <f>BNVFE!M29*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>2.9074003911273041E-4</v>
+        <v>3.1541166444595039E-4</v>
       </c>
       <c r="N7" s="4">
         <f>BNVFE!N29*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>2.9226290833281419E-4</v>
+        <v>3.1892634075550175E-4</v>
       </c>
       <c r="O7" s="4">
         <f>BNVFE!O29*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>2.937887619941194E-4</v>
+        <v>3.2243546366012341E-4</v>
       </c>
       <c r="P7" s="4">
         <f>BNVFE!P29*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.0033596504796238E-4</v>
+        <v>3.2850767173068688E-4</v>
       </c>
       <c r="Q7" s="4">
         <f>BNVFE!Q29*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.0561694929662176E-4</v>
+        <v>3.3335716351672539E-4</v>
       </c>
       <c r="R7" s="4">
         <f>BNVFE!R29*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.1033762400137736E-4</v>
+        <v>3.3778444703873312E-4</v>
       </c>
       <c r="S7" s="4">
         <f>BNVFE!S29*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.231400555609079E-4</v>
+        <v>3.4986487595933905E-4</v>
       </c>
       <c r="T7" s="4">
         <f>BNVFE!T29*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.2695932283305509E-4</v>
+        <v>3.534107056332161E-4</v>
       </c>
       <c r="U7" s="4">
         <f>BNVFE!U29*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.3032276638030907E-4</v>
+        <v>3.5662399303793859E-4</v>
       </c>
       <c r="V7" s="4">
         <f>BNVFE!V29*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.4154676660143898E-4</v>
+        <v>3.6721085010863982E-4</v>
       </c>
       <c r="W7" s="4">
         <f>BNVFE!W29*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.420449768741958E-4</v>
+        <v>3.6762499919934348E-4</v>
       </c>
       <c r="X7" s="4">
         <f>BNVFE!X29*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.4216652058283842E-4</v>
+        <v>3.6773337479207668E-4</v>
       </c>
       <c r="Y7" s="4">
         <f>BNVFE!Y29*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.418502489054371E-4</v>
+        <v>3.6736921672179983E-4</v>
       </c>
       <c r="Z7" s="4">
         <f>BNVFE!Z29*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.422529850790624E-4</v>
+        <v>3.6772730994967127E-4</v>
       </c>
       <c r="AA7" s="4">
         <f>BNVFE!AA29*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.4093529749808124E-4</v>
+        <v>3.6618194153426438E-4</v>
       </c>
       <c r="AB7" s="4">
         <f>BNVFE!AB29*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.4218633785776896E-4</v>
+        <v>3.6737880391439015E-4</v>
       </c>
       <c r="AC7" s="4">
         <f>BNVFE!AC29*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.4301574950155089E-4</v>
+        <v>3.6808897076111757E-4</v>
       </c>
       <c r="AD7" s="4">
         <f>BNVFE!AD29*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.4382818379754854E-4</v>
+        <v>3.6878469932448562E-4</v>
       </c>
       <c r="AE7" s="4">
         <f>BNVFE!AE29*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.4435480774975858E-4</v>
+        <v>3.6920309090080676E-4</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>

</xml_diff>

<commit_message>
Use AEO No IRA tables in recently edited files
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BBB26-2C5B-4C09-BC97-E4961155787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8D3F70-2927-4DF5-84AD-7C05BAAAFE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1815,91 +1815,91 @@
                   <c:v>3.8560342544165043E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>3.938977091004229E-4</c:v>
+                  <c:v>3.9320167803958366E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.0102815590911211E-4</c:v>
+                  <c:v>4.005442502794511E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.0668872915977704E-4</c:v>
+                  <c:v>4.0645945816058469E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>4.2148439524556525E-4</c:v>
+                  <c:v>4.1828300792889542E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>4.2638034079782157E-4</c:v>
+                  <c:v>4.2432642927896187E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>4.2993928617474374E-4</c:v>
+                  <c:v>4.3013868224805557E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>4.4295232919176118E-4</c:v>
+                  <c:v>4.4159741220930354E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.4402927119422075E-4</c:v>
+                  <c:v>4.4283756012174485E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>4.4423001272194757E-4</c:v>
+                  <c:v>4.4369894861174625E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.4444787060954387E-4</c:v>
+                  <c:v>4.4433519283804937E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>4.4510595798899477E-4</c:v>
+                  <c:v>4.4502983096465825E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.4626178063197816E-4</c:v>
+                  <c:v>4.4619804232655445E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>4.4757258182247277E-4</c:v>
+                  <c:v>4.4736157163053795E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>4.4919390205042781E-4</c:v>
+                  <c:v>4.4858409986435515E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>4.5078104437884211E-4</c:v>
+                  <c:v>4.5062348863147132E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.5211629450069859E-4</c:v>
+                  <c:v>4.5195274509021602E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>4.5326957425061224E-4</c:v>
+                  <c:v>4.524452263539576E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>4.5520696339484528E-4</c:v>
+                  <c:v>4.5513787440342439E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>4.5553578115777672E-4</c:v>
+                  <c:v>4.5560000309037107E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>4.5584944646724456E-4</c:v>
+                  <c:v>4.5628219603308817E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>4.559561094704881E-4</c:v>
+                  <c:v>4.5746355401689185E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>4.5572121425237108E-4</c:v>
+                  <c:v>4.577201565564958E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>4.550985416964502E-4</c:v>
+                  <c:v>4.5688423750485098E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>4.5449905971852166E-4</c:v>
+                  <c:v>4.5637498609098584E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>4.5443664862698183E-4</c:v>
+                  <c:v>4.5582206387129149E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>4.5380063490385911E-4</c:v>
+                  <c:v>4.5519749041800602E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>4.5343326114607497E-4</c:v>
+                  <c:v>4.5459553666078392E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>4.5494560422822621E-4</c:v>
+                  <c:v>4.5420742164487069E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>4.5447278785524218E-4</c:v>
+                  <c:v>4.5366186695498144E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3232,136 +3232,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>7.5108389563240119E-5</c:v>
+                  <c:v>7.7947123371766881E-5</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>7.7552820431472588E-5</c:v>
+                  <c:v>8.0186690650322842E-5</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.9997251299705058E-5</c:v>
+                  <c:v>8.2426257928877936E-5</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>8.2441682167937527E-5</c:v>
+                  <c:v>8.4665825207433897E-5</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>8.4886113036169997E-5</c:v>
+                  <c:v>8.6905392485989857E-5</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>8.7330543904402466E-5</c:v>
+                  <c:v>8.9144959764544951E-5</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>8.9774974772634936E-5</c:v>
+                  <c:v>9.1384527043100912E-5</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>9.2219405640867405E-5</c:v>
+                  <c:v>9.3624094321656005E-5</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>9.4663836509099875E-5</c:v>
+                  <c:v>9.5863661600211966E-5</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>9.7108267377332344E-5</c:v>
+                  <c:v>9.810322887876706E-5</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>9.9552698245564814E-5</c:v>
+                  <c:v>1.0034279615732302E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>1.0199712911379728E-4</c:v>
+                  <c:v>1.0258236343587811E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>1.0444155998202975E-4</c:v>
+                  <c:v>1.0482193071443408E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>1.0688599085026222E-4</c:v>
+                  <c:v>1.0706149799298917E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
                   <c:v>1.0748894488887501E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>1.1376628742778099E-4</c:v>
+                  <c:v>1.1340183318243619E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>1.1487084665170681E-4</c:v>
+                  <c:v>1.146278256602771E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>1.1675219072501874E-4</c:v>
+                  <c:v>1.1598939507763969E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>1.1821814758141852E-4</c:v>
+                  <c:v>1.1739300033405102E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>1.1769306557695523E-4</c:v>
+                  <c:v>1.1760985601866623E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>1.1740735707916262E-4</c:v>
+                  <c:v>1.1770623326767235E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>1.1551151797500483E-4</c:v>
+                  <c:v>1.1580915845333066E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>1.1449785838376007E-4</c:v>
+                  <c:v>1.1434896370073045E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.13287341804607E-4</c:v>
+                  <c:v>1.1339009149021013E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>1.1212406398402511E-4</c:v>
+                  <c:v>1.1219566215487321E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.1076186329973974E-4</c:v>
+                  <c:v>1.1066260788344435E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>1.0947685788155618E-4</c:v>
+                  <c:v>1.093041603920123E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>1.0833659526703707E-4</c:v>
+                  <c:v>1.080839088666242E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>1.0725258337875167E-4</c:v>
+                  <c:v>1.0723515259083896E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>1.0627237374881068E-4</c:v>
+                  <c:v>1.0607167803261324E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>1.053872190542009E-4</c:v>
+                  <c:v>1.0514634456433018E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>1.0457070988285631E-4</c:v>
+                  <c:v>1.0424762201930517E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>1.0382785746559407E-4</c:v>
+                  <c:v>1.0356841044901005E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>1.0317553743970813E-4</c:v>
+                  <c:v>1.0310079801566161E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>1.0260660677729319E-4</c:v>
+                  <c:v>1.0253359756446476E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.0212195692865432E-4</c:v>
+                  <c:v>1.0217654907137221E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.0164270384030296E-4</c:v>
+                  <c:v>1.0162236577213031E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.0120623842325044E-4</c:v>
+                  <c:v>1.0123288850628106E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.0086620530512349E-4</c:v>
+                  <c:v>1.0091473811361892E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>1.0054219744424832E-4</c:v>
+                  <c:v>1.0075212418516603E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>9.9850684341711718E-5</c:v>
+                  <c:v>1.0011436735388883E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>9.9621972535475967E-5</c:v>
+                  <c:v>1.0002070036019407E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>9.9483752435656976E-5</c:v>
+                  <c:v>9.9828102035601804E-5</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>9.9383928406132565E-5</c:v>
+                  <c:v>9.9636624901656103E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3785,91 +3785,91 @@
                   <c:v>1.1137362177939013E-3</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>1.1868928349938494E-3</c:v>
+                  <c:v>1.1925426392408319E-3</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>1.2242021544325342E-3</c:v>
+                  <c:v>1.2281409269793643E-3</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>1.2625148116111296E-3</c:v>
+                  <c:v>1.2637392147178965E-3</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>1.2984724640643824E-3</c:v>
+                  <c:v>1.2993375024564287E-3</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>1.3325458991476347E-3</c:v>
+                  <c:v>1.3349357901949611E-3</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>1.3625499159680566E-3</c:v>
+                  <c:v>1.3705340779334933E-3</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>1.3753174198569201E-3</c:v>
+                  <c:v>1.3705340779334933E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>1.3946841343267524E-3</c:v>
+                  <c:v>1.3883332218027598E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.4146533498165595E-3</c:v>
+                  <c:v>1.4061323656720257E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>1.4334182752321722E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.4445909758303492E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>1.4455847020325701E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>1.4457021763821076E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>1.4456854451868699E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>1.4457034223221783E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>1.4456555426251702E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>1.4455629870770495E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>1.4452171497116701E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>1.4450916657473916E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>1.4448529792281048E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.443856049179987E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.4432142120520614E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.443266541535037E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.4434251319069122E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>1.4437811147842976E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>1.4442054463741406E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>1.4447501001765403E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>1.4451804834752992E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>1.4456904289471535E-3</c:v>
+                  <c:v>1.4417306534105579E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4293,91 +4293,91 @@
                   <c:v>7.3612054146182692E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>7.8447318350072194E-4</c:v>
+                  <c:v>7.8820740431081668E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>8.0913266389472246E-4</c:v>
+                  <c:v>8.1173598354397538E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>8.3445529729440947E-4</c:v>
+                  <c:v>8.3526456277713398E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>8.582213975349269E-4</c:v>
+                  <c:v>8.5879314201029269E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>8.8074213007663328E-4</c:v>
+                  <c:v>8.823217212434515E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>9.0057319308330108E-4</c:v>
+                  <c:v>9.058503004766101E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>9.0901183566816969E-4</c:v>
+                  <c:v>9.058503004766101E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>9.2181220627128113E-4</c:v>
+                  <c:v>9.1761459009318956E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>9.3501079807791388E-4</c:v>
+                  <c:v>9.2937887970976892E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>9.4741341804908898E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>9.5479798028431191E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>9.5545478057360543E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>9.5553242488507497E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>9.5552136645283517E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>9.5553324838534815E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>9.5550160244627959E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>9.5544042814027313E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>9.5521184799302321E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>9.5512890975122625E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>9.5497115062746795E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>9.5431223276604333E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>9.5388801248246955E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>9.5392259949394229E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>9.5402741931442593E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>9.5426270510675759E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>9.5454316577121671E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>9.5490315303348411E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>9.5518761355641295E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>9.555246604539279E-4</c:v>
+                  <c:v>9.5290745894292751E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5207,79 +5207,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>3.6038411832808568E-5</c:v>
+                  <c:v>3.6038260344938299E-5</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>3.647844074325616E-5</c:v>
+                  <c:v>3.6478359505012103E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>3.6918469653703644E-5</c:v>
+                  <c:v>3.6918458665085799E-5</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>3.7358498564151237E-5</c:v>
+                  <c:v>3.7358557825159494E-5</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>3.7798527474598721E-5</c:v>
+                  <c:v>3.7798656985233299E-5</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>3.8238556385046314E-5</c:v>
+                  <c:v>3.8238756145306995E-5</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>3.8678585295493906E-5</c:v>
+                  <c:v>3.867885530538069E-5</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>3.9118614205941391E-5</c:v>
+                  <c:v>3.9118954465454495E-5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>3.9558643116388983E-5</c:v>
+                  <c:v>3.955905362552819E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>3.9998672026836467E-5</c:v>
+                  <c:v>3.9999152785601886E-5</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.043870093728406E-5</c:v>
+                  <c:v>4.0439251945675691E-5</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>4.0878729847731653E-5</c:v>
+                  <c:v>4.0879351105749386E-5</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>4.1318758758179137E-5</c:v>
+                  <c:v>4.1319450265823082E-5</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>4.1758787668626729E-5</c:v>
+                  <c:v>4.1759549425896887E-5</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>4.2198816579074322E-5</c:v>
+                  <c:v>4.2199648585970582E-5</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>4.2638845489521806E-5</c:v>
+                  <c:v>4.2639747746044278E-5</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>4.3078874399969399E-5</c:v>
+                  <c:v>4.3079846906117974E-5</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>4.3518903310416883E-5</c:v>
+                  <c:v>4.3519946066191778E-5</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>4.3958932220864476E-5</c:v>
+                  <c:v>4.3960045226265474E-5</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>4.4398961131312068E-5</c:v>
+                  <c:v>4.440014438633917E-5</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>4.4838990041759552E-5</c:v>
+                  <c:v>4.4840243546412974E-5</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>4.5279018952207145E-5</c:v>
+                  <c:v>4.528034270648667E-5</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>4.5719047862654629E-5</c:v>
+                  <c:v>4.5720441866560366E-5</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>4.6159076773102222E-5</c:v>
+                  <c:v>4.616054102663417E-5</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>4.6599105683549815E-5</c:v>
+                  <c:v>4.6600640186707866E-5</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
                   <c:v>4.8563096039282174E-5</c:v>
@@ -5288,88 +5288,88 @@
                   <c:v>4.7951937565239972E-5</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.8199148542133818E-5</c:v>
+                  <c:v>4.8199163709058256E-5</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.8463289763291303E-5</c:v>
+                  <c:v>4.8462484597433007E-5</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>4.8810101273548841E-5</c:v>
+                  <c:v>4.8807912620409042E-5</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>4.9248402309752346E-5</c:v>
+                  <c:v>4.9249126365536466E-5</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>4.9544253613324154E-5</c:v>
+                  <c:v>4.9546819461280452E-5</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>4.9847838070065696E-5</c:v>
+                  <c:v>4.985094728957582E-5</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>5.0132631366857999E-5</c:v>
+                  <c:v>5.0135212381738722E-5</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>5.0441473470928121E-5</c:v>
+                  <c:v>5.0441951558763717E-5</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>5.0785598457265348E-5</c:v>
+                  <c:v>5.0784808458331483E-5</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>5.1172517250624796E-5</c:v>
+                  <c:v>5.1171299280649147E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>5.161151266819503E-5</c:v>
+                  <c:v>5.1611160531775431E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.2082892766601423E-5</c:v>
+                  <c:v>5.2084633665754489E-5</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>5.2576863009813412E-5</c:v>
+                  <c:v>5.2581159206018821E-5</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>5.3077126867236362E-5</c:v>
+                  <c:v>5.3082228229300067E-5</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>5.3586049060219874E-5</c:v>
+                  <c:v>5.3590934128752432E-5</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>5.4105334878616127E-5</c:v>
+                  <c:v>5.4110456683056242E-5</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>5.4610539196817424E-5</c:v>
+                  <c:v>5.4614996953739692E-5</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>5.5125025672775793E-5</c:v>
+                  <c:v>5.5129609381114051E-5</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>5.5644352375924891E-5</c:v>
+                  <c:v>5.5651209804066108E-5</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>5.6164574587047429E-5</c:v>
+                  <c:v>5.6171220337677975E-5</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>5.6693978062907934E-5</c:v>
+                  <c:v>5.6698732564004017E-5</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>5.721493949673903E-5</c:v>
+                  <c:v>5.7217304218088618E-5</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>5.7733179456780447E-5</c:v>
+                  <c:v>5.7733823061921899E-5</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>5.8241709288023016E-5</c:v>
+                  <c:v>5.8241543111285681E-5</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>5.8749514404049965E-5</c:v>
+                  <c:v>5.8747929790161759E-5</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>5.9249763094548476E-5</c:v>
+                  <c:v>5.9248827361253699E-5</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>5.9740125588038328E-5</c:v>
+                  <c:v>5.974092547844464E-5</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>6.0224657388228372E-5</c:v>
+                  <c:v>6.0225517946332457E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10004,99 +10004,99 @@
       </c>
       <c r="B2" s="4">
         <f>B$5/(1-'Other Values'!$B$3)</f>
-        <v>1.1722254425066041E-4</v>
+        <v>1.1722228319362329E-4</v>
       </c>
       <c r="C2" s="4">
         <f>C$5/(1-'Other Values'!$B$3)</f>
-        <v>1.1863656599543676E-4</v>
+        <v>1.1863653068379199E-4</v>
       </c>
       <c r="D2" s="4">
         <f>D$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2005058774021348E-4</v>
+        <v>1.2005077817396067E-4</v>
       </c>
       <c r="E2" s="4">
         <f>E$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2146460948498984E-4</v>
+        <v>1.2146502566412971E-4</v>
       </c>
       <c r="F2" s="4">
         <f>F$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2287863122976655E-4</v>
+        <v>1.2287927315429839E-4</v>
       </c>
       <c r="G2" s="4">
         <f>G$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2429265297454325E-4</v>
+        <v>1.2429352064446708E-4</v>
       </c>
       <c r="H2" s="4">
         <f>H$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2570667471931959E-4</v>
+        <v>1.2570776813463613E-4</v>
       </c>
       <c r="I2" s="4">
         <f>I$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2712069646409632E-4</v>
+        <v>1.2712201562480483E-4</v>
       </c>
       <c r="J2" s="4">
         <f>J$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2853471820887266E-4</v>
+        <v>1.285362631149735E-4</v>
       </c>
       <c r="K2" s="4">
         <f>K$5/(1-'Other Values'!$B$3)</f>
-        <v>1.2994873995364939E-4</v>
+        <v>1.2995051060514255E-4</v>
       </c>
       <c r="L2" s="4">
         <f>L$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3136276169842609E-4</v>
+        <v>1.3136475809531124E-4</v>
       </c>
       <c r="M2" s="4">
         <f>M$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3277678344320243E-4</v>
+        <v>1.3277900558547991E-4</v>
       </c>
       <c r="N2" s="4">
         <f>N$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3419080518797916E-4</v>
+        <v>1.3419325307564896E-4</v>
       </c>
       <c r="O2" s="4">
         <f>O$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3560482693275586E-4</v>
+        <v>1.3560750056581766E-4</v>
       </c>
       <c r="P2" s="4">
         <f>P$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3701884867753223E-4</v>
+        <v>1.3702174805598635E-4</v>
       </c>
       <c r="Q2" s="4">
         <f>Q$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3843287042230893E-4</v>
+        <v>1.3843599554615502E-4</v>
       </c>
       <c r="R2" s="4">
         <f>R$5/(1-'Other Values'!$B$3)</f>
-        <v>1.3984689216708527E-4</v>
+        <v>1.3985024303632407E-4</v>
       </c>
       <c r="S2" s="4">
         <f>S$5/(1-'Other Values'!$B$3)</f>
-        <v>1.41260913911862E-4</v>
+        <v>1.4126449052649276E-4</v>
       </c>
       <c r="T2" s="4">
         <f>T$5/(1-'Other Values'!$B$3)</f>
-        <v>1.426749356566387E-4</v>
+        <v>1.4267873801666143E-4</v>
       </c>
       <c r="U2" s="4">
         <f>U$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4408895740141507E-4</v>
+        <v>1.4409298550683048E-4</v>
       </c>
       <c r="V2" s="4">
         <f>V$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4550297914619177E-4</v>
+        <v>1.4550723299699918E-4</v>
       </c>
       <c r="W2" s="4">
         <f>W$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4691700089096812E-4</v>
+        <v>1.4692148048716787E-4</v>
       </c>
       <c r="X2" s="4">
         <f>X$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4833102263574484E-4</v>
+        <v>1.4833572797733689E-4</v>
       </c>
       <c r="Y2" s="4">
         <f>Y$5/(1-'Other Values'!$B$3)</f>
-        <v>1.4974504438052154E-4</v>
+        <v>1.4974997546750559E-4</v>
       </c>
       <c r="Z2" s="4">
         <f>Z$5/(1-'Other Values'!$B$3)</f>
@@ -10108,19 +10108,19 @@
       </c>
       <c r="AB2" s="4">
         <f>AB$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5488674153017263E-4</v>
+        <v>1.5488679026869968E-4</v>
       </c>
       <c r="AC2" s="4">
         <f>AC$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5573555264585283E-4</v>
+        <v>1.5573296526578585E-4</v>
       </c>
       <c r="AD2" s="4">
         <f>AD$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5685002263907255E-4</v>
+        <v>1.568429894577111E-4</v>
       </c>
       <c r="AE2" s="4">
         <f>AE$5/(1-'Other Values'!$B$3)</f>
-        <v>1.5825849190378402E-4</v>
+        <v>1.5826081863868456E-4</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
@@ -10321,99 +10321,99 @@
       </c>
       <c r="B5" s="4">
         <f>Extrapolations!Q7</f>
-        <v>3.647844074325616E-5</v>
+        <v>3.6478359505012103E-5</v>
       </c>
       <c r="C5" s="4">
         <f>Extrapolations!R7</f>
-        <v>3.6918469653703644E-5</v>
+        <v>3.6918458665085799E-5</v>
       </c>
       <c r="D5" s="4">
         <f>Extrapolations!S7</f>
-        <v>3.7358498564151237E-5</v>
+        <v>3.7358557825159494E-5</v>
       </c>
       <c r="E5" s="4">
         <f>Extrapolations!T7</f>
-        <v>3.7798527474598721E-5</v>
+        <v>3.7798656985233299E-5</v>
       </c>
       <c r="F5" s="4">
         <f>Extrapolations!U7</f>
-        <v>3.8238556385046314E-5</v>
+        <v>3.8238756145306995E-5</v>
       </c>
       <c r="G5" s="4">
         <f>Extrapolations!V7</f>
-        <v>3.8678585295493906E-5</v>
+        <v>3.867885530538069E-5</v>
       </c>
       <c r="H5" s="4">
         <f>Extrapolations!W7</f>
-        <v>3.9118614205941391E-5</v>
+        <v>3.9118954465454495E-5</v>
       </c>
       <c r="I5" s="4">
         <f>Extrapolations!X7</f>
-        <v>3.9558643116388983E-5</v>
+        <v>3.955905362552819E-5</v>
       </c>
       <c r="J5" s="4">
         <f>Extrapolations!Y7</f>
-        <v>3.9998672026836467E-5</v>
+        <v>3.9999152785601886E-5</v>
       </c>
       <c r="K5" s="4">
         <f>Extrapolations!Z7</f>
-        <v>4.043870093728406E-5</v>
+        <v>4.0439251945675691E-5</v>
       </c>
       <c r="L5" s="4">
         <f>Extrapolations!AA7</f>
-        <v>4.0878729847731653E-5</v>
+        <v>4.0879351105749386E-5</v>
       </c>
       <c r="M5" s="4">
         <f>Extrapolations!AB7</f>
-        <v>4.1318758758179137E-5</v>
+        <v>4.1319450265823082E-5</v>
       </c>
       <c r="N5" s="4">
         <f>Extrapolations!AC7</f>
-        <v>4.1758787668626729E-5</v>
+        <v>4.1759549425896887E-5</v>
       </c>
       <c r="O5" s="4">
         <f>Extrapolations!AD7</f>
-        <v>4.2198816579074322E-5</v>
+        <v>4.2199648585970582E-5</v>
       </c>
       <c r="P5" s="4">
         <f>Extrapolations!AE7</f>
-        <v>4.2638845489521806E-5</v>
+        <v>4.2639747746044278E-5</v>
       </c>
       <c r="Q5" s="4">
         <f>Extrapolations!AF7</f>
-        <v>4.3078874399969399E-5</v>
+        <v>4.3079846906117974E-5</v>
       </c>
       <c r="R5" s="4">
         <f>Extrapolations!AG7</f>
-        <v>4.3518903310416883E-5</v>
+        <v>4.3519946066191778E-5</v>
       </c>
       <c r="S5" s="4">
         <f>Extrapolations!AH7</f>
-        <v>4.3958932220864476E-5</v>
+        <v>4.3960045226265474E-5</v>
       </c>
       <c r="T5" s="4">
         <f>Extrapolations!AI7</f>
-        <v>4.4398961131312068E-5</v>
+        <v>4.440014438633917E-5</v>
       </c>
       <c r="U5" s="4">
         <f>Extrapolations!AJ7</f>
-        <v>4.4838990041759552E-5</v>
+        <v>4.4840243546412974E-5</v>
       </c>
       <c r="V5" s="4">
         <f>Extrapolations!AK7</f>
-        <v>4.5279018952207145E-5</v>
+        <v>4.528034270648667E-5</v>
       </c>
       <c r="W5" s="4">
         <f>Extrapolations!AL7</f>
-        <v>4.5719047862654629E-5</v>
+        <v>4.5720441866560366E-5</v>
       </c>
       <c r="X5" s="4">
         <f>Extrapolations!AM7</f>
-        <v>4.6159076773102222E-5</v>
+        <v>4.616054102663417E-5</v>
       </c>
       <c r="Y5" s="4">
         <f>Extrapolations!AN7</f>
-        <v>4.6599105683549815E-5</v>
+        <v>4.6600640186707866E-5</v>
       </c>
       <c r="Z5" s="4">
         <f>Extrapolations!AO7</f>
@@ -10425,19 +10425,19 @@
       </c>
       <c r="AB5" s="4">
         <f>Extrapolations!AQ7</f>
-        <v>4.8199148542133818E-5</v>
+        <v>4.8199163709058256E-5</v>
       </c>
       <c r="AC5" s="4">
         <f>Extrapolations!AR7</f>
-        <v>4.8463289763291303E-5</v>
+        <v>4.8462484597433007E-5</v>
       </c>
       <c r="AD5" s="4">
         <f>Extrapolations!AS7</f>
-        <v>4.8810101273548841E-5</v>
+        <v>4.8807912620409042E-5</v>
       </c>
       <c r="AE5" s="4">
         <f>Extrapolations!AT7</f>
-        <v>4.9248402309752346E-5</v>
+        <v>4.9249126365536466E-5</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -10638,99 +10638,99 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.0943532222976846E-4</v>
+        <v>1.0943507851503629E-4</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.1075540896111091E-4</v>
+        <v>1.1075537599525738E-4</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.1207549569245369E-4</v>
+        <v>1.1207567347547847E-4</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.1339558242379614E-4</v>
+        <v>1.1339597095569988E-4</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.1471566915513892E-4</v>
+        <v>1.1471626843592097E-4</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.160357558864817E-4</v>
+        <v>1.1603656591614206E-4</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.1735584261782415E-4</v>
+        <v>1.1735686339636347E-4</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.1867592934916693E-4</v>
+        <v>1.1867716087658456E-4</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.1999601608050938E-4</v>
+        <v>1.1999745835680565E-4</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.2131610281185216E-4</v>
+        <v>1.2131775583702706E-4</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.2263618954319494E-4</v>
+        <v>1.2263805331724813E-4</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.2395627627453739E-4</v>
+        <v>1.2395835079746922E-4</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.2527636300588017E-4</v>
+        <v>1.2527864827769063E-4</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.2659644973722295E-4</v>
+        <v>1.2659894575791172E-4</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.279165364685654E-4</v>
+        <v>1.2791924323813281E-4</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.2923662319990818E-4</v>
+        <v>1.292395407183539E-4</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.3055670993125063E-4</v>
+        <v>1.3055983819857531E-4</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.3187679666259341E-4</v>
+        <v>1.318801356787964E-4</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.3319688339393618E-4</v>
+        <v>1.3320043315901748E-4</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.3451697012527864E-4</v>
+        <v>1.345207306392389E-4</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.3583705685662141E-4</v>
+        <v>1.3584102811945998E-4</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.3715714358796387E-4</v>
+        <v>1.3716132559968107E-4</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.3847723031930665E-4</v>
+        <v>1.3848162307990248E-4</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.3979731705064942E-4</v>
+        <v>1.3980192056012357E-4</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
@@ -10742,19 +10742,19 @@
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.4459744562640142E-4</v>
+        <v>1.4459749112717473E-4</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.4538986928987389E-4</v>
+        <v>1.4538745379229901E-4</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.464303038206465E-4</v>
+        <v>1.4642373786122711E-4</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.47745206929257E-4</v>
+        <v>1.4774737909660938E-4</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4"/>
@@ -16200,7 +16200,7 @@
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16384,91 +16384,91 @@
         <v>3.8560342544165043E-4</v>
       </c>
       <c r="E8" s="4">
-        <v>3.938977091004229E-4</v>
+        <v>3.9320167803958366E-4</v>
       </c>
       <c r="F8" s="4">
-        <v>4.0102815590911211E-4</v>
+        <v>4.005442502794511E-4</v>
       </c>
       <c r="G8" s="4">
-        <v>4.0668872915977704E-4</v>
+        <v>4.0645945816058469E-4</v>
       </c>
       <c r="H8" s="4">
-        <v>4.2148439524556525E-4</v>
+        <v>4.1828300792889542E-4</v>
       </c>
       <c r="I8" s="4">
-        <v>4.2638034079782157E-4</v>
+        <v>4.2432642927896187E-4</v>
       </c>
       <c r="J8" s="4">
-        <v>4.2993928617474374E-4</v>
+        <v>4.3013868224805557E-4</v>
       </c>
       <c r="K8" s="4">
-        <v>4.4295232919176118E-4</v>
+        <v>4.4159741220930354E-4</v>
       </c>
       <c r="L8" s="4">
-        <v>4.4402927119422075E-4</v>
+        <v>4.4283756012174485E-4</v>
       </c>
       <c r="M8" s="4">
-        <v>4.4423001272194757E-4</v>
+        <v>4.4369894861174625E-4</v>
       </c>
       <c r="N8" s="4">
-        <v>4.4444787060954387E-4</v>
+        <v>4.4433519283804937E-4</v>
       </c>
       <c r="O8" s="4">
-        <v>4.4510595798899477E-4</v>
+        <v>4.4502983096465825E-4</v>
       </c>
       <c r="P8" s="4">
-        <v>4.4626178063197816E-4</v>
+        <v>4.4619804232655445E-4</v>
       </c>
       <c r="Q8" s="4">
-        <v>4.4757258182247277E-4</v>
+        <v>4.4736157163053795E-4</v>
       </c>
       <c r="R8" s="4">
-        <v>4.4919390205042781E-4</v>
+        <v>4.4858409986435515E-4</v>
       </c>
       <c r="S8" s="4">
-        <v>4.5078104437884211E-4</v>
+        <v>4.5062348863147132E-4</v>
       </c>
       <c r="T8" s="4">
-        <v>4.5211629450069859E-4</v>
+        <v>4.5195274509021602E-4</v>
       </c>
       <c r="U8" s="4">
-        <v>4.5326957425061224E-4</v>
+        <v>4.524452263539576E-4</v>
       </c>
       <c r="V8" s="4">
-        <v>4.5520696339484528E-4</v>
+        <v>4.5513787440342439E-4</v>
       </c>
       <c r="W8" s="4">
-        <v>4.5553578115777672E-4</v>
+        <v>4.5560000309037107E-4</v>
       </c>
       <c r="X8" s="4">
-        <v>4.5584944646724456E-4</v>
+        <v>4.5628219603308817E-4</v>
       </c>
       <c r="Y8" s="4">
-        <v>4.559561094704881E-4</v>
+        <v>4.5746355401689185E-4</v>
       </c>
       <c r="Z8" s="4">
-        <v>4.5572121425237108E-4</v>
+        <v>4.577201565564958E-4</v>
       </c>
       <c r="AA8" s="4">
-        <v>4.550985416964502E-4</v>
+        <v>4.5688423750485098E-4</v>
       </c>
       <c r="AB8" s="4">
-        <v>4.5449905971852166E-4</v>
+        <v>4.5637498609098584E-4</v>
       </c>
       <c r="AC8" s="4">
-        <v>4.5443664862698183E-4</v>
+        <v>4.5582206387129149E-4</v>
       </c>
       <c r="AD8" s="4">
-        <v>4.5380063490385911E-4</v>
+        <v>4.5519749041800602E-4</v>
       </c>
       <c r="AE8" s="4">
-        <v>4.5343326114607497E-4</v>
+        <v>4.5459553666078392E-4</v>
       </c>
       <c r="AF8" s="4">
-        <v>4.5494560422822621E-4</v>
+        <v>4.5420742164487069E-4</v>
       </c>
       <c r="AG8" s="4">
-        <v>4.5447278785524218E-4</v>
+        <v>4.5366186695498144E-4</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -16489,91 +16489,91 @@
         <v>1.0748894488887501E-4</v>
       </c>
       <c r="E9" s="4">
-        <v>1.1376628742778099E-4</v>
+        <v>1.1340183318243619E-4</v>
       </c>
       <c r="F9" s="4">
-        <v>1.1487084665170681E-4</v>
+        <v>1.146278256602771E-4</v>
       </c>
       <c r="G9" s="4">
-        <v>1.1675219072501874E-4</v>
+        <v>1.1598939507763969E-4</v>
       </c>
       <c r="H9" s="4">
-        <v>1.1821814758141852E-4</v>
+        <v>1.1739300033405102E-4</v>
       </c>
       <c r="I9" s="4">
-        <v>1.1769306557695523E-4</v>
+        <v>1.1760985601866623E-4</v>
       </c>
       <c r="J9" s="4">
-        <v>1.1740735707916262E-4</v>
+        <v>1.1770623326767235E-4</v>
       </c>
       <c r="K9" s="4">
-        <v>1.1551151797500483E-4</v>
+        <v>1.1580915845333066E-4</v>
       </c>
       <c r="L9" s="4">
-        <v>1.1449785838376007E-4</v>
+        <v>1.1434896370073045E-4</v>
       </c>
       <c r="M9" s="4">
-        <v>1.13287341804607E-4</v>
+        <v>1.1339009149021013E-4</v>
       </c>
       <c r="N9" s="4">
-        <v>1.1212406398402511E-4</v>
+        <v>1.1219566215487321E-4</v>
       </c>
       <c r="O9" s="4">
-        <v>1.1076186329973974E-4</v>
+        <v>1.1066260788344435E-4</v>
       </c>
       <c r="P9" s="4">
-        <v>1.0947685788155618E-4</v>
+        <v>1.093041603920123E-4</v>
       </c>
       <c r="Q9" s="4">
-        <v>1.0833659526703707E-4</v>
+        <v>1.080839088666242E-4</v>
       </c>
       <c r="R9" s="4">
-        <v>1.0725258337875167E-4</v>
+        <v>1.0723515259083896E-4</v>
       </c>
       <c r="S9" s="4">
-        <v>1.0627237374881068E-4</v>
+        <v>1.0607167803261324E-4</v>
       </c>
       <c r="T9" s="4">
-        <v>1.053872190542009E-4</v>
+        <v>1.0514634456433018E-4</v>
       </c>
       <c r="U9" s="4">
-        <v>1.0457070988285631E-4</v>
+        <v>1.0424762201930517E-4</v>
       </c>
       <c r="V9" s="4">
-        <v>1.0382785746559407E-4</v>
+        <v>1.0356841044901005E-4</v>
       </c>
       <c r="W9" s="4">
-        <v>1.0317553743970813E-4</v>
+        <v>1.0310079801566161E-4</v>
       </c>
       <c r="X9" s="4">
-        <v>1.0260660677729319E-4</v>
+        <v>1.0253359756446476E-4</v>
       </c>
       <c r="Y9" s="4">
-        <v>1.0212195692865432E-4</v>
+        <v>1.0217654907137221E-4</v>
       </c>
       <c r="Z9" s="4">
-        <v>1.0164270384030296E-4</v>
+        <v>1.0162236577213031E-4</v>
       </c>
       <c r="AA9" s="4">
-        <v>1.0120623842325044E-4</v>
+        <v>1.0123288850628106E-4</v>
       </c>
       <c r="AB9" s="4">
-        <v>1.0086620530512349E-4</v>
+        <v>1.0091473811361892E-4</v>
       </c>
       <c r="AC9" s="4">
-        <v>1.0054219744424832E-4</v>
+        <v>1.0075212418516603E-4</v>
       </c>
       <c r="AD9" s="4">
-        <v>9.9850684341711718E-5</v>
+        <v>1.0011436735388883E-4</v>
       </c>
       <c r="AE9" s="4">
-        <v>9.9621972535475967E-5</v>
+        <v>1.0002070036019407E-4</v>
       </c>
       <c r="AF9" s="4">
-        <v>9.9483752435656976E-5</v>
+        <v>9.9828102035601804E-5</v>
       </c>
       <c r="AG9" s="4">
-        <v>9.9383928406132565E-5</v>
+        <v>9.9636624901656103E-5</v>
       </c>
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
@@ -16594,91 +16594,91 @@
         <v>1.1137362177939013E-3</v>
       </c>
       <c r="E10" s="4">
-        <v>1.1868928349938494E-3</v>
+        <v>1.1925426392408319E-3</v>
       </c>
       <c r="F10" s="4">
-        <v>1.2242021544325342E-3</v>
+        <v>1.2281409269793643E-3</v>
       </c>
       <c r="G10" s="4">
-        <v>1.2625148116111296E-3</v>
+        <v>1.2637392147178965E-3</v>
       </c>
       <c r="H10" s="4">
-        <v>1.2984724640643824E-3</v>
+        <v>1.2993375024564287E-3</v>
       </c>
       <c r="I10" s="4">
-        <v>1.3325458991476347E-3</v>
+        <v>1.3349357901949611E-3</v>
       </c>
       <c r="J10" s="4">
-        <v>1.3625499159680566E-3</v>
+        <v>1.3705340779334933E-3</v>
       </c>
       <c r="K10" s="4">
-        <v>1.3753174198569201E-3</v>
+        <v>1.3705340779334933E-3</v>
       </c>
       <c r="L10" s="4">
-        <v>1.3946841343267524E-3</v>
+        <v>1.3883332218027598E-3</v>
       </c>
       <c r="M10" s="4">
-        <v>1.4146533498165595E-3</v>
+        <v>1.4061323656720257E-3</v>
       </c>
       <c r="N10" s="4">
-        <v>1.4334182752321722E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="O10" s="4">
-        <v>1.4445909758303492E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="P10" s="4">
-        <v>1.4455847020325701E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="Q10" s="4">
-        <v>1.4457021763821076E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="R10" s="4">
-        <v>1.4456854451868699E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="S10" s="4">
-        <v>1.4457034223221783E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="T10" s="4">
-        <v>1.4456555426251702E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="U10" s="4">
-        <v>1.4455629870770495E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="V10" s="4">
-        <v>1.4452171497116701E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="W10" s="4">
-        <v>1.4450916657473916E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="X10" s="4">
-        <v>1.4448529792281048E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="Y10" s="4">
-        <v>1.443856049179987E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="Z10" s="4">
-        <v>1.4432142120520614E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AA10" s="4">
-        <v>1.443266541535037E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AB10" s="4">
-        <v>1.4434251319069122E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AC10" s="4">
-        <v>1.4437811147842976E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AD10" s="4">
-        <v>1.4442054463741406E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AE10" s="4">
-        <v>1.4447501001765403E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AF10" s="4">
-        <v>1.4451804834752992E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AG10" s="4">
-        <v>1.4456904289471535E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
@@ -16699,91 +16699,91 @@
         <v>7.3612054146182692E-4</v>
       </c>
       <c r="E11" s="4">
-        <v>7.8447318350072194E-4</v>
+        <v>7.8820740431081668E-4</v>
       </c>
       <c r="F11" s="4">
-        <v>8.0913266389472246E-4</v>
+        <v>8.1173598354397538E-4</v>
       </c>
       <c r="G11" s="4">
-        <v>8.3445529729440947E-4</v>
+        <v>8.3526456277713398E-4</v>
       </c>
       <c r="H11" s="4">
-        <v>8.582213975349269E-4</v>
+        <v>8.5879314201029269E-4</v>
       </c>
       <c r="I11" s="4">
-        <v>8.8074213007663328E-4</v>
+        <v>8.823217212434515E-4</v>
       </c>
       <c r="J11" s="4">
-        <v>9.0057319308330108E-4</v>
+        <v>9.058503004766101E-4</v>
       </c>
       <c r="K11" s="4">
-        <v>9.0901183566816969E-4</v>
+        <v>9.058503004766101E-4</v>
       </c>
       <c r="L11" s="4">
-        <v>9.2181220627128113E-4</v>
+        <v>9.1761459009318956E-4</v>
       </c>
       <c r="M11" s="4">
-        <v>9.3501079807791388E-4</v>
+        <v>9.2937887970976892E-4</v>
       </c>
       <c r="N11" s="4">
-        <v>9.4741341804908898E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="O11" s="4">
-        <v>9.5479798028431191E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="P11" s="4">
-        <v>9.5545478057360543E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="Q11" s="4">
-        <v>9.5553242488507497E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="R11" s="4">
-        <v>9.5552136645283517E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="S11" s="4">
-        <v>9.5553324838534815E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="T11" s="4">
-        <v>9.5550160244627959E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="U11" s="4">
-        <v>9.5544042814027313E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="V11" s="4">
-        <v>9.5521184799302321E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="W11" s="4">
-        <v>9.5512890975122625E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="X11" s="4">
-        <v>9.5497115062746795E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="Y11" s="4">
-        <v>9.5431223276604333E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="Z11" s="4">
-        <v>9.5388801248246955E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AA11" s="4">
-        <v>9.5392259949394229E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AB11" s="4">
-        <v>9.5402741931442593E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AC11" s="4">
-        <v>9.5426270510675759E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AD11" s="4">
-        <v>9.5454316577121671E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AE11" s="4">
-        <v>9.5490315303348411E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AF11" s="4">
-        <v>9.5518761355641295E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AG11" s="4">
-        <v>9.555246604539279E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
@@ -16912,88 +16912,88 @@
         <v>4.7951937565239972E-5</v>
       </c>
       <c r="F13" s="4">
-        <v>4.8199148542133818E-5</v>
+        <v>4.8199163709058256E-5</v>
       </c>
       <c r="G13" s="4">
-        <v>4.8463289763291303E-5</v>
+        <v>4.8462484597433007E-5</v>
       </c>
       <c r="H13" s="4">
-        <v>4.8810101273548841E-5</v>
+        <v>4.8807912620409042E-5</v>
       </c>
       <c r="I13" s="4">
-        <v>4.9248402309752346E-5</v>
+        <v>4.9249126365536466E-5</v>
       </c>
       <c r="J13" s="4">
-        <v>4.9544253613324154E-5</v>
+        <v>4.9546819461280452E-5</v>
       </c>
       <c r="K13" s="4">
-        <v>4.9847838070065696E-5</v>
+        <v>4.985094728957582E-5</v>
       </c>
       <c r="L13" s="4">
-        <v>5.0132631366857999E-5</v>
+        <v>5.0135212381738722E-5</v>
       </c>
       <c r="M13" s="4">
-        <v>5.0441473470928121E-5</v>
+        <v>5.0441951558763717E-5</v>
       </c>
       <c r="N13" s="4">
-        <v>5.0785598457265348E-5</v>
+        <v>5.0784808458331483E-5</v>
       </c>
       <c r="O13" s="4">
-        <v>5.1172517250624796E-5</v>
+        <v>5.1171299280649147E-5</v>
       </c>
       <c r="P13" s="4">
-        <v>5.161151266819503E-5</v>
+        <v>5.1611160531775431E-5</v>
       </c>
       <c r="Q13" s="4">
-        <v>5.2082892766601423E-5</v>
+        <v>5.2084633665754489E-5</v>
       </c>
       <c r="R13" s="4">
-        <v>5.2576863009813412E-5</v>
+        <v>5.2581159206018821E-5</v>
       </c>
       <c r="S13" s="4">
-        <v>5.3077126867236362E-5</v>
+        <v>5.3082228229300067E-5</v>
       </c>
       <c r="T13" s="4">
-        <v>5.3586049060219874E-5</v>
+        <v>5.3590934128752432E-5</v>
       </c>
       <c r="U13" s="4">
-        <v>5.4105334878616127E-5</v>
+        <v>5.4110456683056242E-5</v>
       </c>
       <c r="V13" s="4">
-        <v>5.4610539196817424E-5</v>
+        <v>5.4614996953739692E-5</v>
       </c>
       <c r="W13" s="4">
-        <v>5.5125025672775793E-5</v>
+        <v>5.5129609381114051E-5</v>
       </c>
       <c r="X13" s="4">
-        <v>5.5644352375924891E-5</v>
+        <v>5.5651209804066108E-5</v>
       </c>
       <c r="Y13" s="4">
-        <v>5.6164574587047429E-5</v>
+        <v>5.6171220337677975E-5</v>
       </c>
       <c r="Z13" s="4">
-        <v>5.6693978062907934E-5</v>
+        <v>5.6698732564004017E-5</v>
       </c>
       <c r="AA13" s="4">
-        <v>5.721493949673903E-5</v>
+        <v>5.7217304218088618E-5</v>
       </c>
       <c r="AB13" s="4">
-        <v>5.7733179456780447E-5</v>
+        <v>5.7733823061921899E-5</v>
       </c>
       <c r="AC13" s="4">
-        <v>5.8241709288023016E-5</v>
+        <v>5.8241543111285681E-5</v>
       </c>
       <c r="AD13" s="4">
-        <v>5.8749514404049965E-5</v>
+        <v>5.8747929790161759E-5</v>
       </c>
       <c r="AE13" s="4">
-        <v>5.9249763094548476E-5</v>
+        <v>5.9248827361253699E-5</v>
       </c>
       <c r="AF13" s="4">
-        <v>5.9740125588038328E-5</v>
+        <v>5.974092547844464E-5</v>
       </c>
       <c r="AG13" s="4">
-        <v>6.0224657388228372E-5</v>
+        <v>6.0225517946332457E-5</v>
       </c>
       <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
@@ -19585,119 +19585,119 @@
       </c>
       <c r="AP2" s="10">
         <f>BNVFE!E8</f>
-        <v>3.938977091004229E-4</v>
+        <v>3.9320167803958366E-4</v>
       </c>
       <c r="AQ2" s="10">
         <f>BNVFE!F8</f>
-        <v>4.0102815590911211E-4</v>
+        <v>4.005442502794511E-4</v>
       </c>
       <c r="AR2" s="10">
         <f>BNVFE!G8</f>
-        <v>4.0668872915977704E-4</v>
+        <v>4.0645945816058469E-4</v>
       </c>
       <c r="AS2" s="10">
         <f>BNVFE!H8</f>
-        <v>4.2148439524556525E-4</v>
+        <v>4.1828300792889542E-4</v>
       </c>
       <c r="AT2" s="10">
         <f>BNVFE!I8</f>
-        <v>4.2638034079782157E-4</v>
+        <v>4.2432642927896187E-4</v>
       </c>
       <c r="AU2" s="10">
         <f>BNVFE!J8</f>
-        <v>4.2993928617474374E-4</v>
+        <v>4.3013868224805557E-4</v>
       </c>
       <c r="AV2" s="10">
         <f>BNVFE!K8</f>
-        <v>4.4295232919176118E-4</v>
+        <v>4.4159741220930354E-4</v>
       </c>
       <c r="AW2" s="10">
         <f>BNVFE!L8</f>
-        <v>4.4402927119422075E-4</v>
+        <v>4.4283756012174485E-4</v>
       </c>
       <c r="AX2" s="10">
         <f>BNVFE!M8</f>
-        <v>4.4423001272194757E-4</v>
+        <v>4.4369894861174625E-4</v>
       </c>
       <c r="AY2" s="10">
         <f>BNVFE!N8</f>
-        <v>4.4444787060954387E-4</v>
+        <v>4.4433519283804937E-4</v>
       </c>
       <c r="AZ2" s="10">
         <f>BNVFE!O8</f>
-        <v>4.4510595798899477E-4</v>
+        <v>4.4502983096465825E-4</v>
       </c>
       <c r="BA2" s="10">
         <f>BNVFE!P8</f>
-        <v>4.4626178063197816E-4</v>
+        <v>4.4619804232655445E-4</v>
       </c>
       <c r="BB2" s="10">
         <f>BNVFE!Q8</f>
-        <v>4.4757258182247277E-4</v>
+        <v>4.4736157163053795E-4</v>
       </c>
       <c r="BC2" s="10">
         <f>BNVFE!R8</f>
-        <v>4.4919390205042781E-4</v>
+        <v>4.4858409986435515E-4</v>
       </c>
       <c r="BD2" s="10">
         <f>BNVFE!S8</f>
-        <v>4.5078104437884211E-4</v>
+        <v>4.5062348863147132E-4</v>
       </c>
       <c r="BE2" s="10">
         <f>BNVFE!T8</f>
-        <v>4.5211629450069859E-4</v>
+        <v>4.5195274509021602E-4</v>
       </c>
       <c r="BF2" s="10">
         <f>BNVFE!U8</f>
-        <v>4.5326957425061224E-4</v>
+        <v>4.524452263539576E-4</v>
       </c>
       <c r="BG2" s="10">
         <f>BNVFE!V8</f>
-        <v>4.5520696339484528E-4</v>
+        <v>4.5513787440342439E-4</v>
       </c>
       <c r="BH2" s="10">
         <f>BNVFE!W8</f>
-        <v>4.5553578115777672E-4</v>
+        <v>4.5560000309037107E-4</v>
       </c>
       <c r="BI2" s="10">
         <f>BNVFE!X8</f>
-        <v>4.5584944646724456E-4</v>
+        <v>4.5628219603308817E-4</v>
       </c>
       <c r="BJ2" s="10">
         <f>BNVFE!Y8</f>
-        <v>4.559561094704881E-4</v>
+        <v>4.5746355401689185E-4</v>
       </c>
       <c r="BK2" s="10">
         <f>BNVFE!Z8</f>
-        <v>4.5572121425237108E-4</v>
+        <v>4.577201565564958E-4</v>
       </c>
       <c r="BL2" s="10">
         <f>BNVFE!AA8</f>
-        <v>4.550985416964502E-4</v>
+        <v>4.5688423750485098E-4</v>
       </c>
       <c r="BM2" s="10">
         <f>BNVFE!AB8</f>
-        <v>4.5449905971852166E-4</v>
+        <v>4.5637498609098584E-4</v>
       </c>
       <c r="BN2" s="10">
         <f>BNVFE!AC8</f>
-        <v>4.5443664862698183E-4</v>
+        <v>4.5582206387129149E-4</v>
       </c>
       <c r="BO2" s="10">
         <f>BNVFE!AD8</f>
-        <v>4.5380063490385911E-4</v>
+        <v>4.5519749041800602E-4</v>
       </c>
       <c r="BP2" s="10">
         <f>BNVFE!AE8</f>
-        <v>4.5343326114607497E-4</v>
+        <v>4.5459553666078392E-4</v>
       </c>
       <c r="BQ2" s="10">
         <f>BNVFE!AF8</f>
-        <v>4.5494560422822621E-4</v>
+        <v>4.5420742164487069E-4</v>
       </c>
       <c r="BR2" s="10">
         <f>BNVFE!AG8</f>
-        <v>4.5447278785524218E-4</v>
+        <v>4.5366186695498144E-4</v>
       </c>
       <c r="BS2" s="10"/>
       <c r="BT2" s="4"/>
@@ -19735,59 +19735,59 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="4" cm="1">
         <f t="array" ref="AA3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AA1)</f>
-        <v>7.5108389563240119E-5</v>
+        <v>7.7947123371766881E-5</v>
       </c>
       <c r="AB3" s="4" cm="1">
         <f t="array" ref="AB3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AB1)</f>
-        <v>7.7552820431472588E-5</v>
+        <v>8.0186690650322842E-5</v>
       </c>
       <c r="AC3" s="4" cm="1">
         <f t="array" ref="AC3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AC1)</f>
-        <v>7.9997251299705058E-5</v>
+        <v>8.2426257928877936E-5</v>
       </c>
       <c r="AD3" s="4" cm="1">
         <f t="array" ref="AD3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AD1)</f>
-        <v>8.2441682167937527E-5</v>
+        <v>8.4665825207433897E-5</v>
       </c>
       <c r="AE3" s="4" cm="1">
         <f t="array" ref="AE3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AE1)</f>
-        <v>8.4886113036169997E-5</v>
+        <v>8.6905392485989857E-5</v>
       </c>
       <c r="AF3" s="4" cm="1">
         <f t="array" ref="AF3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AF1)</f>
-        <v>8.7330543904402466E-5</v>
+        <v>8.9144959764544951E-5</v>
       </c>
       <c r="AG3" s="4" cm="1">
         <f t="array" ref="AG3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AG1)</f>
-        <v>8.9774974772634936E-5</v>
+        <v>9.1384527043100912E-5</v>
       </c>
       <c r="AH3" s="4" cm="1">
         <f t="array" ref="AH3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AH1)</f>
-        <v>9.2219405640867405E-5</v>
+        <v>9.3624094321656005E-5</v>
       </c>
       <c r="AI3" s="4" cm="1">
         <f t="array" ref="AI3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AI1)</f>
-        <v>9.4663836509099875E-5</v>
+        <v>9.5863661600211966E-5</v>
       </c>
       <c r="AJ3" s="4" cm="1">
         <f t="array" ref="AJ3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AJ1)</f>
-        <v>9.7108267377332344E-5</v>
+        <v>9.810322887876706E-5</v>
       </c>
       <c r="AK3" s="4" cm="1">
         <f t="array" ref="AK3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AK1)</f>
-        <v>9.9552698245564814E-5</v>
+        <v>1.0034279615732302E-4</v>
       </c>
       <c r="AL3" s="4" cm="1">
         <f t="array" ref="AL3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AL1)</f>
-        <v>1.0199712911379728E-4</v>
+        <v>1.0258236343587811E-4</v>
       </c>
       <c r="AM3" s="4" cm="1">
         <f t="array" ref="AM3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AM1)</f>
-        <v>1.0444155998202975E-4</v>
+        <v>1.0482193071443408E-4</v>
       </c>
       <c r="AN3" s="26" cm="1">
         <f t="array" ref="AN3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AN1)</f>
-        <v>1.0688599085026222E-4</v>
+        <v>1.0706149799298917E-4</v>
       </c>
       <c r="AO3" s="10">
         <f>BNVFE!D9</f>
@@ -19795,119 +19795,119 @@
       </c>
       <c r="AP3" s="10">
         <f>BNVFE!E9</f>
-        <v>1.1376628742778099E-4</v>
+        <v>1.1340183318243619E-4</v>
       </c>
       <c r="AQ3" s="10">
         <f>BNVFE!F9</f>
-        <v>1.1487084665170681E-4</v>
+        <v>1.146278256602771E-4</v>
       </c>
       <c r="AR3" s="10">
         <f>BNVFE!G9</f>
-        <v>1.1675219072501874E-4</v>
+        <v>1.1598939507763969E-4</v>
       </c>
       <c r="AS3" s="10">
         <f>BNVFE!H9</f>
-        <v>1.1821814758141852E-4</v>
+        <v>1.1739300033405102E-4</v>
       </c>
       <c r="AT3" s="10">
         <f>BNVFE!I9</f>
-        <v>1.1769306557695523E-4</v>
+        <v>1.1760985601866623E-4</v>
       </c>
       <c r="AU3" s="10">
         <f>BNVFE!J9</f>
-        <v>1.1740735707916262E-4</v>
+        <v>1.1770623326767235E-4</v>
       </c>
       <c r="AV3" s="10">
         <f>BNVFE!K9</f>
-        <v>1.1551151797500483E-4</v>
+        <v>1.1580915845333066E-4</v>
       </c>
       <c r="AW3" s="10">
         <f>BNVFE!L9</f>
-        <v>1.1449785838376007E-4</v>
+        <v>1.1434896370073045E-4</v>
       </c>
       <c r="AX3" s="10">
         <f>BNVFE!M9</f>
-        <v>1.13287341804607E-4</v>
+        <v>1.1339009149021013E-4</v>
       </c>
       <c r="AY3" s="10">
         <f>BNVFE!N9</f>
-        <v>1.1212406398402511E-4</v>
+        <v>1.1219566215487321E-4</v>
       </c>
       <c r="AZ3" s="10">
         <f>BNVFE!O9</f>
-        <v>1.1076186329973974E-4</v>
+        <v>1.1066260788344435E-4</v>
       </c>
       <c r="BA3" s="10">
         <f>BNVFE!P9</f>
-        <v>1.0947685788155618E-4</v>
+        <v>1.093041603920123E-4</v>
       </c>
       <c r="BB3" s="10">
         <f>BNVFE!Q9</f>
-        <v>1.0833659526703707E-4</v>
+        <v>1.080839088666242E-4</v>
       </c>
       <c r="BC3" s="10">
         <f>BNVFE!R9</f>
-        <v>1.0725258337875167E-4</v>
+        <v>1.0723515259083896E-4</v>
       </c>
       <c r="BD3" s="10">
         <f>BNVFE!S9</f>
-        <v>1.0627237374881068E-4</v>
+        <v>1.0607167803261324E-4</v>
       </c>
       <c r="BE3" s="10">
         <f>BNVFE!T9</f>
-        <v>1.053872190542009E-4</v>
+        <v>1.0514634456433018E-4</v>
       </c>
       <c r="BF3" s="10">
         <f>BNVFE!U9</f>
-        <v>1.0457070988285631E-4</v>
+        <v>1.0424762201930517E-4</v>
       </c>
       <c r="BG3" s="10">
         <f>BNVFE!V9</f>
-        <v>1.0382785746559407E-4</v>
+        <v>1.0356841044901005E-4</v>
       </c>
       <c r="BH3" s="10">
         <f>BNVFE!W9</f>
-        <v>1.0317553743970813E-4</v>
+        <v>1.0310079801566161E-4</v>
       </c>
       <c r="BI3" s="10">
         <f>BNVFE!X9</f>
-        <v>1.0260660677729319E-4</v>
+        <v>1.0253359756446476E-4</v>
       </c>
       <c r="BJ3" s="10">
         <f>BNVFE!Y9</f>
-        <v>1.0212195692865432E-4</v>
+        <v>1.0217654907137221E-4</v>
       </c>
       <c r="BK3" s="10">
         <f>BNVFE!Z9</f>
-        <v>1.0164270384030296E-4</v>
+        <v>1.0162236577213031E-4</v>
       </c>
       <c r="BL3" s="10">
         <f>BNVFE!AA9</f>
-        <v>1.0120623842325044E-4</v>
+        <v>1.0123288850628106E-4</v>
       </c>
       <c r="BM3" s="10">
         <f>BNVFE!AB9</f>
-        <v>1.0086620530512349E-4</v>
+        <v>1.0091473811361892E-4</v>
       </c>
       <c r="BN3" s="10">
         <f>BNVFE!AC9</f>
-        <v>1.0054219744424832E-4</v>
+        <v>1.0075212418516603E-4</v>
       </c>
       <c r="BO3" s="10">
         <f>BNVFE!AD9</f>
-        <v>9.9850684341711718E-5</v>
+        <v>1.0011436735388883E-4</v>
       </c>
       <c r="BP3" s="10">
         <f>BNVFE!AE9</f>
-        <v>9.9621972535475967E-5</v>
+        <v>1.0002070036019407E-4</v>
       </c>
       <c r="BQ3" s="10">
         <f>BNVFE!AF9</f>
-        <v>9.9483752435656976E-5</v>
+        <v>9.9828102035601804E-5</v>
       </c>
       <c r="BR3" s="10">
         <f>BNVFE!AG9</f>
-        <v>9.9383928406132565E-5</v>
+        <v>9.9636624901656103E-5</v>
       </c>
       <c r="BS3" s="10"/>
       <c r="BT3" s="4"/>
@@ -20050,119 +20050,119 @@
       </c>
       <c r="AP4" s="10">
         <f>BNVFE!E10</f>
-        <v>1.1868928349938494E-3</v>
+        <v>1.1925426392408319E-3</v>
       </c>
       <c r="AQ4" s="10">
         <f>BNVFE!F10</f>
-        <v>1.2242021544325342E-3</v>
+        <v>1.2281409269793643E-3</v>
       </c>
       <c r="AR4" s="10">
         <f>BNVFE!G10</f>
-        <v>1.2625148116111296E-3</v>
+        <v>1.2637392147178965E-3</v>
       </c>
       <c r="AS4" s="10">
         <f>BNVFE!H10</f>
-        <v>1.2984724640643824E-3</v>
+        <v>1.2993375024564287E-3</v>
       </c>
       <c r="AT4" s="10">
         <f>BNVFE!I10</f>
-        <v>1.3325458991476347E-3</v>
+        <v>1.3349357901949611E-3</v>
       </c>
       <c r="AU4" s="10">
         <f>BNVFE!J10</f>
-        <v>1.3625499159680566E-3</v>
+        <v>1.3705340779334933E-3</v>
       </c>
       <c r="AV4" s="10">
         <f>BNVFE!K10</f>
-        <v>1.3753174198569201E-3</v>
+        <v>1.3705340779334933E-3</v>
       </c>
       <c r="AW4" s="10">
         <f>BNVFE!L10</f>
-        <v>1.3946841343267524E-3</v>
+        <v>1.3883332218027598E-3</v>
       </c>
       <c r="AX4" s="10">
         <f>BNVFE!M10</f>
-        <v>1.4146533498165595E-3</v>
+        <v>1.4061323656720257E-3</v>
       </c>
       <c r="AY4" s="10">
         <f>BNVFE!N10</f>
-        <v>1.4334182752321722E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="AZ4" s="10">
         <f>BNVFE!O10</f>
-        <v>1.4445909758303492E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BA4" s="10">
         <f>BNVFE!P10</f>
-        <v>1.4455847020325701E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BB4" s="10">
         <f>BNVFE!Q10</f>
-        <v>1.4457021763821076E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BC4" s="10">
         <f>BNVFE!R10</f>
-        <v>1.4456854451868699E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BD4" s="10">
         <f>BNVFE!S10</f>
-        <v>1.4457034223221783E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BE4" s="10">
         <f>BNVFE!T10</f>
-        <v>1.4456555426251702E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BF4" s="10">
         <f>BNVFE!U10</f>
-        <v>1.4455629870770495E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BG4" s="10">
         <f>BNVFE!V10</f>
-        <v>1.4452171497116701E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BH4" s="10">
         <f>BNVFE!W10</f>
-        <v>1.4450916657473916E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BI4" s="10">
         <f>BNVFE!X10</f>
-        <v>1.4448529792281048E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BJ4" s="10">
         <f>BNVFE!Y10</f>
-        <v>1.443856049179987E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BK4" s="10">
         <f>BNVFE!Z10</f>
-        <v>1.4432142120520614E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BL4" s="10">
         <f>BNVFE!AA10</f>
-        <v>1.443266541535037E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BM4" s="10">
         <f>BNVFE!AB10</f>
-        <v>1.4434251319069122E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BN4" s="10">
         <f>BNVFE!AC10</f>
-        <v>1.4437811147842976E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BO4" s="10">
         <f>BNVFE!AD10</f>
-        <v>1.4442054463741406E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BP4" s="10">
         <f>BNVFE!AE10</f>
-        <v>1.4447501001765403E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BQ4" s="10">
         <f>BNVFE!AF10</f>
-        <v>1.4451804834752992E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BR4" s="10">
         <f>BNVFE!AG10</f>
-        <v>1.4456904289471535E-3</v>
+        <v>1.4417306534105579E-3</v>
       </c>
       <c r="BS4" s="10"/>
       <c r="BT4" s="4"/>
@@ -20305,119 +20305,119 @@
       </c>
       <c r="AP5" s="10">
         <f>BNVFE!E11</f>
-        <v>7.8447318350072194E-4</v>
+        <v>7.8820740431081668E-4</v>
       </c>
       <c r="AQ5" s="10">
         <f>BNVFE!F11</f>
-        <v>8.0913266389472246E-4</v>
+        <v>8.1173598354397538E-4</v>
       </c>
       <c r="AR5" s="10">
         <f>BNVFE!G11</f>
-        <v>8.3445529729440947E-4</v>
+        <v>8.3526456277713398E-4</v>
       </c>
       <c r="AS5" s="10">
         <f>BNVFE!H11</f>
-        <v>8.582213975349269E-4</v>
+        <v>8.5879314201029269E-4</v>
       </c>
       <c r="AT5" s="10">
         <f>BNVFE!I11</f>
-        <v>8.8074213007663328E-4</v>
+        <v>8.823217212434515E-4</v>
       </c>
       <c r="AU5" s="10">
         <f>BNVFE!J11</f>
-        <v>9.0057319308330108E-4</v>
+        <v>9.058503004766101E-4</v>
       </c>
       <c r="AV5" s="10">
         <f>BNVFE!K11</f>
-        <v>9.0901183566816969E-4</v>
+        <v>9.058503004766101E-4</v>
       </c>
       <c r="AW5" s="10">
         <f>BNVFE!L11</f>
-        <v>9.2181220627128113E-4</v>
+        <v>9.1761459009318956E-4</v>
       </c>
       <c r="AX5" s="10">
         <f>BNVFE!M11</f>
-        <v>9.3501079807791388E-4</v>
+        <v>9.2937887970976892E-4</v>
       </c>
       <c r="AY5" s="10">
         <f>BNVFE!N11</f>
-        <v>9.4741341804908898E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="AZ5" s="10">
         <f>BNVFE!O11</f>
-        <v>9.5479798028431191E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BA5" s="10">
         <f>BNVFE!P11</f>
-        <v>9.5545478057360543E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BB5" s="10">
         <f>BNVFE!Q11</f>
-        <v>9.5553242488507497E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BC5" s="10">
         <f>BNVFE!R11</f>
-        <v>9.5552136645283517E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BD5" s="10">
         <f>BNVFE!S11</f>
-        <v>9.5553324838534815E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BE5" s="10">
         <f>BNVFE!T11</f>
-        <v>9.5550160244627959E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BF5" s="10">
         <f>BNVFE!U11</f>
-        <v>9.5544042814027313E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BG5" s="10">
         <f>BNVFE!V11</f>
-        <v>9.5521184799302321E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BH5" s="10">
         <f>BNVFE!W11</f>
-        <v>9.5512890975122625E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BI5" s="10">
         <f>BNVFE!X11</f>
-        <v>9.5497115062746795E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BJ5" s="10">
         <f>BNVFE!Y11</f>
-        <v>9.5431223276604333E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BK5" s="10">
         <f>BNVFE!Z11</f>
-        <v>9.5388801248246955E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BL5" s="10">
         <f>BNVFE!AA11</f>
-        <v>9.5392259949394229E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BM5" s="10">
         <f>BNVFE!AB11</f>
-        <v>9.5402741931442593E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BN5" s="10">
         <f>BNVFE!AC11</f>
-        <v>9.5426270510675759E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BO5" s="10">
         <f>BNVFE!AD11</f>
-        <v>9.5454316577121671E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BP5" s="10">
         <f>BNVFE!AE11</f>
-        <v>9.5490315303348411E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BQ5" s="10">
         <f>BNVFE!AF11</f>
-        <v>9.5518761355641295E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BR5" s="10">
         <f>BNVFE!AG11</f>
-        <v>9.555246604539279E-4</v>
+        <v>9.5290745894292751E-4</v>
       </c>
       <c r="BS5" s="10"/>
       <c r="BT5" s="4"/>
@@ -20687,103 +20687,103 @@
       <c r="O7" s="9"/>
       <c r="P7" s="4">
         <f>TREND($AO7:$BR7,$AO$1:$BR$1,P$1)-($AR7-$AO7)</f>
-        <v>3.6038411832808568E-5</v>
+        <v>3.6038260344938299E-5</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" ref="Q7:AN7" si="5">TREND($AO7:$BR7,$AO$1:$BR$1,Q$1)-($AR7-$AO7)</f>
-        <v>3.647844074325616E-5</v>
+        <v>3.6478359505012103E-5</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="5"/>
-        <v>3.6918469653703644E-5</v>
+        <v>3.6918458665085799E-5</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="5"/>
-        <v>3.7358498564151237E-5</v>
+        <v>3.7358557825159494E-5</v>
       </c>
       <c r="T7" s="4">
         <f t="shared" si="5"/>
-        <v>3.7798527474598721E-5</v>
+        <v>3.7798656985233299E-5</v>
       </c>
       <c r="U7" s="4">
         <f t="shared" si="5"/>
-        <v>3.8238556385046314E-5</v>
+        <v>3.8238756145306995E-5</v>
       </c>
       <c r="V7" s="4">
         <f t="shared" si="5"/>
-        <v>3.8678585295493906E-5</v>
+        <v>3.867885530538069E-5</v>
       </c>
       <c r="W7" s="4">
         <f t="shared" si="5"/>
-        <v>3.9118614205941391E-5</v>
+        <v>3.9118954465454495E-5</v>
       </c>
       <c r="X7" s="4">
         <f t="shared" si="5"/>
-        <v>3.9558643116388983E-5</v>
+        <v>3.955905362552819E-5</v>
       </c>
       <c r="Y7" s="4">
         <f t="shared" si="5"/>
-        <v>3.9998672026836467E-5</v>
+        <v>3.9999152785601886E-5</v>
       </c>
       <c r="Z7" s="4">
         <f t="shared" si="5"/>
-        <v>4.043870093728406E-5</v>
+        <v>4.0439251945675691E-5</v>
       </c>
       <c r="AA7" s="4">
         <f t="shared" si="5"/>
-        <v>4.0878729847731653E-5</v>
+        <v>4.0879351105749386E-5</v>
       </c>
       <c r="AB7" s="4">
         <f t="shared" si="5"/>
-        <v>4.1318758758179137E-5</v>
+        <v>4.1319450265823082E-5</v>
       </c>
       <c r="AC7" s="4">
         <f t="shared" si="5"/>
-        <v>4.1758787668626729E-5</v>
+        <v>4.1759549425896887E-5</v>
       </c>
       <c r="AD7" s="4">
         <f t="shared" si="5"/>
-        <v>4.2198816579074322E-5</v>
+        <v>4.2199648585970582E-5</v>
       </c>
       <c r="AE7" s="4">
         <f t="shared" si="5"/>
-        <v>4.2638845489521806E-5</v>
+        <v>4.2639747746044278E-5</v>
       </c>
       <c r="AF7" s="4">
         <f t="shared" si="5"/>
-        <v>4.3078874399969399E-5</v>
+        <v>4.3079846906117974E-5</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
-        <v>4.3518903310416883E-5</v>
+        <v>4.3519946066191778E-5</v>
       </c>
       <c r="AH7" s="4">
         <f t="shared" si="5"/>
-        <v>4.3958932220864476E-5</v>
+        <v>4.3960045226265474E-5</v>
       </c>
       <c r="AI7" s="4">
         <f t="shared" si="5"/>
-        <v>4.4398961131312068E-5</v>
+        <v>4.440014438633917E-5</v>
       </c>
       <c r="AJ7" s="4">
         <f t="shared" si="5"/>
-        <v>4.4838990041759552E-5</v>
+        <v>4.4840243546412974E-5</v>
       </c>
       <c r="AK7" s="4">
         <f t="shared" si="5"/>
-        <v>4.5279018952207145E-5</v>
+        <v>4.528034270648667E-5</v>
       </c>
       <c r="AL7" s="4">
         <f t="shared" si="5"/>
-        <v>4.5719047862654629E-5</v>
+        <v>4.5720441866560366E-5</v>
       </c>
       <c r="AM7" s="4">
         <f t="shared" si="5"/>
-        <v>4.6159076773102222E-5</v>
+        <v>4.616054102663417E-5</v>
       </c>
       <c r="AN7" s="26">
         <f t="shared" si="5"/>
-        <v>4.6599105683549815E-5</v>
+        <v>4.6600640186707866E-5</v>
       </c>
       <c r="AO7" s="10">
         <f>BNVFE!D13</f>
@@ -20795,115 +20795,115 @@
       </c>
       <c r="AQ7" s="10">
         <f>BNVFE!F13</f>
-        <v>4.8199148542133818E-5</v>
+        <v>4.8199163709058256E-5</v>
       </c>
       <c r="AR7" s="10">
         <f>BNVFE!G13</f>
-        <v>4.8463289763291303E-5</v>
+        <v>4.8462484597433007E-5</v>
       </c>
       <c r="AS7" s="10">
         <f>BNVFE!H13</f>
-        <v>4.8810101273548841E-5</v>
+        <v>4.8807912620409042E-5</v>
       </c>
       <c r="AT7" s="10">
         <f>BNVFE!I13</f>
-        <v>4.9248402309752346E-5</v>
+        <v>4.9249126365536466E-5</v>
       </c>
       <c r="AU7" s="10">
         <f>BNVFE!J13</f>
-        <v>4.9544253613324154E-5</v>
+        <v>4.9546819461280452E-5</v>
       </c>
       <c r="AV7" s="10">
         <f>BNVFE!K13</f>
-        <v>4.9847838070065696E-5</v>
+        <v>4.985094728957582E-5</v>
       </c>
       <c r="AW7" s="10">
         <f>BNVFE!L13</f>
-        <v>5.0132631366857999E-5</v>
+        <v>5.0135212381738722E-5</v>
       </c>
       <c r="AX7" s="10">
         <f>BNVFE!M13</f>
-        <v>5.0441473470928121E-5</v>
+        <v>5.0441951558763717E-5</v>
       </c>
       <c r="AY7" s="10">
         <f>BNVFE!N13</f>
-        <v>5.0785598457265348E-5</v>
+        <v>5.0784808458331483E-5</v>
       </c>
       <c r="AZ7" s="10">
         <f>BNVFE!O13</f>
-        <v>5.1172517250624796E-5</v>
+        <v>5.1171299280649147E-5</v>
       </c>
       <c r="BA7" s="10">
         <f>BNVFE!P13</f>
-        <v>5.161151266819503E-5</v>
+        <v>5.1611160531775431E-5</v>
       </c>
       <c r="BB7" s="10">
         <f>BNVFE!Q13</f>
-        <v>5.2082892766601423E-5</v>
+        <v>5.2084633665754489E-5</v>
       </c>
       <c r="BC7" s="10">
         <f>BNVFE!R13</f>
-        <v>5.2576863009813412E-5</v>
+        <v>5.2581159206018821E-5</v>
       </c>
       <c r="BD7" s="10">
         <f>BNVFE!S13</f>
-        <v>5.3077126867236362E-5</v>
+        <v>5.3082228229300067E-5</v>
       </c>
       <c r="BE7" s="10">
         <f>BNVFE!T13</f>
-        <v>5.3586049060219874E-5</v>
+        <v>5.3590934128752432E-5</v>
       </c>
       <c r="BF7" s="10">
         <f>BNVFE!U13</f>
-        <v>5.4105334878616127E-5</v>
+        <v>5.4110456683056242E-5</v>
       </c>
       <c r="BG7" s="10">
         <f>BNVFE!V13</f>
-        <v>5.4610539196817424E-5</v>
+        <v>5.4614996953739692E-5</v>
       </c>
       <c r="BH7" s="10">
         <f>BNVFE!W13</f>
-        <v>5.5125025672775793E-5</v>
+        <v>5.5129609381114051E-5</v>
       </c>
       <c r="BI7" s="10">
         <f>BNVFE!X13</f>
-        <v>5.5644352375924891E-5</v>
+        <v>5.5651209804066108E-5</v>
       </c>
       <c r="BJ7" s="10">
         <f>BNVFE!Y13</f>
-        <v>5.6164574587047429E-5</v>
+        <v>5.6171220337677975E-5</v>
       </c>
       <c r="BK7" s="10">
         <f>BNVFE!Z13</f>
-        <v>5.6693978062907934E-5</v>
+        <v>5.6698732564004017E-5</v>
       </c>
       <c r="BL7" s="10">
         <f>BNVFE!AA13</f>
-        <v>5.721493949673903E-5</v>
+        <v>5.7217304218088618E-5</v>
       </c>
       <c r="BM7" s="10">
         <f>BNVFE!AB13</f>
-        <v>5.7733179456780447E-5</v>
+        <v>5.7733823061921899E-5</v>
       </c>
       <c r="BN7" s="10">
         <f>BNVFE!AC13</f>
-        <v>5.8241709288023016E-5</v>
+        <v>5.8241543111285681E-5</v>
       </c>
       <c r="BO7" s="10">
         <f>BNVFE!AD13</f>
-        <v>5.8749514404049965E-5</v>
+        <v>5.8747929790161759E-5</v>
       </c>
       <c r="BP7" s="10">
         <f>BNVFE!AE13</f>
-        <v>5.9249763094548476E-5</v>
+        <v>5.9248827361253699E-5</v>
       </c>
       <c r="BQ7" s="10">
         <f>BNVFE!AF13</f>
-        <v>5.9740125588038328E-5</v>
+        <v>5.974092547844464E-5</v>
       </c>
       <c r="BR7" s="10">
         <f>BNVFE!AG13</f>
-        <v>6.0224657388228372E-5</v>
+        <v>6.0225517946332457E-5</v>
       </c>
       <c r="BS7" s="10"/>
       <c r="BT7" s="4"/>
@@ -23022,67 +23022,67 @@
       </c>
       <c r="P3" s="4">
         <f>BNVFE!P25*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.6148257419113056E-4</v>
+        <v>3.6084382181005237E-4</v>
       </c>
       <c r="Q3" s="4">
         <f>BNVFE!Q25*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.664339997180947E-4</v>
+        <v>3.6599183755878001E-4</v>
       </c>
       <c r="R3" s="4">
         <f>BNVFE!R25*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.7106858296827262E-4</v>
+        <v>3.7085939284647651E-4</v>
       </c>
       <c r="S3" s="4">
         <f>BNVFE!S25*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.8411030958242069E-4</v>
+        <v>3.8119279736329608E-4</v>
       </c>
       <c r="T3" s="4">
         <f>BNVFE!T25*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.8812122876113119E-4</v>
+        <v>3.8625161474240119E-4</v>
       </c>
       <c r="U3" s="4">
         <f>BNVFE!U25*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.9150340258291803E-4</v>
+        <v>3.9168497296662925E-4</v>
       </c>
       <c r="V3" s="4">
         <f>BNVFE!V25*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>4.03112372133042E-4</v>
+        <v>4.0187931890621188E-4</v>
       </c>
       <c r="W3" s="4">
         <f>BNVFE!W25*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.0360787000657248E-4</v>
+        <v>4.0252464419505865E-4</v>
       </c>
       <c r="X3" s="4">
         <f>BNVFE!X25*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.0382283711848821E-4</v>
+        <v>4.0334007861606453E-4</v>
       </c>
       <c r="Y3" s="4">
         <f>BNVFE!Y25*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.0343001609921412E-4</v>
+        <v>4.0332773729854013E-4</v>
       </c>
       <c r="Z3" s="4">
         <f>BNVFE!Z25*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.0399408750656777E-4</v>
+        <v>4.0392499189645641E-4</v>
       </c>
       <c r="AA3" s="4">
         <f>BNVFE!AA25*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.0250398522270639E-4</v>
+        <v>4.0244649671919154E-4</v>
       </c>
       <c r="AB3" s="4">
         <f>BNVFE!AB25*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.0381262204317188E-4</v>
+        <v>4.036222426894231E-4</v>
       </c>
       <c r="AC3" s="4">
         <f>BNVFE!AC25*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.0464211986551089E-4</v>
+        <v>4.0409279885259258E-4</v>
       </c>
       <c r="AD3" s="4">
         <f>BNVFE!AD25*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.061398198412998E-4</v>
+        <v>4.0599786697160823E-4</v>
       </c>
       <c r="AE3" s="4">
         <f>BNVFE!AE25*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.0676965949352643E-4</v>
+        <v>4.0662251386125979E-4</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -23149,67 +23149,67 @@
       </c>
       <c r="P4" s="4">
         <f>Extrapolations!AP2</f>
-        <v>3.938977091004229E-4</v>
+        <v>3.9320167803958366E-4</v>
       </c>
       <c r="Q4" s="4">
         <f>Extrapolations!AQ2</f>
-        <v>4.0102815590911211E-4</v>
+        <v>4.005442502794511E-4</v>
       </c>
       <c r="R4" s="4">
         <f>Extrapolations!AR2</f>
-        <v>4.0668872915977704E-4</v>
+        <v>4.0645945816058469E-4</v>
       </c>
       <c r="S4" s="4">
         <f>Extrapolations!AS2</f>
-        <v>4.2148439524556525E-4</v>
+        <v>4.1828300792889542E-4</v>
       </c>
       <c r="T4" s="4">
         <f>Extrapolations!AT2</f>
-        <v>4.2638034079782157E-4</v>
+        <v>4.2432642927896187E-4</v>
       </c>
       <c r="U4" s="4">
         <f>Extrapolations!AU2</f>
-        <v>4.2993928617474374E-4</v>
+        <v>4.3013868224805557E-4</v>
       </c>
       <c r="V4" s="4">
         <f>Extrapolations!AV2</f>
-        <v>4.4295232919176118E-4</v>
+        <v>4.4159741220930354E-4</v>
       </c>
       <c r="W4" s="4">
         <f>Extrapolations!AW2</f>
-        <v>4.4402927119422075E-4</v>
+        <v>4.4283756012174485E-4</v>
       </c>
       <c r="X4" s="4">
         <f>Extrapolations!AX2</f>
-        <v>4.4423001272194757E-4</v>
+        <v>4.4369894861174625E-4</v>
       </c>
       <c r="Y4" s="4">
         <f>Extrapolations!AY2</f>
-        <v>4.4444787060954387E-4</v>
+        <v>4.4433519283804937E-4</v>
       </c>
       <c r="Z4" s="4">
         <f>Extrapolations!AZ2</f>
-        <v>4.4510595798899477E-4</v>
+        <v>4.4502983096465825E-4</v>
       </c>
       <c r="AA4" s="4">
         <f>Extrapolations!BA2</f>
-        <v>4.4626178063197816E-4</v>
+        <v>4.4619804232655445E-4</v>
       </c>
       <c r="AB4" s="4">
         <f>Extrapolations!BB2</f>
-        <v>4.4757258182247277E-4</v>
+        <v>4.4736157163053795E-4</v>
       </c>
       <c r="AC4" s="4">
         <f>Extrapolations!BC2</f>
-        <v>4.4919390205042781E-4</v>
+        <v>4.4858409986435515E-4</v>
       </c>
       <c r="AD4" s="4">
         <f>Extrapolations!BD2</f>
-        <v>4.5078104437884211E-4</v>
+        <v>4.5062348863147132E-4</v>
       </c>
       <c r="AE4" s="4">
         <f>Extrapolations!BE2</f>
-        <v>4.5211629450069859E-4</v>
+        <v>4.5195274509021602E-4</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -23276,67 +23276,67 @@
       </c>
       <c r="P5" s="4">
         <f>BNVFE!P27*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.5586083055954025E-4</v>
+        <v>3.5523201199654035E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>BNVFE!Q27*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.6129198091988776E-4</v>
+        <v>3.6085602344173472E-4</v>
       </c>
       <c r="R5" s="4">
         <f>BNVFE!R27*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.6638008253103504E-4</v>
+        <v>3.6617353555399044E-4</v>
       </c>
       <c r="S5" s="4">
         <f>BNVFE!S27*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.797656838426424E-4</v>
+        <v>3.7688117125504842E-4</v>
       </c>
       <c r="T5" s="4">
         <f>BNVFE!T27*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.8379386561392104E-4</v>
+        <v>3.8194509688322124E-4</v>
       </c>
       <c r="U5" s="4">
         <f>BNVFE!U27*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.8757523740699085E-4</v>
+        <v>3.8775498599693582E-4</v>
       </c>
       <c r="V5" s="4">
         <f>BNVFE!V27*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.9950134420415153E-4</v>
+        <v>3.9827933650692478E-4</v>
       </c>
       <c r="W5" s="4">
         <f>BNVFE!W27*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.0035850605750056E-4</v>
+        <v>3.9928400107420195E-4</v>
       </c>
       <c r="X5" s="4">
         <f>BNVFE!X27*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.0109394743594799E-4</v>
+        <v>4.0061445124207976E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>BNVFE!Y27*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.012761936991058E-4</v>
+        <v>4.0117446094201597E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>BNVFE!Z27*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.0222683786844709E-4</v>
+        <v>4.0215804451323436E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>BNVFE!AA27*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.0134683501182901E-4</v>
+        <v>4.0128951178079942E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>BNVFE!AB27*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.0302096346638407E-4</v>
+        <v>4.0283095734378266E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>BNVFE!AC27*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.0423921136844502E-4</v>
+        <v>4.0369043732306389E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>BNVFE!AD27*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.0550880062563649E-4</v>
+        <v>4.0536706830804082E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>BNVFE!AE27*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.0641720967975257E-4</v>
+        <v>4.0627019154335358E-4</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -23403,67 +23403,67 @@
       </c>
       <c r="P6" s="4">
         <f>BNVFE!P28*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>5.4302083063339991E-4</v>
+        <v>5.4206129378900759E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>BNVFE!Q28*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>5.522766833965494E-4</v>
+        <v>5.5161027184342474E-4</v>
       </c>
       <c r="R6" s="4">
         <f>BNVFE!R28*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>5.601254580107081E-4</v>
+        <v>5.5980968696955707E-4</v>
       </c>
       <c r="S6" s="4">
         <f>BNVFE!S28*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>5.807089207832928E-4</v>
+        <v>5.7629814260349915E-4</v>
       </c>
       <c r="T6" s="4">
         <f>BNVFE!T28*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>5.8731627063682789E-4</v>
+        <v>5.8448711662091439E-4</v>
       </c>
       <c r="U6" s="4">
         <f>BNVFE!U28*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>5.931554855531328E-4</v>
+        <v>5.9343057759167386E-4</v>
       </c>
       <c r="V6" s="4">
         <f>BNVFE!V28*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>6.1114222360517459E-4</v>
+        <v>6.0927284190676371E-4</v>
       </c>
       <c r="W6" s="4">
         <f>BNVFE!W28*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>6.1263586196471168E-4</v>
+        <v>6.1099163491153661E-4</v>
       </c>
       <c r="X6" s="4">
         <f>BNVFE!X28*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>6.1341880221425316E-4</v>
+        <v>6.1268547780786605E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>BNVFE!Y28*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>6.1418182638870312E-4</v>
+        <v>6.1402611715019335E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>BNVFE!Z28*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>6.1565016430071618E-4</v>
+        <v>6.1554486888914216E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>BNVFE!AA28*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>6.1529793989050126E-4</v>
+        <v>6.1521005862949832E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>BNVFE!AB28*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>6.1772279652446511E-4</v>
+        <v>6.1743156821613928E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>BNVFE!AC28*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>6.2010047833741867E-4</v>
+        <v>6.1925866230752883E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>BNVFE!AD28*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>6.2160289507864192E-4</v>
+        <v>6.2138563414914358E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>BNVFE!AE28*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>6.234661580070439E-4</v>
+        <v>6.2324062417020104E-4</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -23530,67 +23530,67 @@
       </c>
       <c r="P7" s="4">
         <f>BNVFE!P29*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.2850767173068688E-4</v>
+        <v>3.2792718715825633E-4</v>
       </c>
       <c r="Q7" s="4">
         <f>BNVFE!Q29*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3335716351672539E-4</v>
+        <v>3.3295491393465338E-4</v>
       </c>
       <c r="R7" s="4">
         <f>BNVFE!R29*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.3778444703873312E-4</v>
+        <v>3.3759402086723777E-4</v>
       </c>
       <c r="S7" s="4">
         <f>BNVFE!S29*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.4986487595933905E-4</v>
+        <v>3.4720747514194476E-4</v>
       </c>
       <c r="T7" s="4">
         <f>BNVFE!T29*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.534107056332161E-4</v>
+        <v>3.5170829525043397E-4</v>
       </c>
       <c r="U7" s="4">
         <f>BNVFE!U29*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.5662399303793859E-4</v>
+        <v>3.5678938714391397E-4</v>
       </c>
       <c r="V7" s="4">
         <f>BNVFE!V29*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.6721085010863982E-4</v>
+        <v>3.6608761362433745E-4</v>
       </c>
       <c r="W7" s="4">
         <f>BNVFE!W29*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.6762499919934348E-4</v>
+        <v>3.6663834626791286E-4</v>
       </c>
       <c r="X7" s="4">
         <f>BNVFE!X29*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.6773337479207668E-4</v>
+        <v>3.6729376019629852E-4</v>
       </c>
       <c r="Y7" s="4">
         <f>BNVFE!Y29*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.6736921672179983E-4</v>
+        <v>3.6727608016430183E-4</v>
       </c>
       <c r="Z7" s="4">
         <f>BNVFE!Z29*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.6772730994967127E-4</v>
+        <v>3.6766441709152974E-4</v>
       </c>
       <c r="AA7" s="4">
         <f>BNVFE!AA29*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.6618194153426438E-4</v>
+        <v>3.6612964080531309E-4</v>
       </c>
       <c r="AB7" s="4">
         <f>BNVFE!AB29*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.6737880391439015E-4</v>
+        <v>3.672056014550011E-4</v>
       </c>
       <c r="AC7" s="4">
         <f>BNVFE!AC29*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.6808897076111757E-4</v>
+        <v>3.6758927239474449E-4</v>
       </c>
       <c r="AD7" s="4">
         <f>BNVFE!AD29*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.6878469932448562E-4</v>
+        <v>3.6865580271349118E-4</v>
       </c>
       <c r="AE7" s="4">
         <f>BNVFE!AE29*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.6920309090080676E-4</v>
+        <v>3.6906953467069598E-4</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>

</xml_diff>

<commit_message>
Corrections to freight fuel economy values
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\BHNVFEAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BBB26-2C5B-4C09-BC97-E4961155787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F0C145-5EB0-4280-9DA6-AA87E9CED957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3232,136 +3232,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>7.5108389563240119E-5</c:v>
+                  <c:v>5.0412726378568952E-5</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>7.7552820431472588E-5</c:v>
+                  <c:v>5.4271492176534604E-5</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.9997251299705058E-5</c:v>
+                  <c:v>5.8130257974500256E-5</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>8.2441682167937527E-5</c:v>
+                  <c:v>6.1989023772465041E-5</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>8.4886113036169997E-5</c:v>
+                  <c:v>6.5847789570430693E-5</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>8.7330543904402466E-5</c:v>
+                  <c:v>6.9706555368396345E-5</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>8.9774974772634936E-5</c:v>
+                  <c:v>7.3565321166361129E-5</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>9.2219405640867405E-5</c:v>
+                  <c:v>7.7424086964326781E-5</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>9.4663836509099875E-5</c:v>
+                  <c:v>8.1282852762291566E-5</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>9.7108267377332344E-5</c:v>
+                  <c:v>8.5141618560257218E-5</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>9.9552698245564814E-5</c:v>
+                  <c:v>8.900038435822287E-5</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>1.0199712911379728E-4</c:v>
+                  <c:v>9.2859150156187655E-5</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>1.0444155998202975E-4</c:v>
+                  <c:v>9.6717915954153307E-5</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>1.0688599085026222E-4</c:v>
+                  <c:v>1.0057668175211809E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>1.0748894488887501E-4</c:v>
+                  <c:v>1.0420515928406728E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>1.1376628742778099E-4</c:v>
+                  <c:v>1.0877081887028839E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>1.1487084665170681E-4</c:v>
+                  <c:v>1.119228749342E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>1.1675219072501874E-4</c:v>
+                  <c:v>1.1596328986495364E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>1.1821814758141852E-4</c:v>
+                  <c:v>1.1990275277656129E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>1.1769306557695523E-4</c:v>
+                  <c:v>1.2199635295884858E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>1.1740735707916262E-4</c:v>
+                  <c:v>1.243467097653028E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>1.1551151797500483E-4</c:v>
+                  <c:v>1.2468075205096364E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>1.1449785838376007E-4</c:v>
+                  <c:v>1.2577381385553893E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.13287341804607E-4</c:v>
+                  <c:v>1.2646319222836433E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>1.1212406398402511E-4</c:v>
+                  <c:v>1.2698406877407795E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.1076186329973974E-4</c:v>
+                  <c:v>1.2710494044541212E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>1.0947685788155618E-4</c:v>
+                  <c:v>1.2713124547346271E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>1.0833659526703707E-4</c:v>
+                  <c:v>1.2714496314152464E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>1.0725258337875167E-4</c:v>
+                  <c:v>1.2712313200368365E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>1.0627237374881068E-4</c:v>
+                  <c:v>1.271005238267318E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>1.053872190542009E-4</c:v>
+                  <c:v>1.2708001023750603E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>1.0457070988285631E-4</c:v>
+                  <c:v>1.2705407014004141E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>1.0382785746559407E-4</c:v>
+                  <c:v>1.2702629811717708E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>1.0317553743970813E-4</c:v>
+                  <c:v>1.2701194080551808E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>1.0260660677729319E-4</c:v>
+                  <c:v>1.2701796387221964E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.0212195692865432E-4</c:v>
+                  <c:v>1.2701802056749482E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.0164270384030296E-4</c:v>
+                  <c:v>1.270327910946451E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.0120623842325044E-4</c:v>
+                  <c:v>1.2702817221538397E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.0086620530512349E-4</c:v>
+                  <c:v>1.2698131801807758E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>1.0054219744424832E-4</c:v>
+                  <c:v>1.2695571200958938E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>9.9850684341711718E-5</c:v>
+                  <c:v>1.2640538596243631E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>9.9621972535475967E-5</c:v>
+                  <c:v>1.2643551327178303E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>9.9483752435656976E-5</c:v>
+                  <c:v>1.2650241733350927E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>9.9383928406132565E-5</c:v>
+                  <c:v>1.2663654108394285E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3695,91 +3695,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1.1807374066651307E-3</c:v>
+                  <c:v>1.1628806678959742E-3</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>1.177387347221569E-3</c:v>
+                  <c:v>1.1604234453908705E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.1740372877780075E-3</c:v>
+                  <c:v>1.1579662228857668E-3</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>1.1706872283344459E-3</c:v>
+                  <c:v>1.1555090003806633E-3</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.1673371688908844E-3</c:v>
+                  <c:v>1.1530517778755595E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1.163987109447323E-3</c:v>
+                  <c:v>1.1505945553704558E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.1606370500037615E-3</c:v>
+                  <c:v>1.1481373328653521E-3</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>1.1572869905602E-3</c:v>
+                  <c:v>1.1456801103602485E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>1.1539369311166386E-3</c:v>
+                  <c:v>1.1432228878551448E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>1.1505868716730771E-3</c:v>
+                  <c:v>1.1407656653500411E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>1.1472368122295155E-3</c:v>
+                  <c:v>1.1383084428449376E-3</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>1.143886752785954E-3</c:v>
+                  <c:v>1.1358512203398338E-3</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>1.1405366933423926E-3</c:v>
+                  <c:v>1.1333939978347303E-3</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>1.1371866338988309E-3</c:v>
+                  <c:v>1.1309367753296266E-3</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>1.1338365744552694E-3</c:v>
+                  <c:v>1.1284795528245229E-3</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>1.130486515011708E-3</c:v>
+                  <c:v>1.1260223303194191E-3</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>1.1271364555681463E-3</c:v>
+                  <c:v>1.1235651078143154E-3</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>1.1237863961245848E-3</c:v>
+                  <c:v>1.1211078853092119E-3</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>1.1204363366810234E-3</c:v>
+                  <c:v>1.1186506628041082E-3</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
                   <c:v>1.1137362177939013E-3</c:v>
@@ -3797,34 +3797,34 @@
                   <c:v>1.2984724640643824E-3</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>1.3325458991476347E-3</c:v>
+                  <c:v>1.3325458991476349E-3</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
                   <c:v>1.3625499159680566E-3</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>1.3753174198569201E-3</c:v>
+                  <c:v>1.3753174198569197E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
                   <c:v>1.3946841343267524E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.4146533498165595E-3</c:v>
+                  <c:v>1.4146533498165597E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>1.4334182752321722E-3</c:v>
+                  <c:v>1.433418275232172E-3</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
                   <c:v>1.4445909758303492E-3</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>1.4455847020325701E-3</c:v>
+                  <c:v>1.4455847020325705E-3</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>1.4457021763821076E-3</c:v>
+                  <c:v>1.4457021763821074E-3</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>1.4456854451868699E-3</c:v>
+                  <c:v>1.4456854451868704E-3</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
                   <c:v>1.4457034223221783E-3</c:v>
@@ -3836,22 +3836,22 @@
                   <c:v>1.4455629870770495E-3</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>1.4452171497116701E-3</c:v>
+                  <c:v>1.4452171497116699E-3</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>1.4450916657473916E-3</c:v>
+                  <c:v>1.4450916657473914E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
                   <c:v>1.4448529792281048E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.443856049179987E-3</c:v>
+                  <c:v>1.4438560491799872E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.4432142120520614E-3</c:v>
+                  <c:v>1.4432142120520612E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.443266541535037E-3</c:v>
+                  <c:v>1.4432665415350372E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
                   <c:v>1.4434251319069122E-3</c:v>
@@ -4236,148 +4236,148 @@
                   <c:v>7.8040477200267344E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>7.7819056047563108E-4</c:v>
+                  <c:v>7.7875573937035282E-4</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>7.7597634894858872E-4</c:v>
+                  <c:v>7.771067067380322E-4</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>7.7376213742154636E-4</c:v>
+                  <c:v>7.7545767410571158E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>7.71547925894504E-4</c:v>
+                  <c:v>7.7380864147339097E-4</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>7.6933371436746164E-4</c:v>
+                  <c:v>7.7215960884107035E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>7.6711950284041929E-4</c:v>
+                  <c:v>7.7051057620874973E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.6490529131337693E-4</c:v>
+                  <c:v>7.6886154357642912E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>7.6269107978633457E-4</c:v>
+                  <c:v>7.672125109441085E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>7.6047686825929221E-4</c:v>
+                  <c:v>7.6556347831178788E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>7.5826265673224985E-4</c:v>
+                  <c:v>7.6391444567946727E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>7.5604844520520749E-4</c:v>
+                  <c:v>7.6226541304714665E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>7.5383423367816514E-4</c:v>
+                  <c:v>7.6061638041482603E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>7.5162002215112278E-4</c:v>
+                  <c:v>7.5896734778250542E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>7.4940581062408042E-4</c:v>
+                  <c:v>7.573183151501848E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>7.4719159909703806E-4</c:v>
+                  <c:v>7.5566928251786418E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>7.449773875699957E-4</c:v>
+                  <c:v>7.5402024988554357E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>7.4276317604295334E-4</c:v>
+                  <c:v>7.5237121725322295E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>7.4054896451591099E-4</c:v>
+                  <c:v>7.5072218462090233E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>7.3612054146182692E-4</c:v>
+                  <c:v>7.4742411935626142E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>7.8447318350072194E-4</c:v>
+                  <c:v>7.9651924557390657E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>8.0913266389472246E-4</c:v>
+                  <c:v>8.2155738726285784E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>8.3445529729440947E-4</c:v>
+                  <c:v>8.4726886507457174E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>8.582213975349269E-4</c:v>
+                  <c:v>8.7139990821531331E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>8.8074213007663328E-4</c:v>
+                  <c:v>8.9426646028002797E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>9.0057319308330108E-4</c:v>
+                  <c:v>9.1440204130079723E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>9.0901183566816969E-4</c:v>
+                  <c:v>9.2297026436659075E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>9.2181220627128113E-4</c:v>
+                  <c:v>9.3596719243283541E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>9.3501079807791388E-4</c:v>
+                  <c:v>9.4936845663098554E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>9.4741341804908898E-4</c:v>
+                  <c:v>9.6196152636282171E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>9.5479798028431191E-4</c:v>
+                  <c:v>9.6945948303515201E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>9.5545478057360543E-4</c:v>
+                  <c:v>9.7012636889170394E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>9.5553242488507497E-4</c:v>
+                  <c:v>9.7020520547872228E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>9.5552136645283517E-4</c:v>
+                  <c:v>9.7019397723754094E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>9.5553324838534815E-4</c:v>
+                  <c:v>9.7020604162434225E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>9.5550160244627959E-4</c:v>
+                  <c:v>9.7017390974266364E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>9.5544042814027313E-4</c:v>
+                  <c:v>9.7011179606804271E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>9.5521184799302321E-4</c:v>
+                  <c:v>9.6987970593383536E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>9.5512890975122625E-4</c:v>
+                  <c:v>9.6979549412497463E-4</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>9.5497115062746795E-4</c:v>
+                  <c:v>9.6963531251407814E-4</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>9.5431223276604333E-4</c:v>
+                  <c:v>9.6896627656878928E-4</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>9.5388801248246955E-4</c:v>
+                  <c:v>9.6853554212517003E-4</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>9.5392259949394229E-4</c:v>
+                  <c:v>9.6857066024120565E-4</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>9.5402741931442593E-4</c:v>
+                  <c:v>9.6867708963368051E-4</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>9.5426270510675759E-4</c:v>
+                  <c:v>9.6891598838222154E-4</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>9.5454316577121671E-4</c:v>
+                  <c:v>9.6920075569048212E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>9.5490315303348411E-4</c:v>
+                  <c:v>9.6956627077574963E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>9.5518761355641295E-4</c:v>
+                  <c:v>9.6985509936273564E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>9.555246604539279E-4</c:v>
+                  <c:v>9.701973218200204E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16200,7 +16200,7 @@
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16486,94 +16486,94 @@
         <v>4</v>
       </c>
       <c r="D9" s="4">
-        <v>1.0748894488887501E-4</v>
+        <v>1.0420515928406728E-4</v>
       </c>
       <c r="E9" s="4">
-        <v>1.1376628742778099E-4</v>
+        <v>1.0877081887028839E-4</v>
       </c>
       <c r="F9" s="4">
-        <v>1.1487084665170681E-4</v>
+        <v>1.119228749342E-4</v>
       </c>
       <c r="G9" s="4">
-        <v>1.1675219072501874E-4</v>
+        <v>1.1596328986495364E-4</v>
       </c>
       <c r="H9" s="4">
-        <v>1.1821814758141852E-4</v>
+        <v>1.1990275277656129E-4</v>
       </c>
       <c r="I9" s="4">
-        <v>1.1769306557695523E-4</v>
+        <v>1.2199635295884858E-4</v>
       </c>
       <c r="J9" s="4">
-        <v>1.1740735707916262E-4</v>
+        <v>1.243467097653028E-4</v>
       </c>
       <c r="K9" s="4">
-        <v>1.1551151797500483E-4</v>
+        <v>1.2468075205096364E-4</v>
       </c>
       <c r="L9" s="4">
-        <v>1.1449785838376007E-4</v>
+        <v>1.2577381385553893E-4</v>
       </c>
       <c r="M9" s="4">
-        <v>1.13287341804607E-4</v>
+        <v>1.2646319222836433E-4</v>
       </c>
       <c r="N9" s="4">
-        <v>1.1212406398402511E-4</v>
+        <v>1.2698406877407795E-4</v>
       </c>
       <c r="O9" s="4">
-        <v>1.1076186329973974E-4</v>
+        <v>1.2710494044541212E-4</v>
       </c>
       <c r="P9" s="4">
-        <v>1.0947685788155618E-4</v>
+        <v>1.2713124547346271E-4</v>
       </c>
       <c r="Q9" s="4">
-        <v>1.0833659526703707E-4</v>
+        <v>1.2714496314152464E-4</v>
       </c>
       <c r="R9" s="4">
-        <v>1.0725258337875167E-4</v>
+        <v>1.2712313200368365E-4</v>
       </c>
       <c r="S9" s="4">
-        <v>1.0627237374881068E-4</v>
+        <v>1.271005238267318E-4</v>
       </c>
       <c r="T9" s="4">
-        <v>1.053872190542009E-4</v>
+        <v>1.2708001023750603E-4</v>
       </c>
       <c r="U9" s="4">
-        <v>1.0457070988285631E-4</v>
+        <v>1.2705407014004141E-4</v>
       </c>
       <c r="V9" s="4">
-        <v>1.0382785746559407E-4</v>
+        <v>1.2702629811717708E-4</v>
       </c>
       <c r="W9" s="4">
-        <v>1.0317553743970813E-4</v>
+        <v>1.2701194080551808E-4</v>
       </c>
       <c r="X9" s="4">
-        <v>1.0260660677729319E-4</v>
+        <v>1.2701796387221964E-4</v>
       </c>
       <c r="Y9" s="4">
-        <v>1.0212195692865432E-4</v>
+        <v>1.2701802056749482E-4</v>
       </c>
       <c r="Z9" s="4">
-        <v>1.0164270384030296E-4</v>
+        <v>1.270327910946451E-4</v>
       </c>
       <c r="AA9" s="4">
-        <v>1.0120623842325044E-4</v>
+        <v>1.2702817221538397E-4</v>
       </c>
       <c r="AB9" s="4">
-        <v>1.0086620530512349E-4</v>
+        <v>1.2698131801807758E-4</v>
       </c>
       <c r="AC9" s="4">
-        <v>1.0054219744424832E-4</v>
+        <v>1.2695571200958938E-4</v>
       </c>
       <c r="AD9" s="4">
-        <v>9.9850684341711718E-5</v>
+        <v>1.2640538596243631E-4</v>
       </c>
       <c r="AE9" s="4">
-        <v>9.9621972535475967E-5</v>
+        <v>1.2643551327178303E-4</v>
       </c>
       <c r="AF9" s="4">
-        <v>9.9483752435656976E-5</v>
+        <v>1.2650241733350927E-4</v>
       </c>
       <c r="AG9" s="4">
-        <v>9.9383928406132565E-5</v>
+        <v>1.2663654108394285E-4</v>
       </c>
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
@@ -16606,34 +16606,34 @@
         <v>1.2984724640643824E-3</v>
       </c>
       <c r="I10" s="4">
-        <v>1.3325458991476347E-3</v>
+        <v>1.3325458991476349E-3</v>
       </c>
       <c r="J10" s="4">
         <v>1.3625499159680566E-3</v>
       </c>
       <c r="K10" s="4">
-        <v>1.3753174198569201E-3</v>
+        <v>1.3753174198569197E-3</v>
       </c>
       <c r="L10" s="4">
         <v>1.3946841343267524E-3</v>
       </c>
       <c r="M10" s="4">
-        <v>1.4146533498165595E-3</v>
+        <v>1.4146533498165597E-3</v>
       </c>
       <c r="N10" s="4">
-        <v>1.4334182752321722E-3</v>
+        <v>1.433418275232172E-3</v>
       </c>
       <c r="O10" s="4">
         <v>1.4445909758303492E-3</v>
       </c>
       <c r="P10" s="4">
-        <v>1.4455847020325701E-3</v>
+        <v>1.4455847020325705E-3</v>
       </c>
       <c r="Q10" s="4">
-        <v>1.4457021763821076E-3</v>
+        <v>1.4457021763821074E-3</v>
       </c>
       <c r="R10" s="4">
-        <v>1.4456854451868699E-3</v>
+        <v>1.4456854451868704E-3</v>
       </c>
       <c r="S10" s="4">
         <v>1.4457034223221783E-3</v>
@@ -16645,22 +16645,22 @@
         <v>1.4455629870770495E-3</v>
       </c>
       <c r="V10" s="4">
-        <v>1.4452171497116701E-3</v>
+        <v>1.4452171497116699E-3</v>
       </c>
       <c r="W10" s="4">
-        <v>1.4450916657473916E-3</v>
+        <v>1.4450916657473914E-3</v>
       </c>
       <c r="X10" s="4">
         <v>1.4448529792281048E-3</v>
       </c>
       <c r="Y10" s="4">
-        <v>1.443856049179987E-3</v>
+        <v>1.4438560491799872E-3</v>
       </c>
       <c r="Z10" s="4">
-        <v>1.4432142120520614E-3</v>
+        <v>1.4432142120520612E-3</v>
       </c>
       <c r="AA10" s="4">
-        <v>1.443266541535037E-3</v>
+        <v>1.4432665415350372E-3</v>
       </c>
       <c r="AB10" s="4">
         <v>1.4434251319069122E-3</v>
@@ -16696,94 +16696,94 @@
         <v>5</v>
       </c>
       <c r="D11" s="4">
-        <v>7.3612054146182692E-4</v>
+        <v>7.4742411935626142E-4</v>
       </c>
       <c r="E11" s="4">
-        <v>7.8447318350072194E-4</v>
+        <v>7.9651924557390657E-4</v>
       </c>
       <c r="F11" s="4">
-        <v>8.0913266389472246E-4</v>
+        <v>8.2155738726285784E-4</v>
       </c>
       <c r="G11" s="4">
-        <v>8.3445529729440947E-4</v>
+        <v>8.4726886507457174E-4</v>
       </c>
       <c r="H11" s="4">
-        <v>8.582213975349269E-4</v>
+        <v>8.7139990821531331E-4</v>
       </c>
       <c r="I11" s="4">
-        <v>8.8074213007663328E-4</v>
+        <v>8.9426646028002797E-4</v>
       </c>
       <c r="J11" s="4">
-        <v>9.0057319308330108E-4</v>
+        <v>9.1440204130079723E-4</v>
       </c>
       <c r="K11" s="4">
-        <v>9.0901183566816969E-4</v>
+        <v>9.2297026436659075E-4</v>
       </c>
       <c r="L11" s="4">
-        <v>9.2181220627128113E-4</v>
+        <v>9.3596719243283541E-4</v>
       </c>
       <c r="M11" s="4">
-        <v>9.3501079807791388E-4</v>
+        <v>9.4936845663098554E-4</v>
       </c>
       <c r="N11" s="4">
-        <v>9.4741341804908898E-4</v>
+        <v>9.6196152636282171E-4</v>
       </c>
       <c r="O11" s="4">
-        <v>9.5479798028431191E-4</v>
+        <v>9.6945948303515201E-4</v>
       </c>
       <c r="P11" s="4">
-        <v>9.5545478057360543E-4</v>
+        <v>9.7012636889170394E-4</v>
       </c>
       <c r="Q11" s="4">
-        <v>9.5553242488507497E-4</v>
+        <v>9.7020520547872228E-4</v>
       </c>
       <c r="R11" s="4">
-        <v>9.5552136645283517E-4</v>
+        <v>9.7019397723754094E-4</v>
       </c>
       <c r="S11" s="4">
-        <v>9.5553324838534815E-4</v>
+        <v>9.7020604162434225E-4</v>
       </c>
       <c r="T11" s="4">
-        <v>9.5550160244627959E-4</v>
+        <v>9.7017390974266364E-4</v>
       </c>
       <c r="U11" s="4">
-        <v>9.5544042814027313E-4</v>
+        <v>9.7011179606804271E-4</v>
       </c>
       <c r="V11" s="4">
-        <v>9.5521184799302321E-4</v>
+        <v>9.6987970593383536E-4</v>
       </c>
       <c r="W11" s="4">
-        <v>9.5512890975122625E-4</v>
+        <v>9.6979549412497463E-4</v>
       </c>
       <c r="X11" s="4">
-        <v>9.5497115062746795E-4</v>
+        <v>9.6963531251407814E-4</v>
       </c>
       <c r="Y11" s="4">
-        <v>9.5431223276604333E-4</v>
+        <v>9.6896627656878928E-4</v>
       </c>
       <c r="Z11" s="4">
-        <v>9.5388801248246955E-4</v>
+        <v>9.6853554212517003E-4</v>
       </c>
       <c r="AA11" s="4">
-        <v>9.5392259949394229E-4</v>
+        <v>9.6857066024120565E-4</v>
       </c>
       <c r="AB11" s="4">
-        <v>9.5402741931442593E-4</v>
+        <v>9.6867708963368051E-4</v>
       </c>
       <c r="AC11" s="4">
-        <v>9.5426270510675759E-4</v>
+        <v>9.6891598838222154E-4</v>
       </c>
       <c r="AD11" s="4">
-        <v>9.5454316577121671E-4</v>
+        <v>9.6920075569048212E-4</v>
       </c>
       <c r="AE11" s="4">
-        <v>9.5490315303348411E-4</v>
+        <v>9.6956627077574963E-4</v>
       </c>
       <c r="AF11" s="4">
-        <v>9.5518761355641295E-4</v>
+        <v>9.6985509936273564E-4</v>
       </c>
       <c r="AG11" s="4">
-        <v>9.555246604539279E-4</v>
+        <v>9.701973218200204E-4</v>
       </c>
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
@@ -17836,94 +17836,94 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>1.0610370953958444E-3</v>
+        <v>1.1058184387710214E-3</v>
       </c>
       <c r="C24">
-        <v>1.1182929641066262E-3</v>
+        <v>1.1654653618777037E-3</v>
       </c>
       <c r="D24">
-        <v>1.1230378075595187E-3</v>
+        <v>1.1704178038241025E-3</v>
       </c>
       <c r="E24">
-        <v>1.1207737467721995E-3</v>
+        <v>1.1680699023993095E-3</v>
       </c>
       <c r="F24">
-        <v>1.1241462933302886E-3</v>
+        <v>1.1715925157363262E-3</v>
       </c>
       <c r="G24">
-        <v>1.1243227034620279E-3</v>
+        <v>1.1717836975623729E-3</v>
       </c>
       <c r="H24">
-        <v>1.1197764855285623E-3</v>
+        <v>1.1670454732039669E-3</v>
       </c>
       <c r="I24">
-        <v>1.1191149559385343E-3</v>
+        <v>1.1663553647253712E-3</v>
       </c>
       <c r="J24">
-        <v>1.1130469624480827E-3</v>
+        <v>1.1600295837550369E-3</v>
       </c>
       <c r="K24">
-        <v>1.1088287076252618E-3</v>
+        <v>1.1556233631186427E-3</v>
       </c>
       <c r="L24">
-        <v>1.1076057889551705E-3</v>
+        <v>1.1543479301738477E-3</v>
       </c>
       <c r="M24">
-        <v>1.1071053032327867E-3</v>
+        <v>1.1538248111999468E-3</v>
       </c>
       <c r="N24">
-        <v>1.1067724143381994E-3</v>
+        <v>1.1534771013398996E-3</v>
       </c>
       <c r="O24">
-        <v>1.1066615139372906E-3</v>
+        <v>1.153358383316175E-3</v>
       </c>
       <c r="P24">
-        <v>1.1066769292084788E-3</v>
+        <v>1.1533777970732827E-3</v>
       </c>
       <c r="Q24">
-        <v>1.1066795967218581E-3</v>
+        <v>1.1533839998503657E-3</v>
       </c>
       <c r="R24">
-        <v>1.1064406824033406E-3</v>
+        <v>1.1531365054505626E-3</v>
       </c>
       <c r="S24">
-        <v>1.10616658964172E-3</v>
+        <v>1.1528517648706005E-3</v>
       </c>
       <c r="T24">
-        <v>1.1060290826740075E-3</v>
+        <v>1.1527114348871379E-3</v>
       </c>
       <c r="U24">
-        <v>1.1055011555537056E-3</v>
+        <v>1.1521628742468084E-3</v>
       </c>
       <c r="V24">
-        <v>1.1050415873555949E-3</v>
+        <v>1.1516853990217147E-3</v>
       </c>
       <c r="W24">
-        <v>1.1045586465345543E-3</v>
+        <v>1.1511845126241146E-3</v>
       </c>
       <c r="X24">
-        <v>1.1038843213708662E-3</v>
+        <v>1.1504833870552749E-3</v>
       </c>
       <c r="Y24">
-        <v>1.1032661366839319E-3</v>
+        <v>1.1498404422001507E-3</v>
       </c>
       <c r="Z24">
-        <v>1.1026899310228654E-3</v>
+        <v>1.1492400691721339E-3</v>
       </c>
       <c r="AA24">
-        <v>1.1033241851303997E-3</v>
+        <v>1.1499032994117962E-3</v>
       </c>
       <c r="AB24">
-        <v>1.1025809057094401E-3</v>
+        <v>1.1491304009395679E-3</v>
       </c>
       <c r="AC24">
-        <v>1.1023701654874632E-3</v>
+        <v>1.148913547482614E-3</v>
       </c>
       <c r="AD24">
-        <v>1.1025099635140992E-3</v>
+        <v>1.1490606826052038E-3</v>
       </c>
       <c r="AE24">
-        <v>1.1022449653531074E-3</v>
+        <v>1.1487858957225897E-3</v>
       </c>
     </row>
     <row r="25" spans="1:37">
@@ -17931,94 +17931,94 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>3.9757641638912632E-4</v>
+        <v>4.1435623124899391E-4</v>
       </c>
       <c r="C25">
-        <v>3.9900747239960505E-4</v>
+        <v>4.1583860682125711E-4</v>
       </c>
       <c r="D25">
-        <v>4.094728037527083E-4</v>
+        <v>4.2674810809389702E-4</v>
       </c>
       <c r="E25">
-        <v>4.1042134222259559E-4</v>
+        <v>4.2774094105362768E-4</v>
       </c>
       <c r="F25">
-        <v>4.2303467685595353E-4</v>
+        <v>4.4088946807188358E-4</v>
       </c>
       <c r="G25">
-        <v>4.2712563186039055E-4</v>
+        <v>4.4515587089355332E-4</v>
       </c>
       <c r="H25">
-        <v>4.2901230740863917E-4</v>
+        <v>4.4712215141194824E-4</v>
       </c>
       <c r="I25">
-        <v>4.4013468861937947E-4</v>
+        <v>4.5871378319881849E-4</v>
       </c>
       <c r="J25">
-        <v>4.4145313646605977E-4</v>
+        <v>4.60087233889707E-4</v>
       </c>
       <c r="K25">
-        <v>4.4134933786440692E-4</v>
+        <v>4.5997510943360454E-4</v>
       </c>
       <c r="L25">
-        <v>4.4091962109341271E-4</v>
+        <v>4.5952689761791997E-4</v>
       </c>
       <c r="M25">
-        <v>4.4021823423990848E-4</v>
+        <v>4.5879531018905696E-4</v>
       </c>
       <c r="N25">
-        <v>4.4027827540505136E-4</v>
+        <v>4.5885757750912214E-4</v>
       </c>
       <c r="O25">
-        <v>4.4040955993276986E-4</v>
+        <v>4.5899315341134275E-4</v>
       </c>
       <c r="P25">
-        <v>4.4116372836744042E-4</v>
+        <v>4.5978047950904734E-4</v>
       </c>
       <c r="Q25">
-        <v>4.4149861084351322E-4</v>
+        <v>4.6013085920391559E-4</v>
       </c>
       <c r="R25">
-        <v>4.4225600784943527E-4</v>
+        <v>4.6092082071518263E-4</v>
       </c>
       <c r="S25">
-        <v>4.4285604557792939E-4</v>
+        <v>4.615465505005841E-4</v>
       </c>
       <c r="T25">
-        <v>4.4414588143789507E-4</v>
+        <v>4.6289202003053275E-4</v>
       </c>
       <c r="U25">
-        <v>4.4411604405746724E-4</v>
+        <v>4.6286158567069468E-4</v>
       </c>
       <c r="V25">
-        <v>4.4420971921594975E-4</v>
+        <v>4.6295981398202245E-4</v>
       </c>
       <c r="W25">
-        <v>4.4397500702864155E-4</v>
+        <v>4.6271617508682986E-4</v>
       </c>
       <c r="X25">
-        <v>4.4370861117360116E-4</v>
+        <v>4.6243920306310218E-4</v>
       </c>
       <c r="Y25">
-        <v>4.424879140459794E-4</v>
+        <v>4.6116751148015295E-4</v>
       </c>
       <c r="Z25">
-        <v>4.4177355237873966E-4</v>
+        <v>4.6042305602918797E-4</v>
       </c>
       <c r="AA25">
-        <v>4.4054153352135982E-4</v>
+        <v>4.591399062500133E-4</v>
       </c>
       <c r="AB25">
-        <v>4.3982519474178468E-4</v>
+        <v>4.5839402783031833E-4</v>
       </c>
       <c r="AC25">
-        <v>4.3880580213641828E-4</v>
+        <v>4.573327059931574E-4</v>
       </c>
       <c r="AD25">
-        <v>4.4035893908705087E-4</v>
+        <v>4.5895199125989522E-4</v>
       </c>
       <c r="AE25">
-        <v>4.3940968502460365E-4</v>
+        <v>4.579632154985259E-4</v>
       </c>
     </row>
     <row r="26" spans="1:37">
@@ -18026,94 +18026,94 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>3.4525981498377545E-4</v>
+        <v>3.8560342544165043E-4</v>
       </c>
       <c r="C26">
-        <v>3.5982944807231638E-4</v>
+        <v>3.938977091004229E-4</v>
       </c>
       <c r="D26">
-        <v>3.6710644959195353E-4</v>
+        <v>4.0102815590911211E-4</v>
       </c>
       <c r="E26">
-        <v>3.7373493890990666E-4</v>
+        <v>4.0668872915977704E-4</v>
       </c>
       <c r="F26">
-        <v>3.9582578415611009E-4</v>
+        <v>4.2148439524556525E-4</v>
       </c>
       <c r="G26">
-        <v>4.3494713071778808E-4</v>
+        <v>4.2638034079782157E-4</v>
       </c>
       <c r="H26">
-        <v>4.4227847691112512E-4</v>
+        <v>4.2993928617474374E-4</v>
       </c>
       <c r="I26">
-        <v>4.5901794912486538E-4</v>
+        <v>4.4295232919176118E-4</v>
       </c>
       <c r="J26">
-        <v>4.6412939868974872E-4</v>
+        <v>4.4402927119422075E-4</v>
       </c>
       <c r="K26">
-        <v>4.6774364798041294E-4</v>
+        <v>4.4423001272194757E-4</v>
       </c>
       <c r="L26">
-        <v>4.6966309910348734E-4</v>
+        <v>4.4444787060954387E-4</v>
       </c>
       <c r="M26">
-        <v>4.7260846794834008E-4</v>
+        <v>4.4510595798899477E-4</v>
       </c>
       <c r="N26">
-        <v>4.7526441798452414E-4</v>
+        <v>4.4626178063197816E-4</v>
       </c>
       <c r="O26">
-        <v>4.7788153153438258E-4</v>
+        <v>4.4757258182247277E-4</v>
       </c>
       <c r="P26">
-        <v>4.8072409114320114E-4</v>
+        <v>4.4919390205042781E-4</v>
       </c>
       <c r="Q26">
-        <v>4.8317943716800202E-4</v>
+        <v>4.5078104437884211E-4</v>
       </c>
       <c r="R26">
-        <v>4.8470967915637789E-4</v>
+        <v>4.5211629450069859E-4</v>
       </c>
       <c r="S26">
-        <v>4.8594611468298545E-4</v>
+        <v>4.5326957425061224E-4</v>
       </c>
       <c r="T26">
-        <v>4.8792763254902827E-4</v>
+        <v>4.5520696339484528E-4</v>
       </c>
       <c r="U26">
-        <v>4.8771717870415681E-4</v>
+        <v>4.5553578115777672E-4</v>
       </c>
       <c r="V26">
-        <v>4.8811136392356582E-4</v>
+        <v>4.5584944646724456E-4</v>
       </c>
       <c r="W26">
-        <v>4.8843918429084768E-4</v>
+        <v>4.559561094704881E-4</v>
       </c>
       <c r="X26">
-        <v>4.8810682276656785E-4</v>
+        <v>4.5572121425237108E-4</v>
       </c>
       <c r="Y26">
-        <v>4.8747689393500613E-4</v>
+        <v>4.550985416964502E-4</v>
       </c>
       <c r="Z26">
-        <v>4.8672999513277174E-4</v>
+        <v>4.5449905971852166E-4</v>
       </c>
       <c r="AA26">
-        <v>4.8843454079791745E-4</v>
+        <v>4.5443664862698183E-4</v>
       </c>
       <c r="AB26">
-        <v>4.8748772875184347E-4</v>
+        <v>4.5380063490385911E-4</v>
       </c>
       <c r="AC26">
-        <v>4.8711906355556337E-4</v>
+        <v>4.5343326114607497E-4</v>
       </c>
       <c r="AD26">
-        <v>4.8876138897384217E-4</v>
+        <v>4.5494560422822621E-4</v>
       </c>
       <c r="AE26">
-        <v>4.8839502633604009E-4</v>
+        <v>4.5447278785524218E-4</v>
       </c>
     </row>
     <row r="27" spans="1:37">
@@ -18121,94 +18121,94 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>3.8826950759574409E-4</v>
+        <v>4.0465652197743196E-4</v>
       </c>
       <c r="C27">
-        <v>3.989339915927411E-4</v>
+        <v>4.1576202640994142E-4</v>
       </c>
       <c r="D27">
-        <v>4.0175941665032688E-4</v>
+        <v>4.1870929984394776E-4</v>
       </c>
       <c r="E27">
-        <v>4.046076403132251E-4</v>
+        <v>4.2168190349906829E-4</v>
       </c>
       <c r="F27">
-        <v>4.1514273478187707E-4</v>
+        <v>4.3266443515270633E-4</v>
       </c>
       <c r="G27">
-        <v>4.1963901427461011E-4</v>
+        <v>4.3735322098718013E-4</v>
       </c>
       <c r="H27">
-        <v>4.2143164929997338E-4</v>
+        <v>4.3922149191073594E-4</v>
       </c>
       <c r="I27">
-        <v>4.2796953665692094E-4</v>
+        <v>4.4603511227335165E-4</v>
       </c>
       <c r="J27">
-        <v>4.2869137838688967E-4</v>
+        <v>4.4678679157952655E-4</v>
       </c>
       <c r="K27">
-        <v>4.2889294118354267E-4</v>
+        <v>4.4699302940114473E-4</v>
       </c>
       <c r="L27">
-        <v>4.2958514978309507E-4</v>
+        <v>4.4771409957447328E-4</v>
       </c>
       <c r="M27">
-        <v>4.3016225956684587E-4</v>
+        <v>4.4831497643516992E-4</v>
       </c>
       <c r="N27">
-        <v>4.314632453320266E-4</v>
+        <v>4.496705619988588E-4</v>
       </c>
       <c r="O27">
-        <v>4.3270248083989658E-4</v>
+        <v>4.5096086515454705E-4</v>
       </c>
       <c r="P27">
-        <v>4.3430279078009501E-4</v>
+        <v>4.5263001592613935E-4</v>
       </c>
       <c r="Q27">
-        <v>4.3530324098676928E-4</v>
+        <v>4.5367403060863823E-4</v>
       </c>
       <c r="R27">
-        <v>4.3666804491927715E-4</v>
+        <v>4.5509702541521833E-4</v>
       </c>
       <c r="S27">
-        <v>4.3784695384923824E-4</v>
+        <v>4.5632605270766956E-4</v>
       </c>
       <c r="T27">
-        <v>4.3919387063071915E-4</v>
+        <v>4.5773099888512522E-4</v>
       </c>
       <c r="U27">
-        <v>4.3965998782187011E-4</v>
+        <v>4.5821744528746784E-4</v>
       </c>
       <c r="V27">
-        <v>4.4023054662472997E-4</v>
+        <v>4.5881268049317148E-4</v>
       </c>
       <c r="W27">
-        <v>4.4040065556194612E-4</v>
+        <v>4.5899094233070158E-4</v>
       </c>
       <c r="X27">
-        <v>4.4071018775672388E-4</v>
+        <v>4.5931420503415025E-4</v>
       </c>
       <c r="Y27">
-        <v>4.4012557028617579E-4</v>
+        <v>4.5870544153793057E-4</v>
       </c>
       <c r="Z27">
-        <v>4.3984103857540357E-4</v>
+        <v>4.584089610106891E-4</v>
       </c>
       <c r="AA27">
-        <v>4.3927502996579274E-4</v>
+        <v>4.5781993462527175E-4</v>
       </c>
       <c r="AB27">
-        <v>4.3896293494925283E-4</v>
+        <v>4.5749536457941731E-4</v>
       </c>
       <c r="AC27">
-        <v>4.3836887632577525E-4</v>
+        <v>4.5687733265413878E-4</v>
       </c>
       <c r="AD27">
-        <v>4.3967475364455565E-4</v>
+        <v>4.5823891780242144E-4</v>
       </c>
       <c r="AE27">
-        <v>4.3902895392029714E-4</v>
+        <v>4.5756640849424067E-4</v>
       </c>
     </row>
     <row r="28" spans="1:37">
@@ -18216,94 +18216,94 @@
         <v>6</v>
       </c>
       <c r="B28">
-        <v>6.2864085446168573E-4</v>
+        <v>6.5517280333083554E-4</v>
       </c>
       <c r="C28">
-        <v>5.8065173143116884E-4</v>
+        <v>6.0514507559113824E-4</v>
       </c>
       <c r="D28">
-        <v>5.7715727565658991E-4</v>
+        <v>6.0150704320725845E-4</v>
       </c>
       <c r="E28">
-        <v>5.8939802003144003E-4</v>
+        <v>6.1427035538190694E-4</v>
       </c>
       <c r="F28">
-        <v>6.1132283966645277E-4</v>
+        <v>6.3712460549070139E-4</v>
       </c>
       <c r="G28">
-        <v>6.2116495269514782E-4</v>
+        <v>6.4738616664415639E-4</v>
       </c>
       <c r="H28">
-        <v>6.2859863293007745E-4</v>
+        <v>6.5513359005477795E-4</v>
       </c>
       <c r="I28">
-        <v>6.4471041145104213E-4</v>
+        <v>6.7192511645025751E-4</v>
       </c>
       <c r="J28">
-        <v>6.4840312593372079E-4</v>
+        <v>6.7577275142821603E-4</v>
       </c>
       <c r="K28">
-        <v>6.5182617183108646E-4</v>
+        <v>6.7933446138261709E-4</v>
       </c>
       <c r="L28">
-        <v>6.5274851137244263E-4</v>
+        <v>6.8029519215282537E-4</v>
       </c>
       <c r="M28">
-        <v>6.5479808482626608E-4</v>
+        <v>6.8243036537951835E-4</v>
       </c>
       <c r="N28">
-        <v>6.5728685533569657E-4</v>
+        <v>6.8502370209035806E-4</v>
       </c>
       <c r="O28">
-        <v>6.599953694386326E-4</v>
+        <v>6.8784464147818671E-4</v>
       </c>
       <c r="P28">
-        <v>6.6271823685959863E-4</v>
+        <v>6.9068440837210285E-4</v>
       </c>
       <c r="Q28">
-        <v>6.6541147575940635E-4</v>
+        <v>6.9349335772620044E-4</v>
       </c>
       <c r="R28">
-        <v>6.6758238321629323E-4</v>
+        <v>6.9575678906731286E-4</v>
       </c>
       <c r="S28">
-        <v>6.695223998790733E-4</v>
+        <v>6.9777923827096409E-4</v>
       </c>
       <c r="T28">
-        <v>6.7209439570581602E-4</v>
+        <v>7.0046159489822399E-4</v>
       </c>
       <c r="U28">
-        <v>6.7286737744009942E-4</v>
+        <v>7.0126820554068138E-4</v>
       </c>
       <c r="V28">
-        <v>6.7344823507195376E-4</v>
+        <v>7.0187448889172854E-4</v>
       </c>
       <c r="W28">
-        <v>6.73909086850441E-4</v>
+        <v>7.0235628151829209E-4</v>
       </c>
       <c r="X28">
-        <v>6.740064696202369E-4</v>
+        <v>7.0245879124624332E-4</v>
       </c>
       <c r="Y28">
-        <v>6.7364356730673243E-4</v>
+        <v>7.0208138504586923E-4</v>
       </c>
       <c r="Z28">
-        <v>6.7322262507433497E-4</v>
+        <v>7.0164276868927991E-4</v>
       </c>
       <c r="AA28">
-        <v>6.7344500418278937E-4</v>
+        <v>7.0187587901977887E-4</v>
       </c>
       <c r="AB28">
-        <v>6.7281217685356582E-4</v>
+        <v>7.0121740957167211E-4</v>
       </c>
       <c r="AC28">
-        <v>6.7245517568083519E-4</v>
+        <v>7.0084703451029598E-4</v>
       </c>
       <c r="AD28">
-        <v>6.7397575425436052E-4</v>
+        <v>7.0243269074363234E-4</v>
       </c>
       <c r="AE28">
-        <v>6.7349435170381685E-4</v>
+        <v>7.0193181770471214E-4</v>
       </c>
     </row>
     <row r="29" spans="1:37">
@@ -18311,94 +18311,94 @@
         <v>84</v>
       </c>
       <c r="B29">
-        <v>3.4585801076062443E-4</v>
+        <v>3.6045503701553509E-4</v>
       </c>
       <c r="C29">
-        <v>3.4495574783075341E-4</v>
+        <v>3.5950684514816466E-4</v>
       </c>
       <c r="D29">
-        <v>3.6039991749266362E-4</v>
+        <v>3.7560487909735457E-4</v>
       </c>
       <c r="E29">
-        <v>3.6434083049787565E-4</v>
+        <v>3.7971585214712964E-4</v>
       </c>
       <c r="F29">
-        <v>3.7594665871961683E-4</v>
+        <v>3.9181403193273731E-4</v>
       </c>
       <c r="G29">
-        <v>3.8265282942463545E-4</v>
+        <v>3.9880573963794092E-4</v>
       </c>
       <c r="H29">
-        <v>3.8491153807264589E-4</v>
+        <v>4.0115976169978224E-4</v>
       </c>
       <c r="I29">
-        <v>3.948653271158722E-4</v>
+        <v>4.1153349812879397E-4</v>
       </c>
       <c r="J29">
-        <v>3.9594612256427204E-4</v>
+        <v>4.1265933176568687E-4</v>
       </c>
       <c r="K29">
-        <v>3.9619175896624695E-4</v>
+        <v>4.129117958327599E-4</v>
       </c>
       <c r="L29">
-        <v>3.9654376773871745E-4</v>
+        <v>4.1327833609856163E-4</v>
       </c>
       <c r="M29">
-        <v>3.9707573055230652E-4</v>
+        <v>4.1383220593268312E-4</v>
       </c>
       <c r="N29">
-        <v>3.9834863581642401E-4</v>
+        <v>4.1515854913946708E-4</v>
       </c>
       <c r="O29">
-        <v>3.9959695124185265E-4</v>
+        <v>4.1645840924083266E-4</v>
       </c>
       <c r="P29">
-        <v>4.0092020917552979E-4</v>
+        <v>4.1783871648228943E-4</v>
       </c>
       <c r="Q29">
-        <v>4.0164593001903277E-4</v>
+        <v>4.185963043514945E-4</v>
       </c>
       <c r="R29">
-        <v>4.025864972614837E-4</v>
+        <v>4.1957711242621983E-4</v>
       </c>
       <c r="S29">
-        <v>4.0337312378417004E-4</v>
+        <v>4.2039727289771742E-4</v>
       </c>
       <c r="T29">
-        <v>4.0442495213179318E-4</v>
+        <v>4.2149458289914189E-4</v>
       </c>
       <c r="U29">
-        <v>4.0454932437130627E-4</v>
+        <v>4.2162480789881447E-4</v>
       </c>
       <c r="V29">
-        <v>4.0464803339247029E-4</v>
+        <v>4.2172822917568159E-4</v>
       </c>
       <c r="W29">
-        <v>4.0439328301694171E-4</v>
+        <v>4.2146361886612633E-4</v>
       </c>
       <c r="X29">
-        <v>4.040545754555679E-4</v>
+        <v>4.2111122291148745E-4</v>
       </c>
       <c r="Y29">
-        <v>4.0293590438237893E-4</v>
+        <v>4.1994581639741166E-4</v>
       </c>
       <c r="Z29">
-        <v>4.0211529090881346E-4</v>
+        <v>4.190906180766014E-4</v>
       </c>
       <c r="AA29">
-        <v>4.0078697353040108E-4</v>
+        <v>4.1770702521979762E-4</v>
       </c>
       <c r="AB29">
-        <v>4.0014215791000135E-4</v>
+        <v>4.170356261122462E-4</v>
       </c>
       <c r="AC29">
-        <v>3.9916649340924858E-4</v>
+        <v>4.1601977841646405E-4</v>
       </c>
       <c r="AD29">
-        <v>3.9985648048380197E-4</v>
+        <v>4.1673941788640924E-4</v>
       </c>
       <c r="AE29">
-        <v>3.9882869849444967E-4</v>
+        <v>4.1566874700402494E-4</v>
       </c>
     </row>
     <row r="30" spans="1:37">
@@ -18406,94 +18406,94 @@
         <v>85</v>
       </c>
       <c r="B30">
-        <v>5.5949994465194052E-4</v>
+        <v>5.8311378364830837E-4</v>
       </c>
       <c r="C30">
-        <v>5.490709016341414E-4</v>
+        <v>5.7223208730528745E-4</v>
       </c>
       <c r="D30">
-        <v>5.4591562691943185E-4</v>
+        <v>5.6894733626181731E-4</v>
       </c>
       <c r="E30">
-        <v>5.4428202142592678E-4</v>
+        <v>5.6725048162098066E-4</v>
       </c>
       <c r="F30">
-        <v>5.4687829275625965E-4</v>
+        <v>5.6996008314341522E-4</v>
       </c>
       <c r="G30">
-        <v>5.4645085655929157E-4</v>
+        <v>5.6951816703823988E-4</v>
       </c>
       <c r="H30">
-        <v>5.4701855850944456E-4</v>
+        <v>5.7010978594149338E-4</v>
       </c>
       <c r="I30">
-        <v>5.5159545353608997E-4</v>
+        <v>5.7487956261865754E-4</v>
       </c>
       <c r="J30">
-        <v>5.5116986450326347E-4</v>
+        <v>5.7443519462267441E-4</v>
       </c>
       <c r="K30">
-        <v>5.5082515994957833E-4</v>
+        <v>5.7407101696939681E-4</v>
       </c>
       <c r="L30">
-        <v>5.5045116908780244E-4</v>
+        <v>5.7368079332420063E-4</v>
       </c>
       <c r="M30">
-        <v>5.5016894781847396E-4</v>
+        <v>5.7338591052819412E-4</v>
       </c>
       <c r="N30">
-        <v>5.5030632856499669E-4</v>
+        <v>5.7352870427450646E-4</v>
       </c>
       <c r="O30">
-        <v>5.5080345075069956E-4</v>
+        <v>5.7404524281558721E-4</v>
       </c>
       <c r="P30">
-        <v>5.5167571643641449E-4</v>
+        <v>5.7495598374617473E-4</v>
       </c>
       <c r="Q30">
-        <v>5.5236107717376317E-4</v>
+        <v>5.7567197447162301E-4</v>
       </c>
       <c r="R30">
-        <v>5.5273978734272802E-4</v>
+        <v>5.7606741774479436E-4</v>
       </c>
       <c r="S30">
-        <v>5.5274410279881891E-4</v>
+        <v>5.7607237499356242E-4</v>
       </c>
       <c r="T30">
-        <v>5.5289670193281145E-4</v>
+        <v>5.762329043721763E-4</v>
       </c>
       <c r="U30">
-        <v>5.5265714178147211E-4</v>
+        <v>5.7598405732017636E-4</v>
       </c>
       <c r="V30">
-        <v>5.5244896195009953E-4</v>
+        <v>5.7576783576552626E-4</v>
       </c>
       <c r="W30">
-        <v>5.5221137170350255E-4</v>
+        <v>5.7552143636232329E-4</v>
       </c>
       <c r="X30">
-        <v>5.5188530920952062E-4</v>
+        <v>5.7518244213933473E-4</v>
       </c>
       <c r="Y30">
-        <v>5.5130828970691593E-4</v>
+        <v>5.7458173195686134E-4</v>
       </c>
       <c r="Z30">
-        <v>5.5089526377585969E-4</v>
+        <v>5.7415134865799545E-4</v>
       </c>
       <c r="AA30">
-        <v>5.5094868459087108E-4</v>
+        <v>5.7420812373722705E-4</v>
       </c>
       <c r="AB30">
-        <v>5.5070873103541993E-4</v>
+        <v>5.7395891913116653E-4</v>
       </c>
       <c r="AC30">
-        <v>5.5038144396247959E-4</v>
+        <v>5.7361920437307709E-4</v>
       </c>
       <c r="AD30">
-        <v>5.5068737415113456E-4</v>
+        <v>5.7393876788858417E-4</v>
       </c>
       <c r="AE30">
-        <v>5.5020714130888889E-4</v>
+        <v>5.7343895733650446E-4</v>
       </c>
     </row>
   </sheetData>
@@ -19735,179 +19735,179 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="4" cm="1">
         <f t="array" ref="AA3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AA1)</f>
-        <v>7.5108389563240119E-5</v>
+        <v>5.0412726378568952E-5</v>
       </c>
       <c r="AB3" s="4" cm="1">
         <f t="array" ref="AB3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AB1)</f>
-        <v>7.7552820431472588E-5</v>
+        <v>5.4271492176534604E-5</v>
       </c>
       <c r="AC3" s="4" cm="1">
         <f t="array" ref="AC3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AC1)</f>
-        <v>7.9997251299705058E-5</v>
+        <v>5.8130257974500256E-5</v>
       </c>
       <c r="AD3" s="4" cm="1">
         <f t="array" ref="AD3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AD1)</f>
-        <v>8.2441682167937527E-5</v>
+        <v>6.1989023772465041E-5</v>
       </c>
       <c r="AE3" s="4" cm="1">
         <f t="array" ref="AE3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AE1)</f>
-        <v>8.4886113036169997E-5</v>
+        <v>6.5847789570430693E-5</v>
       </c>
       <c r="AF3" s="4" cm="1">
         <f t="array" ref="AF3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AF1)</f>
-        <v>8.7330543904402466E-5</v>
+        <v>6.9706555368396345E-5</v>
       </c>
       <c r="AG3" s="4" cm="1">
         <f t="array" ref="AG3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AG1)</f>
-        <v>8.9774974772634936E-5</v>
+        <v>7.3565321166361129E-5</v>
       </c>
       <c r="AH3" s="4" cm="1">
         <f t="array" ref="AH3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AH1)</f>
-        <v>9.2219405640867405E-5</v>
+        <v>7.7424086964326781E-5</v>
       </c>
       <c r="AI3" s="4" cm="1">
         <f t="array" ref="AI3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AI1)</f>
-        <v>9.4663836509099875E-5</v>
+        <v>8.1282852762291566E-5</v>
       </c>
       <c r="AJ3" s="4" cm="1">
         <f t="array" ref="AJ3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AJ1)</f>
-        <v>9.7108267377332344E-5</v>
+        <v>8.5141618560257218E-5</v>
       </c>
       <c r="AK3" s="4" cm="1">
         <f t="array" ref="AK3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AK1)</f>
-        <v>9.9552698245564814E-5</v>
+        <v>8.900038435822287E-5</v>
       </c>
       <c r="AL3" s="4" cm="1">
         <f t="array" ref="AL3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AL1)</f>
-        <v>1.0199712911379728E-4</v>
+        <v>9.2859150156187655E-5</v>
       </c>
       <c r="AM3" s="4" cm="1">
         <f t="array" ref="AM3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AM1)</f>
-        <v>1.0444155998202975E-4</v>
+        <v>9.6717915954153307E-5</v>
       </c>
       <c r="AN3" s="26" cm="1">
         <f t="array" ref="AN3">TREND($AO$3:$AS$3,$AO$1:$AS$1,AN1)</f>
-        <v>1.0688599085026222E-4</v>
+        <v>1.0057668175211809E-4</v>
       </c>
       <c r="AO3" s="10">
         <f>BNVFE!D9</f>
-        <v>1.0748894488887501E-4</v>
+        <v>1.0420515928406728E-4</v>
       </c>
       <c r="AP3" s="10">
         <f>BNVFE!E9</f>
-        <v>1.1376628742778099E-4</v>
+        <v>1.0877081887028839E-4</v>
       </c>
       <c r="AQ3" s="10">
         <f>BNVFE!F9</f>
-        <v>1.1487084665170681E-4</v>
+        <v>1.119228749342E-4</v>
       </c>
       <c r="AR3" s="10">
         <f>BNVFE!G9</f>
-        <v>1.1675219072501874E-4</v>
+        <v>1.1596328986495364E-4</v>
       </c>
       <c r="AS3" s="10">
         <f>BNVFE!H9</f>
-        <v>1.1821814758141852E-4</v>
+        <v>1.1990275277656129E-4</v>
       </c>
       <c r="AT3" s="10">
         <f>BNVFE!I9</f>
-        <v>1.1769306557695523E-4</v>
+        <v>1.2199635295884858E-4</v>
       </c>
       <c r="AU3" s="10">
         <f>BNVFE!J9</f>
-        <v>1.1740735707916262E-4</v>
+        <v>1.243467097653028E-4</v>
       </c>
       <c r="AV3" s="10">
         <f>BNVFE!K9</f>
-        <v>1.1551151797500483E-4</v>
+        <v>1.2468075205096364E-4</v>
       </c>
       <c r="AW3" s="10">
         <f>BNVFE!L9</f>
-        <v>1.1449785838376007E-4</v>
+        <v>1.2577381385553893E-4</v>
       </c>
       <c r="AX3" s="10">
         <f>BNVFE!M9</f>
-        <v>1.13287341804607E-4</v>
+        <v>1.2646319222836433E-4</v>
       </c>
       <c r="AY3" s="10">
         <f>BNVFE!N9</f>
-        <v>1.1212406398402511E-4</v>
+        <v>1.2698406877407795E-4</v>
       </c>
       <c r="AZ3" s="10">
         <f>BNVFE!O9</f>
-        <v>1.1076186329973974E-4</v>
+        <v>1.2710494044541212E-4</v>
       </c>
       <c r="BA3" s="10">
         <f>BNVFE!P9</f>
-        <v>1.0947685788155618E-4</v>
+        <v>1.2713124547346271E-4</v>
       </c>
       <c r="BB3" s="10">
         <f>BNVFE!Q9</f>
-        <v>1.0833659526703707E-4</v>
+        <v>1.2714496314152464E-4</v>
       </c>
       <c r="BC3" s="10">
         <f>BNVFE!R9</f>
-        <v>1.0725258337875167E-4</v>
+        <v>1.2712313200368365E-4</v>
       </c>
       <c r="BD3" s="10">
         <f>BNVFE!S9</f>
-        <v>1.0627237374881068E-4</v>
+        <v>1.271005238267318E-4</v>
       </c>
       <c r="BE3" s="10">
         <f>BNVFE!T9</f>
-        <v>1.053872190542009E-4</v>
+        <v>1.2708001023750603E-4</v>
       </c>
       <c r="BF3" s="10">
         <f>BNVFE!U9</f>
-        <v>1.0457070988285631E-4</v>
+        <v>1.2705407014004141E-4</v>
       </c>
       <c r="BG3" s="10">
         <f>BNVFE!V9</f>
-        <v>1.0382785746559407E-4</v>
+        <v>1.2702629811717708E-4</v>
       </c>
       <c r="BH3" s="10">
         <f>BNVFE!W9</f>
-        <v>1.0317553743970813E-4</v>
+        <v>1.2701194080551808E-4</v>
       </c>
       <c r="BI3" s="10">
         <f>BNVFE!X9</f>
-        <v>1.0260660677729319E-4</v>
+        <v>1.2701796387221964E-4</v>
       </c>
       <c r="BJ3" s="10">
         <f>BNVFE!Y9</f>
-        <v>1.0212195692865432E-4</v>
+        <v>1.2701802056749482E-4</v>
       </c>
       <c r="BK3" s="10">
         <f>BNVFE!Z9</f>
-        <v>1.0164270384030296E-4</v>
+        <v>1.270327910946451E-4</v>
       </c>
       <c r="BL3" s="10">
         <f>BNVFE!AA9</f>
-        <v>1.0120623842325044E-4</v>
+        <v>1.2702817221538397E-4</v>
       </c>
       <c r="BM3" s="10">
         <f>BNVFE!AB9</f>
-        <v>1.0086620530512349E-4</v>
+        <v>1.2698131801807758E-4</v>
       </c>
       <c r="BN3" s="10">
         <f>BNVFE!AC9</f>
-        <v>1.0054219744424832E-4</v>
+        <v>1.2695571200958938E-4</v>
       </c>
       <c r="BO3" s="10">
         <f>BNVFE!AD9</f>
-        <v>9.9850684341711718E-5</v>
+        <v>1.2640538596243631E-4</v>
       </c>
       <c r="BP3" s="10">
         <f>BNVFE!AE9</f>
-        <v>9.9621972535475967E-5</v>
+        <v>1.2643551327178303E-4</v>
       </c>
       <c r="BQ3" s="10">
         <f>BNVFE!AF9</f>
-        <v>9.9483752435656976E-5</v>
+        <v>1.2650241733350927E-4</v>
       </c>
       <c r="BR3" s="10">
         <f>BNVFE!AG9</f>
-        <v>9.9383928406132565E-5</v>
+        <v>1.2663654108394285E-4</v>
       </c>
       <c r="BS3" s="10"/>
       <c r="BT3" s="4"/>
@@ -19930,119 +19930,119 @@
       <c r="K4" s="9"/>
       <c r="L4" s="4">
         <f>L5/M5*M4</f>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4:AI4" si="1">M5/N5*N4</f>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="T4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1807374066651307E-3</v>
+        <v>1.1628806678959742E-3</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="1"/>
-        <v>1.177387347221569E-3</v>
+        <v>1.1604234453908705E-3</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1740372877780075E-3</v>
+        <v>1.1579662228857668E-3</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1706872283344459E-3</v>
+        <v>1.1555090003806633E-3</v>
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1673371688908844E-3</v>
+        <v>1.1530517778755595E-3</v>
       </c>
       <c r="AA4" s="4">
         <f t="shared" si="1"/>
-        <v>1.163987109447323E-3</v>
+        <v>1.1505945553704558E-3</v>
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1606370500037615E-3</v>
+        <v>1.1481373328653521E-3</v>
       </c>
       <c r="AC4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1572869905602E-3</v>
+        <v>1.1456801103602485E-3</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1539369311166386E-3</v>
+        <v>1.1432228878551448E-3</v>
       </c>
       <c r="AE4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1505868716730771E-3</v>
+        <v>1.1407656653500411E-3</v>
       </c>
       <c r="AF4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1472368122295155E-3</v>
+        <v>1.1383084428449376E-3</v>
       </c>
       <c r="AG4" s="4">
         <f>AG5/AH5*AH4</f>
-        <v>1.143886752785954E-3</v>
+        <v>1.1358512203398338E-3</v>
       </c>
       <c r="AH4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1405366933423926E-3</v>
+        <v>1.1333939978347303E-3</v>
       </c>
       <c r="AI4" s="4">
         <f t="shared" si="1"/>
-        <v>1.1371866338988309E-3</v>
+        <v>1.1309367753296266E-3</v>
       </c>
       <c r="AJ4" s="4">
         <f>AJ5/AK5*AK4</f>
-        <v>1.1338365744552694E-3</v>
+        <v>1.1284795528245229E-3</v>
       </c>
       <c r="AK4" s="19">
         <f>AK5/AL5*AL4</f>
-        <v>1.130486515011708E-3</v>
+        <v>1.1260223303194191E-3</v>
       </c>
       <c r="AL4" s="19">
         <f>AL5/AM5*AM4</f>
-        <v>1.1271364555681463E-3</v>
+        <v>1.1235651078143154E-3</v>
       </c>
       <c r="AM4" s="19">
         <f>AM5/AN5*AN4</f>
-        <v>1.1237863961245848E-3</v>
+        <v>1.1211078853092119E-3</v>
       </c>
       <c r="AN4" s="27">
         <f>AN5/AO5*AO4</f>
-        <v>1.1204363366810234E-3</v>
+        <v>1.1186506628041082E-3</v>
       </c>
       <c r="AO4" s="10">
         <f>BNVFE!D10</f>
@@ -20066,7 +20066,7 @@
       </c>
       <c r="AT4" s="10">
         <f>BNVFE!I10</f>
-        <v>1.3325458991476347E-3</v>
+        <v>1.3325458991476349E-3</v>
       </c>
       <c r="AU4" s="10">
         <f>BNVFE!J10</f>
@@ -20074,7 +20074,7 @@
       </c>
       <c r="AV4" s="10">
         <f>BNVFE!K10</f>
-        <v>1.3753174198569201E-3</v>
+        <v>1.3753174198569197E-3</v>
       </c>
       <c r="AW4" s="10">
         <f>BNVFE!L10</f>
@@ -20082,11 +20082,11 @@
       </c>
       <c r="AX4" s="10">
         <f>BNVFE!M10</f>
-        <v>1.4146533498165595E-3</v>
+        <v>1.4146533498165597E-3</v>
       </c>
       <c r="AY4" s="10">
         <f>BNVFE!N10</f>
-        <v>1.4334182752321722E-3</v>
+        <v>1.433418275232172E-3</v>
       </c>
       <c r="AZ4" s="10">
         <f>BNVFE!O10</f>
@@ -20094,15 +20094,15 @@
       </c>
       <c r="BA4" s="10">
         <f>BNVFE!P10</f>
-        <v>1.4455847020325701E-3</v>
+        <v>1.4455847020325705E-3</v>
       </c>
       <c r="BB4" s="10">
         <f>BNVFE!Q10</f>
-        <v>1.4457021763821076E-3</v>
+        <v>1.4457021763821074E-3</v>
       </c>
       <c r="BC4" s="10">
         <f>BNVFE!R10</f>
-        <v>1.4456854451868699E-3</v>
+        <v>1.4456854451868704E-3</v>
       </c>
       <c r="BD4" s="10">
         <f>BNVFE!S10</f>
@@ -20118,11 +20118,11 @@
       </c>
       <c r="BG4" s="10">
         <f>BNVFE!V10</f>
-        <v>1.4452171497116701E-3</v>
+        <v>1.4452171497116699E-3</v>
       </c>
       <c r="BH4" s="10">
         <f>BNVFE!W10</f>
-        <v>1.4450916657473916E-3</v>
+        <v>1.4450916657473914E-3</v>
       </c>
       <c r="BI4" s="10">
         <f>BNVFE!X10</f>
@@ -20130,15 +20130,15 @@
       </c>
       <c r="BJ4" s="10">
         <f>BNVFE!Y10</f>
-        <v>1.443856049179987E-3</v>
+        <v>1.4438560491799872E-3</v>
       </c>
       <c r="BK4" s="10">
         <f>BNVFE!Z10</f>
-        <v>1.4432142120520614E-3</v>
+        <v>1.4432142120520612E-3</v>
       </c>
       <c r="BL4" s="10">
         <f>BNVFE!AA10</f>
-        <v>1.443266541535037E-3</v>
+        <v>1.4432665415350372E-3</v>
       </c>
       <c r="BM4" s="10">
         <f>BNVFE!AB10</f>
@@ -20229,195 +20229,195 @@
       </c>
       <c r="W5" s="4">
         <f>($AO$5-$V$5)/COUNT($V$1:$AO$1)+V5</f>
-        <v>7.7819056047563108E-4</v>
+        <v>7.7875573937035282E-4</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" ref="X5:AN5" si="3">($AO$5-$V$5)/COUNT($V$1:$AO$1)+W5</f>
-        <v>7.7597634894858872E-4</v>
+        <v>7.771067067380322E-4</v>
       </c>
       <c r="Y5" s="4">
         <f t="shared" si="3"/>
-        <v>7.7376213742154636E-4</v>
+        <v>7.7545767410571158E-4</v>
       </c>
       <c r="Z5" s="4">
         <f t="shared" si="3"/>
-        <v>7.71547925894504E-4</v>
+        <v>7.7380864147339097E-4</v>
       </c>
       <c r="AA5" s="4">
         <f t="shared" si="3"/>
-        <v>7.6933371436746164E-4</v>
+        <v>7.7215960884107035E-4</v>
       </c>
       <c r="AB5" s="4">
         <f t="shared" si="3"/>
-        <v>7.6711950284041929E-4</v>
+        <v>7.7051057620874973E-4</v>
       </c>
       <c r="AC5" s="4">
         <f t="shared" si="3"/>
-        <v>7.6490529131337693E-4</v>
+        <v>7.6886154357642912E-4</v>
       </c>
       <c r="AD5" s="4">
         <f t="shared" si="3"/>
-        <v>7.6269107978633457E-4</v>
+        <v>7.672125109441085E-4</v>
       </c>
       <c r="AE5" s="4">
         <f t="shared" si="3"/>
-        <v>7.6047686825929221E-4</v>
+        <v>7.6556347831178788E-4</v>
       </c>
       <c r="AF5" s="4">
         <f t="shared" si="3"/>
-        <v>7.5826265673224985E-4</v>
+        <v>7.6391444567946727E-4</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="3"/>
-        <v>7.5604844520520749E-4</v>
+        <v>7.6226541304714665E-4</v>
       </c>
       <c r="AH5" s="4">
         <f t="shared" si="3"/>
-        <v>7.5383423367816514E-4</v>
+        <v>7.6061638041482603E-4</v>
       </c>
       <c r="AI5" s="4">
         <f t="shared" si="3"/>
-        <v>7.5162002215112278E-4</v>
+        <v>7.5896734778250542E-4</v>
       </c>
       <c r="AJ5" s="4">
         <f t="shared" si="3"/>
-        <v>7.4940581062408042E-4</v>
+        <v>7.573183151501848E-4</v>
       </c>
       <c r="AK5" s="4">
         <f t="shared" si="3"/>
-        <v>7.4719159909703806E-4</v>
+        <v>7.5566928251786418E-4</v>
       </c>
       <c r="AL5" s="4">
         <f t="shared" si="3"/>
-        <v>7.449773875699957E-4</v>
+        <v>7.5402024988554357E-4</v>
       </c>
       <c r="AM5" s="4">
         <f t="shared" si="3"/>
-        <v>7.4276317604295334E-4</v>
+        <v>7.5237121725322295E-4</v>
       </c>
       <c r="AN5" s="26">
         <f t="shared" si="3"/>
-        <v>7.4054896451591099E-4</v>
+        <v>7.5072218462090233E-4</v>
       </c>
       <c r="AO5" s="10">
         <f>BNVFE!D11</f>
-        <v>7.3612054146182692E-4</v>
+        <v>7.4742411935626142E-4</v>
       </c>
       <c r="AP5" s="10">
         <f>BNVFE!E11</f>
-        <v>7.8447318350072194E-4</v>
+        <v>7.9651924557390657E-4</v>
       </c>
       <c r="AQ5" s="10">
         <f>BNVFE!F11</f>
-        <v>8.0913266389472246E-4</v>
+        <v>8.2155738726285784E-4</v>
       </c>
       <c r="AR5" s="10">
         <f>BNVFE!G11</f>
-        <v>8.3445529729440947E-4</v>
+        <v>8.4726886507457174E-4</v>
       </c>
       <c r="AS5" s="10">
         <f>BNVFE!H11</f>
-        <v>8.582213975349269E-4</v>
+        <v>8.7139990821531331E-4</v>
       </c>
       <c r="AT5" s="10">
         <f>BNVFE!I11</f>
-        <v>8.8074213007663328E-4</v>
+        <v>8.9426646028002797E-4</v>
       </c>
       <c r="AU5" s="10">
         <f>BNVFE!J11</f>
-        <v>9.0057319308330108E-4</v>
+        <v>9.1440204130079723E-4</v>
       </c>
       <c r="AV5" s="10">
         <f>BNVFE!K11</f>
-        <v>9.0901183566816969E-4</v>
+        <v>9.2297026436659075E-4</v>
       </c>
       <c r="AW5" s="10">
         <f>BNVFE!L11</f>
-        <v>9.2181220627128113E-4</v>
+        <v>9.3596719243283541E-4</v>
       </c>
       <c r="AX5" s="10">
         <f>BNVFE!M11</f>
-        <v>9.3501079807791388E-4</v>
+        <v>9.4936845663098554E-4</v>
       </c>
       <c r="AY5" s="10">
         <f>BNVFE!N11</f>
-        <v>9.4741341804908898E-4</v>
+        <v>9.6196152636282171E-4</v>
       </c>
       <c r="AZ5" s="10">
         <f>BNVFE!O11</f>
-        <v>9.5479798028431191E-4</v>
+        <v>9.6945948303515201E-4</v>
       </c>
       <c r="BA5" s="10">
         <f>BNVFE!P11</f>
-        <v>9.5545478057360543E-4</v>
+        <v>9.7012636889170394E-4</v>
       </c>
       <c r="BB5" s="10">
         <f>BNVFE!Q11</f>
-        <v>9.5553242488507497E-4</v>
+        <v>9.7020520547872228E-4</v>
       </c>
       <c r="BC5" s="10">
         <f>BNVFE!R11</f>
-        <v>9.5552136645283517E-4</v>
+        <v>9.7019397723754094E-4</v>
       </c>
       <c r="BD5" s="10">
         <f>BNVFE!S11</f>
-        <v>9.5553324838534815E-4</v>
+        <v>9.7020604162434225E-4</v>
       </c>
       <c r="BE5" s="10">
         <f>BNVFE!T11</f>
-        <v>9.5550160244627959E-4</v>
+        <v>9.7017390974266364E-4</v>
       </c>
       <c r="BF5" s="10">
         <f>BNVFE!U11</f>
-        <v>9.5544042814027313E-4</v>
+        <v>9.7011179606804271E-4</v>
       </c>
       <c r="BG5" s="10">
         <f>BNVFE!V11</f>
-        <v>9.5521184799302321E-4</v>
+        <v>9.6987970593383536E-4</v>
       </c>
       <c r="BH5" s="10">
         <f>BNVFE!W11</f>
-        <v>9.5512890975122625E-4</v>
+        <v>9.6979549412497463E-4</v>
       </c>
       <c r="BI5" s="10">
         <f>BNVFE!X11</f>
-        <v>9.5497115062746795E-4</v>
+        <v>9.6963531251407814E-4</v>
       </c>
       <c r="BJ5" s="10">
         <f>BNVFE!Y11</f>
-        <v>9.5431223276604333E-4</v>
+        <v>9.6896627656878928E-4</v>
       </c>
       <c r="BK5" s="10">
         <f>BNVFE!Z11</f>
-        <v>9.5388801248246955E-4</v>
+        <v>9.6853554212517003E-4</v>
       </c>
       <c r="BL5" s="10">
         <f>BNVFE!AA11</f>
-        <v>9.5392259949394229E-4</v>
+        <v>9.6857066024120565E-4</v>
       </c>
       <c r="BM5" s="10">
         <f>BNVFE!AB11</f>
-        <v>9.5402741931442593E-4</v>
+        <v>9.6867708963368051E-4</v>
       </c>
       <c r="BN5" s="10">
         <f>BNVFE!AC11</f>
-        <v>9.5426270510675759E-4</v>
+        <v>9.6891598838222154E-4</v>
       </c>
       <c r="BO5" s="10">
         <f>BNVFE!AD11</f>
-        <v>9.5454316577121671E-4</v>
+        <v>9.6920075569048212E-4</v>
       </c>
       <c r="BP5" s="10">
         <f>BNVFE!AE11</f>
-        <v>9.5490315303348411E-4</v>
+        <v>9.6956627077574963E-4</v>
       </c>
       <c r="BQ5" s="10">
         <f>BNVFE!AF11</f>
-        <v>9.5518761355641295E-4</v>
+        <v>9.6985509936273564E-4</v>
       </c>
       <c r="BR5" s="10">
         <f>BNVFE!AG11</f>
-        <v>9.555246604539279E-4</v>
+        <v>9.701973218200204E-4</v>
       </c>
       <c r="BS5" s="10"/>
       <c r="BT5" s="4"/>
@@ -22966,123 +22966,123 @@
       </c>
       <c r="B3" s="4">
         <f>BNVFE!B25*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.6773655474057739E-4</v>
+        <v>3.4315885705159878E-4</v>
       </c>
       <c r="C3" s="4">
         <f>BNVFE!C25*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.5976842082089582E-4</v>
+        <v>3.4251537077170018E-4</v>
       </c>
       <c r="D3" s="4">
         <f>BNVFE!D25*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.6757085434956571E-4</v>
+        <v>3.5067496258556929E-4</v>
       </c>
       <c r="E3" s="4">
         <f>BNVFE!E25*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.67485043084539E-4</v>
+        <v>3.5195903261955489E-4</v>
       </c>
       <c r="F3" s="4">
         <f>BNVFE!F25*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.6308639538755298E-4</v>
+        <v>3.5537454196456301E-4</v>
       </c>
       <c r="G3" s="4">
         <f>BNVFE!G25*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.3862900642764912E-4</v>
+        <v>3.6001444402488291E-4</v>
       </c>
       <c r="H3" s="4">
         <f>BNVFE!H25*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.3943057282821812E-4</v>
+        <v>3.639117399264578E-4</v>
       </c>
       <c r="I3" s="4">
         <f>BNVFE!I25*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.4041823774591409E-4</v>
+        <v>3.6765602654358315E-4</v>
       </c>
       <c r="J3" s="4">
         <f>BNVFE!J25*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.4252539976387765E-4</v>
+        <v>3.7314346130715945E-4</v>
       </c>
       <c r="K3" s="4">
         <f>BNVFE!K25*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.4460787718934045E-4</v>
+        <v>3.7816127565462235E-4</v>
       </c>
       <c r="L3" s="4">
         <f>BNVFE!L25*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.4765012147470174E-4</v>
+        <v>3.8287720134892478E-4</v>
       </c>
       <c r="M3" s="4">
         <f>BNVFE!M25*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.4968132096095504E-4</v>
+        <v>3.8695589546632644E-4</v>
       </c>
       <c r="N3" s="4">
         <f>BNVFE!N25*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.5249609679543592E-4</v>
+        <v>3.9124659466938441E-4</v>
       </c>
       <c r="O3" s="4">
         <f>BNVFE!O25*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.5536722744245131E-4</v>
+        <v>3.9544274917153121E-4</v>
       </c>
       <c r="P3" s="4">
         <f>BNVFE!P25*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.6148257419113056E-4</v>
+        <v>4.0318106889032553E-4</v>
       </c>
       <c r="Q3" s="4">
         <f>BNVFE!Q25*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.664339997180947E-4</v>
+        <v>4.0934602784305208E-4</v>
       </c>
       <c r="R3" s="4">
         <f>BNVFE!R25*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.7106858296827262E-4</v>
+        <v>4.1460859761082873E-4</v>
       </c>
       <c r="S3" s="4">
         <f>BNVFE!S25*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.8411030958242069E-4</v>
+        <v>4.2918095492519738E-4</v>
       </c>
       <c r="T3" s="4">
         <f>BNVFE!T25*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.8812122876113119E-4</v>
+        <v>4.335787303895307E-4</v>
       </c>
       <c r="U3" s="4">
         <f>BNVFE!U25*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.9150340258291803E-4</v>
+        <v>4.3685345470599412E-4</v>
       </c>
       <c r="V3" s="4">
         <f>BNVFE!V25*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>4.03112372133042E-4</v>
+        <v>4.4986152668336464E-4</v>
       </c>
       <c r="W3" s="4">
         <f>BNVFE!W25*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.0360787000657248E-4</v>
+        <v>4.506125079279828E-4</v>
       </c>
       <c r="X3" s="4">
         <f>BNVFE!X25*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.0382283711848821E-4</v>
+        <v>4.5077860462753374E-4</v>
       </c>
       <c r="Y3" s="4">
         <f>BNVFE!Y25*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.0343001609921412E-4</v>
+        <v>4.5037480829452432E-4</v>
       </c>
       <c r="Z3" s="4">
         <f>BNVFE!Z25*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.0399408750656777E-4</v>
+        <v>4.5090752346333351E-4</v>
       </c>
       <c r="AA3" s="4">
         <f>BNVFE!AA25*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.0250398522270639E-4</v>
+        <v>4.5088043127990992E-4</v>
       </c>
       <c r="AB3" s="4">
         <f>BNVFE!AB25*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.0381262204317188E-4</v>
+        <v>4.5210293408135845E-4</v>
       </c>
       <c r="AC3" s="4">
         <f>BNVFE!AC25*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.0464211986551089E-4</v>
+        <v>4.5305688916845286E-4</v>
       </c>
       <c r="AD3" s="4">
         <f>BNVFE!AD25*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.061398198412998E-4</v>
+        <v>4.5475075705116326E-4</v>
       </c>
       <c r="AE3" s="4">
         <f>BNVFE!AE25*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.0676965949352643E-4</v>
+        <v>4.5558862387767087E-4</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -23220,123 +23220,123 @@
       </c>
       <c r="B5" s="4">
         <f>BNVFE!B27*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.5912817045549592E-4</v>
+        <v>3.3512581471667653E-4</v>
       </c>
       <c r="C5" s="4">
         <f>BNVFE!C27*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.5970216623752401E-4</v>
+        <v>3.4245229349232932E-4</v>
       </c>
       <c r="D5" s="4">
         <f>BNVFE!D27*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.6064678940271876E-4</v>
+        <v>3.4406917165453311E-4</v>
       </c>
       <c r="E5" s="4">
         <f>BNVFE!E27*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.6227954259795134E-4</v>
+        <v>3.4697346123362365E-4</v>
       </c>
       <c r="F5" s="4">
         <f>BNVFE!F27*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.5631282112271915E-4</v>
+        <v>3.4874483652143026E-4</v>
       </c>
       <c r="G5" s="4">
         <f>BNVFE!G27*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.3269354930339661E-4</v>
+        <v>3.5370414497766343E-4</v>
       </c>
       <c r="H5" s="4">
         <f>BNVFE!H27*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.3343282619064117E-4</v>
+        <v>3.5748141045927891E-4</v>
       </c>
       <c r="I5" s="4">
         <f>BNVFE!I27*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.3100920978231121E-4</v>
+        <v>3.5749415666950872E-4</v>
       </c>
       <c r="J5" s="4">
         <f>BNVFE!J27*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.326234964208629E-4</v>
+        <v>3.6235643503264504E-4</v>
       </c>
       <c r="K5" s="4">
         <f>BNVFE!K27*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.3488185734666483E-4</v>
+        <v>3.6748826347409249E-4</v>
       </c>
       <c r="L5" s="4">
         <f>BNVFE!L27*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.387132764367971E-4</v>
+        <v>3.7303479369352893E-4</v>
       </c>
       <c r="M5" s="4">
         <f>BNVFE!M27*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.4169349530148885E-4</v>
+        <v>3.7811660081257293E-4</v>
       </c>
       <c r="N5" s="4">
         <f>BNVFE!N27*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.4543859732872489E-4</v>
+        <v>3.8341325223429322E-4</v>
       </c>
       <c r="O5" s="4">
         <f>BNVFE!O27*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.4914837213574049E-4</v>
+        <v>3.8852258026095287E-4</v>
       </c>
       <c r="P5" s="4">
         <f>BNVFE!P27*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.5586083055954025E-4</v>
+        <v>3.9691083411764322E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>BNVFE!Q27*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.6129198091988776E-4</v>
+        <v>4.0360184206400415E-4</v>
       </c>
       <c r="R5" s="4">
         <f>BNVFE!R27*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.6638008253103504E-4</v>
+        <v>4.0936996335181616E-4</v>
       </c>
       <c r="S5" s="4">
         <f>BNVFE!S27*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.797656838426424E-4</v>
+        <v>4.2432654051018792E-4</v>
       </c>
       <c r="T5" s="4">
         <f>BNVFE!T27*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.8379386561392104E-4</v>
+        <v>4.2874453818290829E-4</v>
       </c>
       <c r="U5" s="4">
         <f>BNVFE!U27*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.8757523740699085E-4</v>
+        <v>4.3247026795349556E-4</v>
       </c>
       <c r="V5" s="4">
         <f>BNVFE!V27*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.9950134420415153E-4</v>
+        <v>4.4583172593973757E-4</v>
       </c>
       <c r="W5" s="4">
         <f>BNVFE!W27*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>4.0035850605750056E-4</v>
+        <v>4.4698471930671959E-4</v>
       </c>
       <c r="X5" s="4">
         <f>BNVFE!X27*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>4.0109394743594799E-4</v>
+        <v>4.4773240473439335E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>BNVFE!Y27*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>4.012761936991058E-4</v>
+        <v>4.4797035817470312E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>BNVFE!Z27*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>4.0222683786844709E-4</v>
+        <v>4.4893505361214171E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>BNVFE!AA27*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>4.0134683501182901E-4</v>
+        <v>4.4958420464541509E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>BNVFE!AB27*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>4.0302096346638407E-4</v>
+        <v>4.5121660426941369E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>BNVFE!AC27*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>4.0423921136844502E-4</v>
+        <v>4.5260577332722303E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>BNVFE!AD27*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>4.0550880062563649E-4</v>
+        <v>4.5404421104897877E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>BNVFE!AE27*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>4.0641720967975257E-4</v>
+        <v>4.5519387436306075E-4</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -23347,123 +23347,123 @@
       </c>
       <c r="B6" s="4">
         <f>BNVFE!B28*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>5.8145858873744711E-4</v>
+        <v>5.4259676434598647E-4</v>
       </c>
       <c r="C6" s="4">
         <f>BNVFE!C28*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>5.2354948444348316E-4</v>
+        <v>4.9844215168280475E-4</v>
       </c>
       <c r="D6" s="4">
         <f>BNVFE!D28*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>5.1809592960240015E-4</v>
+        <v>4.9428094904465346E-4</v>
       </c>
       <c r="E6" s="4">
         <f>BNVFE!E28*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>5.2773804503500592E-4</v>
+        <v>5.0544144667222896E-4</v>
       </c>
       <c r="F6" s="4">
         <f>BNVFE!F28*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>5.2469222599488079E-4</v>
+        <v>5.1354790995754805E-4</v>
       </c>
       <c r="G6" s="4">
         <f>BNVFE!G28*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>4.9246510878464057E-4</v>
+        <v>5.235657577332682E-4</v>
       </c>
       <c r="H6" s="4">
         <f>BNVFE!H28*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>4.9734142906827569E-4</v>
+        <v>5.332117943345761E-4</v>
       </c>
       <c r="I6" s="4">
         <f>BNVFE!I28*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>4.9864550056494565E-4</v>
+        <v>5.3854348287996328E-4</v>
       </c>
       <c r="J6" s="4">
         <f>BNVFE!J28*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>5.0309879253892425E-4</v>
+        <v>5.480703765526247E-4</v>
       </c>
       <c r="K6" s="4">
         <f>BNVFE!K28*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>5.0894929277128537E-4</v>
+        <v>5.5850410433932053E-4</v>
       </c>
       <c r="L6" s="4">
         <f>BNVFE!L28*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>5.1466999519847565E-4</v>
+        <v>5.6682105141791681E-4</v>
       </c>
       <c r="M6" s="4">
         <f>BNVFE!M28*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>5.2012988435178866E-4</v>
+        <v>5.7557356682662623E-4</v>
       </c>
       <c r="N6" s="4">
         <f>BNVFE!N28*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>5.2623775444660776E-4</v>
+        <v>5.8408796944263018E-4</v>
       </c>
       <c r="O6" s="4">
         <f>BNVFE!O28*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>5.3255139284003441E-4</v>
+        <v>5.9260835157877673E-4</v>
       </c>
       <c r="P6" s="4">
         <f>BNVFE!P28*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>5.4302083063339991E-4</v>
+        <v>6.0566050635881105E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>BNVFE!Q28*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>5.522766833965494E-4</v>
+        <v>6.1695221183796919E-4</v>
       </c>
       <c r="R6" s="4">
         <f>BNVFE!R28*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>5.601254580107081E-4</v>
+        <v>6.2584880879500203E-4</v>
       </c>
       <c r="S6" s="4">
         <f>BNVFE!S28*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>5.807089207832928E-4</v>
+        <v>6.4884800781915975E-4</v>
       </c>
       <c r="T6" s="4">
         <f>BNVFE!T28*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>5.8731627063682789E-4</v>
+        <v>6.5610387706092899E-4</v>
       </c>
       <c r="U6" s="4">
         <f>BNVFE!U28*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>5.931554855531328E-4</v>
+        <v>6.6186403829994044E-4</v>
       </c>
       <c r="V6" s="4">
         <f>BNVFE!V28*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>6.1114222360517459E-4</v>
+        <v>6.8201670982440869E-4</v>
       </c>
       <c r="W6" s="4">
         <f>BNVFE!W28*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>6.1263586196471168E-4</v>
+        <v>6.8398414084949516E-4</v>
       </c>
       <c r="X6" s="4">
         <f>BNVFE!X28*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>6.1341880221425316E-4</v>
+        <v>6.847459982390736E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>BNVFE!Y28*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>6.1418182638870312E-4</v>
+        <v>6.8565057452186899E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>BNVFE!Z28*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>6.1565016430071618E-4</v>
+        <v>6.8714196442322276E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>BNVFE!AA28*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>6.1529793989050126E-4</v>
+        <v>6.892498228308697E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>BNVFE!AB28*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>6.1772279652446511E-4</v>
+        <v>6.9159375787861133E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>BNVFE!AC28*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>6.2010047833741867E-4</v>
+        <v>6.942944886231706E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>BNVFE!AD28*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>6.2160289507864192E-4</v>
+        <v>6.9600264074737327E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>BNVFE!AE28*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>6.234661580070439E-4</v>
+        <v>6.98292220994049E-4</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -23474,123 +23474,123 @@
       </c>
       <c r="B7" s="4">
         <f>BNVFE!B29*('BHNVFEAL-LDVs-psgr'!B$4/BNVFE!B$26)</f>
-        <v>3.1989984330977049E-4</v>
+        <v>2.9851931548825495E-4</v>
       </c>
       <c r="C7" s="4">
         <f>BNVFE!C29*('BHNVFEAL-LDVs-psgr'!C$4/BNVFE!C$26)</f>
-        <v>3.1103223181211821E-4</v>
+        <v>2.9611637385514933E-4</v>
       </c>
       <c r="D7" s="4">
         <f>BNVFE!D29*('BHNVFEAL-LDVs-psgr'!D$4/BNVFE!D$26)</f>
-        <v>3.2351966813477334E-4</v>
+        <v>3.0864864876083039E-4</v>
       </c>
       <c r="E7" s="4">
         <f>BNVFE!E29*('BHNVFEAL-LDVs-psgr'!E$4/BNVFE!E$26)</f>
-        <v>3.2622525200054595E-4</v>
+        <v>3.1244244159283816E-4</v>
       </c>
       <c r="F7" s="4">
         <f>BNVFE!F29*('BHNVFEAL-LDVs-psgr'!F$4/BNVFE!F$26)</f>
-        <v>3.2267122446555342E-4</v>
+        <v>3.1581777796216959E-4</v>
       </c>
       <c r="G7" s="4">
         <f>BNVFE!G29*('BHNVFEAL-LDVs-psgr'!G$4/BNVFE!G$26)</f>
-        <v>3.0337057242480451E-4</v>
+        <v>3.2252933414421414E-4</v>
       </c>
       <c r="H7" s="4">
         <f>BNVFE!H29*('BHNVFEAL-LDVs-psgr'!H$4/BNVFE!H$26)</f>
-        <v>3.0453845169467914E-4</v>
+        <v>3.2650305158812983E-4</v>
       </c>
       <c r="I7" s="4">
         <f>BNVFE!I29*('BHNVFEAL-LDVs-psgr'!I$4/BNVFE!I$26)</f>
-        <v>3.0540505504212268E-4</v>
+        <v>3.298413438909791E-4</v>
       </c>
       <c r="J7" s="4">
         <f>BNVFE!J29*('BHNVFEAL-LDVs-psgr'!J$4/BNVFE!J$26)</f>
-        <v>3.0721631066429536E-4</v>
+        <v>3.3467812200296891E-4</v>
       </c>
       <c r="K7" s="4">
         <f>BNVFE!K29*('BHNVFEAL-LDVs-psgr'!K$4/BNVFE!K$26)</f>
-        <v>3.093486028050069E-4</v>
+        <v>3.3946891525767797E-4</v>
       </c>
       <c r="L7" s="4">
         <f>BNVFE!L29*('BHNVFEAL-LDVs-psgr'!L$4/BNVFE!L$26)</f>
-        <v>3.1266127073803886E-4</v>
+        <v>3.443429612582203E-4</v>
       </c>
       <c r="M7" s="4">
         <f>BNVFE!M29*('BHNVFEAL-LDVs-psgr'!M$4/BNVFE!M$26)</f>
-        <v>3.1541166444595039E-4</v>
+        <v>3.4903323609280015E-4</v>
       </c>
       <c r="N7" s="4">
         <f>BNVFE!N29*('BHNVFEAL-LDVs-psgr'!N$4/BNVFE!N$26)</f>
-        <v>3.1892634075550175E-4</v>
+        <v>3.5398645802132289E-4</v>
       </c>
       <c r="O7" s="4">
         <f>BNVFE!O29*('BHNVFEAL-LDVs-psgr'!O$4/BNVFE!O$26)</f>
-        <v>3.2243546366012341E-4</v>
+        <v>3.5879720000574574E-4</v>
       </c>
       <c r="P7" s="4">
         <f>BNVFE!P29*('BHNVFEAL-LDVs-psgr'!P$4/BNVFE!P$26)</f>
-        <v>3.2850767173068688E-4</v>
+        <v>3.6640237644490118E-4</v>
       </c>
       <c r="Q7" s="4">
         <f>BNVFE!Q29*('BHNVFEAL-LDVs-psgr'!Q$4/BNVFE!Q$26)</f>
-        <v>3.3335716351672539E-4</v>
+        <v>3.7239565881871939E-4</v>
       </c>
       <c r="R7" s="4">
         <f>BNVFE!R29*('BHNVFEAL-LDVs-psgr'!R$4/BNVFE!R$26)</f>
-        <v>3.3778444703873312E-4</v>
+        <v>3.774190063766538E-4</v>
       </c>
       <c r="S7" s="4">
         <f>BNVFE!S29*('BHNVFEAL-LDVs-psgr'!S$4/BNVFE!S$26)</f>
-        <v>3.4986487595933905E-4</v>
+        <v>3.9091723865015179E-4</v>
       </c>
       <c r="T7" s="4">
         <f>BNVFE!T29*('BHNVFEAL-LDVs-psgr'!T$4/BNVFE!T$26)</f>
-        <v>3.534107056332161E-4</v>
+        <v>3.9480284431652184E-4</v>
       </c>
       <c r="U7" s="4">
         <f>BNVFE!U29*('BHNVFEAL-LDVs-psgr'!U$4/BNVFE!U$26)</f>
-        <v>3.5662399303793859E-4</v>
+        <v>3.9793376599498131E-4</v>
       </c>
       <c r="V7" s="4">
         <f>BNVFE!V29*('BHNVFEAL-LDVs-psgr'!V$4/BNVFE!V$26)</f>
-        <v>3.6721085010863982E-4</v>
+        <v>4.0979648620174003E-4</v>
       </c>
       <c r="W7" s="4">
         <f>BNVFE!W29*('BHNVFEAL-LDVs-psgr'!W$4/BNVFE!W$26)</f>
-        <v>3.6762499919934348E-4</v>
+        <v>4.1043903049645998E-4</v>
       </c>
       <c r="X7" s="4">
         <f>BNVFE!X29*('BHNVFEAL-LDVs-psgr'!X$4/BNVFE!X$26)</f>
-        <v>3.6773337479207668E-4</v>
+        <v>4.1049272682690713E-4</v>
       </c>
       <c r="Y7" s="4">
         <f>BNVFE!Y29*('BHNVFEAL-LDVs-psgr'!Y$4/BNVFE!Y$26)</f>
-        <v>3.6736921672179983E-4</v>
+        <v>4.1011782453415828E-4</v>
       </c>
       <c r="Z7" s="4">
         <f>BNVFE!Z29*('BHNVFEAL-LDVs-psgr'!Z$4/BNVFE!Z$26)</f>
-        <v>3.6772730994967127E-4</v>
+        <v>4.1042930024698523E-4</v>
       </c>
       <c r="AA7" s="4">
         <f>BNVFE!AA29*('BHNVFEAL-LDVs-psgr'!AA$4/BNVFE!AA$26)</f>
-        <v>3.6618194153426438E-4</v>
+        <v>4.1019288699596694E-4</v>
       </c>
       <c r="AB7" s="4">
         <f>BNVFE!AB29*('BHNVFEAL-LDVs-psgr'!AB$4/BNVFE!AB$26)</f>
-        <v>3.6737880391439015E-4</v>
+        <v>4.1131214355959064E-4</v>
       </c>
       <c r="AC7" s="4">
         <f>BNVFE!AC29*('BHNVFEAL-LDVs-psgr'!AC$4/BNVFE!AC$26)</f>
-        <v>3.6808897076111757E-4</v>
+        <v>4.1213021542511836E-4</v>
       </c>
       <c r="AD7" s="4">
         <f>BNVFE!AD29*('BHNVFEAL-LDVs-psgr'!AD$4/BNVFE!AD$26)</f>
-        <v>3.6878469932448562E-4</v>
+        <v>4.1292459644126167E-4</v>
       </c>
       <c r="AE7" s="4">
         <f>BNVFE!AE29*('BHNVFEAL-LDVs-psgr'!AE$4/BNVFE!AE$26)</f>
-        <v>3.6920309090080676E-4</v>
+        <v>4.135134570368764E-4</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>

</xml_diff>